<commit_message>
Up lai file tesst case
</commit_message>
<xml_diff>
--- a/TestCase-Reup.xlsx
+++ b/TestCase-Reup.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="634">
   <si>
     <t>ID</t>
   </si>
@@ -2627,15 +2627,6 @@
   </si>
   <si>
     <t>Actual results</t>
-  </si>
-  <si>
-    <t>ádafsafsdfaE</t>
-  </si>
-  <si>
-    <t>Tên : Nguyễn Thành Duy</t>
-  </si>
-  <si>
-    <t>sdasdahskvhas</t>
   </si>
 </sst>
 </file>
@@ -2939,6 +2930,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2957,6 +2957,30 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2974,39 +2998,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3375,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3415,20 +3406,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E7" s="4" t="s">
-        <v>635</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>636</v>
-      </c>
-    </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
@@ -3446,11 +3429,11 @@
       <c r="F14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
@@ -3514,15 +3497,13 @@
         <v>6</v>
       </c>
       <c r="J16" s="8"/>
-      <c r="K16" s="8" t="s">
-        <v>634</v>
-      </c>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>2</v>
       </c>
-      <c r="B17" s="53"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="26" t="s">
         <v>23</v>
       </c>
@@ -3551,7 +3532,7 @@
       <c r="A18" s="22">
         <v>3</v>
       </c>
-      <c r="B18" s="53"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="26" t="s">
         <v>27</v>
       </c>
@@ -3580,7 +3561,7 @@
       <c r="A19" s="22">
         <v>4</v>
       </c>
-      <c r="B19" s="53"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="26" t="s">
         <v>23</v>
       </c>
@@ -3609,7 +3590,7 @@
       <c r="A20" s="22">
         <v>5</v>
       </c>
-      <c r="B20" s="53"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="26" t="s">
         <v>54</v>
       </c>
@@ -3638,7 +3619,7 @@
       <c r="A21" s="22">
         <v>6</v>
       </c>
-      <c r="B21" s="54"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="26" t="s">
         <v>59</v>
       </c>
@@ -3668,7 +3649,7 @@
       <c r="B22" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="43" t="s">
         <v>71</v>
       </c>
       <c r="D22" s="10" t="s">
@@ -3694,8 +3675,8 @@
       <c r="A23" s="22">
         <v>8</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="10" t="s">
         <v>65</v>
       </c>
@@ -3719,8 +3700,8 @@
       <c r="A24" s="22">
         <v>9</v>
       </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="40" t="s">
+      <c r="B24" s="50"/>
+      <c r="C24" s="43" t="s">
         <v>70</v>
       </c>
       <c r="D24" s="10" t="s">
@@ -3746,8 +3727,8 @@
       <c r="A25" s="22">
         <v>10</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="42"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="45"/>
       <c r="D25" s="10" t="s">
         <v>65</v>
       </c>
@@ -3771,7 +3752,7 @@
       <c r="A26" s="22">
         <v>11</v>
       </c>
-      <c r="B26" s="53"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="26" t="s">
         <v>72</v>
       </c>
@@ -3798,7 +3779,7 @@
       <c r="A27" s="22">
         <v>12</v>
       </c>
-      <c r="B27" s="53"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="26" t="s">
         <v>73</v>
       </c>
@@ -3825,7 +3806,7 @@
       <c r="A28" s="22">
         <v>13</v>
       </c>
-      <c r="B28" s="53"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="26" t="s">
         <v>74</v>
       </c>
@@ -3852,7 +3833,7 @@
       <c r="A29" s="22">
         <v>14</v>
       </c>
-      <c r="B29" s="53"/>
+      <c r="B29" s="50"/>
       <c r="C29" s="26" t="s">
         <v>76</v>
       </c>
@@ -3879,7 +3860,7 @@
       <c r="A30" s="22">
         <v>15</v>
       </c>
-      <c r="B30" s="53"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="26" t="s">
         <v>78</v>
       </c>
@@ -3908,7 +3889,7 @@
       <c r="A31" s="22">
         <v>16</v>
       </c>
-      <c r="B31" s="53"/>
+      <c r="B31" s="50"/>
       <c r="C31" s="26" t="s">
         <v>79</v>
       </c>
@@ -3937,7 +3918,7 @@
       <c r="A32" s="22">
         <v>17</v>
       </c>
-      <c r="B32" s="53"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="26" t="s">
         <v>79</v>
       </c>
@@ -3966,7 +3947,7 @@
       <c r="A33" s="22">
         <v>18</v>
       </c>
-      <c r="B33" s="53"/>
+      <c r="B33" s="50"/>
       <c r="C33" s="26" t="s">
         <v>84</v>
       </c>
@@ -3993,7 +3974,7 @@
       <c r="A34" s="22">
         <v>19</v>
       </c>
-      <c r="B34" s="53"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="26" t="s">
         <v>85</v>
       </c>
@@ -4020,7 +4001,7 @@
       <c r="A35" s="22">
         <v>20</v>
       </c>
-      <c r="B35" s="53"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="26" t="s">
         <v>88</v>
       </c>
@@ -4047,7 +4028,7 @@
       <c r="A36" s="22">
         <v>21</v>
       </c>
-      <c r="B36" s="54"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="26" t="s">
         <v>88</v>
       </c>
@@ -4103,7 +4084,7 @@
       <c r="A38" s="22">
         <v>23</v>
       </c>
-      <c r="B38" s="53"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="26" t="s">
         <v>94</v>
       </c>
@@ -4132,7 +4113,7 @@
       <c r="A39" s="22">
         <v>24</v>
       </c>
-      <c r="B39" s="53"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="26" t="s">
         <v>99</v>
       </c>
@@ -4161,7 +4142,7 @@
       <c r="A40" s="22">
         <v>25</v>
       </c>
-      <c r="B40" s="53"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="26" t="s">
         <v>100</v>
       </c>
@@ -4192,7 +4173,7 @@
       <c r="A41" s="22">
         <v>26</v>
       </c>
-      <c r="B41" s="53"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="26" t="s">
         <v>103</v>
       </c>
@@ -4223,7 +4204,7 @@
       <c r="A42" s="22">
         <v>27</v>
       </c>
-      <c r="B42" s="53"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="26" t="s">
         <v>105</v>
       </c>
@@ -4252,7 +4233,7 @@
       <c r="A43" s="22">
         <v>28</v>
       </c>
-      <c r="B43" s="54"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="26" t="s">
         <v>108</v>
       </c>
@@ -4312,7 +4293,7 @@
       <c r="A45" s="22">
         <v>30</v>
       </c>
-      <c r="B45" s="53"/>
+      <c r="B45" s="50"/>
       <c r="C45" s="26" t="s">
         <v>113</v>
       </c>
@@ -4341,7 +4322,7 @@
       <c r="A46" s="22">
         <v>31</v>
       </c>
-      <c r="B46" s="53"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="26" t="s">
         <v>94</v>
       </c>
@@ -4370,7 +4351,7 @@
       <c r="A47" s="22">
         <v>32</v>
       </c>
-      <c r="B47" s="53"/>
+      <c r="B47" s="50"/>
       <c r="C47" s="26" t="s">
         <v>99</v>
       </c>
@@ -4399,7 +4380,7 @@
       <c r="A48" s="22">
         <v>33</v>
       </c>
-      <c r="B48" s="53"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="26" t="s">
         <v>116</v>
       </c>
@@ -4428,7 +4409,7 @@
       <c r="A49" s="22">
         <v>34</v>
       </c>
-      <c r="B49" s="54"/>
+      <c r="B49" s="51"/>
       <c r="C49" s="26" t="s">
         <v>117</v>
       </c>
@@ -4457,7 +4438,7 @@
       <c r="A50" s="22">
         <v>35</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="57" t="s">
         <v>123</v>
       </c>
       <c r="C50" s="26" t="s">
@@ -4486,7 +4467,7 @@
       <c r="A51" s="22">
         <v>36</v>
       </c>
-      <c r="B51" s="47"/>
+      <c r="B51" s="58"/>
       <c r="C51" s="26" t="s">
         <v>94</v>
       </c>
@@ -4515,7 +4496,7 @@
       <c r="A52" s="22">
         <v>37</v>
       </c>
-      <c r="B52" s="48"/>
+      <c r="B52" s="59"/>
       <c r="C52" s="26" t="s">
         <v>99</v>
       </c>
@@ -4571,7 +4552,7 @@
       <c r="A54" s="22">
         <v>39</v>
       </c>
-      <c r="B54" s="53"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="26" t="s">
         <v>94</v>
       </c>
@@ -4600,7 +4581,7 @@
       <c r="A55" s="22">
         <v>40</v>
       </c>
-      <c r="B55" s="53"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="26" t="s">
         <v>99</v>
       </c>
@@ -4629,7 +4610,7 @@
       <c r="A56" s="22">
         <v>41</v>
       </c>
-      <c r="B56" s="53"/>
+      <c r="B56" s="50"/>
       <c r="C56" s="26" t="s">
         <v>99</v>
       </c>
@@ -4658,7 +4639,7 @@
       <c r="A57" s="22">
         <v>42</v>
       </c>
-      <c r="B57" s="54"/>
+      <c r="B57" s="51"/>
       <c r="C57" s="26" t="s">
         <v>99</v>
       </c>
@@ -4717,10 +4698,10 @@
       <c r="A60" s="22">
         <v>45</v>
       </c>
-      <c r="B60" s="55" t="s">
+      <c r="B60" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="56" t="s">
+      <c r="C60" s="54" t="s">
         <v>21</v>
       </c>
       <c r="D60" s="10" t="s">
@@ -4746,8 +4727,8 @@
       <c r="A61" s="22">
         <v>46</v>
       </c>
-      <c r="B61" s="55"/>
-      <c r="C61" s="56"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="54"/>
       <c r="D61" s="10" t="s">
         <v>36</v>
       </c>
@@ -4771,8 +4752,8 @@
       <c r="A62" s="22">
         <v>47</v>
       </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="56"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="54"/>
       <c r="D62" s="10" t="s">
         <v>35</v>
       </c>
@@ -4796,8 +4777,8 @@
       <c r="A63" s="22">
         <v>48</v>
       </c>
-      <c r="B63" s="55"/>
-      <c r="C63" s="56"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="54"/>
       <c r="D63" s="10" t="s">
         <v>34</v>
       </c>
@@ -4821,8 +4802,8 @@
       <c r="A64" s="22">
         <v>49</v>
       </c>
-      <c r="B64" s="55"/>
-      <c r="C64" s="56"/>
+      <c r="B64" s="53"/>
+      <c r="C64" s="54"/>
       <c r="D64" s="10" t="s">
         <v>33</v>
       </c>
@@ -4846,10 +4827,10 @@
       <c r="A65" s="22">
         <v>50</v>
       </c>
-      <c r="B65" s="55" t="s">
+      <c r="B65" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="54" t="s">
         <v>145</v>
       </c>
       <c r="D65" s="10" t="s">
@@ -4875,8 +4856,8 @@
       <c r="A66" s="22">
         <v>51</v>
       </c>
-      <c r="B66" s="55"/>
-      <c r="C66" s="56"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
       <c r="D66" s="10" t="s">
         <v>148</v>
       </c>
@@ -4900,8 +4881,8 @@
       <c r="A67" s="22">
         <v>52</v>
       </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="56"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="54"/>
       <c r="D67" s="10" t="s">
         <v>150</v>
       </c>
@@ -4927,8 +4908,8 @@
       <c r="A68" s="22">
         <v>53</v>
       </c>
-      <c r="B68" s="55"/>
-      <c r="C68" s="56"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="54"/>
       <c r="D68" s="10" t="s">
         <v>153</v>
       </c>
@@ -4954,8 +4935,8 @@
       <c r="A69" s="22">
         <v>54</v>
       </c>
-      <c r="B69" s="55"/>
-      <c r="C69" s="56"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="54"/>
       <c r="D69" s="10" t="s">
         <v>156</v>
       </c>
@@ -4981,8 +4962,8 @@
       <c r="A70" s="22">
         <v>55</v>
       </c>
-      <c r="B70" s="55"/>
-      <c r="C70" s="56"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="54"/>
       <c r="D70" s="10" t="s">
         <v>159</v>
       </c>
@@ -5008,8 +4989,8 @@
       <c r="A71" s="22">
         <v>56</v>
       </c>
-      <c r="B71" s="55"/>
-      <c r="C71" s="56" t="s">
+      <c r="B71" s="53"/>
+      <c r="C71" s="54" t="s">
         <v>160</v>
       </c>
       <c r="D71" s="10" t="s">
@@ -5035,8 +5016,8 @@
       <c r="A72" s="22">
         <v>57</v>
       </c>
-      <c r="B72" s="55"/>
-      <c r="C72" s="56"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="54"/>
       <c r="D72" s="10" t="s">
         <v>162</v>
       </c>
@@ -5060,8 +5041,8 @@
       <c r="A73" s="22">
         <v>58</v>
       </c>
-      <c r="B73" s="55"/>
-      <c r="C73" s="56"/>
+      <c r="B73" s="53"/>
+      <c r="C73" s="54"/>
       <c r="D73" s="10" t="s">
         <v>164</v>
       </c>
@@ -5085,8 +5066,8 @@
       <c r="A74" s="22">
         <v>59</v>
       </c>
-      <c r="B74" s="55"/>
-      <c r="C74" s="56"/>
+      <c r="B74" s="53"/>
+      <c r="C74" s="54"/>
       <c r="D74" s="10" t="s">
         <v>166</v>
       </c>
@@ -5110,8 +5091,8 @@
       <c r="A75" s="22">
         <v>60</v>
       </c>
-      <c r="B75" s="55"/>
-      <c r="C75" s="56"/>
+      <c r="B75" s="53"/>
+      <c r="C75" s="54"/>
       <c r="D75" s="10" t="s">
         <v>168</v>
       </c>
@@ -5135,8 +5116,8 @@
       <c r="A76" s="22">
         <v>61</v>
       </c>
-      <c r="B76" s="55"/>
-      <c r="C76" s="56"/>
+      <c r="B76" s="53"/>
+      <c r="C76" s="54"/>
       <c r="D76" s="10" t="s">
         <v>170</v>
       </c>
@@ -5160,7 +5141,7 @@
       <c r="A77" s="22">
         <v>62</v>
       </c>
-      <c r="B77" s="55"/>
+      <c r="B77" s="53"/>
       <c r="C77" s="26" t="s">
         <v>172</v>
       </c>
@@ -5187,8 +5168,8 @@
       <c r="A78" s="22">
         <v>63</v>
       </c>
-      <c r="B78" s="55"/>
-      <c r="C78" s="56" t="s">
+      <c r="B78" s="53"/>
+      <c r="C78" s="54" t="s">
         <v>174</v>
       </c>
       <c r="D78" s="10" t="s">
@@ -5214,8 +5195,8 @@
       <c r="A79" s="22">
         <v>64</v>
       </c>
-      <c r="B79" s="55"/>
-      <c r="C79" s="56"/>
+      <c r="B79" s="53"/>
+      <c r="C79" s="54"/>
       <c r="D79" s="10" t="s">
         <v>42</v>
       </c>
@@ -5239,8 +5220,8 @@
       <c r="A80" s="22">
         <v>65</v>
       </c>
-      <c r="B80" s="55"/>
-      <c r="C80" s="56"/>
+      <c r="B80" s="53"/>
+      <c r="C80" s="54"/>
       <c r="D80" s="10" t="s">
         <v>44</v>
       </c>
@@ -5264,7 +5245,7 @@
       <c r="A81" s="22">
         <v>66</v>
       </c>
-      <c r="B81" s="55"/>
+      <c r="B81" s="53"/>
       <c r="C81" s="26"/>
       <c r="D81" s="10" t="s">
         <v>175</v>
@@ -5283,10 +5264,10 @@
       <c r="A82" s="22">
         <v>67</v>
       </c>
-      <c r="B82" s="55" t="s">
+      <c r="B82" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C82" s="56" t="s">
+      <c r="C82" s="54" t="s">
         <v>177</v>
       </c>
       <c r="D82" s="10" t="s">
@@ -5314,8 +5295,8 @@
       <c r="A83" s="22">
         <v>68</v>
       </c>
-      <c r="B83" s="55"/>
-      <c r="C83" s="56"/>
+      <c r="B83" s="53"/>
+      <c r="C83" s="54"/>
       <c r="D83" s="10" t="s">
         <v>181</v>
       </c>
@@ -5339,8 +5320,8 @@
       <c r="A84" s="22">
         <v>69</v>
       </c>
-      <c r="B84" s="55"/>
-      <c r="C84" s="56" t="s">
+      <c r="B84" s="53"/>
+      <c r="C84" s="54" t="s">
         <v>183</v>
       </c>
       <c r="D84" s="10" t="s">
@@ -5366,8 +5347,8 @@
       <c r="A85" s="22">
         <v>70</v>
       </c>
-      <c r="B85" s="55"/>
-      <c r="C85" s="56"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="54"/>
       <c r="D85" s="10" t="s">
         <v>186</v>
       </c>
@@ -5391,8 +5372,8 @@
       <c r="A86" s="22">
         <v>71</v>
       </c>
-      <c r="B86" s="55"/>
-      <c r="C86" s="56"/>
+      <c r="B86" s="53"/>
+      <c r="C86" s="54"/>
       <c r="D86" s="10" t="s">
         <v>188</v>
       </c>
@@ -5416,8 +5397,8 @@
       <c r="A87" s="22">
         <v>72</v>
       </c>
-      <c r="B87" s="55"/>
-      <c r="C87" s="56"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="54"/>
       <c r="D87" s="10" t="s">
         <v>190</v>
       </c>
@@ -5441,7 +5422,7 @@
       <c r="A88" s="22">
         <v>73</v>
       </c>
-      <c r="B88" s="55"/>
+      <c r="B88" s="53"/>
       <c r="C88" s="26" t="s">
         <v>172</v>
       </c>
@@ -5468,7 +5449,7 @@
       <c r="A89" s="22">
         <v>74</v>
       </c>
-      <c r="B89" s="55"/>
+      <c r="B89" s="53"/>
       <c r="C89" s="26"/>
       <c r="D89" s="10" t="s">
         <v>175</v>
@@ -5487,10 +5468,10 @@
       <c r="A90" s="22">
         <v>75</v>
       </c>
-      <c r="B90" s="55" t="s">
+      <c r="B90" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="56" t="s">
+      <c r="C90" s="54" t="s">
         <v>177</v>
       </c>
       <c r="D90" s="10" t="s">
@@ -5516,8 +5497,8 @@
       <c r="A91" s="22">
         <v>76</v>
       </c>
-      <c r="B91" s="55"/>
-      <c r="C91" s="56"/>
+      <c r="B91" s="53"/>
+      <c r="C91" s="54"/>
       <c r="D91" s="10" t="s">
         <v>181</v>
       </c>
@@ -5541,8 +5522,8 @@
       <c r="A92" s="22">
         <v>77</v>
       </c>
-      <c r="B92" s="55"/>
-      <c r="C92" s="56" t="s">
+      <c r="B92" s="53"/>
+      <c r="C92" s="54" t="s">
         <v>183</v>
       </c>
       <c r="D92" s="10" t="s">
@@ -5568,8 +5549,8 @@
       <c r="A93" s="22">
         <v>78</v>
       </c>
-      <c r="B93" s="55"/>
-      <c r="C93" s="56"/>
+      <c r="B93" s="53"/>
+      <c r="C93" s="54"/>
       <c r="D93" s="10" t="s">
         <v>186</v>
       </c>
@@ -5593,8 +5574,8 @@
       <c r="A94" s="22">
         <v>79</v>
       </c>
-      <c r="B94" s="55"/>
-      <c r="C94" s="56"/>
+      <c r="B94" s="53"/>
+      <c r="C94" s="54"/>
       <c r="D94" s="10" t="s">
         <v>188</v>
       </c>
@@ -5618,8 +5599,8 @@
       <c r="A95" s="22">
         <v>80</v>
       </c>
-      <c r="B95" s="55"/>
-      <c r="C95" s="56"/>
+      <c r="B95" s="53"/>
+      <c r="C95" s="54"/>
       <c r="D95" s="10" t="s">
         <v>190</v>
       </c>
@@ -5643,7 +5624,7 @@
       <c r="A96" s="22">
         <v>81</v>
       </c>
-      <c r="B96" s="55"/>
+      <c r="B96" s="53"/>
       <c r="C96" s="26" t="s">
         <v>172</v>
       </c>
@@ -5670,7 +5651,7 @@
       <c r="A97" s="22">
         <v>82</v>
       </c>
-      <c r="B97" s="55"/>
+      <c r="B97" s="53"/>
       <c r="C97" s="26"/>
       <c r="D97" s="10" t="s">
         <v>175</v>
@@ -5689,7 +5670,7 @@
       <c r="A98" s="22">
         <v>83</v>
       </c>
-      <c r="B98" s="55" t="s">
+      <c r="B98" s="53" t="s">
         <v>49</v>
       </c>
       <c r="C98" s="26" t="s">
@@ -5718,7 +5699,7 @@
       <c r="A99" s="22">
         <v>84</v>
       </c>
-      <c r="B99" s="55"/>
+      <c r="B99" s="53"/>
       <c r="C99" s="26"/>
       <c r="D99" s="10" t="s">
         <v>175</v>
@@ -5737,7 +5718,7 @@
       <c r="A100" s="22">
         <v>85</v>
       </c>
-      <c r="B100" s="55" t="s">
+      <c r="B100" s="53" t="s">
         <v>196</v>
       </c>
       <c r="C100" s="26" t="s">
@@ -5766,7 +5747,7 @@
       <c r="A101" s="22">
         <v>86</v>
       </c>
-      <c r="B101" s="55"/>
+      <c r="B101" s="53"/>
       <c r="C101" s="26" t="s">
         <v>172</v>
       </c>
@@ -5793,7 +5774,7 @@
       <c r="A102" s="22">
         <v>87</v>
       </c>
-      <c r="B102" s="55"/>
+      <c r="B102" s="53"/>
       <c r="C102" s="26"/>
       <c r="D102" s="10" t="s">
         <v>175</v>
@@ -5812,7 +5793,7 @@
       <c r="A103" s="22">
         <v>88</v>
       </c>
-      <c r="B103" s="55" t="s">
+      <c r="B103" s="53" t="s">
         <v>198</v>
       </c>
       <c r="C103" s="26" t="s">
@@ -5843,7 +5824,7 @@
       <c r="A104" s="22">
         <v>89</v>
       </c>
-      <c r="B104" s="55"/>
+      <c r="B104" s="53"/>
       <c r="C104" s="26" t="s">
         <v>200</v>
       </c>
@@ -5872,8 +5853,8 @@
       <c r="A105" s="22">
         <v>90</v>
       </c>
-      <c r="B105" s="55"/>
-      <c r="C105" s="56" t="s">
+      <c r="B105" s="53"/>
+      <c r="C105" s="54" t="s">
         <v>203</v>
       </c>
       <c r="D105" s="10" t="s">
@@ -5899,8 +5880,8 @@
       <c r="A106" s="22">
         <v>91</v>
       </c>
-      <c r="B106" s="55"/>
-      <c r="C106" s="56"/>
+      <c r="B106" s="53"/>
+      <c r="C106" s="54"/>
       <c r="D106" s="10" t="s">
         <v>206</v>
       </c>
@@ -5924,8 +5905,8 @@
       <c r="A107" s="22">
         <v>92</v>
       </c>
-      <c r="B107" s="55"/>
-      <c r="C107" s="56"/>
+      <c r="B107" s="53"/>
+      <c r="C107" s="54"/>
       <c r="D107" s="10" t="s">
         <v>207</v>
       </c>
@@ -5949,8 +5930,8 @@
       <c r="A108" s="22">
         <v>93</v>
       </c>
-      <c r="B108" s="55"/>
-      <c r="C108" s="56"/>
+      <c r="B108" s="53"/>
+      <c r="C108" s="54"/>
       <c r="D108" s="10" t="s">
         <v>209</v>
       </c>
@@ -5974,7 +5955,7 @@
       <c r="A109" s="22">
         <v>94</v>
       </c>
-      <c r="B109" s="55"/>
+      <c r="B109" s="53"/>
       <c r="C109" s="26" t="s">
         <v>210</v>
       </c>
@@ -6001,7 +5982,7 @@
       <c r="A110" s="22">
         <v>95</v>
       </c>
-      <c r="B110" s="55"/>
+      <c r="B110" s="53"/>
       <c r="C110" s="26"/>
       <c r="D110" s="10" t="s">
         <v>175</v>
@@ -6026,7 +6007,7 @@
       <c r="A111" s="22">
         <v>96</v>
       </c>
-      <c r="B111" s="55" t="s">
+      <c r="B111" s="53" t="s">
         <v>213</v>
       </c>
       <c r="C111" s="26"/>
@@ -6053,7 +6034,7 @@
       <c r="A112" s="22">
         <v>97</v>
       </c>
-      <c r="B112" s="55"/>
+      <c r="B112" s="53"/>
       <c r="C112" s="26"/>
       <c r="D112" s="10" t="s">
         <v>216</v>
@@ -6078,7 +6059,7 @@
       <c r="A113" s="22">
         <v>98</v>
       </c>
-      <c r="B113" s="55"/>
+      <c r="B113" s="53"/>
       <c r="C113" s="26"/>
       <c r="D113" s="10" t="s">
         <v>218</v>
@@ -6103,7 +6084,7 @@
       <c r="A114" s="22">
         <v>99</v>
       </c>
-      <c r="B114" s="55"/>
+      <c r="B114" s="53"/>
       <c r="C114" s="26"/>
       <c r="D114" s="10" t="s">
         <v>220</v>
@@ -6128,7 +6109,7 @@
       <c r="A115" s="22">
         <v>100</v>
       </c>
-      <c r="B115" s="55" t="s">
+      <c r="B115" s="53" t="s">
         <v>222</v>
       </c>
       <c r="C115" s="26" t="s">
@@ -6157,8 +6138,8 @@
       <c r="A116" s="22">
         <v>101</v>
       </c>
-      <c r="B116" s="55"/>
-      <c r="C116" s="56" t="s">
+      <c r="B116" s="53"/>
+      <c r="C116" s="54" t="s">
         <v>226</v>
       </c>
       <c r="D116" s="10" t="s">
@@ -6184,8 +6165,8 @@
       <c r="A117" s="22">
         <v>102</v>
       </c>
-      <c r="B117" s="55"/>
-      <c r="C117" s="56"/>
+      <c r="B117" s="53"/>
+      <c r="C117" s="54"/>
       <c r="D117" s="10" t="s">
         <v>229</v>
       </c>
@@ -6209,8 +6190,8 @@
       <c r="A118" s="22">
         <v>103</v>
       </c>
-      <c r="B118" s="55"/>
-      <c r="C118" s="56"/>
+      <c r="B118" s="53"/>
+      <c r="C118" s="54"/>
       <c r="D118" s="10" t="s">
         <v>231</v>
       </c>
@@ -6234,8 +6215,8 @@
       <c r="A119" s="22">
         <v>104</v>
       </c>
-      <c r="B119" s="55"/>
-      <c r="C119" s="56"/>
+      <c r="B119" s="53"/>
+      <c r="C119" s="54"/>
       <c r="D119" s="10" t="s">
         <v>233</v>
       </c>
@@ -6259,8 +6240,8 @@
       <c r="A120" s="22">
         <v>105</v>
       </c>
-      <c r="B120" s="55"/>
-      <c r="C120" s="56" t="s">
+      <c r="B120" s="53"/>
+      <c r="C120" s="54" t="s">
         <v>234</v>
       </c>
       <c r="D120" s="10" t="s">
@@ -6286,8 +6267,8 @@
       <c r="A121" s="22">
         <v>106</v>
       </c>
-      <c r="B121" s="55"/>
-      <c r="C121" s="56"/>
+      <c r="B121" s="53"/>
+      <c r="C121" s="54"/>
       <c r="D121" s="10" t="s">
         <v>237</v>
       </c>
@@ -6311,8 +6292,8 @@
       <c r="A122" s="22">
         <v>107</v>
       </c>
-      <c r="B122" s="55"/>
-      <c r="C122" s="56"/>
+      <c r="B122" s="53"/>
+      <c r="C122" s="54"/>
       <c r="D122" s="10" t="s">
         <v>239</v>
       </c>
@@ -6336,8 +6317,8 @@
       <c r="A123" s="22">
         <v>108</v>
       </c>
-      <c r="B123" s="55"/>
-      <c r="C123" s="56"/>
+      <c r="B123" s="53"/>
+      <c r="C123" s="54"/>
       <c r="D123" s="10" t="s">
         <v>240</v>
       </c>
@@ -6361,8 +6342,8 @@
       <c r="A124" s="22">
         <v>109</v>
       </c>
-      <c r="B124" s="55"/>
-      <c r="C124" s="56" t="s">
+      <c r="B124" s="53"/>
+      <c r="C124" s="54" t="s">
         <v>241</v>
       </c>
       <c r="D124" s="10" t="s">
@@ -6388,8 +6369,8 @@
       <c r="A125" s="22">
         <v>110</v>
       </c>
-      <c r="B125" s="55"/>
-      <c r="C125" s="56"/>
+      <c r="B125" s="53"/>
+      <c r="C125" s="54"/>
       <c r="D125" s="10" t="s">
         <v>244</v>
       </c>
@@ -6413,8 +6394,8 @@
       <c r="A126" s="22">
         <v>111</v>
       </c>
-      <c r="B126" s="55"/>
-      <c r="C126" s="56"/>
+      <c r="B126" s="53"/>
+      <c r="C126" s="54"/>
       <c r="D126" s="10" t="s">
         <v>245</v>
       </c>
@@ -6438,8 +6419,8 @@
       <c r="A127" s="22">
         <v>112</v>
       </c>
-      <c r="B127" s="55"/>
-      <c r="C127" s="56" t="s">
+      <c r="B127" s="53"/>
+      <c r="C127" s="54" t="s">
         <v>247</v>
       </c>
       <c r="D127" s="10" t="s">
@@ -6465,8 +6446,8 @@
       <c r="A128" s="22">
         <v>113</v>
       </c>
-      <c r="B128" s="55"/>
-      <c r="C128" s="56"/>
+      <c r="B128" s="53"/>
+      <c r="C128" s="54"/>
       <c r="D128" s="10" t="s">
         <v>250</v>
       </c>
@@ -6490,8 +6471,8 @@
       <c r="A129" s="22">
         <v>114</v>
       </c>
-      <c r="B129" s="55"/>
-      <c r="C129" s="56" t="s">
+      <c r="B129" s="53"/>
+      <c r="C129" s="54" t="s">
         <v>252</v>
       </c>
       <c r="D129" s="10" t="s">
@@ -6517,8 +6498,8 @@
       <c r="A130" s="22">
         <v>115</v>
       </c>
-      <c r="B130" s="55"/>
-      <c r="C130" s="56"/>
+      <c r="B130" s="53"/>
+      <c r="C130" s="54"/>
       <c r="D130" s="10" t="s">
         <v>255</v>
       </c>
@@ -6542,8 +6523,8 @@
       <c r="A131" s="22">
         <v>116</v>
       </c>
-      <c r="B131" s="55"/>
-      <c r="C131" s="56"/>
+      <c r="B131" s="53"/>
+      <c r="C131" s="54"/>
       <c r="D131" s="10" t="s">
         <v>257</v>
       </c>
@@ -6567,7 +6548,7 @@
       <c r="A132" s="22">
         <v>117</v>
       </c>
-      <c r="B132" s="55"/>
+      <c r="B132" s="53"/>
       <c r="C132" s="26"/>
       <c r="D132" s="27" t="s">
         <v>175</v>
@@ -6592,10 +6573,10 @@
       <c r="A133" s="22">
         <v>118</v>
       </c>
-      <c r="B133" s="55" t="s">
+      <c r="B133" s="53" t="s">
         <v>260</v>
       </c>
-      <c r="C133" s="56" t="s">
+      <c r="C133" s="54" t="s">
         <v>261</v>
       </c>
       <c r="D133" s="10" t="s">
@@ -6621,8 +6602,8 @@
       <c r="A134" s="22">
         <v>119</v>
       </c>
-      <c r="B134" s="55"/>
-      <c r="C134" s="56"/>
+      <c r="B134" s="53"/>
+      <c r="C134" s="54"/>
       <c r="D134" s="10" t="s">
         <v>264</v>
       </c>
@@ -6646,8 +6627,8 @@
       <c r="A135" s="22">
         <v>120</v>
       </c>
-      <c r="B135" s="55"/>
-      <c r="C135" s="56" t="s">
+      <c r="B135" s="53"/>
+      <c r="C135" s="54" t="s">
         <v>266</v>
       </c>
       <c r="D135" s="10" t="s">
@@ -6673,8 +6654,8 @@
       <c r="A136" s="22">
         <v>121</v>
       </c>
-      <c r="B136" s="55"/>
-      <c r="C136" s="56"/>
+      <c r="B136" s="53"/>
+      <c r="C136" s="54"/>
       <c r="D136" s="10" t="s">
         <v>269</v>
       </c>
@@ -6698,8 +6679,8 @@
       <c r="A137" s="22">
         <v>122</v>
       </c>
-      <c r="B137" s="55"/>
-      <c r="C137" s="56"/>
+      <c r="B137" s="53"/>
+      <c r="C137" s="54"/>
       <c r="D137" s="10" t="s">
         <v>270</v>
       </c>
@@ -6724,8 +6705,8 @@
       <c r="A138" s="22">
         <v>123</v>
       </c>
-      <c r="B138" s="55"/>
-      <c r="C138" s="56"/>
+      <c r="B138" s="53"/>
+      <c r="C138" s="54"/>
       <c r="D138" s="10" t="s">
         <v>271</v>
       </c>
@@ -6749,8 +6730,8 @@
       <c r="A139" s="22">
         <v>124</v>
       </c>
-      <c r="B139" s="55"/>
-      <c r="C139" s="56"/>
+      <c r="B139" s="53"/>
+      <c r="C139" s="54"/>
       <c r="D139" s="10" t="s">
         <v>272</v>
       </c>
@@ -6774,8 +6755,8 @@
       <c r="A140" s="22">
         <v>125</v>
       </c>
-      <c r="B140" s="55"/>
-      <c r="C140" s="56" t="s">
+      <c r="B140" s="53"/>
+      <c r="C140" s="54" t="s">
         <v>274</v>
       </c>
       <c r="D140" s="10" t="s">
@@ -6801,8 +6782,8 @@
       <c r="A141" s="22">
         <v>126</v>
       </c>
-      <c r="B141" s="55"/>
-      <c r="C141" s="56"/>
+      <c r="B141" s="53"/>
+      <c r="C141" s="54"/>
       <c r="D141" s="10" t="s">
         <v>277</v>
       </c>
@@ -6826,7 +6807,7 @@
       <c r="A142" s="22">
         <v>127</v>
       </c>
-      <c r="B142" s="55"/>
+      <c r="B142" s="53"/>
       <c r="C142" s="26" t="s">
         <v>279</v>
       </c>
@@ -6853,8 +6834,8 @@
       <c r="A143" s="22">
         <v>128</v>
       </c>
-      <c r="B143" s="55"/>
-      <c r="C143" s="56" t="s">
+      <c r="B143" s="53"/>
+      <c r="C143" s="54" t="s">
         <v>282</v>
       </c>
       <c r="D143" s="10" t="s">
@@ -6880,8 +6861,8 @@
       <c r="A144" s="22">
         <v>129</v>
       </c>
-      <c r="B144" s="55"/>
-      <c r="C144" s="56"/>
+      <c r="B144" s="53"/>
+      <c r="C144" s="54"/>
       <c r="D144" s="10" t="s">
         <v>285</v>
       </c>
@@ -6905,8 +6886,8 @@
       <c r="A145" s="22">
         <v>130</v>
       </c>
-      <c r="B145" s="55"/>
-      <c r="C145" s="56"/>
+      <c r="B145" s="53"/>
+      <c r="C145" s="54"/>
       <c r="D145" s="10" t="s">
         <v>287</v>
       </c>
@@ -6930,7 +6911,7 @@
       <c r="A146" s="22">
         <v>131</v>
       </c>
-      <c r="B146" s="55"/>
+      <c r="B146" s="53"/>
       <c r="C146" s="26"/>
       <c r="D146" s="10" t="s">
         <v>175</v>
@@ -6955,10 +6936,10 @@
       <c r="A147" s="22">
         <v>132</v>
       </c>
-      <c r="B147" s="55" t="s">
+      <c r="B147" s="53" t="s">
         <v>289</v>
       </c>
-      <c r="C147" s="56" t="s">
+      <c r="C147" s="54" t="s">
         <v>290</v>
       </c>
       <c r="D147" s="10" t="s">
@@ -6984,8 +6965,8 @@
       <c r="A148" s="22">
         <v>133</v>
       </c>
-      <c r="B148" s="55"/>
-      <c r="C148" s="56"/>
+      <c r="B148" s="53"/>
+      <c r="C148" s="54"/>
       <c r="D148" s="10" t="s">
         <v>293</v>
       </c>
@@ -7009,7 +6990,7 @@
       <c r="A149" s="22">
         <v>134</v>
       </c>
-      <c r="B149" s="55"/>
+      <c r="B149" s="53"/>
       <c r="C149" s="26"/>
       <c r="D149" s="10" t="s">
         <v>175</v>
@@ -7037,7 +7018,7 @@
       <c r="B150" s="52" t="s">
         <v>295</v>
       </c>
-      <c r="C150" s="40" t="s">
+      <c r="C150" s="43" t="s">
         <v>296</v>
       </c>
       <c r="D150" s="10" t="s">
@@ -7063,8 +7044,8 @@
       <c r="A151" s="22">
         <v>136</v>
       </c>
-      <c r="B151" s="53"/>
-      <c r="C151" s="41"/>
+      <c r="B151" s="50"/>
+      <c r="C151" s="44"/>
       <c r="D151" s="10" t="s">
         <v>299</v>
       </c>
@@ -7088,8 +7069,8 @@
       <c r="A152" s="22">
         <v>137</v>
       </c>
-      <c r="B152" s="53"/>
-      <c r="C152" s="41"/>
+      <c r="B152" s="50"/>
+      <c r="C152" s="44"/>
       <c r="D152" s="10" t="s">
         <v>301</v>
       </c>
@@ -7113,8 +7094,8 @@
       <c r="A153" s="22">
         <v>138</v>
       </c>
-      <c r="B153" s="53"/>
-      <c r="C153" s="42"/>
+      <c r="B153" s="50"/>
+      <c r="C153" s="45"/>
       <c r="D153" s="10" t="s">
         <v>303</v>
       </c>
@@ -7138,8 +7119,8 @@
       <c r="A154" s="22">
         <v>139</v>
       </c>
-      <c r="B154" s="53"/>
-      <c r="C154" s="40" t="s">
+      <c r="B154" s="50"/>
+      <c r="C154" s="43" t="s">
         <v>290</v>
       </c>
       <c r="D154" s="10" t="s">
@@ -7165,8 +7146,8 @@
       <c r="A155" s="22">
         <v>140</v>
       </c>
-      <c r="B155" s="53"/>
-      <c r="C155" s="42"/>
+      <c r="B155" s="50"/>
+      <c r="C155" s="45"/>
       <c r="D155" s="10" t="s">
         <v>307</v>
       </c>
@@ -7190,7 +7171,7 @@
       <c r="A156" s="22">
         <v>141</v>
       </c>
-      <c r="B156" s="54"/>
+      <c r="B156" s="51"/>
       <c r="C156" s="26"/>
       <c r="D156" s="10" t="s">
         <v>175</v>
@@ -7244,7 +7225,7 @@
       <c r="A158" s="22">
         <v>143</v>
       </c>
-      <c r="B158" s="53"/>
+      <c r="B158" s="50"/>
       <c r="C158" s="26" t="s">
         <v>313</v>
       </c>
@@ -7271,7 +7252,7 @@
       <c r="A159" s="22">
         <v>144</v>
       </c>
-      <c r="B159" s="53"/>
+      <c r="B159" s="50"/>
       <c r="C159" s="26" t="s">
         <v>316</v>
       </c>
@@ -7298,7 +7279,7 @@
       <c r="A160" s="22">
         <v>145</v>
       </c>
-      <c r="B160" s="54"/>
+      <c r="B160" s="51"/>
       <c r="C160" s="26"/>
       <c r="D160" s="10" t="s">
         <v>175</v>
@@ -7352,8 +7333,8 @@
       <c r="A162" s="22">
         <v>147</v>
       </c>
-      <c r="B162" s="53"/>
-      <c r="C162" s="40" t="s">
+      <c r="B162" s="50"/>
+      <c r="C162" s="43" t="s">
         <v>322</v>
       </c>
       <c r="D162" s="10" t="s">
@@ -7379,8 +7360,8 @@
       <c r="A163" s="22">
         <v>148</v>
       </c>
-      <c r="B163" s="53"/>
-      <c r="C163" s="42"/>
+      <c r="B163" s="50"/>
+      <c r="C163" s="45"/>
       <c r="D163" s="10" t="s">
         <v>325</v>
       </c>
@@ -7404,8 +7385,8 @@
       <c r="A164" s="22">
         <v>149</v>
       </c>
-      <c r="B164" s="53"/>
-      <c r="C164" s="40" t="s">
+      <c r="B164" s="50"/>
+      <c r="C164" s="43" t="s">
         <v>327</v>
       </c>
       <c r="D164" s="10" t="s">
@@ -7431,8 +7412,8 @@
       <c r="A165" s="22">
         <v>150</v>
       </c>
-      <c r="B165" s="53"/>
-      <c r="C165" s="42"/>
+      <c r="B165" s="50"/>
+      <c r="C165" s="45"/>
       <c r="D165" s="10" t="s">
         <v>328</v>
       </c>
@@ -7456,7 +7437,7 @@
       <c r="A166" s="22">
         <v>151</v>
       </c>
-      <c r="B166" s="53"/>
+      <c r="B166" s="50"/>
       <c r="C166" s="26" t="s">
         <v>331</v>
       </c>
@@ -7483,8 +7464,8 @@
       <c r="A167" s="22">
         <v>152</v>
       </c>
-      <c r="B167" s="53"/>
-      <c r="C167" s="40" t="s">
+      <c r="B167" s="50"/>
+      <c r="C167" s="43" t="s">
         <v>334</v>
       </c>
       <c r="D167" s="10" t="s">
@@ -7510,8 +7491,8 @@
       <c r="A168" s="22">
         <v>153</v>
       </c>
-      <c r="B168" s="53"/>
-      <c r="C168" s="42"/>
+      <c r="B168" s="50"/>
+      <c r="C168" s="45"/>
       <c r="D168" s="10" t="s">
         <v>338</v>
       </c>
@@ -7535,8 +7516,8 @@
       <c r="A169" s="22">
         <v>154</v>
       </c>
-      <c r="B169" s="53"/>
-      <c r="C169" s="40" t="s">
+      <c r="B169" s="50"/>
+      <c r="C169" s="43" t="s">
         <v>337</v>
       </c>
       <c r="D169" s="10" t="s">
@@ -7562,8 +7543,8 @@
       <c r="A170" s="22">
         <v>155</v>
       </c>
-      <c r="B170" s="53"/>
-      <c r="C170" s="42"/>
+      <c r="B170" s="50"/>
+      <c r="C170" s="45"/>
       <c r="D170" s="10" t="s">
         <v>340</v>
       </c>
@@ -7587,8 +7568,8 @@
       <c r="A171" s="22">
         <v>156</v>
       </c>
-      <c r="B171" s="53"/>
-      <c r="C171" s="40" t="s">
+      <c r="B171" s="50"/>
+      <c r="C171" s="43" t="s">
         <v>344</v>
       </c>
       <c r="D171" s="10" t="s">
@@ -7614,8 +7595,8 @@
       <c r="A172" s="22">
         <v>157</v>
       </c>
-      <c r="B172" s="53"/>
-      <c r="C172" s="41"/>
+      <c r="B172" s="50"/>
+      <c r="C172" s="44"/>
       <c r="D172" s="10" t="s">
         <v>347</v>
       </c>
@@ -7639,8 +7620,8 @@
       <c r="A173" s="22">
         <v>158</v>
       </c>
-      <c r="B173" s="53"/>
-      <c r="C173" s="42"/>
+      <c r="B173" s="50"/>
+      <c r="C173" s="45"/>
       <c r="D173" s="10" t="s">
         <v>349</v>
       </c>
@@ -7664,8 +7645,8 @@
       <c r="A174" s="22">
         <v>159</v>
       </c>
-      <c r="B174" s="53"/>
-      <c r="C174" s="40" t="s">
+      <c r="B174" s="50"/>
+      <c r="C174" s="43" t="s">
         <v>351</v>
       </c>
       <c r="D174" s="10" t="s">
@@ -7691,8 +7672,8 @@
       <c r="A175" s="22">
         <v>160</v>
       </c>
-      <c r="B175" s="53"/>
-      <c r="C175" s="42"/>
+      <c r="B175" s="50"/>
+      <c r="C175" s="45"/>
       <c r="D175" s="10" t="s">
         <v>352</v>
       </c>
@@ -7716,7 +7697,7 @@
       <c r="A176" s="22">
         <v>161</v>
       </c>
-      <c r="B176" s="53" t="s">
+      <c r="B176" s="50" t="s">
         <v>355</v>
       </c>
       <c r="C176" s="26" t="s">
@@ -7745,7 +7726,7 @@
       <c r="A177" s="22">
         <v>162</v>
       </c>
-      <c r="B177" s="53"/>
+      <c r="B177" s="50"/>
       <c r="C177" s="26" t="s">
         <v>356</v>
       </c>
@@ -7772,8 +7753,8 @@
       <c r="A178" s="22">
         <v>163</v>
       </c>
-      <c r="B178" s="53"/>
-      <c r="C178" s="40" t="s">
+      <c r="B178" s="50"/>
+      <c r="C178" s="43" t="s">
         <v>360</v>
       </c>
       <c r="D178" s="10" t="s">
@@ -7799,8 +7780,8 @@
       <c r="A179" s="22">
         <v>164</v>
       </c>
-      <c r="B179" s="54"/>
-      <c r="C179" s="42"/>
+      <c r="B179" s="51"/>
+      <c r="C179" s="45"/>
       <c r="D179" s="10" t="s">
         <v>362</v>
       </c>
@@ -7824,7 +7805,7 @@
       <c r="A180" s="22">
         <v>165</v>
       </c>
-      <c r="B180" s="59" t="s">
+      <c r="B180" s="49" t="s">
         <v>364</v>
       </c>
       <c r="C180" s="34"/>
@@ -7851,7 +7832,7 @@
       <c r="A181" s="22">
         <v>166</v>
       </c>
-      <c r="B181" s="59"/>
+      <c r="B181" s="49"/>
       <c r="C181" s="34"/>
       <c r="D181" s="33" t="s">
         <v>367</v>
@@ -7876,7 +7857,7 @@
       <c r="A182" s="22">
         <v>167</v>
       </c>
-      <c r="B182" s="59"/>
+      <c r="B182" s="49"/>
       <c r="C182" s="34"/>
       <c r="D182" s="33" t="s">
         <v>369</v>
@@ -7901,7 +7882,7 @@
       <c r="A183" s="22">
         <v>168</v>
       </c>
-      <c r="B183" s="59"/>
+      <c r="B183" s="49"/>
       <c r="C183" s="34"/>
       <c r="D183" s="33" t="s">
         <v>371</v>
@@ -7926,7 +7907,7 @@
       <c r="A184" s="22">
         <v>169</v>
       </c>
-      <c r="B184" s="59" t="s">
+      <c r="B184" s="49" t="s">
         <v>373</v>
       </c>
       <c r="C184" s="34" t="s">
@@ -7955,7 +7936,7 @@
       <c r="A185" s="22">
         <v>170</v>
       </c>
-      <c r="B185" s="59"/>
+      <c r="B185" s="49"/>
       <c r="C185" s="34" t="s">
         <v>377</v>
       </c>
@@ -7982,7 +7963,7 @@
       <c r="A186" s="22">
         <v>171</v>
       </c>
-      <c r="B186" s="59"/>
+      <c r="B186" s="49"/>
       <c r="C186" s="34" t="s">
         <v>380</v>
       </c>
@@ -8009,7 +7990,7 @@
       <c r="A187" s="22">
         <v>172</v>
       </c>
-      <c r="B187" s="59"/>
+      <c r="B187" s="49"/>
       <c r="C187" s="34" t="s">
         <v>383</v>
       </c>
@@ -8036,7 +8017,7 @@
       <c r="A188" s="22">
         <v>173</v>
       </c>
-      <c r="B188" s="59" t="s">
+      <c r="B188" s="49" t="s">
         <v>386</v>
       </c>
       <c r="C188" s="34" t="s">
@@ -8065,7 +8046,7 @@
       <c r="A189" s="22">
         <v>174</v>
       </c>
-      <c r="B189" s="59"/>
+      <c r="B189" s="49"/>
       <c r="C189" s="34" t="s">
         <v>390</v>
       </c>
@@ -8092,7 +8073,7 @@
       <c r="A190" s="22">
         <v>175</v>
       </c>
-      <c r="B190" s="59"/>
+      <c r="B190" s="49"/>
       <c r="C190" s="34" t="s">
         <v>393</v>
       </c>
@@ -8119,7 +8100,7 @@
       <c r="A191" s="22">
         <v>176</v>
       </c>
-      <c r="B191" s="59"/>
+      <c r="B191" s="49"/>
       <c r="C191" s="34" t="s">
         <v>396</v>
       </c>
@@ -8146,7 +8127,7 @@
       <c r="A192" s="22">
         <v>177</v>
       </c>
-      <c r="B192" s="59"/>
+      <c r="B192" s="49"/>
       <c r="C192" s="34" t="s">
         <v>398</v>
       </c>
@@ -8173,7 +8154,7 @@
       <c r="A193" s="22">
         <v>178</v>
       </c>
-      <c r="B193" s="59" t="s">
+      <c r="B193" s="49" t="s">
         <v>400</v>
       </c>
       <c r="C193" s="34" t="s">
@@ -8202,7 +8183,7 @@
       <c r="A194" s="22">
         <v>179</v>
       </c>
-      <c r="B194" s="59"/>
+      <c r="B194" s="49"/>
       <c r="C194" s="34"/>
       <c r="D194" s="33" t="s">
         <v>404</v>
@@ -8227,7 +8208,7 @@
       <c r="A195" s="22">
         <v>180</v>
       </c>
-      <c r="B195" s="59"/>
+      <c r="B195" s="49"/>
       <c r="C195" s="34"/>
       <c r="D195" s="33" t="s">
         <v>406</v>
@@ -8252,7 +8233,7 @@
       <c r="A196" s="22">
         <v>181</v>
       </c>
-      <c r="B196" s="59"/>
+      <c r="B196" s="49"/>
       <c r="C196" s="34"/>
       <c r="D196" s="33" t="s">
         <v>408</v>
@@ -8277,7 +8258,7 @@
       <c r="A197" s="22">
         <v>182</v>
       </c>
-      <c r="B197" s="59"/>
+      <c r="B197" s="49"/>
       <c r="C197" s="34" t="s">
         <v>410</v>
       </c>
@@ -8304,7 +8285,7 @@
       <c r="A198" s="22">
         <v>183</v>
       </c>
-      <c r="B198" s="59"/>
+      <c r="B198" s="49"/>
       <c r="C198" s="34" t="s">
         <v>413</v>
       </c>
@@ -8331,7 +8312,7 @@
       <c r="A199" s="22">
         <v>184</v>
       </c>
-      <c r="B199" s="59"/>
+      <c r="B199" s="49"/>
       <c r="C199" s="34"/>
       <c r="D199" s="33" t="s">
         <v>416</v>
@@ -8356,7 +8337,7 @@
       <c r="A200" s="22">
         <v>185</v>
       </c>
-      <c r="B200" s="59"/>
+      <c r="B200" s="49"/>
       <c r="C200" s="34"/>
       <c r="D200" s="33" t="s">
         <v>418</v>
@@ -8381,7 +8362,7 @@
       <c r="A201" s="22">
         <v>186</v>
       </c>
-      <c r="B201" s="59"/>
+      <c r="B201" s="49"/>
       <c r="C201" s="34" t="s">
         <v>420</v>
       </c>
@@ -8408,7 +8389,7 @@
       <c r="A202" s="22">
         <v>187</v>
       </c>
-      <c r="B202" s="59"/>
+      <c r="B202" s="49"/>
       <c r="C202" s="34" t="s">
         <v>398</v>
       </c>
@@ -8435,7 +8416,7 @@
       <c r="A203" s="22">
         <v>188</v>
       </c>
-      <c r="B203" s="59"/>
+      <c r="B203" s="49"/>
       <c r="C203" s="34" t="s">
         <v>423</v>
       </c>
@@ -8462,7 +8443,7 @@
       <c r="A204" s="22">
         <v>189</v>
       </c>
-      <c r="B204" s="59" t="s">
+      <c r="B204" s="49" t="s">
         <v>425</v>
       </c>
       <c r="C204" s="34" t="s">
@@ -8491,7 +8472,7 @@
       <c r="A205" s="22">
         <v>190</v>
       </c>
-      <c r="B205" s="59"/>
+      <c r="B205" s="49"/>
       <c r="C205" s="34"/>
       <c r="D205" s="33" t="s">
         <v>394</v>
@@ -8516,7 +8497,7 @@
       <c r="A206" s="22">
         <v>191</v>
       </c>
-      <c r="B206" s="59"/>
+      <c r="B206" s="49"/>
       <c r="C206" s="34" t="s">
         <v>423</v>
       </c>
@@ -8543,7 +8524,7 @@
       <c r="A207" s="22">
         <v>192</v>
       </c>
-      <c r="B207" s="59"/>
+      <c r="B207" s="49"/>
       <c r="C207" s="34" t="s">
         <v>429</v>
       </c>
@@ -8570,7 +8551,7 @@
       <c r="A208" s="22">
         <v>193</v>
       </c>
-      <c r="B208" s="59"/>
+      <c r="B208" s="49"/>
       <c r="C208" s="35" t="s">
         <v>432</v>
       </c>
@@ -8626,8 +8607,8 @@
       <c r="A210" s="22">
         <v>195</v>
       </c>
-      <c r="B210" s="53"/>
-      <c r="C210" s="40" t="s">
+      <c r="B210" s="50"/>
+      <c r="C210" s="43" t="s">
         <v>438</v>
       </c>
       <c r="D210" s="10" t="s">
@@ -8653,8 +8634,8 @@
       <c r="A211" s="22">
         <v>196</v>
       </c>
-      <c r="B211" s="53"/>
-      <c r="C211" s="41"/>
+      <c r="B211" s="50"/>
+      <c r="C211" s="44"/>
       <c r="D211" s="10" t="s">
         <v>441</v>
       </c>
@@ -8678,8 +8659,8 @@
       <c r="A212" s="22">
         <v>197</v>
       </c>
-      <c r="B212" s="53"/>
-      <c r="C212" s="42"/>
+      <c r="B212" s="50"/>
+      <c r="C212" s="45"/>
       <c r="D212" s="10" t="s">
         <v>443</v>
       </c>
@@ -8703,7 +8684,7 @@
       <c r="A213" s="22">
         <v>198</v>
       </c>
-      <c r="B213" s="53"/>
+      <c r="B213" s="50"/>
       <c r="C213" s="26" t="s">
         <v>445</v>
       </c>
@@ -8730,7 +8711,7 @@
       <c r="A214" s="22">
         <v>199</v>
       </c>
-      <c r="B214" s="53"/>
+      <c r="B214" s="50"/>
       <c r="C214" s="26" t="s">
         <v>448</v>
       </c>
@@ -8757,8 +8738,8 @@
       <c r="A215" s="22">
         <v>200</v>
       </c>
-      <c r="B215" s="53"/>
-      <c r="C215" s="40" t="s">
+      <c r="B215" s="50"/>
+      <c r="C215" s="43" t="s">
         <v>451</v>
       </c>
       <c r="D215" s="10" t="s">
@@ -8784,8 +8765,8 @@
       <c r="A216" s="22">
         <v>201</v>
       </c>
-      <c r="B216" s="53"/>
-      <c r="C216" s="41"/>
+      <c r="B216" s="50"/>
+      <c r="C216" s="44"/>
       <c r="D216" s="10" t="s">
         <v>452</v>
       </c>
@@ -8809,8 +8790,8 @@
       <c r="A217" s="22">
         <v>202</v>
       </c>
-      <c r="B217" s="53"/>
-      <c r="C217" s="42"/>
+      <c r="B217" s="50"/>
+      <c r="C217" s="45"/>
       <c r="D217" s="10" t="s">
         <v>452</v>
       </c>
@@ -8834,7 +8815,7 @@
       <c r="A218" s="22">
         <v>203</v>
       </c>
-      <c r="B218" s="53"/>
+      <c r="B218" s="50"/>
       <c r="C218" s="26" t="s">
         <v>398</v>
       </c>
@@ -8861,7 +8842,7 @@
       <c r="A219" s="22">
         <v>204</v>
       </c>
-      <c r="B219" s="53"/>
+      <c r="B219" s="50"/>
       <c r="C219" s="26" t="s">
         <v>423</v>
       </c>
@@ -8888,7 +8869,7 @@
       <c r="A220" s="22">
         <v>205</v>
       </c>
-      <c r="B220" s="54"/>
+      <c r="B220" s="51"/>
       <c r="C220" s="26" t="s">
         <v>459</v>
       </c>
@@ -8915,7 +8896,7 @@
       <c r="A221" s="22">
         <v>206</v>
       </c>
-      <c r="B221" s="49" t="s">
+      <c r="B221" s="60" t="s">
         <v>462</v>
       </c>
       <c r="C221" s="26" t="s">
@@ -8944,8 +8925,8 @@
       <c r="A222" s="22">
         <v>207</v>
       </c>
-      <c r="B222" s="50"/>
-      <c r="C222" s="40" t="s">
+      <c r="B222" s="61"/>
+      <c r="C222" s="43" t="s">
         <v>438</v>
       </c>
       <c r="D222" s="10" t="s">
@@ -8971,8 +8952,8 @@
       <c r="A223" s="22">
         <v>208</v>
       </c>
-      <c r="B223" s="50"/>
-      <c r="C223" s="41"/>
+      <c r="B223" s="61"/>
+      <c r="C223" s="44"/>
       <c r="D223" s="10" t="s">
         <v>475</v>
       </c>
@@ -8996,8 +8977,8 @@
       <c r="A224" s="22">
         <v>209</v>
       </c>
-      <c r="B224" s="50"/>
-      <c r="C224" s="42"/>
+      <c r="B224" s="61"/>
+      <c r="C224" s="45"/>
       <c r="D224" s="10" t="s">
         <v>475</v>
       </c>
@@ -9021,7 +9002,7 @@
       <c r="A225" s="22">
         <v>210</v>
       </c>
-      <c r="B225" s="50"/>
+      <c r="B225" s="61"/>
       <c r="C225" s="26" t="s">
         <v>448</v>
       </c>
@@ -9048,8 +9029,8 @@
       <c r="A226" s="22">
         <v>211</v>
       </c>
-      <c r="B226" s="50"/>
-      <c r="C226" s="40" t="s">
+      <c r="B226" s="61"/>
+      <c r="C226" s="43" t="s">
         <v>451</v>
       </c>
       <c r="D226" s="10" t="s">
@@ -9075,8 +9056,8 @@
       <c r="A227" s="22">
         <v>212</v>
       </c>
-      <c r="B227" s="50"/>
-      <c r="C227" s="41"/>
+      <c r="B227" s="61"/>
+      <c r="C227" s="44"/>
       <c r="D227" s="10" t="s">
         <v>477</v>
       </c>
@@ -9100,8 +9081,8 @@
       <c r="A228" s="22">
         <v>213</v>
       </c>
-      <c r="B228" s="50"/>
-      <c r="C228" s="42"/>
+      <c r="B228" s="61"/>
+      <c r="C228" s="45"/>
       <c r="D228" s="10" t="s">
         <v>477</v>
       </c>
@@ -9125,7 +9106,7 @@
       <c r="A229" s="22">
         <v>214</v>
       </c>
-      <c r="B229" s="50"/>
+      <c r="B229" s="61"/>
       <c r="C229" s="26" t="s">
         <v>398</v>
       </c>
@@ -9152,7 +9133,7 @@
       <c r="A230" s="22">
         <v>215</v>
       </c>
-      <c r="B230" s="51"/>
+      <c r="B230" s="62"/>
       <c r="C230" s="26" t="s">
         <v>423</v>
       </c>
@@ -9179,7 +9160,7 @@
       <c r="A231" s="22">
         <v>216</v>
       </c>
-      <c r="B231" s="43" t="s">
+      <c r="B231" s="46" t="s">
         <v>465</v>
       </c>
       <c r="C231" s="26" t="s">
@@ -9208,8 +9189,8 @@
       <c r="A232" s="22">
         <v>217</v>
       </c>
-      <c r="B232" s="44"/>
-      <c r="C232" s="40" t="s">
+      <c r="B232" s="47"/>
+      <c r="C232" s="43" t="s">
         <v>438</v>
       </c>
       <c r="D232" s="10" t="s">
@@ -9235,8 +9216,8 @@
       <c r="A233" s="22">
         <v>218</v>
       </c>
-      <c r="B233" s="44"/>
-      <c r="C233" s="41"/>
+      <c r="B233" s="47"/>
+      <c r="C233" s="44"/>
       <c r="D233" s="10" t="s">
         <v>469</v>
       </c>
@@ -9260,8 +9241,8 @@
       <c r="A234" s="22">
         <v>219</v>
       </c>
-      <c r="B234" s="44"/>
-      <c r="C234" s="42"/>
+      <c r="B234" s="47"/>
+      <c r="C234" s="45"/>
       <c r="D234" s="10" t="s">
         <v>469</v>
       </c>
@@ -9285,7 +9266,7 @@
       <c r="A235" s="22">
         <v>220</v>
       </c>
-      <c r="B235" s="44"/>
+      <c r="B235" s="47"/>
       <c r="C235" s="26" t="s">
         <v>448</v>
       </c>
@@ -9312,8 +9293,8 @@
       <c r="A236" s="22">
         <v>221</v>
       </c>
-      <c r="B236" s="44"/>
-      <c r="C236" s="40" t="s">
+      <c r="B236" s="47"/>
+      <c r="C236" s="43" t="s">
         <v>451</v>
       </c>
       <c r="D236" s="10" t="s">
@@ -9339,8 +9320,8 @@
       <c r="A237" s="22">
         <v>222</v>
       </c>
-      <c r="B237" s="44"/>
-      <c r="C237" s="41"/>
+      <c r="B237" s="47"/>
+      <c r="C237" s="44"/>
       <c r="D237" s="10" t="s">
         <v>471</v>
       </c>
@@ -9364,8 +9345,8 @@
       <c r="A238" s="22">
         <v>223</v>
       </c>
-      <c r="B238" s="44"/>
-      <c r="C238" s="42"/>
+      <c r="B238" s="47"/>
+      <c r="C238" s="45"/>
       <c r="D238" s="10" t="s">
         <v>471</v>
       </c>
@@ -9389,7 +9370,7 @@
       <c r="A239" s="22">
         <v>224</v>
       </c>
-      <c r="B239" s="44"/>
+      <c r="B239" s="47"/>
       <c r="C239" s="26" t="s">
         <v>398</v>
       </c>
@@ -9416,7 +9397,7 @@
       <c r="A240" s="22">
         <v>225</v>
       </c>
-      <c r="B240" s="44"/>
+      <c r="B240" s="47"/>
       <c r="C240" s="26" t="s">
         <v>423</v>
       </c>
@@ -9443,7 +9424,7 @@
       <c r="A241" s="22">
         <v>226</v>
       </c>
-      <c r="B241" s="45"/>
+      <c r="B241" s="48"/>
       <c r="C241" s="26" t="s">
         <v>445</v>
       </c>
@@ -9470,7 +9451,7 @@
       <c r="A242" s="22">
         <v>227</v>
       </c>
-      <c r="B242" s="43" t="s">
+      <c r="B242" s="46" t="s">
         <v>480</v>
       </c>
       <c r="C242" s="26" t="s">
@@ -9499,7 +9480,7 @@
       <c r="A243" s="22">
         <v>228</v>
       </c>
-      <c r="B243" s="44"/>
+      <c r="B243" s="47"/>
       <c r="C243" s="26" t="s">
         <v>483</v>
       </c>
@@ -9526,7 +9507,7 @@
       <c r="A244" s="22">
         <v>229</v>
       </c>
-      <c r="B244" s="44"/>
+      <c r="B244" s="47"/>
       <c r="C244" s="26" t="s">
         <v>486</v>
       </c>
@@ -9553,7 +9534,7 @@
       <c r="A245" s="22">
         <v>230</v>
       </c>
-      <c r="B245" s="44"/>
+      <c r="B245" s="47"/>
       <c r="C245" s="26"/>
       <c r="D245" s="10" t="s">
         <v>489</v>
@@ -9578,7 +9559,7 @@
       <c r="A246" s="22">
         <v>231</v>
       </c>
-      <c r="B246" s="45"/>
+      <c r="B246" s="48"/>
       <c r="C246" s="26"/>
       <c r="D246" s="10" t="s">
         <v>491</v>
@@ -9603,7 +9584,7 @@
       <c r="A247" s="22">
         <v>232</v>
       </c>
-      <c r="B247" s="43" t="s">
+      <c r="B247" s="46" t="s">
         <v>493</v>
       </c>
       <c r="C247" s="32" t="s">
@@ -9626,8 +9607,8 @@
       <c r="A248" s="22">
         <v>233</v>
       </c>
-      <c r="B248" s="44"/>
-      <c r="C248" s="40" t="s">
+      <c r="B248" s="47"/>
+      <c r="C248" s="43" t="s">
         <v>494</v>
       </c>
       <c r="D248" s="10" t="s">
@@ -9647,8 +9628,8 @@
       <c r="A249" s="22">
         <v>234</v>
       </c>
-      <c r="B249" s="44"/>
-      <c r="C249" s="41"/>
+      <c r="B249" s="47"/>
+      <c r="C249" s="44"/>
       <c r="D249" s="10" t="s">
         <v>500</v>
       </c>
@@ -9666,8 +9647,8 @@
       <c r="A250" s="22">
         <v>235</v>
       </c>
-      <c r="B250" s="44"/>
-      <c r="C250" s="41"/>
+      <c r="B250" s="47"/>
+      <c r="C250" s="44"/>
       <c r="D250" s="10" t="s">
         <v>501</v>
       </c>
@@ -9685,8 +9666,8 @@
       <c r="A251" s="22">
         <v>236</v>
       </c>
-      <c r="B251" s="44"/>
-      <c r="C251" s="42"/>
+      <c r="B251" s="47"/>
+      <c r="C251" s="45"/>
       <c r="D251" s="10" t="s">
         <v>503</v>
       </c>
@@ -9704,7 +9685,7 @@
       <c r="A252" s="22">
         <v>237</v>
       </c>
-      <c r="B252" s="44"/>
+      <c r="B252" s="47"/>
       <c r="C252" s="32" t="s">
         <v>505</v>
       </c>
@@ -9725,7 +9706,7 @@
       <c r="A253" s="22">
         <v>238</v>
       </c>
-      <c r="B253" s="44"/>
+      <c r="B253" s="47"/>
       <c r="C253" s="32" t="s">
         <v>508</v>
       </c>
@@ -9746,7 +9727,7 @@
       <c r="A254" s="22">
         <v>239</v>
       </c>
-      <c r="B254" s="44"/>
+      <c r="B254" s="47"/>
       <c r="C254" s="32" t="s">
         <v>511</v>
       </c>
@@ -9767,7 +9748,7 @@
       <c r="A255" s="22">
         <v>240</v>
       </c>
-      <c r="B255" s="44"/>
+      <c r="B255" s="47"/>
       <c r="C255" s="32" t="s">
         <v>514</v>
       </c>
@@ -9788,7 +9769,7 @@
       <c r="A256" s="22">
         <v>241</v>
       </c>
-      <c r="B256" s="45"/>
+      <c r="B256" s="48"/>
       <c r="C256" s="32" t="s">
         <v>517</v>
       </c>
@@ -9809,7 +9790,7 @@
       <c r="A257" s="22">
         <v>242</v>
       </c>
-      <c r="B257" s="43" t="s">
+      <c r="B257" s="46" t="s">
         <v>520</v>
       </c>
       <c r="C257" s="32" t="s">
@@ -9832,7 +9813,7 @@
       <c r="A258" s="22">
         <v>243</v>
       </c>
-      <c r="B258" s="44"/>
+      <c r="B258" s="47"/>
       <c r="C258" s="26" t="s">
         <v>523</v>
       </c>
@@ -9853,7 +9834,7 @@
       <c r="A259" s="22">
         <v>244</v>
       </c>
-      <c r="B259" s="44"/>
+      <c r="B259" s="47"/>
       <c r="C259" s="26" t="s">
         <v>177</v>
       </c>
@@ -9874,8 +9855,8 @@
       <c r="A260" s="22">
         <v>245</v>
       </c>
-      <c r="B260" s="44"/>
-      <c r="C260" s="40" t="s">
+      <c r="B260" s="47"/>
+      <c r="C260" s="43" t="s">
         <v>528</v>
       </c>
       <c r="D260" s="10" t="s">
@@ -9895,8 +9876,8 @@
       <c r="A261" s="22">
         <v>246</v>
       </c>
-      <c r="B261" s="44"/>
-      <c r="C261" s="41"/>
+      <c r="B261" s="47"/>
+      <c r="C261" s="44"/>
       <c r="D261" s="10" t="s">
         <v>531</v>
       </c>
@@ -9914,8 +9895,8 @@
       <c r="A262" s="22">
         <v>247</v>
       </c>
-      <c r="B262" s="44"/>
-      <c r="C262" s="42"/>
+      <c r="B262" s="47"/>
+      <c r="C262" s="45"/>
       <c r="D262" s="10" t="s">
         <v>533</v>
       </c>
@@ -9933,7 +9914,7 @@
       <c r="A263" s="22">
         <v>248</v>
       </c>
-      <c r="B263" s="44"/>
+      <c r="B263" s="47"/>
       <c r="C263" s="39" t="s">
         <v>535</v>
       </c>
@@ -9954,7 +9935,7 @@
       <c r="A264" s="22">
         <v>249</v>
       </c>
-      <c r="B264" s="44"/>
+      <c r="B264" s="47"/>
       <c r="C264" s="32" t="s">
         <v>538</v>
       </c>
@@ -9975,7 +9956,7 @@
       <c r="A265" s="22">
         <v>250</v>
       </c>
-      <c r="B265" s="44"/>
+      <c r="B265" s="47"/>
       <c r="C265" s="32" t="s">
         <v>541</v>
       </c>
@@ -9996,7 +9977,7 @@
       <c r="A266" s="22">
         <v>251</v>
       </c>
-      <c r="B266" s="45"/>
+      <c r="B266" s="48"/>
       <c r="C266" s="32" t="s">
         <v>544</v>
       </c>
@@ -10017,7 +9998,7 @@
       <c r="A267" s="22">
         <v>252</v>
       </c>
-      <c r="B267" s="43" t="s">
+      <c r="B267" s="46" t="s">
         <v>547</v>
       </c>
       <c r="C267" s="32" t="s">
@@ -10040,7 +10021,7 @@
       <c r="A268" s="22">
         <v>253</v>
       </c>
-      <c r="B268" s="44"/>
+      <c r="B268" s="47"/>
       <c r="C268" s="32" t="s">
         <v>550</v>
       </c>
@@ -10061,7 +10042,7 @@
       <c r="A269" s="22">
         <v>254</v>
       </c>
-      <c r="B269" s="44"/>
+      <c r="B269" s="47"/>
       <c r="C269" s="32" t="s">
         <v>553</v>
       </c>
@@ -10082,7 +10063,7 @@
       <c r="A270" s="22">
         <v>255</v>
       </c>
-      <c r="B270" s="44"/>
+      <c r="B270" s="47"/>
       <c r="C270" s="32" t="s">
         <v>556</v>
       </c>
@@ -10103,7 +10084,7 @@
       <c r="A271" s="22">
         <v>256</v>
       </c>
-      <c r="B271" s="44"/>
+      <c r="B271" s="47"/>
       <c r="C271" s="32" t="s">
         <v>541</v>
       </c>
@@ -10124,7 +10105,7 @@
       <c r="A272" s="22">
         <v>257</v>
       </c>
-      <c r="B272" s="45"/>
+      <c r="B272" s="48"/>
       <c r="C272" s="32" t="s">
         <v>538</v>
       </c>
@@ -10145,7 +10126,7 @@
       <c r="A273" s="22">
         <v>258</v>
       </c>
-      <c r="B273" s="43" t="s">
+      <c r="B273" s="46" t="s">
         <v>561</v>
       </c>
       <c r="C273" s="32" t="s">
@@ -10168,7 +10149,7 @@
       <c r="A274" s="22">
         <v>259</v>
       </c>
-      <c r="B274" s="44"/>
+      <c r="B274" s="47"/>
       <c r="C274" s="32" t="s">
         <v>523</v>
       </c>
@@ -10189,7 +10170,7 @@
       <c r="A275" s="22">
         <v>260</v>
       </c>
-      <c r="B275" s="44"/>
+      <c r="B275" s="47"/>
       <c r="C275" s="32" t="s">
         <v>177</v>
       </c>
@@ -10210,8 +10191,8 @@
       <c r="A276" s="22">
         <v>261</v>
       </c>
-      <c r="B276" s="44"/>
-      <c r="C276" s="40" t="s">
+      <c r="B276" s="47"/>
+      <c r="C276" s="43" t="s">
         <v>528</v>
       </c>
       <c r="D276" s="10" t="s">
@@ -10231,8 +10212,8 @@
       <c r="A277" s="22">
         <v>262</v>
       </c>
-      <c r="B277" s="44"/>
-      <c r="C277" s="41"/>
+      <c r="B277" s="47"/>
+      <c r="C277" s="44"/>
       <c r="D277" s="10" t="s">
         <v>531</v>
       </c>
@@ -10250,8 +10231,8 @@
       <c r="A278" s="22">
         <v>263</v>
       </c>
-      <c r="B278" s="44"/>
-      <c r="C278" s="42"/>
+      <c r="B278" s="47"/>
+      <c r="C278" s="45"/>
       <c r="D278" s="10" t="s">
         <v>533</v>
       </c>
@@ -10269,7 +10250,7 @@
       <c r="A279" s="22">
         <v>264</v>
       </c>
-      <c r="B279" s="44"/>
+      <c r="B279" s="47"/>
       <c r="C279" s="39" t="s">
         <v>535</v>
       </c>
@@ -10290,7 +10271,7 @@
       <c r="A280" s="22">
         <v>265</v>
       </c>
-      <c r="B280" s="44"/>
+      <c r="B280" s="47"/>
       <c r="C280" s="32" t="s">
         <v>538</v>
       </c>
@@ -10311,7 +10292,7 @@
       <c r="A281" s="22">
         <v>266</v>
       </c>
-      <c r="B281" s="45"/>
+      <c r="B281" s="48"/>
       <c r="C281" s="32" t="s">
         <v>541</v>
       </c>
@@ -10332,7 +10313,7 @@
       <c r="A282" s="22">
         <v>267</v>
       </c>
-      <c r="B282" s="43" t="s">
+      <c r="B282" s="46" t="s">
         <v>571</v>
       </c>
       <c r="C282" s="32" t="s">
@@ -10355,7 +10336,7 @@
       <c r="A283" s="22">
         <v>268</v>
       </c>
-      <c r="B283" s="44"/>
+      <c r="B283" s="47"/>
       <c r="C283" s="32" t="s">
         <v>523</v>
       </c>
@@ -10376,7 +10357,7 @@
       <c r="A284" s="22">
         <v>269</v>
       </c>
-      <c r="B284" s="44"/>
+      <c r="B284" s="47"/>
       <c r="C284" s="32" t="s">
         <v>177</v>
       </c>
@@ -10397,7 +10378,7 @@
       <c r="A285" s="22">
         <v>270</v>
       </c>
-      <c r="B285" s="44"/>
+      <c r="B285" s="47"/>
       <c r="C285" s="32" t="s">
         <v>541</v>
       </c>
@@ -10418,7 +10399,7 @@
       <c r="A286" s="22">
         <v>271</v>
       </c>
-      <c r="B286" s="44"/>
+      <c r="B286" s="47"/>
       <c r="C286" s="32" t="s">
         <v>538</v>
       </c>
@@ -10439,8 +10420,8 @@
       <c r="A287" s="22">
         <v>272</v>
       </c>
-      <c r="B287" s="44"/>
-      <c r="C287" s="40" t="s">
+      <c r="B287" s="47"/>
+      <c r="C287" s="43" t="s">
         <v>528</v>
       </c>
       <c r="D287" s="10" t="s">
@@ -10460,8 +10441,8 @@
       <c r="A288" s="22">
         <v>273</v>
       </c>
-      <c r="B288" s="44"/>
-      <c r="C288" s="41"/>
+      <c r="B288" s="47"/>
+      <c r="C288" s="44"/>
       <c r="D288" s="10" t="s">
         <v>531</v>
       </c>
@@ -10479,8 +10460,8 @@
       <c r="A289" s="22">
         <v>274</v>
       </c>
-      <c r="B289" s="44"/>
-      <c r="C289" s="41"/>
+      <c r="B289" s="47"/>
+      <c r="C289" s="44"/>
       <c r="D289" s="10" t="s">
         <v>533</v>
       </c>
@@ -10498,8 +10479,8 @@
       <c r="A290" s="22">
         <v>275</v>
       </c>
-      <c r="B290" s="44"/>
-      <c r="C290" s="41"/>
+      <c r="B290" s="47"/>
+      <c r="C290" s="44"/>
       <c r="D290" s="10" t="s">
         <v>581</v>
       </c>
@@ -10517,8 +10498,8 @@
       <c r="A291" s="22">
         <v>276</v>
       </c>
-      <c r="B291" s="44"/>
-      <c r="C291" s="41"/>
+      <c r="B291" s="47"/>
+      <c r="C291" s="44"/>
       <c r="D291" s="10" t="s">
         <v>578</v>
       </c>
@@ -10536,8 +10517,8 @@
       <c r="A292" s="22">
         <v>277</v>
       </c>
-      <c r="B292" s="45"/>
-      <c r="C292" s="42"/>
+      <c r="B292" s="48"/>
+      <c r="C292" s="45"/>
       <c r="D292" s="10" t="s">
         <v>578</v>
       </c>
@@ -10555,7 +10536,7 @@
       <c r="A293" s="22">
         <v>278</v>
       </c>
-      <c r="B293" s="43" t="s">
+      <c r="B293" s="46" t="s">
         <v>585</v>
       </c>
       <c r="C293" s="32" t="s">
@@ -10578,7 +10559,7 @@
       <c r="A294" s="22">
         <v>279</v>
       </c>
-      <c r="B294" s="44"/>
+      <c r="B294" s="47"/>
       <c r="C294" s="32" t="s">
         <v>523</v>
       </c>
@@ -10599,7 +10580,7 @@
       <c r="A295" s="22">
         <v>280</v>
       </c>
-      <c r="B295" s="44"/>
+      <c r="B295" s="47"/>
       <c r="C295" s="32" t="s">
         <v>177</v>
       </c>
@@ -10620,7 +10601,7 @@
       <c r="A296" s="22">
         <v>281</v>
       </c>
-      <c r="B296" s="44"/>
+      <c r="B296" s="47"/>
       <c r="C296" s="32" t="s">
         <v>538</v>
       </c>
@@ -10641,8 +10622,8 @@
       <c r="A297" s="22">
         <v>282</v>
       </c>
-      <c r="B297" s="44"/>
-      <c r="C297" s="40" t="s">
+      <c r="B297" s="47"/>
+      <c r="C297" s="43" t="s">
         <v>528</v>
       </c>
       <c r="D297" s="10" t="s">
@@ -10662,8 +10643,8 @@
       <c r="A298" s="22">
         <v>283</v>
       </c>
-      <c r="B298" s="44"/>
-      <c r="C298" s="41"/>
+      <c r="B298" s="47"/>
+      <c r="C298" s="44"/>
       <c r="D298" s="10" t="s">
         <v>531</v>
       </c>
@@ -10681,8 +10662,8 @@
       <c r="A299" s="22">
         <v>284</v>
       </c>
-      <c r="B299" s="44"/>
-      <c r="C299" s="41"/>
+      <c r="B299" s="47"/>
+      <c r="C299" s="44"/>
       <c r="D299" s="10" t="s">
         <v>533</v>
       </c>
@@ -10700,8 +10681,8 @@
       <c r="A300" s="22">
         <v>285</v>
       </c>
-      <c r="B300" s="44"/>
-      <c r="C300" s="42"/>
+      <c r="B300" s="47"/>
+      <c r="C300" s="45"/>
       <c r="D300" s="10" t="s">
         <v>591</v>
       </c>
@@ -10719,7 +10700,7 @@
       <c r="A301" s="22">
         <v>286</v>
       </c>
-      <c r="B301" s="44"/>
+      <c r="B301" s="47"/>
       <c r="C301" s="32" t="s">
         <v>593</v>
       </c>
@@ -10740,7 +10721,7 @@
       <c r="A302" s="22">
         <v>287</v>
       </c>
-      <c r="B302" s="45"/>
+      <c r="B302" s="48"/>
       <c r="C302" s="32" t="s">
         <v>541</v>
       </c>
@@ -10761,7 +10742,7 @@
       <c r="A303" s="22">
         <v>288</v>
       </c>
-      <c r="B303" s="60" t="s">
+      <c r="B303" s="40" t="s">
         <v>597</v>
       </c>
       <c r="C303" s="32" t="s">
@@ -10784,7 +10765,7 @@
       <c r="A304" s="22">
         <v>289</v>
       </c>
-      <c r="B304" s="61"/>
+      <c r="B304" s="41"/>
       <c r="C304" s="32" t="s">
         <v>593</v>
       </c>
@@ -10805,7 +10786,7 @@
       <c r="A305" s="22">
         <v>290</v>
       </c>
-      <c r="B305" s="61"/>
+      <c r="B305" s="41"/>
       <c r="C305" s="32" t="s">
         <v>541</v>
       </c>
@@ -10826,7 +10807,7 @@
       <c r="A306" s="22">
         <v>291</v>
       </c>
-      <c r="B306" s="61"/>
+      <c r="B306" s="41"/>
       <c r="C306" s="32" t="s">
         <v>538</v>
       </c>
@@ -10847,7 +10828,7 @@
       <c r="A307" s="22">
         <v>292</v>
       </c>
-      <c r="B307" s="62"/>
+      <c r="B307" s="42"/>
       <c r="C307" s="32" t="s">
         <v>602</v>
       </c>
@@ -10868,7 +10849,7 @@
       <c r="A308" s="22">
         <v>293</v>
       </c>
-      <c r="B308" s="43" t="s">
+      <c r="B308" s="46" t="s">
         <v>605</v>
       </c>
       <c r="C308" s="32" t="s">
@@ -10891,7 +10872,7 @@
       <c r="A309" s="22">
         <v>294</v>
       </c>
-      <c r="B309" s="44"/>
+      <c r="B309" s="47"/>
       <c r="C309" s="32" t="s">
         <v>541</v>
       </c>
@@ -10912,7 +10893,7 @@
       <c r="A310" s="22">
         <v>295</v>
       </c>
-      <c r="B310" s="44"/>
+      <c r="B310" s="47"/>
       <c r="C310" s="32" t="s">
         <v>538</v>
       </c>
@@ -10933,8 +10914,8 @@
       <c r="A311" s="22">
         <v>296</v>
       </c>
-      <c r="B311" s="44"/>
-      <c r="C311" s="40" t="s">
+      <c r="B311" s="47"/>
+      <c r="C311" s="43" t="s">
         <v>528</v>
       </c>
       <c r="D311" s="10" t="s">
@@ -10954,8 +10935,8 @@
       <c r="A312" s="22">
         <v>297</v>
       </c>
-      <c r="B312" s="44"/>
-      <c r="C312" s="41"/>
+      <c r="B312" s="47"/>
+      <c r="C312" s="44"/>
       <c r="D312" s="10" t="s">
         <v>531</v>
       </c>
@@ -10973,8 +10954,8 @@
       <c r="A313" s="22">
         <v>298</v>
       </c>
-      <c r="B313" s="44"/>
-      <c r="C313" s="42"/>
+      <c r="B313" s="47"/>
+      <c r="C313" s="45"/>
       <c r="D313" s="10" t="s">
         <v>533</v>
       </c>
@@ -10992,8 +10973,8 @@
       <c r="A314" s="22">
         <v>299</v>
       </c>
-      <c r="B314" s="44"/>
-      <c r="C314" s="40" t="s">
+      <c r="B314" s="47"/>
+      <c r="C314" s="43" t="s">
         <v>610</v>
       </c>
       <c r="D314" s="10" t="s">
@@ -11013,8 +10994,8 @@
       <c r="A315" s="22">
         <v>300</v>
       </c>
-      <c r="B315" s="44"/>
-      <c r="C315" s="41"/>
+      <c r="B315" s="47"/>
+      <c r="C315" s="44"/>
       <c r="D315" s="10" t="s">
         <v>614</v>
       </c>
@@ -11032,8 +11013,8 @@
       <c r="A316" s="22">
         <v>301</v>
       </c>
-      <c r="B316" s="44"/>
-      <c r="C316" s="42"/>
+      <c r="B316" s="47"/>
+      <c r="C316" s="45"/>
       <c r="D316" s="10" t="s">
         <v>615</v>
       </c>
@@ -11051,8 +11032,8 @@
       <c r="A317" s="22">
         <v>302</v>
       </c>
-      <c r="B317" s="44"/>
-      <c r="C317" s="40" t="s">
+      <c r="B317" s="47"/>
+      <c r="C317" s="43" t="s">
         <v>617</v>
       </c>
       <c r="D317" s="10" t="s">
@@ -11072,8 +11053,8 @@
       <c r="A318" s="22">
         <v>303</v>
       </c>
-      <c r="B318" s="44"/>
-      <c r="C318" s="42"/>
+      <c r="B318" s="47"/>
+      <c r="C318" s="45"/>
       <c r="D318" s="10" t="s">
         <v>620</v>
       </c>
@@ -11091,7 +11072,7 @@
       <c r="A319" s="22">
         <v>304</v>
       </c>
-      <c r="B319" s="45"/>
+      <c r="B319" s="48"/>
       <c r="C319" s="32" t="s">
         <v>622</v>
       </c>
@@ -11403,74 +11384,6 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="B303:B307"/>
-    <mergeCell ref="C311:C313"/>
-    <mergeCell ref="C314:C316"/>
-    <mergeCell ref="C317:C318"/>
-    <mergeCell ref="B308:B319"/>
-    <mergeCell ref="C276:C278"/>
-    <mergeCell ref="B273:B281"/>
-    <mergeCell ref="C287:C292"/>
-    <mergeCell ref="B282:B292"/>
-    <mergeCell ref="C297:C300"/>
-    <mergeCell ref="B293:B302"/>
-    <mergeCell ref="C248:C251"/>
-    <mergeCell ref="B247:B256"/>
-    <mergeCell ref="C260:C262"/>
-    <mergeCell ref="B257:B266"/>
-    <mergeCell ref="B267:B272"/>
-    <mergeCell ref="B204:B208"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="B176:B179"/>
-    <mergeCell ref="C164:C165"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="C169:C170"/>
-    <mergeCell ref="C171:C173"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B161:B175"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="B180:B183"/>
-    <mergeCell ref="B184:B187"/>
-    <mergeCell ref="B188:B192"/>
-    <mergeCell ref="B193:B203"/>
-    <mergeCell ref="B147:B149"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="B150:B156"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="B133:B146"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="C135:C139"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C143:C145"/>
-    <mergeCell ref="B115:B132"/>
-    <mergeCell ref="C116:C119"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C124:C126"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="C129:C131"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B22:B36"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="B100:B102"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B82:B89"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="C60:C64"/>
-    <mergeCell ref="B65:B81"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="C78:C80"/>
     <mergeCell ref="C236:C238"/>
     <mergeCell ref="B231:B241"/>
     <mergeCell ref="B242:B246"/>
@@ -11487,6 +11400,74 @@
     <mergeCell ref="B111:B114"/>
     <mergeCell ref="B53:B57"/>
     <mergeCell ref="B90:B97"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="B100:B102"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="B82:B89"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="B65:B81"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B22:B36"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B115:B132"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C124:C126"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C129:C131"/>
+    <mergeCell ref="B133:B146"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="C135:C139"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C143:C145"/>
+    <mergeCell ref="B147:B149"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="B150:B156"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="B180:B183"/>
+    <mergeCell ref="B184:B187"/>
+    <mergeCell ref="B188:B192"/>
+    <mergeCell ref="B193:B203"/>
+    <mergeCell ref="B204:B208"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="B176:B179"/>
+    <mergeCell ref="C164:C165"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="C169:C170"/>
+    <mergeCell ref="C171:C173"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B161:B175"/>
+    <mergeCell ref="C162:C163"/>
+    <mergeCell ref="C248:C251"/>
+    <mergeCell ref="B247:B256"/>
+    <mergeCell ref="C260:C262"/>
+    <mergeCell ref="B257:B266"/>
+    <mergeCell ref="B267:B272"/>
+    <mergeCell ref="C276:C278"/>
+    <mergeCell ref="B273:B281"/>
+    <mergeCell ref="C287:C292"/>
+    <mergeCell ref="B282:B292"/>
+    <mergeCell ref="C297:C300"/>
+    <mergeCell ref="B293:B302"/>
+    <mergeCell ref="B303:B307"/>
+    <mergeCell ref="C311:C313"/>
+    <mergeCell ref="C314:C316"/>
+    <mergeCell ref="C317:C318"/>
+    <mergeCell ref="B308:B319"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G60:I246 G16:I57">

</xml_diff>

<commit_message>
update sua loi vang app
</commit_message>
<xml_diff>
--- a/TestCase-Reup.xlsx
+++ b/TestCase-Reup.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="633">
   <si>
     <t>ID</t>
   </si>
@@ -2621,9 +2621,6 @@
   </si>
   <si>
     <t>Actual results</t>
-  </si>
-  <si>
-    <t>Thoát Ứng Dụng</t>
   </si>
   <si>
     <t>Nhập từ vựng và để trống nghĩa từ vựng nhưng vẫn lưu dc</t>
@@ -2817,7 +2814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2921,14 +2918,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2948,27 +2939,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2987,11 +2957,55 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3410,8 +3424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K81" sqref="K81"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3451,11 +3465,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G13" s="52" t="s">
+      <c r="G13" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
@@ -3473,11 +3487,11 @@
       <c r="F14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
@@ -3518,7 +3532,7 @@
       <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="50" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="22" t="s">
@@ -3547,7 +3561,7 @@
       <c r="A17" s="7">
         <v>2</v>
       </c>
-      <c r="B17" s="47"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="22" t="s">
         <v>23</v>
       </c>
@@ -3576,7 +3590,7 @@
       <c r="A18" s="18">
         <v>3</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="22" t="s">
         <v>27</v>
       </c>
@@ -3590,24 +3604,22 @@
         <v>52</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>632</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>4</v>
       </c>
-      <c r="B19" s="47"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="22" t="s">
         <v>23</v>
       </c>
@@ -3636,7 +3648,7 @@
       <c r="A20" s="18">
         <v>5</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="22" t="s">
         <v>54</v>
       </c>
@@ -3650,24 +3662,22 @@
         <v>58</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>632</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J20" s="8"/>
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>6</v>
       </c>
-      <c r="B21" s="48"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="22" t="s">
         <v>59</v>
       </c>
@@ -3694,10 +3704,10 @@
       <c r="A22" s="18">
         <v>7</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="38" t="s">
         <v>71</v>
       </c>
       <c r="D22" s="10" t="s">
@@ -3723,8 +3733,8 @@
       <c r="A23" s="18">
         <v>8</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="10" t="s">
         <v>65</v>
       </c>
@@ -3748,8 +3758,8 @@
       <c r="A24" s="18">
         <v>9</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="40" t="s">
+      <c r="B24" s="51"/>
+      <c r="C24" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D24" s="10" t="s">
@@ -3775,8 +3785,8 @@
       <c r="A25" s="18">
         <v>10</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="42"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="10" t="s">
         <v>65</v>
       </c>
@@ -3800,7 +3810,7 @@
       <c r="A26" s="18">
         <v>11</v>
       </c>
-      <c r="B26" s="47"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="22" t="s">
         <v>72</v>
       </c>
@@ -3827,7 +3837,7 @@
       <c r="A27" s="18">
         <v>12</v>
       </c>
-      <c r="B27" s="47"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="22" t="s">
         <v>73</v>
       </c>
@@ -3854,7 +3864,7 @@
       <c r="A28" s="18">
         <v>13</v>
       </c>
-      <c r="B28" s="47"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="22" t="s">
         <v>74</v>
       </c>
@@ -3881,7 +3891,7 @@
       <c r="A29" s="18">
         <v>14</v>
       </c>
-      <c r="B29" s="47"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="22" t="s">
         <v>76</v>
       </c>
@@ -3908,7 +3918,7 @@
       <c r="A30" s="18">
         <v>15</v>
       </c>
-      <c r="B30" s="47"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="22" t="s">
         <v>78</v>
       </c>
@@ -3922,24 +3932,22 @@
         <v>51</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>632</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J30" s="8"/>
       <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <v>16</v>
       </c>
-      <c r="B31" s="47"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="22" t="s">
         <v>79</v>
       </c>
@@ -3953,24 +3961,22 @@
         <v>52</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>632</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J31" s="8"/>
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
         <v>17</v>
       </c>
-      <c r="B32" s="47"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="22" t="s">
         <v>79</v>
       </c>
@@ -3999,7 +4005,7 @@
       <c r="A33" s="18">
         <v>18</v>
       </c>
-      <c r="B33" s="47"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="22" t="s">
         <v>84</v>
       </c>
@@ -4026,7 +4032,7 @@
       <c r="A34" s="18">
         <v>19</v>
       </c>
-      <c r="B34" s="47"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="22" t="s">
         <v>85</v>
       </c>
@@ -4053,7 +4059,7 @@
       <c r="A35" s="18">
         <v>20</v>
       </c>
-      <c r="B35" s="47"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="22" t="s">
         <v>88</v>
       </c>
@@ -4080,7 +4086,7 @@
       <c r="A36" s="18">
         <v>21</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="22" t="s">
         <v>88</v>
       </c>
@@ -4107,7 +4113,7 @@
       <c r="A37" s="18">
         <v>22</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="50" t="s">
         <v>93</v>
       </c>
       <c r="C37" s="22" t="s">
@@ -4136,7 +4142,7 @@
       <c r="A38" s="18">
         <v>23</v>
       </c>
-      <c r="B38" s="47"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="22" t="s">
         <v>94</v>
       </c>
@@ -4165,7 +4171,7 @@
       <c r="A39" s="18">
         <v>24</v>
       </c>
-      <c r="B39" s="47"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="22" t="s">
         <v>99</v>
       </c>
@@ -4194,7 +4200,7 @@
       <c r="A40" s="18">
         <v>25</v>
       </c>
-      <c r="B40" s="47"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="22" t="s">
         <v>100</v>
       </c>
@@ -4223,7 +4229,7 @@
       <c r="A41" s="18">
         <v>26</v>
       </c>
-      <c r="B41" s="47"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="22" t="s">
         <v>103</v>
       </c>
@@ -4252,7 +4258,7 @@
       <c r="A42" s="18">
         <v>27</v>
       </c>
-      <c r="B42" s="47"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="22" t="s">
         <v>105</v>
       </c>
@@ -4279,7 +4285,7 @@
       <c r="A43" s="18">
         <v>28</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="22" t="s">
         <v>108</v>
       </c>
@@ -4306,7 +4312,7 @@
       <c r="A44" s="18">
         <v>29</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="50" t="s">
         <v>93</v>
       </c>
       <c r="C44" s="22" t="s">
@@ -4335,7 +4341,7 @@
       <c r="A45" s="18">
         <v>30</v>
       </c>
-      <c r="B45" s="47"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="22" t="s">
         <v>113</v>
       </c>
@@ -4362,7 +4368,7 @@
       <c r="A46" s="18">
         <v>31</v>
       </c>
-      <c r="B46" s="47"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="22" t="s">
         <v>94</v>
       </c>
@@ -4391,7 +4397,7 @@
       <c r="A47" s="18">
         <v>32</v>
       </c>
-      <c r="B47" s="47"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="22" t="s">
         <v>99</v>
       </c>
@@ -4420,7 +4426,7 @@
       <c r="A48" s="18">
         <v>33</v>
       </c>
-      <c r="B48" s="47"/>
+      <c r="B48" s="51"/>
       <c r="C48" s="22" t="s">
         <v>116</v>
       </c>
@@ -4449,7 +4455,7 @@
       <c r="A49" s="18">
         <v>34</v>
       </c>
-      <c r="B49" s="48"/>
+      <c r="B49" s="52"/>
       <c r="C49" s="22" t="s">
         <v>117</v>
       </c>
@@ -4478,7 +4484,7 @@
       <c r="A50" s="18">
         <v>35</v>
       </c>
-      <c r="B50" s="53" t="s">
+      <c r="B50" s="44" t="s">
         <v>123</v>
       </c>
       <c r="C50" s="22" t="s">
@@ -4507,7 +4513,7 @@
       <c r="A51" s="18">
         <v>36</v>
       </c>
-      <c r="B51" s="54"/>
+      <c r="B51" s="45"/>
       <c r="C51" s="22" t="s">
         <v>94</v>
       </c>
@@ -4536,7 +4542,7 @@
       <c r="A52" s="18">
         <v>37</v>
       </c>
-      <c r="B52" s="55"/>
+      <c r="B52" s="46"/>
       <c r="C52" s="22" t="s">
         <v>99</v>
       </c>
@@ -4563,7 +4569,7 @@
       <c r="A53" s="18">
         <v>38</v>
       </c>
-      <c r="B53" s="49" t="s">
+      <c r="B53" s="50" t="s">
         <v>131</v>
       </c>
       <c r="C53" s="22" t="s">
@@ -4592,7 +4598,7 @@
       <c r="A54" s="18">
         <v>39</v>
       </c>
-      <c r="B54" s="47"/>
+      <c r="B54" s="51"/>
       <c r="C54" s="22" t="s">
         <v>94</v>
       </c>
@@ -4621,7 +4627,7 @@
       <c r="A55" s="18">
         <v>40</v>
       </c>
-      <c r="B55" s="47"/>
+      <c r="B55" s="51"/>
       <c r="C55" s="22" t="s">
         <v>99</v>
       </c>
@@ -4650,7 +4656,7 @@
       <c r="A56" s="18">
         <v>41</v>
       </c>
-      <c r="B56" s="47"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="22" t="s">
         <v>99</v>
       </c>
@@ -4679,7 +4685,7 @@
       <c r="A57" s="18">
         <v>42</v>
       </c>
-      <c r="B57" s="48"/>
+      <c r="B57" s="52"/>
       <c r="C57" s="22" t="s">
         <v>99</v>
       </c>
@@ -4750,10 +4756,10 @@
       <c r="A60" s="18">
         <v>45</v>
       </c>
-      <c r="B60" s="46" t="s">
+      <c r="B60" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="50" t="s">
+      <c r="C60" s="54" t="s">
         <v>21</v>
       </c>
       <c r="D60" s="10" t="s">
@@ -4779,8 +4785,8 @@
       <c r="A61" s="18">
         <v>46</v>
       </c>
-      <c r="B61" s="46"/>
-      <c r="C61" s="50"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="54"/>
       <c r="D61" s="10" t="s">
         <v>36</v>
       </c>
@@ -4804,8 +4810,8 @@
       <c r="A62" s="18">
         <v>47</v>
       </c>
-      <c r="B62" s="46"/>
-      <c r="C62" s="50"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="54"/>
       <c r="D62" s="10" t="s">
         <v>35</v>
       </c>
@@ -4829,8 +4835,8 @@
       <c r="A63" s="18">
         <v>48</v>
       </c>
-      <c r="B63" s="46"/>
-      <c r="C63" s="50"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="54"/>
       <c r="D63" s="10" t="s">
         <v>34</v>
       </c>
@@ -4854,8 +4860,8 @@
       <c r="A64" s="18">
         <v>49</v>
       </c>
-      <c r="B64" s="46"/>
-      <c r="C64" s="50"/>
+      <c r="B64" s="53"/>
+      <c r="C64" s="54"/>
       <c r="D64" s="10" t="s">
         <v>33</v>
       </c>
@@ -4879,10 +4885,10 @@
       <c r="A65" s="18">
         <v>50</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="50" t="s">
+      <c r="C65" s="54" t="s">
         <v>145</v>
       </c>
       <c r="D65" s="10" t="s">
@@ -4908,8 +4914,8 @@
       <c r="A66" s="18">
         <v>51</v>
       </c>
-      <c r="B66" s="46"/>
-      <c r="C66" s="50"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
       <c r="D66" s="10" t="s">
         <v>148</v>
       </c>
@@ -4933,8 +4939,8 @@
       <c r="A67" s="18">
         <v>52</v>
       </c>
-      <c r="B67" s="46"/>
-      <c r="C67" s="50"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="54"/>
       <c r="D67" s="10" t="s">
         <v>150</v>
       </c>
@@ -4954,7 +4960,7 @@
         <v>5</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K67" s="9"/>
     </row>
@@ -4962,8 +4968,8 @@
       <c r="A68" s="18">
         <v>53</v>
       </c>
-      <c r="B68" s="46"/>
-      <c r="C68" s="50"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="54"/>
       <c r="D68" s="10" t="s">
         <v>153</v>
       </c>
@@ -4983,7 +4989,7 @@
         <v>5</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K68" s="9"/>
     </row>
@@ -4991,8 +4997,8 @@
       <c r="A69" s="18">
         <v>54</v>
       </c>
-      <c r="B69" s="46"/>
-      <c r="C69" s="50"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="54"/>
       <c r="D69" s="10" t="s">
         <v>156</v>
       </c>
@@ -5018,8 +5024,8 @@
       <c r="A70" s="18">
         <v>55</v>
       </c>
-      <c r="B70" s="46"/>
-      <c r="C70" s="50"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="54"/>
       <c r="D70" s="10" t="s">
         <v>159</v>
       </c>
@@ -5045,8 +5051,8 @@
       <c r="A71" s="18">
         <v>56</v>
       </c>
-      <c r="B71" s="46"/>
-      <c r="C71" s="50" t="s">
+      <c r="B71" s="53"/>
+      <c r="C71" s="54" t="s">
         <v>160</v>
       </c>
       <c r="D71" s="10" t="s">
@@ -5072,8 +5078,8 @@
       <c r="A72" s="18">
         <v>57</v>
       </c>
-      <c r="B72" s="46"/>
-      <c r="C72" s="50"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="54"/>
       <c r="D72" s="10" t="s">
         <v>162</v>
       </c>
@@ -5097,8 +5103,8 @@
       <c r="A73" s="18">
         <v>58</v>
       </c>
-      <c r="B73" s="46"/>
-      <c r="C73" s="50"/>
+      <c r="B73" s="53"/>
+      <c r="C73" s="54"/>
       <c r="D73" s="10" t="s">
         <v>164</v>
       </c>
@@ -5122,8 +5128,8 @@
       <c r="A74" s="18">
         <v>59</v>
       </c>
-      <c r="B74" s="46"/>
-      <c r="C74" s="50"/>
+      <c r="B74" s="53"/>
+      <c r="C74" s="54"/>
       <c r="D74" s="10" t="s">
         <v>166</v>
       </c>
@@ -5147,8 +5153,8 @@
       <c r="A75" s="18">
         <v>60</v>
       </c>
-      <c r="B75" s="46"/>
-      <c r="C75" s="50"/>
+      <c r="B75" s="53"/>
+      <c r="C75" s="54"/>
       <c r="D75" s="10" t="s">
         <v>168</v>
       </c>
@@ -5172,8 +5178,8 @@
       <c r="A76" s="18">
         <v>61</v>
       </c>
-      <c r="B76" s="46"/>
-      <c r="C76" s="50"/>
+      <c r="B76" s="53"/>
+      <c r="C76" s="54"/>
       <c r="D76" s="10" t="s">
         <v>170</v>
       </c>
@@ -5197,7 +5203,7 @@
       <c r="A77" s="18">
         <v>62</v>
       </c>
-      <c r="B77" s="46"/>
+      <c r="B77" s="53"/>
       <c r="C77" s="22" t="s">
         <v>172</v>
       </c>
@@ -5224,8 +5230,8 @@
       <c r="A78" s="18">
         <v>63</v>
       </c>
-      <c r="B78" s="46"/>
-      <c r="C78" s="50" t="s">
+      <c r="B78" s="53"/>
+      <c r="C78" s="54" t="s">
         <v>174</v>
       </c>
       <c r="D78" s="10" t="s">
@@ -5251,8 +5257,8 @@
       <c r="A79" s="18">
         <v>64</v>
       </c>
-      <c r="B79" s="46"/>
-      <c r="C79" s="50"/>
+      <c r="B79" s="53"/>
+      <c r="C79" s="54"/>
       <c r="D79" s="10" t="s">
         <v>42</v>
       </c>
@@ -5276,8 +5282,8 @@
       <c r="A80" s="18">
         <v>65</v>
       </c>
-      <c r="B80" s="46"/>
-      <c r="C80" s="50"/>
+      <c r="B80" s="53"/>
+      <c r="C80" s="54"/>
       <c r="D80" s="10" t="s">
         <v>44</v>
       </c>
@@ -5301,7 +5307,7 @@
       <c r="A81" s="18">
         <v>66</v>
       </c>
-      <c r="B81" s="46"/>
+      <c r="B81" s="53"/>
       <c r="C81" s="22"/>
       <c r="D81" s="10" t="s">
         <v>175</v>
@@ -5313,10 +5319,10 @@
       <c r="G81" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H81" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="I81" s="33" t="s">
+      <c r="H81" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I81" s="37" t="s">
         <v>6</v>
       </c>
       <c r="J81" s="8"/>
@@ -5326,10 +5332,10 @@
       <c r="A82" s="18">
         <v>67</v>
       </c>
-      <c r="B82" s="46" t="s">
+      <c r="B82" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C82" s="50" t="s">
+      <c r="C82" s="54" t="s">
         <v>177</v>
       </c>
       <c r="D82" s="10" t="s">
@@ -5341,14 +5347,14 @@
       <c r="F82" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="G82" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H82" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I82" s="21" t="s">
-        <v>10</v>
+      <c r="G82" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H82" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I82" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="9"/>
@@ -5357,8 +5363,8 @@
       <c r="A83" s="18">
         <v>68</v>
       </c>
-      <c r="B83" s="46"/>
-      <c r="C83" s="50"/>
+      <c r="B83" s="53"/>
+      <c r="C83" s="54"/>
       <c r="D83" s="10" t="s">
         <v>181</v>
       </c>
@@ -5366,14 +5372,14 @@
         <v>182</v>
       </c>
       <c r="F83" s="10"/>
-      <c r="G83" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H83" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I83" s="21" t="s">
-        <v>10</v>
+      <c r="G83" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H83" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I83" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J83" s="8"/>
       <c r="K83" s="9"/>
@@ -5382,8 +5388,8 @@
       <c r="A84" s="18">
         <v>69</v>
       </c>
-      <c r="B84" s="46"/>
-      <c r="C84" s="50" t="s">
+      <c r="B84" s="53"/>
+      <c r="C84" s="54" t="s">
         <v>183</v>
       </c>
       <c r="D84" s="10" t="s">
@@ -5393,14 +5399,14 @@
         <v>185</v>
       </c>
       <c r="F84" s="10"/>
-      <c r="G84" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H84" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I84" s="21" t="s">
-        <v>10</v>
+      <c r="G84" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H84" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I84" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="9"/>
@@ -5409,8 +5415,8 @@
       <c r="A85" s="18">
         <v>70</v>
       </c>
-      <c r="B85" s="46"/>
-      <c r="C85" s="50"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="54"/>
       <c r="D85" s="10" t="s">
         <v>186</v>
       </c>
@@ -5418,14 +5424,14 @@
         <v>187</v>
       </c>
       <c r="F85" s="10"/>
-      <c r="G85" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H85" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I85" s="21" t="s">
-        <v>10</v>
+      <c r="G85" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H85" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I85" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J85" s="8"/>
       <c r="K85" s="9"/>
@@ -5434,8 +5440,8 @@
       <c r="A86" s="18">
         <v>71</v>
       </c>
-      <c r="B86" s="46"/>
-      <c r="C86" s="50"/>
+      <c r="B86" s="53"/>
+      <c r="C86" s="54"/>
       <c r="D86" s="10" t="s">
         <v>188</v>
       </c>
@@ -5443,14 +5449,14 @@
         <v>189</v>
       </c>
       <c r="F86" s="10"/>
-      <c r="G86" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H86" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I86" s="21" t="s">
-        <v>10</v>
+      <c r="G86" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H86" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I86" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="9"/>
@@ -5459,8 +5465,8 @@
       <c r="A87" s="18">
         <v>72</v>
       </c>
-      <c r="B87" s="46"/>
-      <c r="C87" s="50"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="54"/>
       <c r="D87" s="10" t="s">
         <v>190</v>
       </c>
@@ -5468,14 +5474,14 @@
         <v>191</v>
       </c>
       <c r="F87" s="10"/>
-      <c r="G87" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H87" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I87" s="21" t="s">
-        <v>10</v>
+      <c r="G87" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H87" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I87" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="9"/>
@@ -5484,7 +5490,7 @@
       <c r="A88" s="18">
         <v>73</v>
       </c>
-      <c r="B88" s="46"/>
+      <c r="B88" s="53"/>
       <c r="C88" s="22" t="s">
         <v>172</v>
       </c>
@@ -5495,14 +5501,14 @@
         <v>40</v>
       </c>
       <c r="F88" s="10"/>
-      <c r="G88" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H88" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I88" s="21" t="s">
-        <v>10</v>
+      <c r="G88" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H88" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I88" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="9"/>
@@ -5511,7 +5517,7 @@
       <c r="A89" s="18">
         <v>74</v>
       </c>
-      <c r="B89" s="46"/>
+      <c r="B89" s="53"/>
       <c r="C89" s="22"/>
       <c r="D89" s="10" t="s">
         <v>175</v>
@@ -5520,9 +5526,15 @@
         <v>176</v>
       </c>
       <c r="F89" s="10"/>
-      <c r="G89" s="21"/>
-      <c r="H89" s="21"/>
-      <c r="I89" s="21"/>
+      <c r="G89" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H89" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I89" s="37" t="s">
+        <v>6</v>
+      </c>
       <c r="J89" s="8"/>
       <c r="K89" s="9"/>
     </row>
@@ -5530,10 +5542,10 @@
       <c r="A90" s="18">
         <v>75</v>
       </c>
-      <c r="B90" s="46" t="s">
+      <c r="B90" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="50" t="s">
+      <c r="C90" s="54" t="s">
         <v>177</v>
       </c>
       <c r="D90" s="10" t="s">
@@ -5543,14 +5555,14 @@
         <v>179</v>
       </c>
       <c r="F90" s="10"/>
-      <c r="G90" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H90" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I90" s="21" t="s">
-        <v>10</v>
+      <c r="G90" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H90" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I90" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J90" s="8"/>
       <c r="K90" s="9"/>
@@ -5559,8 +5571,8 @@
       <c r="A91" s="18">
         <v>76</v>
       </c>
-      <c r="B91" s="46"/>
-      <c r="C91" s="50"/>
+      <c r="B91" s="53"/>
+      <c r="C91" s="54"/>
       <c r="D91" s="10" t="s">
         <v>181</v>
       </c>
@@ -5568,14 +5580,14 @@
         <v>182</v>
       </c>
       <c r="F91" s="10"/>
-      <c r="G91" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I91" s="21" t="s">
-        <v>10</v>
+      <c r="G91" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H91" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I91" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="9"/>
@@ -5584,8 +5596,8 @@
       <c r="A92" s="18">
         <v>77</v>
       </c>
-      <c r="B92" s="46"/>
-      <c r="C92" s="50" t="s">
+      <c r="B92" s="53"/>
+      <c r="C92" s="54" t="s">
         <v>183</v>
       </c>
       <c r="D92" s="10" t="s">
@@ -5595,14 +5607,14 @@
         <v>185</v>
       </c>
       <c r="F92" s="10"/>
-      <c r="G92" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I92" s="21" t="s">
-        <v>10</v>
+      <c r="G92" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H92" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I92" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J92" s="8"/>
       <c r="K92" s="9"/>
@@ -5611,8 +5623,8 @@
       <c r="A93" s="18">
         <v>78</v>
       </c>
-      <c r="B93" s="46"/>
-      <c r="C93" s="50"/>
+      <c r="B93" s="53"/>
+      <c r="C93" s="54"/>
       <c r="D93" s="10" t="s">
         <v>186</v>
       </c>
@@ -5620,14 +5632,14 @@
         <v>187</v>
       </c>
       <c r="F93" s="10"/>
-      <c r="G93" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I93" s="21" t="s">
-        <v>10</v>
+      <c r="G93" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I93" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="9"/>
@@ -5636,8 +5648,8 @@
       <c r="A94" s="18">
         <v>79</v>
       </c>
-      <c r="B94" s="46"/>
-      <c r="C94" s="50"/>
+      <c r="B94" s="53"/>
+      <c r="C94" s="54"/>
       <c r="D94" s="10" t="s">
         <v>188</v>
       </c>
@@ -5645,14 +5657,14 @@
         <v>189</v>
       </c>
       <c r="F94" s="10"/>
-      <c r="G94" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I94" s="21" t="s">
-        <v>10</v>
+      <c r="G94" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H94" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I94" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J94" s="8"/>
       <c r="K94" s="9"/>
@@ -5661,8 +5673,8 @@
       <c r="A95" s="18">
         <v>80</v>
       </c>
-      <c r="B95" s="46"/>
-      <c r="C95" s="50"/>
+      <c r="B95" s="53"/>
+      <c r="C95" s="54"/>
       <c r="D95" s="10" t="s">
         <v>190</v>
       </c>
@@ -5670,14 +5682,14 @@
         <v>192</v>
       </c>
       <c r="F95" s="10"/>
-      <c r="G95" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I95" s="21" t="s">
-        <v>10</v>
+      <c r="G95" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H95" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I95" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J95" s="8"/>
       <c r="K95" s="9"/>
@@ -5686,7 +5698,7 @@
       <c r="A96" s="18">
         <v>81</v>
       </c>
-      <c r="B96" s="46"/>
+      <c r="B96" s="53"/>
       <c r="C96" s="22" t="s">
         <v>172</v>
       </c>
@@ -5697,14 +5709,14 @@
         <v>40</v>
       </c>
       <c r="F96" s="10"/>
-      <c r="G96" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H96" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I96" s="21" t="s">
-        <v>10</v>
+      <c r="G96" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H96" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I96" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="9"/>
@@ -5713,7 +5725,7 @@
       <c r="A97" s="18">
         <v>82</v>
       </c>
-      <c r="B97" s="46"/>
+      <c r="B97" s="53"/>
       <c r="C97" s="22"/>
       <c r="D97" s="10" t="s">
         <v>175</v>
@@ -5722,9 +5734,15 @@
         <v>176</v>
       </c>
       <c r="F97" s="10"/>
-      <c r="G97" s="21"/>
-      <c r="H97" s="21"/>
-      <c r="I97" s="21"/>
+      <c r="G97" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I97" s="37" t="s">
+        <v>6</v>
+      </c>
       <c r="J97" s="8"/>
       <c r="K97" s="9"/>
     </row>
@@ -5732,7 +5750,7 @@
       <c r="A98" s="18">
         <v>83</v>
       </c>
-      <c r="B98" s="46" t="s">
+      <c r="B98" s="53" t="s">
         <v>49</v>
       </c>
       <c r="C98" s="22" t="s">
@@ -5745,14 +5763,14 @@
         <v>195</v>
       </c>
       <c r="F98" s="10"/>
-      <c r="G98" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H98" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I98" s="21" t="s">
-        <v>10</v>
+      <c r="G98" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H98" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I98" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="9"/>
@@ -5761,7 +5779,7 @@
       <c r="A99" s="18">
         <v>84</v>
       </c>
-      <c r="B99" s="46"/>
+      <c r="B99" s="53"/>
       <c r="C99" s="22"/>
       <c r="D99" s="10" t="s">
         <v>175</v>
@@ -5770,9 +5788,15 @@
         <v>176</v>
       </c>
       <c r="F99" s="10"/>
-      <c r="G99" s="21"/>
-      <c r="H99" s="21"/>
-      <c r="I99" s="21"/>
+      <c r="G99" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H99" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I99" s="37" t="s">
+        <v>6</v>
+      </c>
       <c r="J99" s="8"/>
       <c r="K99" s="9"/>
     </row>
@@ -5780,7 +5804,7 @@
       <c r="A100" s="18">
         <v>85</v>
       </c>
-      <c r="B100" s="46" t="s">
+      <c r="B100" s="53" t="s">
         <v>196</v>
       </c>
       <c r="C100" s="22" t="s">
@@ -5793,14 +5817,14 @@
         <v>197</v>
       </c>
       <c r="F100" s="10"/>
-      <c r="G100" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H100" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I100" s="21" t="s">
-        <v>10</v>
+      <c r="G100" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H100" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I100" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="9"/>
@@ -5809,7 +5833,7 @@
       <c r="A101" s="18">
         <v>86</v>
       </c>
-      <c r="B101" s="46"/>
+      <c r="B101" s="53"/>
       <c r="C101" s="22" t="s">
         <v>172</v>
       </c>
@@ -5820,14 +5844,14 @@
         <v>40</v>
       </c>
       <c r="F101" s="10"/>
-      <c r="G101" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H101" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I101" s="21" t="s">
-        <v>10</v>
+      <c r="G101" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H101" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I101" s="37" t="s">
+        <v>6</v>
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="9"/>
@@ -5836,7 +5860,7 @@
       <c r="A102" s="18">
         <v>87</v>
       </c>
-      <c r="B102" s="46"/>
+      <c r="B102" s="53"/>
       <c r="C102" s="22"/>
       <c r="D102" s="10" t="s">
         <v>175</v>
@@ -5845,9 +5869,15 @@
         <v>176</v>
       </c>
       <c r="F102" s="10"/>
-      <c r="G102" s="21"/>
-      <c r="H102" s="21"/>
-      <c r="I102" s="21"/>
+      <c r="G102" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H102" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I102" s="37" t="s">
+        <v>6</v>
+      </c>
       <c r="J102" s="8"/>
       <c r="K102" s="9"/>
     </row>
@@ -5855,7 +5885,7 @@
       <c r="A103" s="18">
         <v>88</v>
       </c>
-      <c r="B103" s="46" t="s">
+      <c r="B103" s="53" t="s">
         <v>198</v>
       </c>
       <c r="C103" s="22" t="s">
@@ -5886,7 +5916,7 @@
       <c r="A104" s="18">
         <v>89</v>
       </c>
-      <c r="B104" s="46"/>
+      <c r="B104" s="53"/>
       <c r="C104" s="22" t="s">
         <v>200</v>
       </c>
@@ -5915,8 +5945,8 @@
       <c r="A105" s="18">
         <v>90</v>
       </c>
-      <c r="B105" s="46"/>
-      <c r="C105" s="50" t="s">
+      <c r="B105" s="53"/>
+      <c r="C105" s="54" t="s">
         <v>203</v>
       </c>
       <c r="D105" s="10" t="s">
@@ -5942,8 +5972,8 @@
       <c r="A106" s="18">
         <v>91</v>
       </c>
-      <c r="B106" s="46"/>
-      <c r="C106" s="50"/>
+      <c r="B106" s="53"/>
+      <c r="C106" s="54"/>
       <c r="D106" s="10" t="s">
         <v>206</v>
       </c>
@@ -5967,8 +5997,8 @@
       <c r="A107" s="18">
         <v>92</v>
       </c>
-      <c r="B107" s="46"/>
-      <c r="C107" s="50"/>
+      <c r="B107" s="53"/>
+      <c r="C107" s="54"/>
       <c r="D107" s="10" t="s">
         <v>207</v>
       </c>
@@ -5992,8 +6022,8 @@
       <c r="A108" s="18">
         <v>93</v>
       </c>
-      <c r="B108" s="46"/>
-      <c r="C108" s="50"/>
+      <c r="B108" s="53"/>
+      <c r="C108" s="54"/>
       <c r="D108" s="10" t="s">
         <v>209</v>
       </c>
@@ -6017,7 +6047,7 @@
       <c r="A109" s="18">
         <v>94</v>
       </c>
-      <c r="B109" s="46"/>
+      <c r="B109" s="53"/>
       <c r="C109" s="22" t="s">
         <v>210</v>
       </c>
@@ -6044,7 +6074,7 @@
       <c r="A110" s="18">
         <v>95</v>
       </c>
-      <c r="B110" s="46"/>
+      <c r="B110" s="53"/>
       <c r="C110" s="22"/>
       <c r="D110" s="10" t="s">
         <v>175</v>
@@ -6069,7 +6099,7 @@
       <c r="A111" s="18">
         <v>96</v>
       </c>
-      <c r="B111" s="46" t="s">
+      <c r="B111" s="53" t="s">
         <v>213</v>
       </c>
       <c r="C111" s="22"/>
@@ -6096,7 +6126,7 @@
       <c r="A112" s="18">
         <v>97</v>
       </c>
-      <c r="B112" s="46"/>
+      <c r="B112" s="53"/>
       <c r="C112" s="22"/>
       <c r="D112" s="10" t="s">
         <v>216</v>
@@ -6121,7 +6151,7 @@
       <c r="A113" s="18">
         <v>98</v>
       </c>
-      <c r="B113" s="46"/>
+      <c r="B113" s="53"/>
       <c r="C113" s="22"/>
       <c r="D113" s="10" t="s">
         <v>218</v>
@@ -6146,7 +6176,7 @@
       <c r="A114" s="18">
         <v>99</v>
       </c>
-      <c r="B114" s="46"/>
+      <c r="B114" s="53"/>
       <c r="C114" s="22"/>
       <c r="D114" s="10" t="s">
         <v>220</v>
@@ -6171,7 +6201,7 @@
       <c r="A115" s="18">
         <v>100</v>
       </c>
-      <c r="B115" s="46" t="s">
+      <c r="B115" s="53" t="s">
         <v>222</v>
       </c>
       <c r="C115" s="22" t="s">
@@ -6200,8 +6230,8 @@
       <c r="A116" s="18">
         <v>101</v>
       </c>
-      <c r="B116" s="46"/>
-      <c r="C116" s="50" t="s">
+      <c r="B116" s="53"/>
+      <c r="C116" s="54" t="s">
         <v>226</v>
       </c>
       <c r="D116" s="10" t="s">
@@ -6227,8 +6257,8 @@
       <c r="A117" s="18">
         <v>102</v>
       </c>
-      <c r="B117" s="46"/>
-      <c r="C117" s="50"/>
+      <c r="B117" s="53"/>
+      <c r="C117" s="54"/>
       <c r="D117" s="10" t="s">
         <v>229</v>
       </c>
@@ -6252,8 +6282,8 @@
       <c r="A118" s="18">
         <v>103</v>
       </c>
-      <c r="B118" s="46"/>
-      <c r="C118" s="50"/>
+      <c r="B118" s="53"/>
+      <c r="C118" s="54"/>
       <c r="D118" s="10" t="s">
         <v>231</v>
       </c>
@@ -6277,8 +6307,8 @@
       <c r="A119" s="18">
         <v>104</v>
       </c>
-      <c r="B119" s="46"/>
-      <c r="C119" s="50"/>
+      <c r="B119" s="53"/>
+      <c r="C119" s="54"/>
       <c r="D119" s="10" t="s">
         <v>233</v>
       </c>
@@ -6302,8 +6332,8 @@
       <c r="A120" s="18">
         <v>105</v>
       </c>
-      <c r="B120" s="46"/>
-      <c r="C120" s="50" t="s">
+      <c r="B120" s="53"/>
+      <c r="C120" s="54" t="s">
         <v>234</v>
       </c>
       <c r="D120" s="10" t="s">
@@ -6329,8 +6359,8 @@
       <c r="A121" s="18">
         <v>106</v>
       </c>
-      <c r="B121" s="46"/>
-      <c r="C121" s="50"/>
+      <c r="B121" s="53"/>
+      <c r="C121" s="54"/>
       <c r="D121" s="10" t="s">
         <v>237</v>
       </c>
@@ -6354,8 +6384,8 @@
       <c r="A122" s="18">
         <v>107</v>
       </c>
-      <c r="B122" s="46"/>
-      <c r="C122" s="50"/>
+      <c r="B122" s="53"/>
+      <c r="C122" s="54"/>
       <c r="D122" s="10" t="s">
         <v>239</v>
       </c>
@@ -6379,8 +6409,8 @@
       <c r="A123" s="18">
         <v>108</v>
       </c>
-      <c r="B123" s="46"/>
-      <c r="C123" s="50"/>
+      <c r="B123" s="53"/>
+      <c r="C123" s="54"/>
       <c r="D123" s="10" t="s">
         <v>240</v>
       </c>
@@ -6404,8 +6434,8 @@
       <c r="A124" s="18">
         <v>109</v>
       </c>
-      <c r="B124" s="46"/>
-      <c r="C124" s="50" t="s">
+      <c r="B124" s="53"/>
+      <c r="C124" s="54" t="s">
         <v>241</v>
       </c>
       <c r="D124" s="10" t="s">
@@ -6431,8 +6461,8 @@
       <c r="A125" s="18">
         <v>110</v>
       </c>
-      <c r="B125" s="46"/>
-      <c r="C125" s="50"/>
+      <c r="B125" s="53"/>
+      <c r="C125" s="54"/>
       <c r="D125" s="10" t="s">
         <v>244</v>
       </c>
@@ -6456,8 +6486,8 @@
       <c r="A126" s="18">
         <v>111</v>
       </c>
-      <c r="B126" s="46"/>
-      <c r="C126" s="50"/>
+      <c r="B126" s="53"/>
+      <c r="C126" s="54"/>
       <c r="D126" s="10" t="s">
         <v>245</v>
       </c>
@@ -6481,8 +6511,8 @@
       <c r="A127" s="18">
         <v>112</v>
       </c>
-      <c r="B127" s="46"/>
-      <c r="C127" s="50" t="s">
+      <c r="B127" s="53"/>
+      <c r="C127" s="54" t="s">
         <v>247</v>
       </c>
       <c r="D127" s="10" t="s">
@@ -6508,8 +6538,8 @@
       <c r="A128" s="18">
         <v>113</v>
       </c>
-      <c r="B128" s="46"/>
-      <c r="C128" s="50"/>
+      <c r="B128" s="53"/>
+      <c r="C128" s="54"/>
       <c r="D128" s="10" t="s">
         <v>250</v>
       </c>
@@ -6533,8 +6563,8 @@
       <c r="A129" s="18">
         <v>114</v>
       </c>
-      <c r="B129" s="46"/>
-      <c r="C129" s="50" t="s">
+      <c r="B129" s="53"/>
+      <c r="C129" s="54" t="s">
         <v>252</v>
       </c>
       <c r="D129" s="10" t="s">
@@ -6560,8 +6590,8 @@
       <c r="A130" s="18">
         <v>115</v>
       </c>
-      <c r="B130" s="46"/>
-      <c r="C130" s="50"/>
+      <c r="B130" s="53"/>
+      <c r="C130" s="54"/>
       <c r="D130" s="10" t="s">
         <v>255</v>
       </c>
@@ -6585,8 +6615,8 @@
       <c r="A131" s="18">
         <v>116</v>
       </c>
-      <c r="B131" s="46"/>
-      <c r="C131" s="50"/>
+      <c r="B131" s="53"/>
+      <c r="C131" s="54"/>
       <c r="D131" s="10" t="s">
         <v>257</v>
       </c>
@@ -6610,7 +6640,7 @@
       <c r="A132" s="18">
         <v>117</v>
       </c>
-      <c r="B132" s="46"/>
+      <c r="B132" s="53"/>
       <c r="C132" s="22"/>
       <c r="D132" s="23" t="s">
         <v>175</v>
@@ -6635,10 +6665,10 @@
       <c r="A133" s="18">
         <v>118</v>
       </c>
-      <c r="B133" s="46" t="s">
+      <c r="B133" s="53" t="s">
         <v>260</v>
       </c>
-      <c r="C133" s="50" t="s">
+      <c r="C133" s="54" t="s">
         <v>261</v>
       </c>
       <c r="D133" s="10" t="s">
@@ -6664,8 +6694,8 @@
       <c r="A134" s="18">
         <v>119</v>
       </c>
-      <c r="B134" s="46"/>
-      <c r="C134" s="50"/>
+      <c r="B134" s="53"/>
+      <c r="C134" s="54"/>
       <c r="D134" s="10" t="s">
         <v>264</v>
       </c>
@@ -6689,8 +6719,8 @@
       <c r="A135" s="18">
         <v>120</v>
       </c>
-      <c r="B135" s="46"/>
-      <c r="C135" s="50" t="s">
+      <c r="B135" s="53"/>
+      <c r="C135" s="54" t="s">
         <v>266</v>
       </c>
       <c r="D135" s="10" t="s">
@@ -6716,8 +6746,8 @@
       <c r="A136" s="18">
         <v>121</v>
       </c>
-      <c r="B136" s="46"/>
-      <c r="C136" s="50"/>
+      <c r="B136" s="53"/>
+      <c r="C136" s="54"/>
       <c r="D136" s="10" t="s">
         <v>269</v>
       </c>
@@ -6741,8 +6771,8 @@
       <c r="A137" s="18">
         <v>122</v>
       </c>
-      <c r="B137" s="46"/>
-      <c r="C137" s="50"/>
+      <c r="B137" s="53"/>
+      <c r="C137" s="54"/>
       <c r="D137" s="10" t="s">
         <v>270</v>
       </c>
@@ -6767,8 +6797,8 @@
       <c r="A138" s="18">
         <v>123</v>
       </c>
-      <c r="B138" s="46"/>
-      <c r="C138" s="50"/>
+      <c r="B138" s="53"/>
+      <c r="C138" s="54"/>
       <c r="D138" s="10" t="s">
         <v>271</v>
       </c>
@@ -6792,8 +6822,8 @@
       <c r="A139" s="18">
         <v>124</v>
       </c>
-      <c r="B139" s="46"/>
-      <c r="C139" s="50"/>
+      <c r="B139" s="53"/>
+      <c r="C139" s="54"/>
       <c r="D139" s="10" t="s">
         <v>272</v>
       </c>
@@ -6817,8 +6847,8 @@
       <c r="A140" s="18">
         <v>125</v>
       </c>
-      <c r="B140" s="46"/>
-      <c r="C140" s="50" t="s">
+      <c r="B140" s="53"/>
+      <c r="C140" s="54" t="s">
         <v>274</v>
       </c>
       <c r="D140" s="10" t="s">
@@ -6844,8 +6874,8 @@
       <c r="A141" s="18">
         <v>126</v>
       </c>
-      <c r="B141" s="46"/>
-      <c r="C141" s="50"/>
+      <c r="B141" s="53"/>
+      <c r="C141" s="54"/>
       <c r="D141" s="10" t="s">
         <v>277</v>
       </c>
@@ -6869,7 +6899,7 @@
       <c r="A142" s="18">
         <v>127</v>
       </c>
-      <c r="B142" s="46"/>
+      <c r="B142" s="53"/>
       <c r="C142" s="22" t="s">
         <v>279</v>
       </c>
@@ -6896,8 +6926,8 @@
       <c r="A143" s="18">
         <v>128</v>
       </c>
-      <c r="B143" s="46"/>
-      <c r="C143" s="50" t="s">
+      <c r="B143" s="53"/>
+      <c r="C143" s="54" t="s">
         <v>282</v>
       </c>
       <c r="D143" s="10" t="s">
@@ -6923,8 +6953,8 @@
       <c r="A144" s="18">
         <v>129</v>
       </c>
-      <c r="B144" s="46"/>
-      <c r="C144" s="50"/>
+      <c r="B144" s="53"/>
+      <c r="C144" s="54"/>
       <c r="D144" s="10" t="s">
         <v>285</v>
       </c>
@@ -6948,8 +6978,8 @@
       <c r="A145" s="18">
         <v>130</v>
       </c>
-      <c r="B145" s="46"/>
-      <c r="C145" s="50"/>
+      <c r="B145" s="53"/>
+      <c r="C145" s="54"/>
       <c r="D145" s="10" t="s">
         <v>287</v>
       </c>
@@ -6973,7 +7003,7 @@
       <c r="A146" s="18">
         <v>131</v>
       </c>
-      <c r="B146" s="46"/>
+      <c r="B146" s="53"/>
       <c r="C146" s="22"/>
       <c r="D146" s="10" t="s">
         <v>175</v>
@@ -6998,10 +7028,10 @@
       <c r="A147" s="18">
         <v>132</v>
       </c>
-      <c r="B147" s="46" t="s">
+      <c r="B147" s="53" t="s">
         <v>289</v>
       </c>
-      <c r="C147" s="50" t="s">
+      <c r="C147" s="54" t="s">
         <v>290</v>
       </c>
       <c r="D147" s="10" t="s">
@@ -7027,8 +7057,8 @@
       <c r="A148" s="18">
         <v>133</v>
       </c>
-      <c r="B148" s="46"/>
-      <c r="C148" s="50"/>
+      <c r="B148" s="53"/>
+      <c r="C148" s="54"/>
       <c r="D148" s="10" t="s">
         <v>293</v>
       </c>
@@ -7052,7 +7082,7 @@
       <c r="A149" s="18">
         <v>134</v>
       </c>
-      <c r="B149" s="46"/>
+      <c r="B149" s="53"/>
       <c r="C149" s="22"/>
       <c r="D149" s="10" t="s">
         <v>175</v>
@@ -7077,10 +7107,10 @@
       <c r="A150" s="18">
         <v>135</v>
       </c>
-      <c r="B150" s="49" t="s">
+      <c r="B150" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="C150" s="40" t="s">
+      <c r="C150" s="38" t="s">
         <v>296</v>
       </c>
       <c r="D150" s="10" t="s">
@@ -7106,8 +7136,8 @@
       <c r="A151" s="18">
         <v>136</v>
       </c>
-      <c r="B151" s="47"/>
-      <c r="C151" s="41"/>
+      <c r="B151" s="51"/>
+      <c r="C151" s="39"/>
       <c r="D151" s="10" t="s">
         <v>299</v>
       </c>
@@ -7131,8 +7161,8 @@
       <c r="A152" s="18">
         <v>137</v>
       </c>
-      <c r="B152" s="47"/>
-      <c r="C152" s="41"/>
+      <c r="B152" s="51"/>
+      <c r="C152" s="39"/>
       <c r="D152" s="10" t="s">
         <v>301</v>
       </c>
@@ -7156,8 +7186,8 @@
       <c r="A153" s="18">
         <v>138</v>
       </c>
-      <c r="B153" s="47"/>
-      <c r="C153" s="42"/>
+      <c r="B153" s="51"/>
+      <c r="C153" s="40"/>
       <c r="D153" s="10" t="s">
         <v>303</v>
       </c>
@@ -7181,8 +7211,8 @@
       <c r="A154" s="18">
         <v>139</v>
       </c>
-      <c r="B154" s="47"/>
-      <c r="C154" s="40" t="s">
+      <c r="B154" s="51"/>
+      <c r="C154" s="38" t="s">
         <v>290</v>
       </c>
       <c r="D154" s="10" t="s">
@@ -7208,8 +7238,8 @@
       <c r="A155" s="18">
         <v>140</v>
       </c>
-      <c r="B155" s="47"/>
-      <c r="C155" s="42"/>
+      <c r="B155" s="51"/>
+      <c r="C155" s="40"/>
       <c r="D155" s="10" t="s">
         <v>307</v>
       </c>
@@ -7233,7 +7263,7 @@
       <c r="A156" s="18">
         <v>141</v>
       </c>
-      <c r="B156" s="48"/>
+      <c r="B156" s="52"/>
       <c r="C156" s="22"/>
       <c r="D156" s="10" t="s">
         <v>175</v>
@@ -7258,7 +7288,7 @@
       <c r="A157" s="18">
         <v>142</v>
       </c>
-      <c r="B157" s="49" t="s">
+      <c r="B157" s="50" t="s">
         <v>309</v>
       </c>
       <c r="C157" s="22" t="s">
@@ -7287,7 +7317,7 @@
       <c r="A158" s="18">
         <v>143</v>
       </c>
-      <c r="B158" s="47"/>
+      <c r="B158" s="51"/>
       <c r="C158" s="22" t="s">
         <v>313</v>
       </c>
@@ -7314,7 +7344,7 @@
       <c r="A159" s="18">
         <v>144</v>
       </c>
-      <c r="B159" s="47"/>
+      <c r="B159" s="51"/>
       <c r="C159" s="22" t="s">
         <v>316</v>
       </c>
@@ -7341,7 +7371,7 @@
       <c r="A160" s="18">
         <v>145</v>
       </c>
-      <c r="B160" s="48"/>
+      <c r="B160" s="52"/>
       <c r="C160" s="22"/>
       <c r="D160" s="10" t="s">
         <v>175</v>
@@ -7366,7 +7396,7 @@
       <c r="A161" s="18">
         <v>146</v>
       </c>
-      <c r="B161" s="49" t="s">
+      <c r="B161" s="50" t="s">
         <v>320</v>
       </c>
       <c r="C161" s="22" t="s">
@@ -7395,8 +7425,8 @@
       <c r="A162" s="18">
         <v>147</v>
       </c>
-      <c r="B162" s="47"/>
-      <c r="C162" s="40" t="s">
+      <c r="B162" s="51"/>
+      <c r="C162" s="38" t="s">
         <v>322</v>
       </c>
       <c r="D162" s="10" t="s">
@@ -7422,8 +7452,8 @@
       <c r="A163" s="18">
         <v>148</v>
       </c>
-      <c r="B163" s="47"/>
-      <c r="C163" s="42"/>
+      <c r="B163" s="51"/>
+      <c r="C163" s="40"/>
       <c r="D163" s="10" t="s">
         <v>325</v>
       </c>
@@ -7447,8 +7477,8 @@
       <c r="A164" s="18">
         <v>149</v>
       </c>
-      <c r="B164" s="47"/>
-      <c r="C164" s="40" t="s">
+      <c r="B164" s="51"/>
+      <c r="C164" s="38" t="s">
         <v>327</v>
       </c>
       <c r="D164" s="10" t="s">
@@ -7474,8 +7504,8 @@
       <c r="A165" s="18">
         <v>150</v>
       </c>
-      <c r="B165" s="47"/>
-      <c r="C165" s="42"/>
+      <c r="B165" s="51"/>
+      <c r="C165" s="40"/>
       <c r="D165" s="10" t="s">
         <v>328</v>
       </c>
@@ -7499,7 +7529,7 @@
       <c r="A166" s="18">
         <v>151</v>
       </c>
-      <c r="B166" s="47"/>
+      <c r="B166" s="51"/>
       <c r="C166" s="22" t="s">
         <v>331</v>
       </c>
@@ -7526,8 +7556,8 @@
       <c r="A167" s="18">
         <v>152</v>
       </c>
-      <c r="B167" s="47"/>
-      <c r="C167" s="40" t="s">
+      <c r="B167" s="51"/>
+      <c r="C167" s="38" t="s">
         <v>334</v>
       </c>
       <c r="D167" s="10" t="s">
@@ -7553,8 +7583,8 @@
       <c r="A168" s="18">
         <v>153</v>
       </c>
-      <c r="B168" s="47"/>
-      <c r="C168" s="42"/>
+      <c r="B168" s="51"/>
+      <c r="C168" s="40"/>
       <c r="D168" s="10" t="s">
         <v>338</v>
       </c>
@@ -7578,8 +7608,8 @@
       <c r="A169" s="18">
         <v>154</v>
       </c>
-      <c r="B169" s="47"/>
-      <c r="C169" s="40" t="s">
+      <c r="B169" s="51"/>
+      <c r="C169" s="38" t="s">
         <v>337</v>
       </c>
       <c r="D169" s="10" t="s">
@@ -7605,8 +7635,8 @@
       <c r="A170" s="18">
         <v>155</v>
       </c>
-      <c r="B170" s="47"/>
-      <c r="C170" s="42"/>
+      <c r="B170" s="51"/>
+      <c r="C170" s="40"/>
       <c r="D170" s="10" t="s">
         <v>340</v>
       </c>
@@ -7630,8 +7660,8 @@
       <c r="A171" s="18">
         <v>156</v>
       </c>
-      <c r="B171" s="47"/>
-      <c r="C171" s="40" t="s">
+      <c r="B171" s="51"/>
+      <c r="C171" s="38" t="s">
         <v>344</v>
       </c>
       <c r="D171" s="10" t="s">
@@ -7657,8 +7687,8 @@
       <c r="A172" s="18">
         <v>157</v>
       </c>
-      <c r="B172" s="47"/>
-      <c r="C172" s="41"/>
+      <c r="B172" s="51"/>
+      <c r="C172" s="39"/>
       <c r="D172" s="10" t="s">
         <v>347</v>
       </c>
@@ -7682,8 +7712,8 @@
       <c r="A173" s="18">
         <v>158</v>
       </c>
-      <c r="B173" s="47"/>
-      <c r="C173" s="42"/>
+      <c r="B173" s="51"/>
+      <c r="C173" s="40"/>
       <c r="D173" s="10" t="s">
         <v>349</v>
       </c>
@@ -7707,8 +7737,8 @@
       <c r="A174" s="18">
         <v>159</v>
       </c>
-      <c r="B174" s="47"/>
-      <c r="C174" s="40" t="s">
+      <c r="B174" s="51"/>
+      <c r="C174" s="38" t="s">
         <v>351</v>
       </c>
       <c r="D174" s="10" t="s">
@@ -7734,8 +7764,8 @@
       <c r="A175" s="18">
         <v>160</v>
       </c>
-      <c r="B175" s="47"/>
-      <c r="C175" s="42"/>
+      <c r="B175" s="51"/>
+      <c r="C175" s="40"/>
       <c r="D175" s="10" t="s">
         <v>352</v>
       </c>
@@ -7759,7 +7789,7 @@
       <c r="A176" s="18">
         <v>161</v>
       </c>
-      <c r="B176" s="47" t="s">
+      <c r="B176" s="51" t="s">
         <v>355</v>
       </c>
       <c r="C176" s="22" t="s">
@@ -7788,7 +7818,7 @@
       <c r="A177" s="18">
         <v>162</v>
       </c>
-      <c r="B177" s="47"/>
+      <c r="B177" s="51"/>
       <c r="C177" s="22" t="s">
         <v>356</v>
       </c>
@@ -7815,8 +7845,8 @@
       <c r="A178" s="18">
         <v>163</v>
       </c>
-      <c r="B178" s="47"/>
-      <c r="C178" s="40" t="s">
+      <c r="B178" s="51"/>
+      <c r="C178" s="38" t="s">
         <v>360</v>
       </c>
       <c r="D178" s="10" t="s">
@@ -7842,8 +7872,8 @@
       <c r="A179" s="18">
         <v>164</v>
       </c>
-      <c r="B179" s="48"/>
-      <c r="C179" s="42"/>
+      <c r="B179" s="52"/>
+      <c r="C179" s="40"/>
       <c r="D179" s="10" t="s">
         <v>362</v>
       </c>
@@ -7867,7 +7897,7 @@
       <c r="A180" s="18">
         <v>165</v>
       </c>
-      <c r="B180" s="46" t="s">
+      <c r="B180" s="53" t="s">
         <v>364</v>
       </c>
       <c r="C180" s="32"/>
@@ -7894,7 +7924,7 @@
       <c r="A181" s="18">
         <v>166</v>
       </c>
-      <c r="B181" s="46"/>
+      <c r="B181" s="53"/>
       <c r="C181" s="32"/>
       <c r="D181" s="10" t="s">
         <v>367</v>
@@ -7919,7 +7949,7 @@
       <c r="A182" s="18">
         <v>167</v>
       </c>
-      <c r="B182" s="46"/>
+      <c r="B182" s="53"/>
       <c r="C182" s="32"/>
       <c r="D182" s="10" t="s">
         <v>369</v>
@@ -7944,7 +7974,7 @@
       <c r="A183" s="18">
         <v>168</v>
       </c>
-      <c r="B183" s="46"/>
+      <c r="B183" s="53"/>
       <c r="C183" s="32"/>
       <c r="D183" s="10" t="s">
         <v>371</v>
@@ -7969,7 +7999,7 @@
       <c r="A184" s="18">
         <v>169</v>
       </c>
-      <c r="B184" s="46" t="s">
+      <c r="B184" s="53" t="s">
         <v>373</v>
       </c>
       <c r="C184" s="32" t="s">
@@ -7998,7 +8028,7 @@
       <c r="A185" s="18">
         <v>170</v>
       </c>
-      <c r="B185" s="46"/>
+      <c r="B185" s="53"/>
       <c r="C185" s="32" t="s">
         <v>377</v>
       </c>
@@ -8025,7 +8055,7 @@
       <c r="A186" s="18">
         <v>171</v>
       </c>
-      <c r="B186" s="46"/>
+      <c r="B186" s="53"/>
       <c r="C186" s="32" t="s">
         <v>380</v>
       </c>
@@ -8052,7 +8082,7 @@
       <c r="A187" s="18">
         <v>172</v>
       </c>
-      <c r="B187" s="46"/>
+      <c r="B187" s="53"/>
       <c r="C187" s="32" t="s">
         <v>383</v>
       </c>
@@ -8079,7 +8109,7 @@
       <c r="A188" s="18">
         <v>173</v>
       </c>
-      <c r="B188" s="46" t="s">
+      <c r="B188" s="53" t="s">
         <v>386</v>
       </c>
       <c r="C188" s="32" t="s">
@@ -8108,7 +8138,7 @@
       <c r="A189" s="18">
         <v>174</v>
       </c>
-      <c r="B189" s="46"/>
+      <c r="B189" s="53"/>
       <c r="C189" s="32" t="s">
         <v>390</v>
       </c>
@@ -8135,7 +8165,7 @@
       <c r="A190" s="18">
         <v>175</v>
       </c>
-      <c r="B190" s="46"/>
+      <c r="B190" s="53"/>
       <c r="C190" s="32" t="s">
         <v>393</v>
       </c>
@@ -8162,7 +8192,7 @@
       <c r="A191" s="18">
         <v>176</v>
       </c>
-      <c r="B191" s="46"/>
+      <c r="B191" s="53"/>
       <c r="C191" s="32" t="s">
         <v>396</v>
       </c>
@@ -8189,7 +8219,7 @@
       <c r="A192" s="18">
         <v>177</v>
       </c>
-      <c r="B192" s="46"/>
+      <c r="B192" s="53"/>
       <c r="C192" s="32" t="s">
         <v>398</v>
       </c>
@@ -8216,7 +8246,7 @@
       <c r="A193" s="18">
         <v>178</v>
       </c>
-      <c r="B193" s="46" t="s">
+      <c r="B193" s="53" t="s">
         <v>400</v>
       </c>
       <c r="C193" s="32" t="s">
@@ -8245,7 +8275,7 @@
       <c r="A194" s="18">
         <v>179</v>
       </c>
-      <c r="B194" s="46"/>
+      <c r="B194" s="53"/>
       <c r="C194" s="32"/>
       <c r="D194" s="10" t="s">
         <v>404</v>
@@ -8270,7 +8300,7 @@
       <c r="A195" s="18">
         <v>180</v>
       </c>
-      <c r="B195" s="46"/>
+      <c r="B195" s="53"/>
       <c r="C195" s="32"/>
       <c r="D195" s="10" t="s">
         <v>406</v>
@@ -8295,7 +8325,7 @@
       <c r="A196" s="18">
         <v>181</v>
       </c>
-      <c r="B196" s="46"/>
+      <c r="B196" s="53"/>
       <c r="C196" s="32"/>
       <c r="D196" s="10" t="s">
         <v>408</v>
@@ -8320,7 +8350,7 @@
       <c r="A197" s="18">
         <v>182</v>
       </c>
-      <c r="B197" s="46"/>
+      <c r="B197" s="53"/>
       <c r="C197" s="32" t="s">
         <v>410</v>
       </c>
@@ -8347,7 +8377,7 @@
       <c r="A198" s="18">
         <v>183</v>
       </c>
-      <c r="B198" s="46"/>
+      <c r="B198" s="53"/>
       <c r="C198" s="32" t="s">
         <v>413</v>
       </c>
@@ -8374,7 +8404,7 @@
       <c r="A199" s="18">
         <v>184</v>
       </c>
-      <c r="B199" s="46"/>
+      <c r="B199" s="53"/>
       <c r="C199" s="32"/>
       <c r="D199" s="10" t="s">
         <v>416</v>
@@ -8399,7 +8429,7 @@
       <c r="A200" s="18">
         <v>185</v>
       </c>
-      <c r="B200" s="46"/>
+      <c r="B200" s="53"/>
       <c r="C200" s="32"/>
       <c r="D200" s="10" t="s">
         <v>418</v>
@@ -8424,7 +8454,7 @@
       <c r="A201" s="18">
         <v>186</v>
       </c>
-      <c r="B201" s="46"/>
+      <c r="B201" s="53"/>
       <c r="C201" s="32" t="s">
         <v>420</v>
       </c>
@@ -8451,7 +8481,7 @@
       <c r="A202" s="18">
         <v>187</v>
       </c>
-      <c r="B202" s="46"/>
+      <c r="B202" s="53"/>
       <c r="C202" s="32" t="s">
         <v>398</v>
       </c>
@@ -8478,7 +8508,7 @@
       <c r="A203" s="18">
         <v>188</v>
       </c>
-      <c r="B203" s="46"/>
+      <c r="B203" s="53"/>
       <c r="C203" s="32" t="s">
         <v>423</v>
       </c>
@@ -8505,7 +8535,7 @@
       <c r="A204" s="18">
         <v>189</v>
       </c>
-      <c r="B204" s="46" t="s">
+      <c r="B204" s="53" t="s">
         <v>425</v>
       </c>
       <c r="C204" s="32" t="s">
@@ -8534,7 +8564,7 @@
       <c r="A205" s="18">
         <v>190</v>
       </c>
-      <c r="B205" s="46"/>
+      <c r="B205" s="53"/>
       <c r="C205" s="32"/>
       <c r="D205" s="10" t="s">
         <v>394</v>
@@ -8559,7 +8589,7 @@
       <c r="A206" s="18">
         <v>191</v>
       </c>
-      <c r="B206" s="46"/>
+      <c r="B206" s="53"/>
       <c r="C206" s="32" t="s">
         <v>423</v>
       </c>
@@ -8586,7 +8616,7 @@
       <c r="A207" s="18">
         <v>192</v>
       </c>
-      <c r="B207" s="46"/>
+      <c r="B207" s="53"/>
       <c r="C207" s="32" t="s">
         <v>429</v>
       </c>
@@ -8613,7 +8643,7 @@
       <c r="A208" s="18">
         <v>193</v>
       </c>
-      <c r="B208" s="46"/>
+      <c r="B208" s="53"/>
       <c r="C208" s="36" t="s">
         <v>432</v>
       </c>
@@ -8640,7 +8670,7 @@
       <c r="A209" s="18">
         <v>194</v>
       </c>
-      <c r="B209" s="49" t="s">
+      <c r="B209" s="50" t="s">
         <v>435</v>
       </c>
       <c r="C209" s="22" t="s">
@@ -8669,8 +8699,8 @@
       <c r="A210" s="18">
         <v>195</v>
       </c>
-      <c r="B210" s="47"/>
-      <c r="C210" s="40" t="s">
+      <c r="B210" s="51"/>
+      <c r="C210" s="38" t="s">
         <v>438</v>
       </c>
       <c r="D210" s="10" t="s">
@@ -8696,8 +8726,8 @@
       <c r="A211" s="18">
         <v>196</v>
       </c>
-      <c r="B211" s="47"/>
-      <c r="C211" s="41"/>
+      <c r="B211" s="51"/>
+      <c r="C211" s="39"/>
       <c r="D211" s="10" t="s">
         <v>441</v>
       </c>
@@ -8721,8 +8751,8 @@
       <c r="A212" s="18">
         <v>197</v>
       </c>
-      <c r="B212" s="47"/>
-      <c r="C212" s="42"/>
+      <c r="B212" s="51"/>
+      <c r="C212" s="40"/>
       <c r="D212" s="10" t="s">
         <v>443</v>
       </c>
@@ -8746,7 +8776,7 @@
       <c r="A213" s="18">
         <v>198</v>
       </c>
-      <c r="B213" s="47"/>
+      <c r="B213" s="51"/>
       <c r="C213" s="22" t="s">
         <v>445</v>
       </c>
@@ -8773,7 +8803,7 @@
       <c r="A214" s="18">
         <v>199</v>
       </c>
-      <c r="B214" s="47"/>
+      <c r="B214" s="51"/>
       <c r="C214" s="22" t="s">
         <v>448</v>
       </c>
@@ -8800,8 +8830,8 @@
       <c r="A215" s="18">
         <v>200</v>
       </c>
-      <c r="B215" s="47"/>
-      <c r="C215" s="40" t="s">
+      <c r="B215" s="51"/>
+      <c r="C215" s="38" t="s">
         <v>451</v>
       </c>
       <c r="D215" s="10" t="s">
@@ -8827,8 +8857,8 @@
       <c r="A216" s="18">
         <v>201</v>
       </c>
-      <c r="B216" s="47"/>
-      <c r="C216" s="41"/>
+      <c r="B216" s="51"/>
+      <c r="C216" s="39"/>
       <c r="D216" s="10" t="s">
         <v>452</v>
       </c>
@@ -8852,8 +8882,8 @@
       <c r="A217" s="18">
         <v>202</v>
       </c>
-      <c r="B217" s="47"/>
-      <c r="C217" s="42"/>
+      <c r="B217" s="51"/>
+      <c r="C217" s="40"/>
       <c r="D217" s="10" t="s">
         <v>452</v>
       </c>
@@ -8877,7 +8907,7 @@
       <c r="A218" s="18">
         <v>203</v>
       </c>
-      <c r="B218" s="47"/>
+      <c r="B218" s="51"/>
       <c r="C218" s="22" t="s">
         <v>398</v>
       </c>
@@ -8904,7 +8934,7 @@
       <c r="A219" s="18">
         <v>204</v>
       </c>
-      <c r="B219" s="47"/>
+      <c r="B219" s="51"/>
       <c r="C219" s="22" t="s">
         <v>423</v>
       </c>
@@ -8931,7 +8961,7 @@
       <c r="A220" s="18">
         <v>205</v>
       </c>
-      <c r="B220" s="48"/>
+      <c r="B220" s="52"/>
       <c r="C220" s="22" t="s">
         <v>459</v>
       </c>
@@ -8958,7 +8988,7 @@
       <c r="A221" s="18">
         <v>206</v>
       </c>
-      <c r="B221" s="56" t="s">
+      <c r="B221" s="47" t="s">
         <v>462</v>
       </c>
       <c r="C221" s="22" t="s">
@@ -8987,8 +9017,8 @@
       <c r="A222" s="18">
         <v>207</v>
       </c>
-      <c r="B222" s="57"/>
-      <c r="C222" s="40" t="s">
+      <c r="B222" s="48"/>
+      <c r="C222" s="38" t="s">
         <v>438</v>
       </c>
       <c r="D222" s="10" t="s">
@@ -9014,8 +9044,8 @@
       <c r="A223" s="18">
         <v>208</v>
       </c>
-      <c r="B223" s="57"/>
-      <c r="C223" s="41"/>
+      <c r="B223" s="48"/>
+      <c r="C223" s="39"/>
       <c r="D223" s="10" t="s">
         <v>475</v>
       </c>
@@ -9039,8 +9069,8 @@
       <c r="A224" s="18">
         <v>209</v>
       </c>
-      <c r="B224" s="57"/>
-      <c r="C224" s="42"/>
+      <c r="B224" s="48"/>
+      <c r="C224" s="40"/>
       <c r="D224" s="10" t="s">
         <v>475</v>
       </c>
@@ -9064,7 +9094,7 @@
       <c r="A225" s="18">
         <v>210</v>
       </c>
-      <c r="B225" s="57"/>
+      <c r="B225" s="48"/>
       <c r="C225" s="22" t="s">
         <v>448</v>
       </c>
@@ -9091,8 +9121,8 @@
       <c r="A226" s="18">
         <v>211</v>
       </c>
-      <c r="B226" s="57"/>
-      <c r="C226" s="40" t="s">
+      <c r="B226" s="48"/>
+      <c r="C226" s="38" t="s">
         <v>451</v>
       </c>
       <c r="D226" s="10" t="s">
@@ -9118,8 +9148,8 @@
       <c r="A227" s="18">
         <v>212</v>
       </c>
-      <c r="B227" s="57"/>
-      <c r="C227" s="41"/>
+      <c r="B227" s="48"/>
+      <c r="C227" s="39"/>
       <c r="D227" s="10" t="s">
         <v>477</v>
       </c>
@@ -9143,8 +9173,8 @@
       <c r="A228" s="18">
         <v>213</v>
       </c>
-      <c r="B228" s="57"/>
-      <c r="C228" s="42"/>
+      <c r="B228" s="48"/>
+      <c r="C228" s="40"/>
       <c r="D228" s="10" t="s">
         <v>477</v>
       </c>
@@ -9168,7 +9198,7 @@
       <c r="A229" s="18">
         <v>214</v>
       </c>
-      <c r="B229" s="57"/>
+      <c r="B229" s="48"/>
       <c r="C229" s="22" t="s">
         <v>398</v>
       </c>
@@ -9195,7 +9225,7 @@
       <c r="A230" s="18">
         <v>215</v>
       </c>
-      <c r="B230" s="58"/>
+      <c r="B230" s="49"/>
       <c r="C230" s="22" t="s">
         <v>423</v>
       </c>
@@ -9222,7 +9252,7 @@
       <c r="A231" s="18">
         <v>216</v>
       </c>
-      <c r="B231" s="43" t="s">
+      <c r="B231" s="41" t="s">
         <v>465</v>
       </c>
       <c r="C231" s="22" t="s">
@@ -9251,8 +9281,8 @@
       <c r="A232" s="18">
         <v>217</v>
       </c>
-      <c r="B232" s="44"/>
-      <c r="C232" s="40" t="s">
+      <c r="B232" s="42"/>
+      <c r="C232" s="38" t="s">
         <v>438</v>
       </c>
       <c r="D232" s="10" t="s">
@@ -9278,8 +9308,8 @@
       <c r="A233" s="18">
         <v>218</v>
       </c>
-      <c r="B233" s="44"/>
-      <c r="C233" s="41"/>
+      <c r="B233" s="42"/>
+      <c r="C233" s="39"/>
       <c r="D233" s="10" t="s">
         <v>469</v>
       </c>
@@ -9303,8 +9333,8 @@
       <c r="A234" s="18">
         <v>219</v>
       </c>
-      <c r="B234" s="44"/>
-      <c r="C234" s="42"/>
+      <c r="B234" s="42"/>
+      <c r="C234" s="40"/>
       <c r="D234" s="10" t="s">
         <v>469</v>
       </c>
@@ -9328,7 +9358,7 @@
       <c r="A235" s="18">
         <v>220</v>
       </c>
-      <c r="B235" s="44"/>
+      <c r="B235" s="42"/>
       <c r="C235" s="22" t="s">
         <v>448</v>
       </c>
@@ -9355,8 +9385,8 @@
       <c r="A236" s="18">
         <v>221</v>
       </c>
-      <c r="B236" s="44"/>
-      <c r="C236" s="40" t="s">
+      <c r="B236" s="42"/>
+      <c r="C236" s="38" t="s">
         <v>451</v>
       </c>
       <c r="D236" s="10" t="s">
@@ -9382,8 +9412,8 @@
       <c r="A237" s="18">
         <v>222</v>
       </c>
-      <c r="B237" s="44"/>
-      <c r="C237" s="41"/>
+      <c r="B237" s="42"/>
+      <c r="C237" s="39"/>
       <c r="D237" s="10" t="s">
         <v>471</v>
       </c>
@@ -9407,8 +9437,8 @@
       <c r="A238" s="18">
         <v>223</v>
       </c>
-      <c r="B238" s="44"/>
-      <c r="C238" s="42"/>
+      <c r="B238" s="42"/>
+      <c r="C238" s="40"/>
       <c r="D238" s="10" t="s">
         <v>471</v>
       </c>
@@ -9432,7 +9462,7 @@
       <c r="A239" s="18">
         <v>224</v>
       </c>
-      <c r="B239" s="44"/>
+      <c r="B239" s="42"/>
       <c r="C239" s="22" t="s">
         <v>398</v>
       </c>
@@ -9459,7 +9489,7 @@
       <c r="A240" s="18">
         <v>225</v>
       </c>
-      <c r="B240" s="44"/>
+      <c r="B240" s="42"/>
       <c r="C240" s="22" t="s">
         <v>423</v>
       </c>
@@ -9486,7 +9516,7 @@
       <c r="A241" s="18">
         <v>226</v>
       </c>
-      <c r="B241" s="45"/>
+      <c r="B241" s="43"/>
       <c r="C241" s="22" t="s">
         <v>445</v>
       </c>
@@ -9513,7 +9543,7 @@
       <c r="A242" s="18">
         <v>227</v>
       </c>
-      <c r="B242" s="43" t="s">
+      <c r="B242" s="41" t="s">
         <v>480</v>
       </c>
       <c r="C242" s="22" t="s">
@@ -9542,7 +9572,7 @@
       <c r="A243" s="18">
         <v>228</v>
       </c>
-      <c r="B243" s="44"/>
+      <c r="B243" s="42"/>
       <c r="C243" s="22" t="s">
         <v>483</v>
       </c>
@@ -9569,7 +9599,7 @@
       <c r="A244" s="18">
         <v>229</v>
       </c>
-      <c r="B244" s="44"/>
+      <c r="B244" s="42"/>
       <c r="C244" s="22" t="s">
         <v>486</v>
       </c>
@@ -9596,7 +9626,7 @@
       <c r="A245" s="18">
         <v>230</v>
       </c>
-      <c r="B245" s="44"/>
+      <c r="B245" s="42"/>
       <c r="C245" s="22"/>
       <c r="D245" s="10" t="s">
         <v>489</v>
@@ -9621,7 +9651,7 @@
       <c r="A246" s="18">
         <v>231</v>
       </c>
-      <c r="B246" s="45"/>
+      <c r="B246" s="43"/>
       <c r="C246" s="22"/>
       <c r="D246" s="10" t="s">
         <v>491</v>
@@ -9646,7 +9676,7 @@
       <c r="A247" s="18">
         <v>232</v>
       </c>
-      <c r="B247" s="43" t="s">
+      <c r="B247" s="41" t="s">
         <v>493</v>
       </c>
       <c r="C247" s="28" t="s">
@@ -9669,8 +9699,8 @@
       <c r="A248" s="18">
         <v>233</v>
       </c>
-      <c r="B248" s="44"/>
-      <c r="C248" s="40" t="s">
+      <c r="B248" s="42"/>
+      <c r="C248" s="38" t="s">
         <v>494</v>
       </c>
       <c r="D248" s="10" t="s">
@@ -9690,8 +9720,8 @@
       <c r="A249" s="18">
         <v>234</v>
       </c>
-      <c r="B249" s="44"/>
-      <c r="C249" s="41"/>
+      <c r="B249" s="42"/>
+      <c r="C249" s="39"/>
       <c r="D249" s="10" t="s">
         <v>500</v>
       </c>
@@ -9709,8 +9739,8 @@
       <c r="A250" s="18">
         <v>235</v>
       </c>
-      <c r="B250" s="44"/>
-      <c r="C250" s="41"/>
+      <c r="B250" s="42"/>
+      <c r="C250" s="39"/>
       <c r="D250" s="10" t="s">
         <v>501</v>
       </c>
@@ -9728,8 +9758,8 @@
       <c r="A251" s="18">
         <v>236</v>
       </c>
-      <c r="B251" s="44"/>
-      <c r="C251" s="42"/>
+      <c r="B251" s="42"/>
+      <c r="C251" s="40"/>
       <c r="D251" s="10" t="s">
         <v>503</v>
       </c>
@@ -9747,7 +9777,7 @@
       <c r="A252" s="18">
         <v>237</v>
       </c>
-      <c r="B252" s="44"/>
+      <c r="B252" s="42"/>
       <c r="C252" s="28" t="s">
         <v>505</v>
       </c>
@@ -9768,7 +9798,7 @@
       <c r="A253" s="18">
         <v>238</v>
       </c>
-      <c r="B253" s="44"/>
+      <c r="B253" s="42"/>
       <c r="C253" s="28" t="s">
         <v>508</v>
       </c>
@@ -9789,7 +9819,7 @@
       <c r="A254" s="18">
         <v>239</v>
       </c>
-      <c r="B254" s="44"/>
+      <c r="B254" s="42"/>
       <c r="C254" s="28" t="s">
         <v>511</v>
       </c>
@@ -9810,7 +9840,7 @@
       <c r="A255" s="18">
         <v>240</v>
       </c>
-      <c r="B255" s="44"/>
+      <c r="B255" s="42"/>
       <c r="C255" s="28" t="s">
         <v>514</v>
       </c>
@@ -9831,7 +9861,7 @@
       <c r="A256" s="18">
         <v>241</v>
       </c>
-      <c r="B256" s="45"/>
+      <c r="B256" s="43"/>
       <c r="C256" s="28" t="s">
         <v>517</v>
       </c>
@@ -9852,7 +9882,7 @@
       <c r="A257" s="18">
         <v>242</v>
       </c>
-      <c r="B257" s="43" t="s">
+      <c r="B257" s="41" t="s">
         <v>520</v>
       </c>
       <c r="C257" s="28" t="s">
@@ -9881,7 +9911,7 @@
       <c r="A258" s="18">
         <v>243</v>
       </c>
-      <c r="B258" s="44"/>
+      <c r="B258" s="42"/>
       <c r="C258" s="22" t="s">
         <v>523</v>
       </c>
@@ -9908,7 +9938,7 @@
       <c r="A259" s="18">
         <v>244</v>
       </c>
-      <c r="B259" s="44"/>
+      <c r="B259" s="42"/>
       <c r="C259" s="22" t="s">
         <v>177</v>
       </c>
@@ -9935,8 +9965,8 @@
       <c r="A260" s="18">
         <v>245</v>
       </c>
-      <c r="B260" s="44"/>
-      <c r="C260" s="40" t="s">
+      <c r="B260" s="42"/>
+      <c r="C260" s="38" t="s">
         <v>528</v>
       </c>
       <c r="D260" s="10" t="s">
@@ -9962,8 +9992,8 @@
       <c r="A261" s="18">
         <v>246</v>
       </c>
-      <c r="B261" s="44"/>
-      <c r="C261" s="41"/>
+      <c r="B261" s="42"/>
+      <c r="C261" s="39"/>
       <c r="D261" s="10" t="s">
         <v>531</v>
       </c>
@@ -9987,8 +10017,8 @@
       <c r="A262" s="18">
         <v>247</v>
       </c>
-      <c r="B262" s="44"/>
-      <c r="C262" s="42"/>
+      <c r="B262" s="42"/>
+      <c r="C262" s="40"/>
       <c r="D262" s="10" t="s">
         <v>533</v>
       </c>
@@ -10012,7 +10042,7 @@
       <c r="A263" s="18">
         <v>248</v>
       </c>
-      <c r="B263" s="44"/>
+      <c r="B263" s="42"/>
       <c r="C263" s="30" t="s">
         <v>535</v>
       </c>
@@ -10039,7 +10069,7 @@
       <c r="A264" s="18">
         <v>249</v>
       </c>
-      <c r="B264" s="44"/>
+      <c r="B264" s="42"/>
       <c r="C264" s="28" t="s">
         <v>538</v>
       </c>
@@ -10066,7 +10096,7 @@
       <c r="A265" s="18">
         <v>250</v>
       </c>
-      <c r="B265" s="44"/>
+      <c r="B265" s="42"/>
       <c r="C265" s="28" t="s">
         <v>541</v>
       </c>
@@ -10093,7 +10123,7 @@
       <c r="A266" s="18">
         <v>251</v>
       </c>
-      <c r="B266" s="45"/>
+      <c r="B266" s="43"/>
       <c r="C266" s="28" t="s">
         <v>544</v>
       </c>
@@ -10120,7 +10150,7 @@
       <c r="A267" s="18">
         <v>252</v>
       </c>
-      <c r="B267" s="43" t="s">
+      <c r="B267" s="41" t="s">
         <v>547</v>
       </c>
       <c r="C267" s="28" t="s">
@@ -10149,7 +10179,7 @@
       <c r="A268" s="18">
         <v>253</v>
       </c>
-      <c r="B268" s="44"/>
+      <c r="B268" s="42"/>
       <c r="C268" s="28" t="s">
         <v>550</v>
       </c>
@@ -10176,7 +10206,7 @@
       <c r="A269" s="18">
         <v>254</v>
       </c>
-      <c r="B269" s="44"/>
+      <c r="B269" s="42"/>
       <c r="C269" s="28" t="s">
         <v>553</v>
       </c>
@@ -10203,7 +10233,7 @@
       <c r="A270" s="18">
         <v>255</v>
       </c>
-      <c r="B270" s="44"/>
+      <c r="B270" s="42"/>
       <c r="C270" s="28" t="s">
         <v>556</v>
       </c>
@@ -10230,7 +10260,7 @@
       <c r="A271" s="18">
         <v>256</v>
       </c>
-      <c r="B271" s="44"/>
+      <c r="B271" s="42"/>
       <c r="C271" s="28" t="s">
         <v>541</v>
       </c>
@@ -10257,7 +10287,7 @@
       <c r="A272" s="18">
         <v>257</v>
       </c>
-      <c r="B272" s="45"/>
+      <c r="B272" s="43"/>
       <c r="C272" s="28" t="s">
         <v>538</v>
       </c>
@@ -10284,7 +10314,7 @@
       <c r="A273" s="18">
         <v>258</v>
       </c>
-      <c r="B273" s="43" t="s">
+      <c r="B273" s="41" t="s">
         <v>561</v>
       </c>
       <c r="C273" s="28" t="s">
@@ -10313,7 +10343,7 @@
       <c r="A274" s="18">
         <v>259</v>
       </c>
-      <c r="B274" s="44"/>
+      <c r="B274" s="42"/>
       <c r="C274" s="28" t="s">
         <v>523</v>
       </c>
@@ -10340,7 +10370,7 @@
       <c r="A275" s="18">
         <v>260</v>
       </c>
-      <c r="B275" s="44"/>
+      <c r="B275" s="42"/>
       <c r="C275" s="28" t="s">
         <v>177</v>
       </c>
@@ -10367,8 +10397,8 @@
       <c r="A276" s="18">
         <v>261</v>
       </c>
-      <c r="B276" s="44"/>
-      <c r="C276" s="40" t="s">
+      <c r="B276" s="42"/>
+      <c r="C276" s="38" t="s">
         <v>528</v>
       </c>
       <c r="D276" s="10" t="s">
@@ -10394,8 +10424,8 @@
       <c r="A277" s="18">
         <v>262</v>
       </c>
-      <c r="B277" s="44"/>
-      <c r="C277" s="41"/>
+      <c r="B277" s="42"/>
+      <c r="C277" s="39"/>
       <c r="D277" s="10" t="s">
         <v>531</v>
       </c>
@@ -10419,8 +10449,8 @@
       <c r="A278" s="18">
         <v>263</v>
       </c>
-      <c r="B278" s="44"/>
-      <c r="C278" s="42"/>
+      <c r="B278" s="42"/>
+      <c r="C278" s="40"/>
       <c r="D278" s="10" t="s">
         <v>533</v>
       </c>
@@ -10444,7 +10474,7 @@
       <c r="A279" s="18">
         <v>264</v>
       </c>
-      <c r="B279" s="44"/>
+      <c r="B279" s="42"/>
       <c r="C279" s="30" t="s">
         <v>535</v>
       </c>
@@ -10471,7 +10501,7 @@
       <c r="A280" s="18">
         <v>265</v>
       </c>
-      <c r="B280" s="44"/>
+      <c r="B280" s="42"/>
       <c r="C280" s="28" t="s">
         <v>538</v>
       </c>
@@ -10498,7 +10528,7 @@
       <c r="A281" s="18">
         <v>266</v>
       </c>
-      <c r="B281" s="45"/>
+      <c r="B281" s="43"/>
       <c r="C281" s="28" t="s">
         <v>541</v>
       </c>
@@ -10525,7 +10555,7 @@
       <c r="A282" s="18">
         <v>267</v>
       </c>
-      <c r="B282" s="43" t="s">
+      <c r="B282" s="41" t="s">
         <v>571</v>
       </c>
       <c r="C282" s="28" t="s">
@@ -10548,7 +10578,7 @@
       <c r="A283" s="18">
         <v>268</v>
       </c>
-      <c r="B283" s="44"/>
+      <c r="B283" s="42"/>
       <c r="C283" s="28" t="s">
         <v>523</v>
       </c>
@@ -10569,7 +10599,7 @@
       <c r="A284" s="18">
         <v>269</v>
       </c>
-      <c r="B284" s="44"/>
+      <c r="B284" s="42"/>
       <c r="C284" s="28" t="s">
         <v>177</v>
       </c>
@@ -10590,7 +10620,7 @@
       <c r="A285" s="18">
         <v>270</v>
       </c>
-      <c r="B285" s="44"/>
+      <c r="B285" s="42"/>
       <c r="C285" s="28" t="s">
         <v>541</v>
       </c>
@@ -10611,7 +10641,7 @@
       <c r="A286" s="18">
         <v>271</v>
       </c>
-      <c r="B286" s="44"/>
+      <c r="B286" s="42"/>
       <c r="C286" s="28" t="s">
         <v>538</v>
       </c>
@@ -10632,8 +10662,8 @@
       <c r="A287" s="18">
         <v>272</v>
       </c>
-      <c r="B287" s="44"/>
-      <c r="C287" s="40" t="s">
+      <c r="B287" s="42"/>
+      <c r="C287" s="38" t="s">
         <v>528</v>
       </c>
       <c r="D287" s="10" t="s">
@@ -10653,8 +10683,8 @@
       <c r="A288" s="18">
         <v>273</v>
       </c>
-      <c r="B288" s="44"/>
-      <c r="C288" s="41"/>
+      <c r="B288" s="42"/>
+      <c r="C288" s="39"/>
       <c r="D288" s="10" t="s">
         <v>531</v>
       </c>
@@ -10672,8 +10702,8 @@
       <c r="A289" s="18">
         <v>274</v>
       </c>
-      <c r="B289" s="44"/>
-      <c r="C289" s="41"/>
+      <c r="B289" s="42"/>
+      <c r="C289" s="39"/>
       <c r="D289" s="10" t="s">
         <v>533</v>
       </c>
@@ -10691,8 +10721,8 @@
       <c r="A290" s="18">
         <v>275</v>
       </c>
-      <c r="B290" s="44"/>
-      <c r="C290" s="41"/>
+      <c r="B290" s="42"/>
+      <c r="C290" s="39"/>
       <c r="D290" s="10" t="s">
         <v>581</v>
       </c>
@@ -10710,8 +10740,8 @@
       <c r="A291" s="18">
         <v>276</v>
       </c>
-      <c r="B291" s="44"/>
-      <c r="C291" s="41"/>
+      <c r="B291" s="42"/>
+      <c r="C291" s="39"/>
       <c r="D291" s="10" t="s">
         <v>578</v>
       </c>
@@ -10729,8 +10759,8 @@
       <c r="A292" s="18">
         <v>277</v>
       </c>
-      <c r="B292" s="45"/>
-      <c r="C292" s="42"/>
+      <c r="B292" s="43"/>
+      <c r="C292" s="40"/>
       <c r="D292" s="10" t="s">
         <v>578</v>
       </c>
@@ -10748,7 +10778,7 @@
       <c r="A293" s="18">
         <v>278</v>
       </c>
-      <c r="B293" s="43" t="s">
+      <c r="B293" s="41" t="s">
         <v>585</v>
       </c>
       <c r="C293" s="28" t="s">
@@ -10771,7 +10801,7 @@
       <c r="A294" s="18">
         <v>279</v>
       </c>
-      <c r="B294" s="44"/>
+      <c r="B294" s="42"/>
       <c r="C294" s="28" t="s">
         <v>523</v>
       </c>
@@ -10792,7 +10822,7 @@
       <c r="A295" s="18">
         <v>280</v>
       </c>
-      <c r="B295" s="44"/>
+      <c r="B295" s="42"/>
       <c r="C295" s="28" t="s">
         <v>177</v>
       </c>
@@ -10813,7 +10843,7 @@
       <c r="A296" s="18">
         <v>281</v>
       </c>
-      <c r="B296" s="44"/>
+      <c r="B296" s="42"/>
       <c r="C296" s="28" t="s">
         <v>538</v>
       </c>
@@ -10834,8 +10864,8 @@
       <c r="A297" s="18">
         <v>282</v>
       </c>
-      <c r="B297" s="44"/>
-      <c r="C297" s="40" t="s">
+      <c r="B297" s="42"/>
+      <c r="C297" s="38" t="s">
         <v>528</v>
       </c>
       <c r="D297" s="10" t="s">
@@ -10855,8 +10885,8 @@
       <c r="A298" s="18">
         <v>283</v>
       </c>
-      <c r="B298" s="44"/>
-      <c r="C298" s="41"/>
+      <c r="B298" s="42"/>
+      <c r="C298" s="39"/>
       <c r="D298" s="10" t="s">
         <v>531</v>
       </c>
@@ -10874,8 +10904,8 @@
       <c r="A299" s="18">
         <v>284</v>
       </c>
-      <c r="B299" s="44"/>
-      <c r="C299" s="41"/>
+      <c r="B299" s="42"/>
+      <c r="C299" s="39"/>
       <c r="D299" s="10" t="s">
         <v>533</v>
       </c>
@@ -10893,8 +10923,8 @@
       <c r="A300" s="18">
         <v>285</v>
       </c>
-      <c r="B300" s="44"/>
-      <c r="C300" s="42"/>
+      <c r="B300" s="42"/>
+      <c r="C300" s="40"/>
       <c r="D300" s="10" t="s">
         <v>591</v>
       </c>
@@ -10912,7 +10942,7 @@
       <c r="A301" s="18">
         <v>286</v>
       </c>
-      <c r="B301" s="44"/>
+      <c r="B301" s="42"/>
       <c r="C301" s="28" t="s">
         <v>593</v>
       </c>
@@ -10933,7 +10963,7 @@
       <c r="A302" s="18">
         <v>287</v>
       </c>
-      <c r="B302" s="45"/>
+      <c r="B302" s="43"/>
       <c r="C302" s="28" t="s">
         <v>541</v>
       </c>
@@ -10954,7 +10984,7 @@
       <c r="A303" s="18">
         <v>288</v>
       </c>
-      <c r="B303" s="37" t="s">
+      <c r="B303" s="57" t="s">
         <v>597</v>
       </c>
       <c r="C303" s="28" t="s">
@@ -10977,7 +11007,7 @@
       <c r="A304" s="18">
         <v>289</v>
       </c>
-      <c r="B304" s="38"/>
+      <c r="B304" s="58"/>
       <c r="C304" s="28" t="s">
         <v>593</v>
       </c>
@@ -10998,7 +11028,7 @@
       <c r="A305" s="18">
         <v>290</v>
       </c>
-      <c r="B305" s="38"/>
+      <c r="B305" s="58"/>
       <c r="C305" s="28" t="s">
         <v>541</v>
       </c>
@@ -11019,7 +11049,7 @@
       <c r="A306" s="18">
         <v>291</v>
       </c>
-      <c r="B306" s="38"/>
+      <c r="B306" s="58"/>
       <c r="C306" s="28" t="s">
         <v>538</v>
       </c>
@@ -11040,7 +11070,7 @@
       <c r="A307" s="18">
         <v>292</v>
       </c>
-      <c r="B307" s="39"/>
+      <c r="B307" s="59"/>
       <c r="C307" s="28" t="s">
         <v>602</v>
       </c>
@@ -11061,7 +11091,7 @@
       <c r="A308" s="18">
         <v>293</v>
       </c>
-      <c r="B308" s="43" t="s">
+      <c r="B308" s="41" t="s">
         <v>605</v>
       </c>
       <c r="C308" s="28" t="s">
@@ -11084,7 +11114,7 @@
       <c r="A309" s="18">
         <v>294</v>
       </c>
-      <c r="B309" s="44"/>
+      <c r="B309" s="42"/>
       <c r="C309" s="28" t="s">
         <v>541</v>
       </c>
@@ -11105,7 +11135,7 @@
       <c r="A310" s="18">
         <v>295</v>
       </c>
-      <c r="B310" s="44"/>
+      <c r="B310" s="42"/>
       <c r="C310" s="28" t="s">
         <v>538</v>
       </c>
@@ -11126,8 +11156,8 @@
       <c r="A311" s="18">
         <v>296</v>
       </c>
-      <c r="B311" s="44"/>
-      <c r="C311" s="40" t="s">
+      <c r="B311" s="42"/>
+      <c r="C311" s="38" t="s">
         <v>528</v>
       </c>
       <c r="D311" s="10" t="s">
@@ -11147,8 +11177,8 @@
       <c r="A312" s="18">
         <v>297</v>
       </c>
-      <c r="B312" s="44"/>
-      <c r="C312" s="41"/>
+      <c r="B312" s="42"/>
+      <c r="C312" s="39"/>
       <c r="D312" s="10" t="s">
         <v>531</v>
       </c>
@@ -11166,8 +11196,8 @@
       <c r="A313" s="18">
         <v>298</v>
       </c>
-      <c r="B313" s="44"/>
-      <c r="C313" s="42"/>
+      <c r="B313" s="42"/>
+      <c r="C313" s="40"/>
       <c r="D313" s="10" t="s">
         <v>533</v>
       </c>
@@ -11185,8 +11215,8 @@
       <c r="A314" s="18">
         <v>299</v>
       </c>
-      <c r="B314" s="44"/>
-      <c r="C314" s="40" t="s">
+      <c r="B314" s="42"/>
+      <c r="C314" s="38" t="s">
         <v>610</v>
       </c>
       <c r="D314" s="10" t="s">
@@ -11206,8 +11236,8 @@
       <c r="A315" s="18">
         <v>300</v>
       </c>
-      <c r="B315" s="44"/>
-      <c r="C315" s="41"/>
+      <c r="B315" s="42"/>
+      <c r="C315" s="39"/>
       <c r="D315" s="10" t="s">
         <v>614</v>
       </c>
@@ -11225,8 +11255,8 @@
       <c r="A316" s="18">
         <v>301</v>
       </c>
-      <c r="B316" s="44"/>
-      <c r="C316" s="42"/>
+      <c r="B316" s="42"/>
+      <c r="C316" s="40"/>
       <c r="D316" s="10" t="s">
         <v>615</v>
       </c>
@@ -11244,8 +11274,8 @@
       <c r="A317" s="18">
         <v>302</v>
       </c>
-      <c r="B317" s="44"/>
-      <c r="C317" s="40" t="s">
+      <c r="B317" s="42"/>
+      <c r="C317" s="38" t="s">
         <v>617</v>
       </c>
       <c r="D317" s="10" t="s">
@@ -11265,8 +11295,8 @@
       <c r="A318" s="18">
         <v>303</v>
       </c>
-      <c r="B318" s="44"/>
-      <c r="C318" s="42"/>
+      <c r="B318" s="42"/>
+      <c r="C318" s="40"/>
       <c r="D318" s="10" t="s">
         <v>620</v>
       </c>
@@ -11284,7 +11314,7 @@
       <c r="A319" s="18">
         <v>304</v>
       </c>
-      <c r="B319" s="45"/>
+      <c r="B319" s="43"/>
       <c r="C319" s="28" t="s">
         <v>622</v>
       </c>
@@ -11596,6 +11626,74 @@
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="B303:B307"/>
+    <mergeCell ref="C311:C313"/>
+    <mergeCell ref="C314:C316"/>
+    <mergeCell ref="C317:C318"/>
+    <mergeCell ref="B308:B319"/>
+    <mergeCell ref="C276:C278"/>
+    <mergeCell ref="B273:B281"/>
+    <mergeCell ref="C287:C292"/>
+    <mergeCell ref="B282:B292"/>
+    <mergeCell ref="C297:C300"/>
+    <mergeCell ref="B293:B302"/>
+    <mergeCell ref="C248:C251"/>
+    <mergeCell ref="B247:B256"/>
+    <mergeCell ref="C260:C262"/>
+    <mergeCell ref="B257:B266"/>
+    <mergeCell ref="B267:B272"/>
+    <mergeCell ref="B204:B208"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="B176:B179"/>
+    <mergeCell ref="C164:C165"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="C169:C170"/>
+    <mergeCell ref="C171:C173"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B161:B175"/>
+    <mergeCell ref="C162:C163"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="B180:B183"/>
+    <mergeCell ref="B184:B187"/>
+    <mergeCell ref="B188:B192"/>
+    <mergeCell ref="B193:B203"/>
+    <mergeCell ref="B147:B149"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="B150:B156"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="B133:B146"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="C135:C139"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C143:C145"/>
+    <mergeCell ref="B115:B132"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C124:C126"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C129:C131"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B22:B36"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="B100:B102"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="B82:B89"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="B65:B81"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="C78:C80"/>
     <mergeCell ref="C236:C238"/>
     <mergeCell ref="B231:B241"/>
     <mergeCell ref="B242:B246"/>
@@ -11612,74 +11710,6 @@
     <mergeCell ref="B111:B114"/>
     <mergeCell ref="B53:B57"/>
     <mergeCell ref="B90:B97"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="B100:B102"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B82:B89"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="C60:C64"/>
-    <mergeCell ref="B65:B81"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B22:B36"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B115:B132"/>
-    <mergeCell ref="C116:C119"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C124:C126"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="C129:C131"/>
-    <mergeCell ref="B133:B146"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="C135:C139"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C143:C145"/>
-    <mergeCell ref="B147:B149"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="B150:B156"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="B180:B183"/>
-    <mergeCell ref="B184:B187"/>
-    <mergeCell ref="B188:B192"/>
-    <mergeCell ref="B193:B203"/>
-    <mergeCell ref="B204:B208"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="B176:B179"/>
-    <mergeCell ref="C164:C165"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="C169:C170"/>
-    <mergeCell ref="C171:C173"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B161:B175"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="C248:C251"/>
-    <mergeCell ref="B247:B256"/>
-    <mergeCell ref="C260:C262"/>
-    <mergeCell ref="B257:B266"/>
-    <mergeCell ref="B267:B272"/>
-    <mergeCell ref="C276:C278"/>
-    <mergeCell ref="B273:B281"/>
-    <mergeCell ref="C287:C292"/>
-    <mergeCell ref="B282:B292"/>
-    <mergeCell ref="C297:C300"/>
-    <mergeCell ref="B293:B302"/>
-    <mergeCell ref="B303:B307"/>
-    <mergeCell ref="C311:C313"/>
-    <mergeCell ref="C314:C316"/>
-    <mergeCell ref="C317:C318"/>
-    <mergeCell ref="B308:B319"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G257:I281 G16:I246">

</xml_diff>

<commit_message>
test chet do huan luyen
</commit_message>
<xml_diff>
--- a/TestCase-Reup.xlsx
+++ b/TestCase-Reup.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ChuyenDe12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952D9E51-FF8B-4B4A-83C4-FB6F26BAE0B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2626,7 +2625,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2790,7 +2789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2849,6 +2848,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2861,22 +2872,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2888,38 +2911,59 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3265,11 +3309,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J203" sqref="A13:K322"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150:B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3459,11 +3503,11 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="2"/>
       <c r="K13" s="9"/>
     </row>
@@ -3484,11 +3528,11 @@
       <c r="F14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="2"/>
       <c r="K14" s="9"/>
     </row>
@@ -3531,7 +3575,7 @@
       <c r="A16" s="4">
         <v>1</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -3560,7 +3604,7 @@
       <c r="A17" s="4">
         <v>2</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="4" t="s">
         <v>23</v>
       </c>
@@ -3589,7 +3633,7 @@
       <c r="A18" s="4">
         <v>3</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
@@ -3618,7 +3662,7 @@
       <c r="A19" s="4">
         <v>4</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
@@ -3647,7 +3691,7 @@
       <c r="A20" s="4">
         <v>5</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3676,7 +3720,7 @@
       <c r="A21" s="4">
         <v>6</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
@@ -3703,10 +3747,10 @@
       <c r="A22" s="4">
         <v>7</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="27" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -3732,8 +3776,8 @@
       <c r="A23" s="4">
         <v>8</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="5" t="s">
         <v>42</v>
       </c>
@@ -3757,8 +3801,8 @@
       <c r="A24" s="4">
         <v>9</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="23" t="s">
+      <c r="B24" s="25"/>
+      <c r="C24" s="27" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -3784,8 +3828,8 @@
       <c r="A25" s="4">
         <v>10</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="5" t="s">
         <v>42</v>
       </c>
@@ -3809,7 +3853,7 @@
       <c r="A26" s="4">
         <v>11</v>
       </c>
-      <c r="B26" s="21"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="4" t="s">
         <v>46</v>
       </c>
@@ -3836,7 +3880,7 @@
       <c r="A27" s="4">
         <v>12</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="4" t="s">
         <v>49</v>
       </c>
@@ -3863,7 +3907,7 @@
       <c r="A28" s="4">
         <v>13</v>
       </c>
-      <c r="B28" s="21"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
@@ -3890,7 +3934,7 @@
       <c r="A29" s="4">
         <v>14</v>
       </c>
-      <c r="B29" s="21"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="4" t="s">
         <v>54</v>
       </c>
@@ -3917,7 +3961,7 @@
       <c r="A30" s="4">
         <v>15</v>
       </c>
-      <c r="B30" s="21"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="4" t="s">
         <v>55</v>
       </c>
@@ -3946,7 +3990,7 @@
       <c r="A31" s="4">
         <v>16</v>
       </c>
-      <c r="B31" s="21"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="4" t="s">
         <v>58</v>
       </c>
@@ -3975,7 +4019,7 @@
       <c r="A32" s="4">
         <v>17</v>
       </c>
-      <c r="B32" s="21"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="4" t="s">
         <v>58</v>
       </c>
@@ -4004,7 +4048,7 @@
       <c r="A33" s="4">
         <v>18</v>
       </c>
-      <c r="B33" s="21"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="4" t="s">
         <v>61</v>
       </c>
@@ -4033,7 +4077,7 @@
       <c r="A34" s="4">
         <v>19</v>
       </c>
-      <c r="B34" s="21"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="4" t="s">
         <v>64</v>
       </c>
@@ -4060,7 +4104,7 @@
       <c r="A35" s="4">
         <v>20</v>
       </c>
-      <c r="B35" s="21"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="4" t="s">
         <v>65</v>
       </c>
@@ -4087,7 +4131,7 @@
       <c r="A36" s="4">
         <v>21</v>
       </c>
-      <c r="B36" s="22"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="4" t="s">
         <v>65</v>
       </c>
@@ -4114,7 +4158,7 @@
       <c r="A37" s="4">
         <v>22</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -4143,7 +4187,7 @@
       <c r="A38" s="4">
         <v>23</v>
       </c>
-      <c r="B38" s="21"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="4" t="s">
         <v>71</v>
       </c>
@@ -4172,7 +4216,7 @@
       <c r="A39" s="4">
         <v>24</v>
       </c>
-      <c r="B39" s="21"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="4" t="s">
         <v>74</v>
       </c>
@@ -4201,7 +4245,7 @@
       <c r="A40" s="4">
         <v>25</v>
       </c>
-      <c r="B40" s="21"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="4" t="s">
         <v>76</v>
       </c>
@@ -4230,7 +4274,7 @@
       <c r="A41" s="4">
         <v>26</v>
       </c>
-      <c r="B41" s="21"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="4" t="s">
         <v>79</v>
       </c>
@@ -4259,7 +4303,7 @@
       <c r="A42" s="4">
         <v>27</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="4" t="s">
         <v>81</v>
       </c>
@@ -4286,7 +4330,7 @@
       <c r="A43" s="4">
         <v>28</v>
       </c>
-      <c r="B43" s="22"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="4" t="s">
         <v>84</v>
       </c>
@@ -4313,7 +4357,7 @@
       <c r="A44" s="4">
         <v>29</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -4342,7 +4386,7 @@
       <c r="A45" s="4">
         <v>30</v>
       </c>
-      <c r="B45" s="21"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="4" t="s">
         <v>89</v>
       </c>
@@ -4369,7 +4413,7 @@
       <c r="A46" s="4">
         <v>31</v>
       </c>
-      <c r="B46" s="21"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="4" t="s">
         <v>71</v>
       </c>
@@ -4398,7 +4442,7 @@
       <c r="A47" s="4">
         <v>32</v>
       </c>
-      <c r="B47" s="21"/>
+      <c r="B47" s="25"/>
       <c r="C47" s="4" t="s">
         <v>74</v>
       </c>
@@ -4427,7 +4471,7 @@
       <c r="A48" s="4">
         <v>33</v>
       </c>
-      <c r="B48" s="21"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="4" t="s">
         <v>92</v>
       </c>
@@ -4456,7 +4500,7 @@
       <c r="A49" s="4">
         <v>34</v>
       </c>
-      <c r="B49" s="22"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="4" t="s">
         <v>96</v>
       </c>
@@ -4485,7 +4529,7 @@
       <c r="A50" s="4">
         <v>35</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="38" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -4514,7 +4558,7 @@
       <c r="A51" s="4">
         <v>36</v>
       </c>
-      <c r="B51" s="31"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="4" t="s">
         <v>71</v>
       </c>
@@ -4543,7 +4587,7 @@
       <c r="A52" s="4">
         <v>37</v>
       </c>
-      <c r="B52" s="32"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="4" t="s">
         <v>74</v>
       </c>
@@ -4570,7 +4614,7 @@
       <c r="A53" s="4">
         <v>38</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="24" t="s">
         <v>107</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -4599,7 +4643,7 @@
       <c r="A54" s="4">
         <v>39</v>
       </c>
-      <c r="B54" s="21"/>
+      <c r="B54" s="25"/>
       <c r="C54" s="4" t="s">
         <v>71</v>
       </c>
@@ -4628,7 +4672,7 @@
       <c r="A55" s="4">
         <v>40</v>
       </c>
-      <c r="B55" s="21"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="4" t="s">
         <v>74</v>
       </c>
@@ -4657,7 +4701,7 @@
       <c r="A56" s="4">
         <v>41</v>
       </c>
-      <c r="B56" s="21"/>
+      <c r="B56" s="25"/>
       <c r="C56" s="4" t="s">
         <v>74</v>
       </c>
@@ -4686,7 +4730,7 @@
       <c r="A57" s="4">
         <v>42</v>
       </c>
-      <c r="B57" s="22"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="4" t="s">
         <v>74</v>
       </c>
@@ -4715,10 +4759,10 @@
       <c r="A58" s="4">
         <v>43</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C58" s="37" t="s">
         <v>19</v>
       </c>
       <c r="D58" s="5" t="s">
@@ -4744,8 +4788,8 @@
       <c r="A59" s="4">
         <v>44</v>
       </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="5" t="s">
         <v>124</v>
       </c>
@@ -4769,8 +4813,8 @@
       <c r="A60" s="4">
         <v>45</v>
       </c>
-      <c r="B60" s="27"/>
-      <c r="C60" s="28"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="5" t="s">
         <v>126</v>
       </c>
@@ -4794,8 +4838,8 @@
       <c r="A61" s="4">
         <v>46</v>
       </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="5" t="s">
         <v>128</v>
       </c>
@@ -4819,8 +4863,8 @@
       <c r="A62" s="4">
         <v>47</v>
       </c>
-      <c r="B62" s="27"/>
-      <c r="C62" s="28"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="37"/>
       <c r="D62" s="5" t="s">
         <v>130</v>
       </c>
@@ -4844,10 +4888,10 @@
       <c r="A63" s="4">
         <v>48</v>
       </c>
-      <c r="B63" s="27" t="s">
+      <c r="B63" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="28" t="s">
+      <c r="C63" s="37" t="s">
         <v>133</v>
       </c>
       <c r="D63" s="5" t="s">
@@ -4873,8 +4917,8 @@
       <c r="A64" s="4">
         <v>49</v>
       </c>
-      <c r="B64" s="27"/>
-      <c r="C64" s="28"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="37"/>
       <c r="D64" s="5" t="s">
         <v>136</v>
       </c>
@@ -4898,8 +4942,8 @@
       <c r="A65" s="4">
         <v>50</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="28"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="37"/>
       <c r="D65" s="5" t="s">
         <v>138</v>
       </c>
@@ -4927,8 +4971,8 @@
       <c r="A66" s="4">
         <v>51</v>
       </c>
-      <c r="B66" s="27"/>
-      <c r="C66" s="28"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="37"/>
       <c r="D66" s="5" t="s">
         <v>143</v>
       </c>
@@ -4956,8 +5000,8 @@
       <c r="A67" s="4">
         <v>52</v>
       </c>
-      <c r="B67" s="27"/>
-      <c r="C67" s="28"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="5" t="s">
         <v>146</v>
       </c>
@@ -4983,8 +5027,8 @@
       <c r="A68" s="4">
         <v>53</v>
       </c>
-      <c r="B68" s="27"/>
-      <c r="C68" s="28"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="37"/>
       <c r="D68" s="5" t="s">
         <v>149</v>
       </c>
@@ -5010,8 +5054,8 @@
       <c r="A69" s="4">
         <v>54</v>
       </c>
-      <c r="B69" s="27"/>
-      <c r="C69" s="28" t="s">
+      <c r="B69" s="36"/>
+      <c r="C69" s="37" t="s">
         <v>151</v>
       </c>
       <c r="D69" s="5" t="s">
@@ -5037,8 +5081,8 @@
       <c r="A70" s="4">
         <v>55</v>
       </c>
-      <c r="B70" s="27"/>
-      <c r="C70" s="28"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="37"/>
       <c r="D70" s="5" t="s">
         <v>153</v>
       </c>
@@ -5062,8 +5106,8 @@
       <c r="A71" s="4">
         <v>56</v>
       </c>
-      <c r="B71" s="27"/>
-      <c r="C71" s="28"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="37"/>
       <c r="D71" s="5" t="s">
         <v>155</v>
       </c>
@@ -5087,8 +5131,8 @@
       <c r="A72" s="4">
         <v>57</v>
       </c>
-      <c r="B72" s="27"/>
-      <c r="C72" s="28"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="37"/>
       <c r="D72" s="5" t="s">
         <v>157</v>
       </c>
@@ -5112,8 +5156,8 @@
       <c r="A73" s="4">
         <v>58</v>
       </c>
-      <c r="B73" s="27"/>
-      <c r="C73" s="28"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="37"/>
       <c r="D73" s="5" t="s">
         <v>159</v>
       </c>
@@ -5137,8 +5181,8 @@
       <c r="A74" s="4">
         <v>59</v>
       </c>
-      <c r="B74" s="27"/>
-      <c r="C74" s="28"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="37"/>
       <c r="D74" s="5" t="s">
         <v>161</v>
       </c>
@@ -5162,7 +5206,7 @@
       <c r="A75" s="4">
         <v>60</v>
       </c>
-      <c r="B75" s="27"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="4" t="s">
         <v>163</v>
       </c>
@@ -5189,8 +5233,8 @@
       <c r="A76" s="4">
         <v>61</v>
       </c>
-      <c r="B76" s="27"/>
-      <c r="C76" s="28" t="s">
+      <c r="B76" s="36"/>
+      <c r="C76" s="37" t="s">
         <v>166</v>
       </c>
       <c r="D76" s="5" t="s">
@@ -5216,8 +5260,8 @@
       <c r="A77" s="4">
         <v>62</v>
       </c>
-      <c r="B77" s="27"/>
-      <c r="C77" s="28"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="37"/>
       <c r="D77" s="5" t="s">
         <v>169</v>
       </c>
@@ -5241,8 +5285,8 @@
       <c r="A78" s="4">
         <v>63</v>
       </c>
-      <c r="B78" s="27"/>
-      <c r="C78" s="28"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="37"/>
       <c r="D78" s="5" t="s">
         <v>171</v>
       </c>
@@ -5266,7 +5310,7 @@
       <c r="A79" s="4">
         <v>64</v>
       </c>
-      <c r="B79" s="27"/>
+      <c r="B79" s="36"/>
       <c r="C79" s="4"/>
       <c r="D79" s="5" t="s">
         <v>173</v>
@@ -5291,10 +5335,10 @@
       <c r="A80" s="4">
         <v>65</v>
       </c>
-      <c r="B80" s="27" t="s">
+      <c r="B80" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="C80" s="28" t="s">
+      <c r="C80" s="37" t="s">
         <v>176</v>
       </c>
       <c r="D80" s="5" t="s">
@@ -5322,8 +5366,8 @@
       <c r="A81" s="4">
         <v>66</v>
       </c>
-      <c r="B81" s="27"/>
-      <c r="C81" s="28"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="37"/>
       <c r="D81" s="5" t="s">
         <v>180</v>
       </c>
@@ -5347,8 +5391,8 @@
       <c r="A82" s="4">
         <v>67</v>
       </c>
-      <c r="B82" s="27"/>
-      <c r="C82" s="28" t="s">
+      <c r="B82" s="36"/>
+      <c r="C82" s="37" t="s">
         <v>182</v>
       </c>
       <c r="D82" s="5" t="s">
@@ -5374,8 +5418,8 @@
       <c r="A83" s="4">
         <v>68</v>
       </c>
-      <c r="B83" s="27"/>
-      <c r="C83" s="28"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="37"/>
       <c r="D83" s="5" t="s">
         <v>185</v>
       </c>
@@ -5399,8 +5443,8 @@
       <c r="A84" s="4">
         <v>69</v>
       </c>
-      <c r="B84" s="27"/>
-      <c r="C84" s="28"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="37"/>
       <c r="D84" s="5" t="s">
         <v>187</v>
       </c>
@@ -5424,8 +5468,8 @@
       <c r="A85" s="4">
         <v>70</v>
       </c>
-      <c r="B85" s="27"/>
-      <c r="C85" s="28"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="37"/>
       <c r="D85" s="5" t="s">
         <v>189</v>
       </c>
@@ -5449,7 +5493,7 @@
       <c r="A86" s="4">
         <v>71</v>
       </c>
-      <c r="B86" s="27"/>
+      <c r="B86" s="36"/>
       <c r="C86" s="4" t="s">
         <v>163</v>
       </c>
@@ -5476,7 +5520,7 @@
       <c r="A87" s="4">
         <v>72</v>
       </c>
-      <c r="B87" s="27"/>
+      <c r="B87" s="36"/>
       <c r="C87" s="4"/>
       <c r="D87" s="5" t="s">
         <v>173</v>
@@ -5501,10 +5545,10 @@
       <c r="A88" s="4">
         <v>73</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="B88" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="C88" s="28" t="s">
+      <c r="C88" s="37" t="s">
         <v>176</v>
       </c>
       <c r="D88" s="5" t="s">
@@ -5530,8 +5574,8 @@
       <c r="A89" s="4">
         <v>74</v>
       </c>
-      <c r="B89" s="27"/>
-      <c r="C89" s="28"/>
+      <c r="B89" s="36"/>
+      <c r="C89" s="37"/>
       <c r="D89" s="5" t="s">
         <v>180</v>
       </c>
@@ -5555,8 +5599,8 @@
       <c r="A90" s="4">
         <v>75</v>
       </c>
-      <c r="B90" s="27"/>
-      <c r="C90" s="28" t="s">
+      <c r="B90" s="36"/>
+      <c r="C90" s="37" t="s">
         <v>182</v>
       </c>
       <c r="D90" s="5" t="s">
@@ -5582,8 +5626,8 @@
       <c r="A91" s="4">
         <v>76</v>
       </c>
-      <c r="B91" s="27"/>
-      <c r="C91" s="28"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="37"/>
       <c r="D91" s="5" t="s">
         <v>185</v>
       </c>
@@ -5607,8 +5651,8 @@
       <c r="A92" s="4">
         <v>77</v>
       </c>
-      <c r="B92" s="27"/>
-      <c r="C92" s="28"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="37"/>
       <c r="D92" s="5" t="s">
         <v>187</v>
       </c>
@@ -5632,8 +5676,8 @@
       <c r="A93" s="4">
         <v>78</v>
       </c>
-      <c r="B93" s="27"/>
-      <c r="C93" s="28"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="37"/>
       <c r="D93" s="5" t="s">
         <v>189</v>
       </c>
@@ -5657,7 +5701,7 @@
       <c r="A94" s="4">
         <v>79</v>
       </c>
-      <c r="B94" s="27"/>
+      <c r="B94" s="36"/>
       <c r="C94" s="4" t="s">
         <v>163</v>
       </c>
@@ -5684,7 +5728,7 @@
       <c r="A95" s="4">
         <v>80</v>
       </c>
-      <c r="B95" s="27"/>
+      <c r="B95" s="36"/>
       <c r="C95" s="4"/>
       <c r="D95" s="5" t="s">
         <v>173</v>
@@ -5709,7 +5753,7 @@
       <c r="A96" s="4">
         <v>81</v>
       </c>
-      <c r="B96" s="27" t="s">
+      <c r="B96" s="36" t="s">
         <v>193</v>
       </c>
       <c r="C96" s="4" t="s">
@@ -5738,7 +5782,7 @@
       <c r="A97" s="4">
         <v>82</v>
       </c>
-      <c r="B97" s="27"/>
+      <c r="B97" s="36"/>
       <c r="C97" s="4"/>
       <c r="D97" s="5" t="s">
         <v>173</v>
@@ -5763,7 +5807,7 @@
       <c r="A98" s="4">
         <v>83</v>
       </c>
-      <c r="B98" s="27" t="s">
+      <c r="B98" s="36" t="s">
         <v>197</v>
       </c>
       <c r="C98" s="4" t="s">
@@ -5792,7 +5836,7 @@
       <c r="A99" s="4">
         <v>84</v>
       </c>
-      <c r="B99" s="27"/>
+      <c r="B99" s="36"/>
       <c r="C99" s="4" t="s">
         <v>163</v>
       </c>
@@ -5819,7 +5863,7 @@
       <c r="A100" s="4">
         <v>85</v>
       </c>
-      <c r="B100" s="27"/>
+      <c r="B100" s="36"/>
       <c r="C100" s="4"/>
       <c r="D100" s="5" t="s">
         <v>173</v>
@@ -5844,7 +5888,7 @@
       <c r="A101" s="4">
         <v>86</v>
       </c>
-      <c r="B101" s="27" t="s">
+      <c r="B101" s="36" t="s">
         <v>199</v>
       </c>
       <c r="C101" s="4" t="s">
@@ -5873,7 +5917,7 @@
       <c r="A102" s="4">
         <v>87</v>
       </c>
-      <c r="B102" s="27"/>
+      <c r="B102" s="36"/>
       <c r="C102" s="4" t="s">
         <v>200</v>
       </c>
@@ -5900,8 +5944,8 @@
       <c r="A103" s="4">
         <v>88</v>
       </c>
-      <c r="B103" s="27"/>
-      <c r="C103" s="28" t="s">
+      <c r="B103" s="36"/>
+      <c r="C103" s="37" t="s">
         <v>203</v>
       </c>
       <c r="D103" s="5" t="s">
@@ -5927,8 +5971,8 @@
       <c r="A104" s="4">
         <v>89</v>
       </c>
-      <c r="B104" s="27"/>
-      <c r="C104" s="28"/>
+      <c r="B104" s="36"/>
+      <c r="C104" s="37"/>
       <c r="D104" s="5" t="s">
         <v>206</v>
       </c>
@@ -5952,8 +5996,8 @@
       <c r="A105" s="4">
         <v>90</v>
       </c>
-      <c r="B105" s="27"/>
-      <c r="C105" s="28"/>
+      <c r="B105" s="36"/>
+      <c r="C105" s="37"/>
       <c r="D105" s="5" t="s">
         <v>207</v>
       </c>
@@ -5977,8 +6021,8 @@
       <c r="A106" s="4">
         <v>91</v>
       </c>
-      <c r="B106" s="27"/>
-      <c r="C106" s="28"/>
+      <c r="B106" s="36"/>
+      <c r="C106" s="37"/>
       <c r="D106" s="5" t="s">
         <v>209</v>
       </c>
@@ -6002,7 +6046,7 @@
       <c r="A107" s="4">
         <v>92</v>
       </c>
-      <c r="B107" s="27"/>
+      <c r="B107" s="36"/>
       <c r="C107" s="4" t="s">
         <v>210</v>
       </c>
@@ -6031,7 +6075,7 @@
       <c r="A108" s="4">
         <v>93</v>
       </c>
-      <c r="B108" s="27"/>
+      <c r="B108" s="36"/>
       <c r="C108" s="4"/>
       <c r="D108" s="5" t="s">
         <v>173</v>
@@ -6056,10 +6100,10 @@
       <c r="A109" s="4">
         <v>94</v>
       </c>
-      <c r="B109" s="27" t="s">
+      <c r="B109" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="C109" s="23" t="s">
+      <c r="C109" s="27" t="s">
         <v>19</v>
       </c>
       <c r="D109" s="5" t="s">
@@ -6085,8 +6129,8 @@
       <c r="A110" s="4">
         <v>95</v>
       </c>
-      <c r="B110" s="27"/>
-      <c r="C110" s="29"/>
+      <c r="B110" s="36"/>
+      <c r="C110" s="28"/>
       <c r="D110" s="5" t="s">
         <v>217</v>
       </c>
@@ -6110,8 +6154,8 @@
       <c r="A111" s="4">
         <v>96</v>
       </c>
-      <c r="B111" s="27"/>
-      <c r="C111" s="29"/>
+      <c r="B111" s="36"/>
+      <c r="C111" s="28"/>
       <c r="D111" s="5" t="s">
         <v>219</v>
       </c>
@@ -6135,8 +6179,8 @@
       <c r="A112" s="4">
         <v>97</v>
       </c>
-      <c r="B112" s="27"/>
-      <c r="C112" s="24"/>
+      <c r="B112" s="36"/>
+      <c r="C112" s="29"/>
       <c r="D112" s="5" t="s">
         <v>221</v>
       </c>
@@ -6160,7 +6204,7 @@
       <c r="A113" s="4">
         <v>98</v>
       </c>
-      <c r="B113" s="27" t="s">
+      <c r="B113" s="36" t="s">
         <v>223</v>
       </c>
       <c r="C113" s="4" t="s">
@@ -6189,8 +6233,8 @@
       <c r="A114" s="4">
         <v>99</v>
       </c>
-      <c r="B114" s="27"/>
-      <c r="C114" s="28" t="s">
+      <c r="B114" s="36"/>
+      <c r="C114" s="37" t="s">
         <v>227</v>
       </c>
       <c r="D114" s="5" t="s">
@@ -6216,8 +6260,8 @@
       <c r="A115" s="4">
         <v>100</v>
       </c>
-      <c r="B115" s="27"/>
-      <c r="C115" s="28"/>
+      <c r="B115" s="36"/>
+      <c r="C115" s="37"/>
       <c r="D115" s="5" t="s">
         <v>230</v>
       </c>
@@ -6241,8 +6285,8 @@
       <c r="A116" s="4">
         <v>101</v>
       </c>
-      <c r="B116" s="27"/>
-      <c r="C116" s="28"/>
+      <c r="B116" s="36"/>
+      <c r="C116" s="37"/>
       <c r="D116" s="5" t="s">
         <v>232</v>
       </c>
@@ -6266,8 +6310,8 @@
       <c r="A117" s="4">
         <v>102</v>
       </c>
-      <c r="B117" s="27"/>
-      <c r="C117" s="28"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="37"/>
       <c r="D117" s="5" t="s">
         <v>234</v>
       </c>
@@ -6291,8 +6335,8 @@
       <c r="A118" s="4">
         <v>103</v>
       </c>
-      <c r="B118" s="27"/>
-      <c r="C118" s="28" t="s">
+      <c r="B118" s="36"/>
+      <c r="C118" s="37" t="s">
         <v>235</v>
       </c>
       <c r="D118" s="5" t="s">
@@ -6318,8 +6362,8 @@
       <c r="A119" s="4">
         <v>104</v>
       </c>
-      <c r="B119" s="27"/>
-      <c r="C119" s="28"/>
+      <c r="B119" s="36"/>
+      <c r="C119" s="37"/>
       <c r="D119" s="5" t="s">
         <v>238</v>
       </c>
@@ -6343,8 +6387,8 @@
       <c r="A120" s="4">
         <v>105</v>
       </c>
-      <c r="B120" s="27"/>
-      <c r="C120" s="28"/>
+      <c r="B120" s="36"/>
+      <c r="C120" s="37"/>
       <c r="D120" s="5" t="s">
         <v>240</v>
       </c>
@@ -6368,8 +6412,8 @@
       <c r="A121" s="4">
         <v>106</v>
       </c>
-      <c r="B121" s="27"/>
-      <c r="C121" s="28"/>
+      <c r="B121" s="36"/>
+      <c r="C121" s="37"/>
       <c r="D121" s="5" t="s">
         <v>241</v>
       </c>
@@ -6393,8 +6437,8 @@
       <c r="A122" s="4">
         <v>107</v>
       </c>
-      <c r="B122" s="27"/>
-      <c r="C122" s="28" t="s">
+      <c r="B122" s="36"/>
+      <c r="C122" s="37" t="s">
         <v>242</v>
       </c>
       <c r="D122" s="5" t="s">
@@ -6420,8 +6464,8 @@
       <c r="A123" s="4">
         <v>108</v>
       </c>
-      <c r="B123" s="27"/>
-      <c r="C123" s="28"/>
+      <c r="B123" s="36"/>
+      <c r="C123" s="37"/>
       <c r="D123" s="5" t="s">
         <v>245</v>
       </c>
@@ -6445,8 +6489,8 @@
       <c r="A124" s="4">
         <v>109</v>
       </c>
-      <c r="B124" s="27"/>
-      <c r="C124" s="28"/>
+      <c r="B124" s="36"/>
+      <c r="C124" s="37"/>
       <c r="D124" s="5" t="s">
         <v>246</v>
       </c>
@@ -6470,8 +6514,8 @@
       <c r="A125" s="4">
         <v>110</v>
       </c>
-      <c r="B125" s="27"/>
-      <c r="C125" s="28" t="s">
+      <c r="B125" s="36"/>
+      <c r="C125" s="37" t="s">
         <v>248</v>
       </c>
       <c r="D125" s="5" t="s">
@@ -6497,8 +6541,8 @@
       <c r="A126" s="4">
         <v>111</v>
       </c>
-      <c r="B126" s="27"/>
-      <c r="C126" s="28"/>
+      <c r="B126" s="36"/>
+      <c r="C126" s="37"/>
       <c r="D126" s="5" t="s">
         <v>251</v>
       </c>
@@ -6522,8 +6566,8 @@
       <c r="A127" s="4">
         <v>112</v>
       </c>
-      <c r="B127" s="27"/>
-      <c r="C127" s="28" t="s">
+      <c r="B127" s="36"/>
+      <c r="C127" s="37" t="s">
         <v>253</v>
       </c>
       <c r="D127" s="5" t="s">
@@ -6549,8 +6593,8 @@
       <c r="A128" s="4">
         <v>113</v>
       </c>
-      <c r="B128" s="27"/>
-      <c r="C128" s="28"/>
+      <c r="B128" s="36"/>
+      <c r="C128" s="37"/>
       <c r="D128" s="5" t="s">
         <v>256</v>
       </c>
@@ -6574,8 +6618,8 @@
       <c r="A129" s="4">
         <v>114</v>
       </c>
-      <c r="B129" s="27"/>
-      <c r="C129" s="28"/>
+      <c r="B129" s="36"/>
+      <c r="C129" s="37"/>
       <c r="D129" s="5" t="s">
         <v>258</v>
       </c>
@@ -6599,7 +6643,7 @@
       <c r="A130" s="4">
         <v>115</v>
       </c>
-      <c r="B130" s="27"/>
+      <c r="B130" s="36"/>
       <c r="C130" s="4"/>
       <c r="D130" s="8" t="s">
         <v>173</v>
@@ -6624,10 +6668,10 @@
       <c r="A131" s="4">
         <v>116</v>
       </c>
-      <c r="B131" s="27" t="s">
+      <c r="B131" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="C131" s="28" t="s">
+      <c r="C131" s="37" t="s">
         <v>263</v>
       </c>
       <c r="D131" s="5" t="s">
@@ -6653,8 +6697,8 @@
       <c r="A132" s="4">
         <v>117</v>
       </c>
-      <c r="B132" s="27"/>
-      <c r="C132" s="28"/>
+      <c r="B132" s="36"/>
+      <c r="C132" s="37"/>
       <c r="D132" s="5" t="s">
         <v>270</v>
       </c>
@@ -6678,8 +6722,8 @@
       <c r="A133" s="4">
         <v>118</v>
       </c>
-      <c r="B133" s="27"/>
-      <c r="C133" s="28"/>
+      <c r="B133" s="36"/>
+      <c r="C133" s="37"/>
       <c r="D133" s="5" t="s">
         <v>271</v>
       </c>
@@ -6703,8 +6747,8 @@
       <c r="A134" s="4">
         <v>119</v>
       </c>
-      <c r="B134" s="27"/>
-      <c r="C134" s="23" t="s">
+      <c r="B134" s="36"/>
+      <c r="C134" s="27" t="s">
         <v>264</v>
       </c>
       <c r="D134" s="5" t="s">
@@ -6730,8 +6774,8 @@
       <c r="A135" s="4">
         <v>120</v>
       </c>
-      <c r="B135" s="27"/>
-      <c r="C135" s="24"/>
+      <c r="B135" s="36"/>
+      <c r="C135" s="29"/>
       <c r="D135" s="5" t="s">
         <v>269</v>
       </c>
@@ -6755,8 +6799,8 @@
       <c r="A136" s="4">
         <v>121</v>
       </c>
-      <c r="B136" s="27"/>
-      <c r="C136" s="23" t="s">
+      <c r="B136" s="36"/>
+      <c r="C136" s="27" t="s">
         <v>265</v>
       </c>
       <c r="D136" s="5" t="s">
@@ -6782,8 +6826,8 @@
       <c r="A137" s="4">
         <v>122</v>
       </c>
-      <c r="B137" s="27"/>
-      <c r="C137" s="29"/>
+      <c r="B137" s="36"/>
+      <c r="C137" s="28"/>
       <c r="D137" s="5" t="s">
         <v>277</v>
       </c>
@@ -6807,8 +6851,8 @@
       <c r="A138" s="4">
         <v>123</v>
       </c>
-      <c r="B138" s="27"/>
-      <c r="C138" s="24"/>
+      <c r="B138" s="36"/>
+      <c r="C138" s="29"/>
       <c r="D138" s="5" t="s">
         <v>279</v>
       </c>
@@ -6832,8 +6876,8 @@
       <c r="A139" s="4">
         <v>124</v>
       </c>
-      <c r="B139" s="27"/>
-      <c r="C139" s="23" t="s">
+      <c r="B139" s="36"/>
+      <c r="C139" s="27" t="s">
         <v>266</v>
       </c>
       <c r="D139" s="5" t="s">
@@ -6859,8 +6903,8 @@
       <c r="A140" s="4">
         <v>125</v>
       </c>
-      <c r="B140" s="27"/>
-      <c r="C140" s="29"/>
+      <c r="B140" s="36"/>
+      <c r="C140" s="28"/>
       <c r="D140" s="5" t="s">
         <v>283</v>
       </c>
@@ -6884,8 +6928,8 @@
       <c r="A141" s="4">
         <v>126</v>
       </c>
-      <c r="B141" s="27"/>
-      <c r="C141" s="29"/>
+      <c r="B141" s="36"/>
+      <c r="C141" s="28"/>
       <c r="D141" s="5" t="s">
         <v>285</v>
       </c>
@@ -6909,8 +6953,8 @@
       <c r="A142" s="4">
         <v>127</v>
       </c>
-      <c r="B142" s="27"/>
-      <c r="C142" s="29"/>
+      <c r="B142" s="36"/>
+      <c r="C142" s="28"/>
       <c r="D142" s="5" t="s">
         <v>284</v>
       </c>
@@ -6934,8 +6978,8 @@
       <c r="A143" s="4">
         <v>128</v>
       </c>
-      <c r="B143" s="27"/>
-      <c r="C143" s="29"/>
+      <c r="B143" s="36"/>
+      <c r="C143" s="28"/>
       <c r="D143" s="5" t="s">
         <v>286</v>
       </c>
@@ -6959,8 +7003,8 @@
       <c r="A144" s="4">
         <v>129</v>
       </c>
-      <c r="B144" s="27"/>
-      <c r="C144" s="24"/>
+      <c r="B144" s="36"/>
+      <c r="C144" s="29"/>
       <c r="D144" s="5" t="s">
         <v>288</v>
       </c>
@@ -6984,7 +7028,7 @@
       <c r="A145" s="4">
         <v>130</v>
       </c>
-      <c r="B145" s="27"/>
+      <c r="B145" s="36"/>
       <c r="C145" s="7" t="s">
         <v>267</v>
       </c>
@@ -7011,7 +7055,7 @@
       <c r="A146" s="4">
         <v>131</v>
       </c>
-      <c r="B146" s="27"/>
+      <c r="B146" s="36"/>
       <c r="C146" s="7"/>
       <c r="D146" s="5" t="s">
         <v>173</v>
@@ -7036,10 +7080,10 @@
       <c r="A147" s="4">
         <v>132</v>
       </c>
-      <c r="B147" s="27" t="s">
+      <c r="B147" s="36" t="s">
         <v>290</v>
       </c>
-      <c r="C147" s="28" t="s">
+      <c r="C147" s="37" t="s">
         <v>291</v>
       </c>
       <c r="D147" s="5" t="s">
@@ -7065,8 +7109,8 @@
       <c r="A148" s="4">
         <v>133</v>
       </c>
-      <c r="B148" s="27"/>
-      <c r="C148" s="28"/>
+      <c r="B148" s="36"/>
+      <c r="C148" s="37"/>
       <c r="D148" s="5" t="s">
         <v>294</v>
       </c>
@@ -7090,7 +7134,7 @@
       <c r="A149" s="4">
         <v>134</v>
       </c>
-      <c r="B149" s="27"/>
+      <c r="B149" s="36"/>
       <c r="C149" s="4"/>
       <c r="D149" s="5" t="s">
         <v>173</v>
@@ -7102,10 +7146,10 @@
       <c r="G149" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H149" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="I149" s="18" t="s">
+      <c r="H149" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I149" s="20" t="s">
         <v>22</v>
       </c>
       <c r="J149" s="6"/>
@@ -7115,10 +7159,10 @@
       <c r="A150" s="4">
         <v>135</v>
       </c>
-      <c r="B150" s="20" t="s">
+      <c r="B150" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="C150" s="23" t="s">
+      <c r="C150" s="27" t="s">
         <v>297</v>
       </c>
       <c r="D150" s="5" t="s">
@@ -7128,14 +7172,14 @@
         <v>299</v>
       </c>
       <c r="F150" s="5"/>
-      <c r="G150" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H150" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I150" s="4" t="s">
-        <v>213</v>
+      <c r="G150" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H150" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I150" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J150" s="6"/>
       <c r="K150" s="7"/>
@@ -7144,8 +7188,8 @@
       <c r="A151" s="4">
         <v>136</v>
       </c>
-      <c r="B151" s="21"/>
-      <c r="C151" s="29"/>
+      <c r="B151" s="25"/>
+      <c r="C151" s="28"/>
       <c r="D151" s="5" t="s">
         <v>300</v>
       </c>
@@ -7153,14 +7197,14 @@
         <v>301</v>
       </c>
       <c r="F151" s="5"/>
-      <c r="G151" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H151" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I151" s="4" t="s">
-        <v>213</v>
+      <c r="G151" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H151" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I151" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J151" s="6"/>
       <c r="K151" s="7"/>
@@ -7169,8 +7213,8 @@
       <c r="A152" s="4">
         <v>137</v>
       </c>
-      <c r="B152" s="21"/>
-      <c r="C152" s="29"/>
+      <c r="B152" s="25"/>
+      <c r="C152" s="28"/>
       <c r="D152" s="5" t="s">
         <v>302</v>
       </c>
@@ -7178,14 +7222,14 @@
         <v>303</v>
       </c>
       <c r="F152" s="5"/>
-      <c r="G152" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H152" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I152" s="4" t="s">
-        <v>213</v>
+      <c r="G152" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H152" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I152" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J152" s="6"/>
       <c r="K152" s="7"/>
@@ -7194,8 +7238,8 @@
       <c r="A153" s="4">
         <v>138</v>
       </c>
-      <c r="B153" s="21"/>
-      <c r="C153" s="24"/>
+      <c r="B153" s="25"/>
+      <c r="C153" s="29"/>
       <c r="D153" s="5" t="s">
         <v>304</v>
       </c>
@@ -7203,14 +7247,14 @@
         <v>305</v>
       </c>
       <c r="F153" s="5"/>
-      <c r="G153" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H153" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I153" s="4" t="s">
-        <v>213</v>
+      <c r="G153" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H153" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I153" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J153" s="6"/>
       <c r="K153" s="7"/>
@@ -7219,8 +7263,8 @@
       <c r="A154" s="4">
         <v>139</v>
       </c>
-      <c r="B154" s="21"/>
-      <c r="C154" s="23" t="s">
+      <c r="B154" s="25"/>
+      <c r="C154" s="27" t="s">
         <v>291</v>
       </c>
       <c r="D154" s="5" t="s">
@@ -7230,14 +7274,14 @@
         <v>307</v>
       </c>
       <c r="F154" s="5"/>
-      <c r="G154" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H154" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I154" s="4" t="s">
-        <v>213</v>
+      <c r="G154" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H154" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I154" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J154" s="6"/>
       <c r="K154" s="7"/>
@@ -7246,8 +7290,8 @@
       <c r="A155" s="4">
         <v>140</v>
       </c>
-      <c r="B155" s="21"/>
-      <c r="C155" s="24"/>
+      <c r="B155" s="25"/>
+      <c r="C155" s="29"/>
       <c r="D155" s="5" t="s">
         <v>308</v>
       </c>
@@ -7255,14 +7299,14 @@
         <v>309</v>
       </c>
       <c r="F155" s="5"/>
-      <c r="G155" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H155" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I155" s="4" t="s">
-        <v>213</v>
+      <c r="G155" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H155" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I155" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J155" s="6"/>
       <c r="K155" s="7"/>
@@ -7271,7 +7315,7 @@
       <c r="A156" s="4">
         <v>141</v>
       </c>
-      <c r="B156" s="22"/>
+      <c r="B156" s="26"/>
       <c r="C156" s="4"/>
       <c r="D156" s="5" t="s">
         <v>173</v>
@@ -7280,14 +7324,14 @@
         <v>260</v>
       </c>
       <c r="F156" s="5"/>
-      <c r="G156" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H156" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I156" s="4" t="s">
-        <v>213</v>
+      <c r="G156" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H156" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I156" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="J156" s="6"/>
       <c r="K156" s="7"/>
@@ -7296,7 +7340,7 @@
       <c r="A157" s="4">
         <v>142</v>
       </c>
-      <c r="B157" s="20" t="s">
+      <c r="B157" s="24" t="s">
         <v>310</v>
       </c>
       <c r="C157" s="4" t="s">
@@ -7325,7 +7369,7 @@
       <c r="A158" s="4">
         <v>143</v>
       </c>
-      <c r="B158" s="21"/>
+      <c r="B158" s="25"/>
       <c r="C158" s="4" t="s">
         <v>314</v>
       </c>
@@ -7352,7 +7396,7 @@
       <c r="A159" s="4">
         <v>144</v>
       </c>
-      <c r="B159" s="21"/>
+      <c r="B159" s="25"/>
       <c r="C159" s="4" t="s">
         <v>317</v>
       </c>
@@ -7379,7 +7423,7 @@
       <c r="A160" s="4">
         <v>145</v>
       </c>
-      <c r="B160" s="22"/>
+      <c r="B160" s="26"/>
       <c r="C160" s="4"/>
       <c r="D160" s="5" t="s">
         <v>173</v>
@@ -7404,7 +7448,7 @@
       <c r="A161" s="4">
         <v>146</v>
       </c>
-      <c r="B161" s="20" t="s">
+      <c r="B161" s="24" t="s">
         <v>320</v>
       </c>
       <c r="C161" s="4" t="s">
@@ -7433,8 +7477,8 @@
       <c r="A162" s="4">
         <v>147</v>
       </c>
-      <c r="B162" s="21"/>
-      <c r="C162" s="23" t="s">
+      <c r="B162" s="25"/>
+      <c r="C162" s="27" t="s">
         <v>323</v>
       </c>
       <c r="D162" s="5" t="s">
@@ -7460,8 +7504,8 @@
       <c r="A163" s="4">
         <v>148</v>
       </c>
-      <c r="B163" s="21"/>
-      <c r="C163" s="24"/>
+      <c r="B163" s="25"/>
+      <c r="C163" s="29"/>
       <c r="D163" s="5" t="s">
         <v>326</v>
       </c>
@@ -7485,8 +7529,8 @@
       <c r="A164" s="4">
         <v>149</v>
       </c>
-      <c r="B164" s="21"/>
-      <c r="C164" s="23" t="s">
+      <c r="B164" s="25"/>
+      <c r="C164" s="27" t="s">
         <v>328</v>
       </c>
       <c r="D164" s="5" t="s">
@@ -7512,8 +7556,8 @@
       <c r="A165" s="4">
         <v>150</v>
       </c>
-      <c r="B165" s="21"/>
-      <c r="C165" s="24"/>
+      <c r="B165" s="25"/>
+      <c r="C165" s="29"/>
       <c r="D165" s="5" t="s">
         <v>329</v>
       </c>
@@ -7537,7 +7581,7 @@
       <c r="A166" s="4">
         <v>151</v>
       </c>
-      <c r="B166" s="21"/>
+      <c r="B166" s="25"/>
       <c r="C166" s="4" t="s">
         <v>332</v>
       </c>
@@ -7564,8 +7608,8 @@
       <c r="A167" s="4">
         <v>152</v>
       </c>
-      <c r="B167" s="21"/>
-      <c r="C167" s="23" t="s">
+      <c r="B167" s="25"/>
+      <c r="C167" s="27" t="s">
         <v>335</v>
       </c>
       <c r="D167" s="5" t="s">
@@ -7591,8 +7635,8 @@
       <c r="A168" s="4">
         <v>153</v>
       </c>
-      <c r="B168" s="21"/>
-      <c r="C168" s="24"/>
+      <c r="B168" s="25"/>
+      <c r="C168" s="29"/>
       <c r="D168" s="5" t="s">
         <v>338</v>
       </c>
@@ -7616,8 +7660,8 @@
       <c r="A169" s="4">
         <v>154</v>
       </c>
-      <c r="B169" s="21"/>
-      <c r="C169" s="23" t="s">
+      <c r="B169" s="25"/>
+      <c r="C169" s="27" t="s">
         <v>340</v>
       </c>
       <c r="D169" s="5" t="s">
@@ -7643,8 +7687,8 @@
       <c r="A170" s="4">
         <v>155</v>
       </c>
-      <c r="B170" s="21"/>
-      <c r="C170" s="24"/>
+      <c r="B170" s="25"/>
+      <c r="C170" s="29"/>
       <c r="D170" s="5" t="s">
         <v>343</v>
       </c>
@@ -7668,8 +7712,8 @@
       <c r="A171" s="4">
         <v>156</v>
       </c>
-      <c r="B171" s="21"/>
-      <c r="C171" s="23" t="s">
+      <c r="B171" s="25"/>
+      <c r="C171" s="27" t="s">
         <v>345</v>
       </c>
       <c r="D171" s="5" t="s">
@@ -7695,8 +7739,8 @@
       <c r="A172" s="4">
         <v>157</v>
       </c>
-      <c r="B172" s="21"/>
-      <c r="C172" s="29"/>
+      <c r="B172" s="25"/>
+      <c r="C172" s="28"/>
       <c r="D172" s="5" t="s">
         <v>348</v>
       </c>
@@ -7720,8 +7764,8 @@
       <c r="A173" s="4">
         <v>158</v>
       </c>
-      <c r="B173" s="21"/>
-      <c r="C173" s="24"/>
+      <c r="B173" s="25"/>
+      <c r="C173" s="29"/>
       <c r="D173" s="5" t="s">
         <v>350</v>
       </c>
@@ -7745,8 +7789,8 @@
       <c r="A174" s="4">
         <v>159</v>
       </c>
-      <c r="B174" s="21"/>
-      <c r="C174" s="23" t="s">
+      <c r="B174" s="25"/>
+      <c r="C174" s="27" t="s">
         <v>352</v>
       </c>
       <c r="D174" s="5" t="s">
@@ -7772,8 +7816,8 @@
       <c r="A175" s="4">
         <v>160</v>
       </c>
-      <c r="B175" s="21"/>
-      <c r="C175" s="24"/>
+      <c r="B175" s="25"/>
+      <c r="C175" s="29"/>
       <c r="D175" s="5" t="s">
         <v>353</v>
       </c>
@@ -7797,7 +7841,7 @@
       <c r="A176" s="4">
         <v>161</v>
       </c>
-      <c r="B176" s="21" t="s">
+      <c r="B176" s="25" t="s">
         <v>356</v>
       </c>
       <c r="C176" s="4" t="s">
@@ -7826,7 +7870,7 @@
       <c r="A177" s="4">
         <v>162</v>
       </c>
-      <c r="B177" s="21"/>
+      <c r="B177" s="25"/>
       <c r="C177" s="4" t="s">
         <v>358</v>
       </c>
@@ -7853,8 +7897,8 @@
       <c r="A178" s="4">
         <v>163</v>
       </c>
-      <c r="B178" s="21"/>
-      <c r="C178" s="23" t="s">
+      <c r="B178" s="25"/>
+      <c r="C178" s="27" t="s">
         <v>361</v>
       </c>
       <c r="D178" s="5" t="s">
@@ -7880,8 +7924,8 @@
       <c r="A179" s="4">
         <v>164</v>
       </c>
-      <c r="B179" s="22"/>
-      <c r="C179" s="24"/>
+      <c r="B179" s="26"/>
+      <c r="C179" s="29"/>
       <c r="D179" s="5" t="s">
         <v>362</v>
       </c>
@@ -7905,7 +7949,7 @@
       <c r="A180" s="4">
         <v>165</v>
       </c>
-      <c r="B180" s="27" t="s">
+      <c r="B180" s="36" t="s">
         <v>365</v>
       </c>
       <c r="C180" s="4"/>
@@ -7932,7 +7976,7 @@
       <c r="A181" s="4">
         <v>166</v>
       </c>
-      <c r="B181" s="27"/>
+      <c r="B181" s="36"/>
       <c r="C181" s="4"/>
       <c r="D181" s="5" t="s">
         <v>368</v>
@@ -7957,7 +8001,7 @@
       <c r="A182" s="4">
         <v>167</v>
       </c>
-      <c r="B182" s="27"/>
+      <c r="B182" s="36"/>
       <c r="C182" s="4"/>
       <c r="D182" s="5" t="s">
         <v>370</v>
@@ -7982,7 +8026,7 @@
       <c r="A183" s="4">
         <v>168</v>
       </c>
-      <c r="B183" s="27"/>
+      <c r="B183" s="36"/>
       <c r="C183" s="4"/>
       <c r="D183" s="5" t="s">
         <v>372</v>
@@ -8007,7 +8051,7 @@
       <c r="A184" s="4">
         <v>169</v>
       </c>
-      <c r="B184" s="20" t="s">
+      <c r="B184" s="24" t="s">
         <v>374</v>
       </c>
       <c r="C184" s="4" t="s">
@@ -8036,7 +8080,7 @@
       <c r="A185" s="18">
         <v>170</v>
       </c>
-      <c r="B185" s="21"/>
+      <c r="B185" s="25"/>
       <c r="C185" s="4" t="s">
         <v>378</v>
       </c>
@@ -8063,7 +8107,7 @@
       <c r="A186" s="18">
         <v>171</v>
       </c>
-      <c r="B186" s="22"/>
+      <c r="B186" s="26"/>
       <c r="C186" s="4" t="s">
         <v>381</v>
       </c>
@@ -8090,7 +8134,7 @@
       <c r="A187" s="18">
         <v>172</v>
       </c>
-      <c r="B187" s="27" t="s">
+      <c r="B187" s="36" t="s">
         <v>384</v>
       </c>
       <c r="C187" s="4" t="s">
@@ -8119,7 +8163,7 @@
       <c r="A188" s="18">
         <v>173</v>
       </c>
-      <c r="B188" s="27"/>
+      <c r="B188" s="36"/>
       <c r="C188" s="4" t="s">
         <v>388</v>
       </c>
@@ -8146,7 +8190,7 @@
       <c r="A189" s="18">
         <v>174</v>
       </c>
-      <c r="B189" s="27"/>
+      <c r="B189" s="36"/>
       <c r="C189" s="4" t="s">
         <v>391</v>
       </c>
@@ -8173,7 +8217,7 @@
       <c r="A190" s="18">
         <v>175</v>
       </c>
-      <c r="B190" s="27"/>
+      <c r="B190" s="36"/>
       <c r="C190" s="4" t="s">
         <v>394</v>
       </c>
@@ -8200,7 +8244,7 @@
       <c r="A191" s="18">
         <v>176</v>
       </c>
-      <c r="B191" s="27"/>
+      <c r="B191" s="36"/>
       <c r="C191" s="4" t="s">
         <v>396</v>
       </c>
@@ -8227,7 +8271,7 @@
       <c r="A192" s="18">
         <v>177</v>
       </c>
-      <c r="B192" s="27" t="s">
+      <c r="B192" s="36" t="s">
         <v>398</v>
       </c>
       <c r="C192" s="4" t="s">
@@ -8256,7 +8300,7 @@
       <c r="A193" s="18">
         <v>178</v>
       </c>
-      <c r="B193" s="27"/>
+      <c r="B193" s="36"/>
       <c r="C193" s="4"/>
       <c r="D193" s="5" t="s">
         <v>402</v>
@@ -8281,7 +8325,7 @@
       <c r="A194" s="18">
         <v>179</v>
       </c>
-      <c r="B194" s="27"/>
+      <c r="B194" s="36"/>
       <c r="C194" s="4"/>
       <c r="D194" s="5" t="s">
         <v>404</v>
@@ -8306,7 +8350,7 @@
       <c r="A195" s="18">
         <v>180</v>
       </c>
-      <c r="B195" s="27"/>
+      <c r="B195" s="36"/>
       <c r="C195" s="4"/>
       <c r="D195" s="5" t="s">
         <v>406</v>
@@ -8331,7 +8375,7 @@
       <c r="A196" s="18">
         <v>181</v>
       </c>
-      <c r="B196" s="27"/>
+      <c r="B196" s="36"/>
       <c r="C196" s="4" t="s">
         <v>408</v>
       </c>
@@ -8358,7 +8402,7 @@
       <c r="A197" s="18">
         <v>182</v>
       </c>
-      <c r="B197" s="27"/>
+      <c r="B197" s="36"/>
       <c r="C197" s="4" t="s">
         <v>411</v>
       </c>
@@ -8385,7 +8429,7 @@
       <c r="A198" s="18">
         <v>183</v>
       </c>
-      <c r="B198" s="27"/>
+      <c r="B198" s="36"/>
       <c r="C198" s="4"/>
       <c r="D198" s="5" t="s">
         <v>414</v>
@@ -8410,7 +8454,7 @@
       <c r="A199" s="18">
         <v>184</v>
       </c>
-      <c r="B199" s="27"/>
+      <c r="B199" s="36"/>
       <c r="C199" s="4"/>
       <c r="D199" s="5" t="s">
         <v>416</v>
@@ -8435,7 +8479,7 @@
       <c r="A200" s="18">
         <v>185</v>
       </c>
-      <c r="B200" s="27"/>
+      <c r="B200" s="36"/>
       <c r="C200" s="4" t="s">
         <v>418</v>
       </c>
@@ -8462,7 +8506,7 @@
       <c r="A201" s="18">
         <v>186</v>
       </c>
-      <c r="B201" s="27"/>
+      <c r="B201" s="36"/>
       <c r="C201" s="4" t="s">
         <v>396</v>
       </c>
@@ -8489,7 +8533,7 @@
       <c r="A202" s="18">
         <v>187</v>
       </c>
-      <c r="B202" s="27"/>
+      <c r="B202" s="36"/>
       <c r="C202" s="4" t="s">
         <v>421</v>
       </c>
@@ -8516,7 +8560,7 @@
       <c r="A203" s="18">
         <v>188</v>
       </c>
-      <c r="B203" s="27" t="s">
+      <c r="B203" s="36" t="s">
         <v>423</v>
       </c>
       <c r="C203" s="4" t="s">
@@ -8545,7 +8589,7 @@
       <c r="A204" s="18">
         <v>189</v>
       </c>
-      <c r="B204" s="27"/>
+      <c r="B204" s="36"/>
       <c r="C204" s="4"/>
       <c r="D204" s="5" t="s">
         <v>392</v>
@@ -8570,7 +8614,7 @@
       <c r="A205" s="18">
         <v>190</v>
       </c>
-      <c r="B205" s="27"/>
+      <c r="B205" s="36"/>
       <c r="C205" s="4" t="s">
         <v>421</v>
       </c>
@@ -8597,7 +8641,7 @@
       <c r="A206" s="18">
         <v>191</v>
       </c>
-      <c r="B206" s="27"/>
+      <c r="B206" s="36"/>
       <c r="C206" s="4" t="s">
         <v>427</v>
       </c>
@@ -8624,7 +8668,7 @@
       <c r="A207" s="18">
         <v>192</v>
       </c>
-      <c r="B207" s="27"/>
+      <c r="B207" s="36"/>
       <c r="C207" s="16" t="s">
         <v>430</v>
       </c>
@@ -8651,7 +8695,7 @@
       <c r="A208" s="18">
         <v>193</v>
       </c>
-      <c r="B208" s="20" t="s">
+      <c r="B208" s="24" t="s">
         <v>433</v>
       </c>
       <c r="C208" s="4" t="s">
@@ -8680,8 +8724,8 @@
       <c r="A209" s="18">
         <v>194</v>
       </c>
-      <c r="B209" s="21"/>
-      <c r="C209" s="23" t="s">
+      <c r="B209" s="25"/>
+      <c r="C209" s="27" t="s">
         <v>436</v>
       </c>
       <c r="D209" s="5" t="s">
@@ -8707,8 +8751,8 @@
       <c r="A210" s="18">
         <v>195</v>
       </c>
-      <c r="B210" s="21"/>
-      <c r="C210" s="29"/>
+      <c r="B210" s="25"/>
+      <c r="C210" s="28"/>
       <c r="D210" s="5" t="s">
         <v>439</v>
       </c>
@@ -8732,8 +8776,8 @@
       <c r="A211" s="18">
         <v>196</v>
       </c>
-      <c r="B211" s="21"/>
-      <c r="C211" s="24"/>
+      <c r="B211" s="25"/>
+      <c r="C211" s="29"/>
       <c r="D211" s="5" t="s">
         <v>441</v>
       </c>
@@ -8757,7 +8801,7 @@
       <c r="A212" s="18">
         <v>197</v>
       </c>
-      <c r="B212" s="21"/>
+      <c r="B212" s="25"/>
       <c r="C212" s="4" t="s">
         <v>443</v>
       </c>
@@ -8784,7 +8828,7 @@
       <c r="A213" s="18">
         <v>198</v>
       </c>
-      <c r="B213" s="21"/>
+      <c r="B213" s="25"/>
       <c r="C213" s="4" t="s">
         <v>446</v>
       </c>
@@ -8811,8 +8855,8 @@
       <c r="A214" s="18">
         <v>199</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="23" t="s">
+      <c r="B214" s="25"/>
+      <c r="C214" s="27" t="s">
         <v>449</v>
       </c>
       <c r="D214" s="5" t="s">
@@ -8838,8 +8882,8 @@
       <c r="A215" s="18">
         <v>200</v>
       </c>
-      <c r="B215" s="21"/>
-      <c r="C215" s="29"/>
+      <c r="B215" s="25"/>
+      <c r="C215" s="28"/>
       <c r="D215" s="5" t="s">
         <v>450</v>
       </c>
@@ -8863,8 +8907,8 @@
       <c r="A216" s="18">
         <v>201</v>
       </c>
-      <c r="B216" s="21"/>
-      <c r="C216" s="24"/>
+      <c r="B216" s="25"/>
+      <c r="C216" s="29"/>
       <c r="D216" s="5" t="s">
         <v>450</v>
       </c>
@@ -8888,7 +8932,7 @@
       <c r="A217" s="18">
         <v>202</v>
       </c>
-      <c r="B217" s="21"/>
+      <c r="B217" s="25"/>
       <c r="C217" s="4" t="s">
         <v>396</v>
       </c>
@@ -8915,7 +8959,7 @@
       <c r="A218" s="18">
         <v>203</v>
       </c>
-      <c r="B218" s="21"/>
+      <c r="B218" s="25"/>
       <c r="C218" s="4" t="s">
         <v>421</v>
       </c>
@@ -8942,7 +8986,7 @@
       <c r="A219" s="18">
         <v>204</v>
       </c>
-      <c r="B219" s="22"/>
+      <c r="B219" s="26"/>
       <c r="C219" s="4" t="s">
         <v>457</v>
       </c>
@@ -8999,7 +9043,7 @@
         <v>206</v>
       </c>
       <c r="B221" s="34"/>
-      <c r="C221" s="23" t="s">
+      <c r="C221" s="27" t="s">
         <v>436</v>
       </c>
       <c r="D221" s="5" t="s">
@@ -9026,7 +9070,7 @@
         <v>207</v>
       </c>
       <c r="B222" s="34"/>
-      <c r="C222" s="29"/>
+      <c r="C222" s="28"/>
       <c r="D222" s="5" t="s">
         <v>463</v>
       </c>
@@ -9051,7 +9095,7 @@
         <v>208</v>
       </c>
       <c r="B223" s="34"/>
-      <c r="C223" s="24"/>
+      <c r="C223" s="29"/>
       <c r="D223" s="5" t="s">
         <v>463</v>
       </c>
@@ -9103,7 +9147,7 @@
         <v>210</v>
       </c>
       <c r="B225" s="34"/>
-      <c r="C225" s="23" t="s">
+      <c r="C225" s="27" t="s">
         <v>449</v>
       </c>
       <c r="D225" s="5" t="s">
@@ -9130,7 +9174,7 @@
         <v>211</v>
       </c>
       <c r="B226" s="34"/>
-      <c r="C226" s="29"/>
+      <c r="C226" s="28"/>
       <c r="D226" s="5" t="s">
         <v>465</v>
       </c>
@@ -9155,7 +9199,7 @@
         <v>212</v>
       </c>
       <c r="B227" s="34"/>
-      <c r="C227" s="24"/>
+      <c r="C227" s="29"/>
       <c r="D227" s="5" t="s">
         <v>465</v>
       </c>
@@ -9233,7 +9277,7 @@
       <c r="A230" s="18">
         <v>215</v>
       </c>
-      <c r="B230" s="36" t="s">
+      <c r="B230" s="21" t="s">
         <v>468</v>
       </c>
       <c r="C230" s="4" t="s">
@@ -9262,8 +9306,8 @@
       <c r="A231" s="18">
         <v>216</v>
       </c>
-      <c r="B231" s="37"/>
-      <c r="C231" s="23" t="s">
+      <c r="B231" s="22"/>
+      <c r="C231" s="27" t="s">
         <v>436</v>
       </c>
       <c r="D231" s="5" t="s">
@@ -9289,8 +9333,8 @@
       <c r="A232" s="18">
         <v>217</v>
       </c>
-      <c r="B232" s="37"/>
-      <c r="C232" s="29"/>
+      <c r="B232" s="22"/>
+      <c r="C232" s="28"/>
       <c r="D232" s="5" t="s">
         <v>472</v>
       </c>
@@ -9314,8 +9358,8 @@
       <c r="A233" s="18">
         <v>218</v>
       </c>
-      <c r="B233" s="37"/>
-      <c r="C233" s="24"/>
+      <c r="B233" s="22"/>
+      <c r="C233" s="29"/>
       <c r="D233" s="5" t="s">
         <v>472</v>
       </c>
@@ -9339,7 +9383,7 @@
       <c r="A234" s="18">
         <v>219</v>
       </c>
-      <c r="B234" s="37"/>
+      <c r="B234" s="22"/>
       <c r="C234" s="4" t="s">
         <v>446</v>
       </c>
@@ -9366,8 +9410,8 @@
       <c r="A235" s="18">
         <v>220</v>
       </c>
-      <c r="B235" s="37"/>
-      <c r="C235" s="23" t="s">
+      <c r="B235" s="22"/>
+      <c r="C235" s="27" t="s">
         <v>449</v>
       </c>
       <c r="D235" s="5" t="s">
@@ -9393,8 +9437,8 @@
       <c r="A236" s="18">
         <v>221</v>
       </c>
-      <c r="B236" s="37"/>
-      <c r="C236" s="29"/>
+      <c r="B236" s="22"/>
+      <c r="C236" s="28"/>
       <c r="D236" s="5" t="s">
         <v>474</v>
       </c>
@@ -9418,8 +9462,8 @@
       <c r="A237" s="18">
         <v>222</v>
       </c>
-      <c r="B237" s="37"/>
-      <c r="C237" s="24"/>
+      <c r="B237" s="22"/>
+      <c r="C237" s="29"/>
       <c r="D237" s="5" t="s">
         <v>474</v>
       </c>
@@ -9443,7 +9487,7 @@
       <c r="A238" s="18">
         <v>223</v>
       </c>
-      <c r="B238" s="37"/>
+      <c r="B238" s="22"/>
       <c r="C238" s="4" t="s">
         <v>396</v>
       </c>
@@ -9470,7 +9514,7 @@
       <c r="A239" s="18">
         <v>224</v>
       </c>
-      <c r="B239" s="37"/>
+      <c r="B239" s="22"/>
       <c r="C239" s="4" t="s">
         <v>421</v>
       </c>
@@ -9497,7 +9541,7 @@
       <c r="A240" s="18">
         <v>225</v>
       </c>
-      <c r="B240" s="38"/>
+      <c r="B240" s="23"/>
       <c r="C240" s="4" t="s">
         <v>443</v>
       </c>
@@ -9524,7 +9568,7 @@
       <c r="A241" s="18">
         <v>226</v>
       </c>
-      <c r="B241" s="36" t="s">
+      <c r="B241" s="21" t="s">
         <v>478</v>
       </c>
       <c r="C241" s="4" t="s">
@@ -9553,7 +9597,7 @@
       <c r="A242" s="18">
         <v>227</v>
       </c>
-      <c r="B242" s="37"/>
+      <c r="B242" s="22"/>
       <c r="C242" s="4" t="s">
         <v>481</v>
       </c>
@@ -9580,7 +9624,7 @@
       <c r="A243" s="18">
         <v>228</v>
       </c>
-      <c r="B243" s="37"/>
+      <c r="B243" s="22"/>
       <c r="C243" s="4" t="s">
         <v>484</v>
       </c>
@@ -9607,7 +9651,7 @@
       <c r="A244" s="18">
         <v>229</v>
       </c>
-      <c r="B244" s="37"/>
+      <c r="B244" s="22"/>
       <c r="C244" s="4"/>
       <c r="D244" s="5" t="s">
         <v>487</v>
@@ -9632,7 +9676,7 @@
       <c r="A245" s="18">
         <v>230</v>
       </c>
-      <c r="B245" s="38"/>
+      <c r="B245" s="23"/>
       <c r="C245" s="4"/>
       <c r="D245" s="5" t="s">
         <v>489</v>
@@ -9657,7 +9701,7 @@
       <c r="A246" s="18">
         <v>231</v>
       </c>
-      <c r="B246" s="36" t="s">
+      <c r="B246" s="21" t="s">
         <v>491</v>
       </c>
       <c r="C246" s="4" t="s">
@@ -9686,8 +9730,8 @@
       <c r="A247" s="18">
         <v>232</v>
       </c>
-      <c r="B247" s="37"/>
-      <c r="C247" s="23" t="s">
+      <c r="B247" s="22"/>
+      <c r="C247" s="27" t="s">
         <v>494</v>
       </c>
       <c r="D247" s="5" t="s">
@@ -9713,8 +9757,8 @@
       <c r="A248" s="18">
         <v>233</v>
       </c>
-      <c r="B248" s="37"/>
-      <c r="C248" s="29"/>
+      <c r="B248" s="22"/>
+      <c r="C248" s="28"/>
       <c r="D248" s="5" t="s">
         <v>497</v>
       </c>
@@ -9738,8 +9782,8 @@
       <c r="A249" s="18">
         <v>234</v>
       </c>
-      <c r="B249" s="37"/>
-      <c r="C249" s="29"/>
+      <c r="B249" s="22"/>
+      <c r="C249" s="28"/>
       <c r="D249" s="5" t="s">
         <v>499</v>
       </c>
@@ -9763,8 +9807,8 @@
       <c r="A250" s="18">
         <v>235</v>
       </c>
-      <c r="B250" s="37"/>
-      <c r="C250" s="24"/>
+      <c r="B250" s="22"/>
+      <c r="C250" s="29"/>
       <c r="D250" s="5" t="s">
         <v>501</v>
       </c>
@@ -9788,7 +9832,7 @@
       <c r="A251" s="18">
         <v>236</v>
       </c>
-      <c r="B251" s="37"/>
+      <c r="B251" s="22"/>
       <c r="C251" s="4" t="s">
         <v>503</v>
       </c>
@@ -9815,7 +9859,7 @@
       <c r="A252" s="18">
         <v>237</v>
       </c>
-      <c r="B252" s="37"/>
+      <c r="B252" s="22"/>
       <c r="C252" s="4" t="s">
         <v>506</v>
       </c>
@@ -9842,7 +9886,7 @@
       <c r="A253" s="18">
         <v>238</v>
       </c>
-      <c r="B253" s="37"/>
+      <c r="B253" s="22"/>
       <c r="C253" s="4" t="s">
         <v>509</v>
       </c>
@@ -9869,7 +9913,7 @@
       <c r="A254" s="18">
         <v>239</v>
       </c>
-      <c r="B254" s="37"/>
+      <c r="B254" s="22"/>
       <c r="C254" s="4" t="s">
         <v>512</v>
       </c>
@@ -9896,7 +9940,7 @@
       <c r="A255" s="18">
         <v>240</v>
       </c>
-      <c r="B255" s="38"/>
+      <c r="B255" s="23"/>
       <c r="C255" s="4" t="s">
         <v>515</v>
       </c>
@@ -9923,7 +9967,7 @@
       <c r="A256" s="18">
         <v>241</v>
       </c>
-      <c r="B256" s="36" t="s">
+      <c r="B256" s="21" t="s">
         <v>518</v>
       </c>
       <c r="C256" s="4" t="s">
@@ -9952,7 +9996,7 @@
       <c r="A257" s="18">
         <v>242</v>
       </c>
-      <c r="B257" s="37"/>
+      <c r="B257" s="22"/>
       <c r="C257" s="4" t="s">
         <v>521</v>
       </c>
@@ -9979,7 +10023,7 @@
       <c r="A258" s="18">
         <v>243</v>
       </c>
-      <c r="B258" s="37"/>
+      <c r="B258" s="22"/>
       <c r="C258" s="4" t="s">
         <v>176</v>
       </c>
@@ -10006,8 +10050,8 @@
       <c r="A259" s="18">
         <v>244</v>
       </c>
-      <c r="B259" s="37"/>
-      <c r="C259" s="23" t="s">
+      <c r="B259" s="22"/>
+      <c r="C259" s="27" t="s">
         <v>526</v>
       </c>
       <c r="D259" s="5" t="s">
@@ -10033,8 +10077,8 @@
       <c r="A260" s="18">
         <v>245</v>
       </c>
-      <c r="B260" s="37"/>
-      <c r="C260" s="29"/>
+      <c r="B260" s="22"/>
+      <c r="C260" s="28"/>
       <c r="D260" s="5" t="s">
         <v>529</v>
       </c>
@@ -10058,8 +10102,8 @@
       <c r="A261" s="18">
         <v>246</v>
       </c>
-      <c r="B261" s="37"/>
-      <c r="C261" s="24"/>
+      <c r="B261" s="22"/>
+      <c r="C261" s="29"/>
       <c r="D261" s="5" t="s">
         <v>531</v>
       </c>
@@ -10083,7 +10127,7 @@
       <c r="A262" s="18">
         <v>247</v>
       </c>
-      <c r="B262" s="37"/>
+      <c r="B262" s="22"/>
       <c r="C262" s="17" t="s">
         <v>533</v>
       </c>
@@ -10110,7 +10154,7 @@
       <c r="A263" s="18">
         <v>248</v>
       </c>
-      <c r="B263" s="37"/>
+      <c r="B263" s="22"/>
       <c r="C263" s="4" t="s">
         <v>536</v>
       </c>
@@ -10137,7 +10181,7 @@
       <c r="A264" s="18">
         <v>249</v>
       </c>
-      <c r="B264" s="37"/>
+      <c r="B264" s="22"/>
       <c r="C264" s="4" t="s">
         <v>539</v>
       </c>
@@ -10164,7 +10208,7 @@
       <c r="A265" s="18">
         <v>250</v>
       </c>
-      <c r="B265" s="38"/>
+      <c r="B265" s="23"/>
       <c r="C265" s="4" t="s">
         <v>542</v>
       </c>
@@ -10191,7 +10235,7 @@
       <c r="A266" s="18">
         <v>251</v>
       </c>
-      <c r="B266" s="36" t="s">
+      <c r="B266" s="21" t="s">
         <v>545</v>
       </c>
       <c r="C266" s="4" t="s">
@@ -10220,7 +10264,7 @@
       <c r="A267" s="18">
         <v>252</v>
       </c>
-      <c r="B267" s="37"/>
+      <c r="B267" s="22"/>
       <c r="C267" s="4" t="s">
         <v>548</v>
       </c>
@@ -10247,7 +10291,7 @@
       <c r="A268" s="18">
         <v>253</v>
       </c>
-      <c r="B268" s="37"/>
+      <c r="B268" s="22"/>
       <c r="C268" s="4" t="s">
         <v>551</v>
       </c>
@@ -10274,7 +10318,7 @@
       <c r="A269" s="18">
         <v>254</v>
       </c>
-      <c r="B269" s="37"/>
+      <c r="B269" s="22"/>
       <c r="C269" s="4" t="s">
         <v>554</v>
       </c>
@@ -10301,7 +10345,7 @@
       <c r="A270" s="18">
         <v>255</v>
       </c>
-      <c r="B270" s="37"/>
+      <c r="B270" s="22"/>
       <c r="C270" s="4" t="s">
         <v>539</v>
       </c>
@@ -10328,7 +10372,7 @@
       <c r="A271" s="18">
         <v>256</v>
       </c>
-      <c r="B271" s="38"/>
+      <c r="B271" s="23"/>
       <c r="C271" s="4" t="s">
         <v>536</v>
       </c>
@@ -10355,7 +10399,7 @@
       <c r="A272" s="18">
         <v>257</v>
       </c>
-      <c r="B272" s="36" t="s">
+      <c r="B272" s="21" t="s">
         <v>559</v>
       </c>
       <c r="C272" s="4" t="s">
@@ -10384,7 +10428,7 @@
       <c r="A273" s="18">
         <v>258</v>
       </c>
-      <c r="B273" s="37"/>
+      <c r="B273" s="22"/>
       <c r="C273" s="4" t="s">
         <v>521</v>
       </c>
@@ -10411,7 +10455,7 @@
       <c r="A274" s="18">
         <v>259</v>
       </c>
-      <c r="B274" s="37"/>
+      <c r="B274" s="22"/>
       <c r="C274" s="4" t="s">
         <v>176</v>
       </c>
@@ -10438,8 +10482,8 @@
       <c r="A275" s="18">
         <v>260</v>
       </c>
-      <c r="B275" s="37"/>
-      <c r="C275" s="23" t="s">
+      <c r="B275" s="22"/>
+      <c r="C275" s="27" t="s">
         <v>526</v>
       </c>
       <c r="D275" s="5" t="s">
@@ -10465,8 +10509,8 @@
       <c r="A276" s="18">
         <v>261</v>
       </c>
-      <c r="B276" s="37"/>
-      <c r="C276" s="29"/>
+      <c r="B276" s="22"/>
+      <c r="C276" s="28"/>
       <c r="D276" s="5" t="s">
         <v>529</v>
       </c>
@@ -10490,8 +10534,8 @@
       <c r="A277" s="18">
         <v>262</v>
       </c>
-      <c r="B277" s="37"/>
-      <c r="C277" s="24"/>
+      <c r="B277" s="22"/>
+      <c r="C277" s="29"/>
       <c r="D277" s="5" t="s">
         <v>531</v>
       </c>
@@ -10515,7 +10559,7 @@
       <c r="A278" s="18">
         <v>263</v>
       </c>
-      <c r="B278" s="37"/>
+      <c r="B278" s="22"/>
       <c r="C278" s="17" t="s">
         <v>533</v>
       </c>
@@ -10542,7 +10586,7 @@
       <c r="A279" s="18">
         <v>264</v>
       </c>
-      <c r="B279" s="37"/>
+      <c r="B279" s="22"/>
       <c r="C279" s="4" t="s">
         <v>536</v>
       </c>
@@ -10569,7 +10613,7 @@
       <c r="A280" s="18">
         <v>265</v>
       </c>
-      <c r="B280" s="38"/>
+      <c r="B280" s="23"/>
       <c r="C280" s="4" t="s">
         <v>539</v>
       </c>
@@ -10596,7 +10640,7 @@
       <c r="A281" s="18">
         <v>266</v>
       </c>
-      <c r="B281" s="36" t="s">
+      <c r="B281" s="21" t="s">
         <v>569</v>
       </c>
       <c r="C281" s="4" t="s">
@@ -10625,7 +10669,7 @@
       <c r="A282" s="18">
         <v>267</v>
       </c>
-      <c r="B282" s="37"/>
+      <c r="B282" s="22"/>
       <c r="C282" s="4" t="s">
         <v>521</v>
       </c>
@@ -10652,7 +10696,7 @@
       <c r="A283" s="18">
         <v>268</v>
       </c>
-      <c r="B283" s="37"/>
+      <c r="B283" s="22"/>
       <c r="C283" s="4" t="s">
         <v>176</v>
       </c>
@@ -10679,7 +10723,7 @@
       <c r="A284" s="18">
         <v>269</v>
       </c>
-      <c r="B284" s="37"/>
+      <c r="B284" s="22"/>
       <c r="C284" s="4" t="s">
         <v>539</v>
       </c>
@@ -10706,7 +10750,7 @@
       <c r="A285" s="18">
         <v>270</v>
       </c>
-      <c r="B285" s="37"/>
+      <c r="B285" s="22"/>
       <c r="C285" s="4" t="s">
         <v>536</v>
       </c>
@@ -10733,8 +10777,8 @@
       <c r="A286" s="18">
         <v>271</v>
       </c>
-      <c r="B286" s="37"/>
-      <c r="C286" s="23" t="s">
+      <c r="B286" s="22"/>
+      <c r="C286" s="27" t="s">
         <v>526</v>
       </c>
       <c r="D286" s="5" t="s">
@@ -10760,8 +10804,8 @@
       <c r="A287" s="18">
         <v>272</v>
       </c>
-      <c r="B287" s="37"/>
-      <c r="C287" s="29"/>
+      <c r="B287" s="22"/>
+      <c r="C287" s="28"/>
       <c r="D287" s="5" t="s">
         <v>529</v>
       </c>
@@ -10785,8 +10829,8 @@
       <c r="A288" s="18">
         <v>273</v>
       </c>
-      <c r="B288" s="37"/>
-      <c r="C288" s="29"/>
+      <c r="B288" s="22"/>
+      <c r="C288" s="28"/>
       <c r="D288" s="5" t="s">
         <v>531</v>
       </c>
@@ -10810,8 +10854,8 @@
       <c r="A289" s="18">
         <v>274</v>
       </c>
-      <c r="B289" s="37"/>
-      <c r="C289" s="29"/>
+      <c r="B289" s="22"/>
+      <c r="C289" s="28"/>
       <c r="D289" s="5" t="s">
         <v>578</v>
       </c>
@@ -10835,8 +10879,8 @@
       <c r="A290" s="18">
         <v>275</v>
       </c>
-      <c r="B290" s="37"/>
-      <c r="C290" s="29"/>
+      <c r="B290" s="22"/>
+      <c r="C290" s="28"/>
       <c r="D290" s="5" t="s">
         <v>580</v>
       </c>
@@ -10860,8 +10904,8 @@
       <c r="A291" s="18">
         <v>276</v>
       </c>
-      <c r="B291" s="38"/>
-      <c r="C291" s="24"/>
+      <c r="B291" s="23"/>
+      <c r="C291" s="29"/>
       <c r="D291" s="5" t="s">
         <v>580</v>
       </c>
@@ -10885,7 +10929,7 @@
       <c r="A292" s="18">
         <v>277</v>
       </c>
-      <c r="B292" s="36" t="s">
+      <c r="B292" s="21" t="s">
         <v>583</v>
       </c>
       <c r="C292" s="4" t="s">
@@ -10914,7 +10958,7 @@
       <c r="A293" s="18">
         <v>278</v>
       </c>
-      <c r="B293" s="37"/>
+      <c r="B293" s="22"/>
       <c r="C293" s="4" t="s">
         <v>521</v>
       </c>
@@ -10941,7 +10985,7 @@
       <c r="A294" s="18">
         <v>279</v>
       </c>
-      <c r="B294" s="37"/>
+      <c r="B294" s="22"/>
       <c r="C294" s="4" t="s">
         <v>176</v>
       </c>
@@ -10968,7 +11012,7 @@
       <c r="A295" s="18">
         <v>280</v>
       </c>
-      <c r="B295" s="37"/>
+      <c r="B295" s="22"/>
       <c r="C295" s="4" t="s">
         <v>536</v>
       </c>
@@ -10995,8 +11039,8 @@
       <c r="A296" s="18">
         <v>281</v>
       </c>
-      <c r="B296" s="37"/>
-      <c r="C296" s="23" t="s">
+      <c r="B296" s="22"/>
+      <c r="C296" s="27" t="s">
         <v>526</v>
       </c>
       <c r="D296" s="5" t="s">
@@ -11022,8 +11066,8 @@
       <c r="A297" s="18">
         <v>282</v>
       </c>
-      <c r="B297" s="37"/>
-      <c r="C297" s="29"/>
+      <c r="B297" s="22"/>
+      <c r="C297" s="28"/>
       <c r="D297" s="5" t="s">
         <v>529</v>
       </c>
@@ -11047,8 +11091,8 @@
       <c r="A298" s="18">
         <v>283</v>
       </c>
-      <c r="B298" s="37"/>
-      <c r="C298" s="29"/>
+      <c r="B298" s="22"/>
+      <c r="C298" s="28"/>
       <c r="D298" s="5" t="s">
         <v>531</v>
       </c>
@@ -11072,8 +11116,8 @@
       <c r="A299" s="18">
         <v>284</v>
       </c>
-      <c r="B299" s="37"/>
-      <c r="C299" s="24"/>
+      <c r="B299" s="22"/>
+      <c r="C299" s="29"/>
       <c r="D299" s="5" t="s">
         <v>589</v>
       </c>
@@ -11097,7 +11141,7 @@
       <c r="A300" s="18">
         <v>285</v>
       </c>
-      <c r="B300" s="37"/>
+      <c r="B300" s="22"/>
       <c r="C300" s="4" t="s">
         <v>591</v>
       </c>
@@ -11124,7 +11168,7 @@
       <c r="A301" s="18">
         <v>286</v>
       </c>
-      <c r="B301" s="38"/>
+      <c r="B301" s="23"/>
       <c r="C301" s="4" t="s">
         <v>539</v>
       </c>
@@ -11151,7 +11195,7 @@
       <c r="A302" s="18">
         <v>287</v>
       </c>
-      <c r="B302" s="39" t="s">
+      <c r="B302" s="30" t="s">
         <v>595</v>
       </c>
       <c r="C302" s="4" t="s">
@@ -11180,7 +11224,7 @@
       <c r="A303" s="18">
         <v>288</v>
       </c>
-      <c r="B303" s="40"/>
+      <c r="B303" s="31"/>
       <c r="C303" s="4" t="s">
         <v>591</v>
       </c>
@@ -11207,7 +11251,7 @@
       <c r="A304" s="18">
         <v>289</v>
       </c>
-      <c r="B304" s="40"/>
+      <c r="B304" s="31"/>
       <c r="C304" s="4" t="s">
         <v>539</v>
       </c>
@@ -11234,7 +11278,7 @@
       <c r="A305" s="18">
         <v>290</v>
       </c>
-      <c r="B305" s="40"/>
+      <c r="B305" s="31"/>
       <c r="C305" s="4" t="s">
         <v>536</v>
       </c>
@@ -11261,7 +11305,7 @@
       <c r="A306" s="18">
         <v>291</v>
       </c>
-      <c r="B306" s="41"/>
+      <c r="B306" s="32"/>
       <c r="C306" s="4" t="s">
         <v>600</v>
       </c>
@@ -11288,7 +11332,7 @@
       <c r="A307" s="18">
         <v>292</v>
       </c>
-      <c r="B307" s="36" t="s">
+      <c r="B307" s="21" t="s">
         <v>603</v>
       </c>
       <c r="C307" s="4" t="s">
@@ -11317,7 +11361,7 @@
       <c r="A308" s="18">
         <v>293</v>
       </c>
-      <c r="B308" s="37"/>
+      <c r="B308" s="22"/>
       <c r="C308" s="4" t="s">
         <v>539</v>
       </c>
@@ -11344,7 +11388,7 @@
       <c r="A309" s="18">
         <v>294</v>
       </c>
-      <c r="B309" s="37"/>
+      <c r="B309" s="22"/>
       <c r="C309" s="4" t="s">
         <v>536</v>
       </c>
@@ -11371,8 +11415,8 @@
       <c r="A310" s="18">
         <v>295</v>
       </c>
-      <c r="B310" s="37"/>
-      <c r="C310" s="23" t="s">
+      <c r="B310" s="22"/>
+      <c r="C310" s="27" t="s">
         <v>526</v>
       </c>
       <c r="D310" s="5" t="s">
@@ -11398,8 +11442,8 @@
       <c r="A311" s="18">
         <v>296</v>
       </c>
-      <c r="B311" s="37"/>
-      <c r="C311" s="29"/>
+      <c r="B311" s="22"/>
+      <c r="C311" s="28"/>
       <c r="D311" s="5" t="s">
         <v>529</v>
       </c>
@@ -11423,8 +11467,8 @@
       <c r="A312" s="18">
         <v>297</v>
       </c>
-      <c r="B312" s="37"/>
-      <c r="C312" s="24"/>
+      <c r="B312" s="22"/>
+      <c r="C312" s="29"/>
       <c r="D312" s="5" t="s">
         <v>531</v>
       </c>
@@ -11448,8 +11492,8 @@
       <c r="A313" s="18">
         <v>298</v>
       </c>
-      <c r="B313" s="37"/>
-      <c r="C313" s="23" t="s">
+      <c r="B313" s="22"/>
+      <c r="C313" s="27" t="s">
         <v>608</v>
       </c>
       <c r="D313" s="5" t="s">
@@ -11475,8 +11519,8 @@
       <c r="A314" s="18">
         <v>299</v>
       </c>
-      <c r="B314" s="37"/>
-      <c r="C314" s="29"/>
+      <c r="B314" s="22"/>
+      <c r="C314" s="28"/>
       <c r="D314" s="5" t="s">
         <v>611</v>
       </c>
@@ -11500,8 +11544,8 @@
       <c r="A315" s="18">
         <v>300</v>
       </c>
-      <c r="B315" s="37"/>
-      <c r="C315" s="24"/>
+      <c r="B315" s="22"/>
+      <c r="C315" s="29"/>
       <c r="D315" s="5" t="s">
         <v>613</v>
       </c>
@@ -11525,8 +11569,8 @@
       <c r="A316" s="18">
         <v>301</v>
       </c>
-      <c r="B316" s="37"/>
-      <c r="C316" s="23" t="s">
+      <c r="B316" s="22"/>
+      <c r="C316" s="27" t="s">
         <v>615</v>
       </c>
       <c r="D316" s="5" t="s">
@@ -11552,8 +11596,8 @@
       <c r="A317" s="18">
         <v>302</v>
       </c>
-      <c r="B317" s="37"/>
-      <c r="C317" s="24"/>
+      <c r="B317" s="22"/>
+      <c r="C317" s="29"/>
       <c r="D317" s="5" t="s">
         <v>618</v>
       </c>
@@ -11577,7 +11621,7 @@
       <c r="A318" s="18">
         <v>303</v>
       </c>
-      <c r="B318" s="38"/>
+      <c r="B318" s="23"/>
       <c r="C318" s="4" t="s">
         <v>620</v>
       </c>
@@ -11604,7 +11648,7 @@
       <c r="A319" s="18">
         <v>304</v>
       </c>
-      <c r="B319" s="36" t="s">
+      <c r="B319" s="21" t="s">
         <v>623</v>
       </c>
       <c r="C319" s="4" t="s">
@@ -11633,7 +11677,7 @@
       <c r="A320" s="18">
         <v>305</v>
       </c>
-      <c r="B320" s="37"/>
+      <c r="B320" s="22"/>
       <c r="C320" s="4" t="s">
         <v>533</v>
       </c>
@@ -11660,7 +11704,7 @@
       <c r="A321" s="18">
         <v>306</v>
       </c>
-      <c r="B321" s="37"/>
+      <c r="B321" s="22"/>
       <c r="C321" s="4" t="s">
         <v>539</v>
       </c>
@@ -11687,7 +11731,7 @@
       <c r="A322" s="18">
         <v>307</v>
       </c>
-      <c r="B322" s="38"/>
+      <c r="B322" s="23"/>
       <c r="C322" s="4" t="s">
         <v>536</v>
       </c>
@@ -11712,6 +11756,76 @@
     </row>
   </sheetData>
   <mergeCells count="86">
+    <mergeCell ref="B22:B36"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B109:B112"/>
+    <mergeCell ref="B113:B130"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="B80:B87"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="B101:B108"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="C127:C129"/>
+    <mergeCell ref="C109:C112"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="C58:C62"/>
+    <mergeCell ref="B63:B79"/>
+    <mergeCell ref="C63:C68"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="B88:B95"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="C136:C138"/>
+    <mergeCell ref="C139:C144"/>
+    <mergeCell ref="B147:B149"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="B131:B146"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="B150:B156"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="B161:B175"/>
+    <mergeCell ref="C162:C163"/>
+    <mergeCell ref="C164:C165"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="C169:C170"/>
+    <mergeCell ref="C171:C173"/>
+    <mergeCell ref="B220:B229"/>
+    <mergeCell ref="C221:C223"/>
+    <mergeCell ref="C225:C227"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B176:B179"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="B180:B183"/>
+    <mergeCell ref="B187:B191"/>
+    <mergeCell ref="B192:B202"/>
+    <mergeCell ref="B203:B207"/>
+    <mergeCell ref="B208:B219"/>
+    <mergeCell ref="C209:C211"/>
+    <mergeCell ref="C214:C216"/>
+    <mergeCell ref="C247:C250"/>
+    <mergeCell ref="B256:B265"/>
+    <mergeCell ref="C259:C261"/>
+    <mergeCell ref="B266:B271"/>
+    <mergeCell ref="B272:B280"/>
+    <mergeCell ref="C275:C277"/>
     <mergeCell ref="B319:B322"/>
     <mergeCell ref="B184:B186"/>
     <mergeCell ref="B292:B301"/>
@@ -11728,82 +11842,12 @@
     <mergeCell ref="C235:C237"/>
     <mergeCell ref="B241:B245"/>
     <mergeCell ref="B246:B255"/>
-    <mergeCell ref="C247:C250"/>
-    <mergeCell ref="B256:B265"/>
-    <mergeCell ref="C259:C261"/>
-    <mergeCell ref="B266:B271"/>
-    <mergeCell ref="B272:B280"/>
-    <mergeCell ref="C275:C277"/>
-    <mergeCell ref="B220:B229"/>
-    <mergeCell ref="C221:C223"/>
-    <mergeCell ref="C225:C227"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B176:B179"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="B180:B183"/>
-    <mergeCell ref="B187:B191"/>
-    <mergeCell ref="B192:B202"/>
-    <mergeCell ref="B203:B207"/>
-    <mergeCell ref="B208:B219"/>
-    <mergeCell ref="C209:C211"/>
-    <mergeCell ref="C214:C216"/>
-    <mergeCell ref="B150:B156"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="B161:B175"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="C164:C165"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="C169:C170"/>
-    <mergeCell ref="C171:C173"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="C136:C138"/>
-    <mergeCell ref="C139:C144"/>
-    <mergeCell ref="B147:B149"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="B131:B146"/>
-    <mergeCell ref="C131:C133"/>
-    <mergeCell ref="B63:B79"/>
-    <mergeCell ref="C63:C68"/>
-    <mergeCell ref="C69:C74"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="B88:B95"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="C58:C62"/>
-    <mergeCell ref="B109:B112"/>
-    <mergeCell ref="B113:B130"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="B80:B87"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="B101:B108"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="C122:C124"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="C127:C129"/>
-    <mergeCell ref="C109:C112"/>
-    <mergeCell ref="B22:B36"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 K54:K57 K59:K212" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 K54:K57 K59:K212">
       <formula1>$C$2:$C$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G16:I322" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G16:I322">
       <formula1>$B$1:$B$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -11835,7 +11879,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G132:I255 G16:I130</xm:sqref>
+          <xm:sqref>G16:I130 G132:I255</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="9" operator="containsText" id="{5F2DFDBD-06DA-4837-B76B-210602F638BB}">

</xml_diff>

<commit_message>
up test giao dien man hnh chinh
</commit_message>
<xml_diff>
--- a/TestCase-Reup.xlsx
+++ b/TestCase-Reup.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ChuyenDe12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F967991-73FD-4ED9-B325-19E9AA8609CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="615">
   <si>
     <t>Kết quả test trên ứng dụng</t>
   </si>
@@ -2486,9 +2485,6 @@
 2. click the Tabbar . Button</t>
   </si>
   <si>
-    <t>Không đăng nhập bằng fb đuọc</t>
-  </si>
-  <si>
     <t>Go to History screen</t>
   </si>
   <si>
@@ -2559,12 +2555,18 @@
   </si>
   <si>
     <t>Answer is wrong, the button will turn red. The screen will appear "Incorrect (Red)". Correct answer, the button will turn green. The screen will appear "Exacly (Green)"</t>
+  </si>
+  <si>
+    <t>Bấm vào không có chuyển sang màn đăng nhập bằng fb</t>
+  </si>
+  <si>
+    <t>Lõi không đăng nhập được</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2728,7 +2730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2796,6 +2798,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2808,22 +2825,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2835,41 +2864,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3313,11 +3346,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M240" sqref="M240"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H181" sqref="H181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3507,11 +3540,11 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="2"/>
       <c r="K13" s="9"/>
     </row>
@@ -3532,11 +3565,11 @@
       <c r="F14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
       <c r="J14" s="2"/>
       <c r="K14" s="9"/>
     </row>
@@ -3575,11 +3608,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -3608,7 +3641,7 @@
       <c r="A17" s="4">
         <v>2</v>
       </c>
-      <c r="B17" s="24"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="4" t="s">
         <v>23</v>
       </c>
@@ -3637,7 +3670,7 @@
       <c r="A18" s="22">
         <v>3</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
@@ -3666,7 +3699,7 @@
       <c r="A19" s="22">
         <v>4</v>
       </c>
-      <c r="B19" s="24"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
@@ -3695,7 +3728,7 @@
       <c r="A20" s="22">
         <v>5</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3724,7 +3757,7 @@
       <c r="A21" s="22">
         <v>6</v>
       </c>
-      <c r="B21" s="25"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
@@ -3751,10 +3784,10 @@
       <c r="A22" s="22">
         <v>7</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -3780,8 +3813,8 @@
       <c r="A23" s="22">
         <v>8</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="5" t="s">
         <v>42</v>
       </c>
@@ -3805,8 +3838,8 @@
       <c r="A24" s="22">
         <v>9</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="31" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -3832,8 +3865,8 @@
       <c r="A25" s="22">
         <v>10</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="5" t="s">
         <v>42</v>
       </c>
@@ -3857,7 +3890,7 @@
       <c r="A26" s="22">
         <v>11</v>
       </c>
-      <c r="B26" s="24"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="4" t="s">
         <v>46</v>
       </c>
@@ -3884,7 +3917,7 @@
       <c r="A27" s="22">
         <v>12</v>
       </c>
-      <c r="B27" s="24"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="4" t="s">
         <v>49</v>
       </c>
@@ -3911,7 +3944,7 @@
       <c r="A28" s="22">
         <v>13</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
@@ -3938,7 +3971,7 @@
       <c r="A29" s="22">
         <v>14</v>
       </c>
-      <c r="B29" s="24"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="4" t="s">
         <v>54</v>
       </c>
@@ -3965,7 +3998,7 @@
       <c r="A30" s="22">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="4" t="s">
         <v>55</v>
       </c>
@@ -3994,7 +4027,7 @@
       <c r="A31" s="22">
         <v>16</v>
       </c>
-      <c r="B31" s="24"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="4" t="s">
         <v>58</v>
       </c>
@@ -4023,7 +4056,7 @@
       <c r="A32" s="22">
         <v>17</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="4" t="s">
         <v>58</v>
       </c>
@@ -4052,7 +4085,7 @@
       <c r="A33" s="22">
         <v>18</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="4" t="s">
         <v>61</v>
       </c>
@@ -4073,15 +4106,17 @@
         <v>132</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="K33" s="5"/>
+        <v>613</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="22">
         <v>19</v>
       </c>
-      <c r="B34" s="24"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="4" t="s">
         <v>64</v>
       </c>
@@ -4093,7 +4128,7 @@
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="11" t="s">
-        <v>22</v>
+        <v>177</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>22</v>
@@ -4108,7 +4143,7 @@
       <c r="A35" s="22">
         <v>20</v>
       </c>
-      <c r="B35" s="24"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="4" t="s">
         <v>65</v>
       </c>
@@ -4135,7 +4170,7 @@
       <c r="A36" s="22">
         <v>21</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="4" t="s">
         <v>65</v>
       </c>
@@ -4162,7 +4197,7 @@
       <c r="A37" s="22">
         <v>22</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -4191,7 +4226,7 @@
       <c r="A38" s="22">
         <v>23</v>
       </c>
-      <c r="B38" s="24"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="4" t="s">
         <v>71</v>
       </c>
@@ -4220,7 +4255,7 @@
       <c r="A39" s="22">
         <v>24</v>
       </c>
-      <c r="B39" s="24"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="4" t="s">
         <v>74</v>
       </c>
@@ -4249,7 +4284,7 @@
       <c r="A40" s="22">
         <v>25</v>
       </c>
-      <c r="B40" s="24"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="4" t="s">
         <v>76</v>
       </c>
@@ -4278,7 +4313,7 @@
       <c r="A41" s="22">
         <v>26</v>
       </c>
-      <c r="B41" s="24"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="4" t="s">
         <v>79</v>
       </c>
@@ -4307,7 +4342,7 @@
       <c r="A42" s="22">
         <v>27</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="4" t="s">
         <v>81</v>
       </c>
@@ -4334,7 +4369,7 @@
       <c r="A43" s="22">
         <v>28</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="4" t="s">
         <v>84</v>
       </c>
@@ -4361,7 +4396,7 @@
       <c r="A44" s="22">
         <v>29</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -4390,7 +4425,7 @@
       <c r="A45" s="22">
         <v>30</v>
       </c>
-      <c r="B45" s="24"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="4" t="s">
         <v>89</v>
       </c>
@@ -4417,7 +4452,7 @@
       <c r="A46" s="22">
         <v>31</v>
       </c>
-      <c r="B46" s="24"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="4" t="s">
         <v>71</v>
       </c>
@@ -4446,7 +4481,7 @@
       <c r="A47" s="22">
         <v>32</v>
       </c>
-      <c r="B47" s="24"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="4" t="s">
         <v>74</v>
       </c>
@@ -4475,7 +4510,7 @@
       <c r="A48" s="22">
         <v>33</v>
       </c>
-      <c r="B48" s="24"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="4" t="s">
         <v>92</v>
       </c>
@@ -4504,7 +4539,7 @@
       <c r="A49" s="22">
         <v>34</v>
       </c>
-      <c r="B49" s="25"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="4" t="s">
         <v>96</v>
       </c>
@@ -4533,7 +4568,7 @@
       <c r="A50" s="22">
         <v>35</v>
       </c>
-      <c r="B50" s="33" t="s">
+      <c r="B50" s="42" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -4562,7 +4597,7 @@
       <c r="A51" s="22">
         <v>36</v>
       </c>
-      <c r="B51" s="34"/>
+      <c r="B51" s="43"/>
       <c r="C51" s="4" t="s">
         <v>71</v>
       </c>
@@ -4591,7 +4626,7 @@
       <c r="A52" s="22">
         <v>37</v>
       </c>
-      <c r="B52" s="35"/>
+      <c r="B52" s="44"/>
       <c r="C52" s="4" t="s">
         <v>74</v>
       </c>
@@ -4618,7 +4653,7 @@
       <c r="A53" s="22">
         <v>38</v>
       </c>
-      <c r="B53" s="23" t="s">
+      <c r="B53" s="28" t="s">
         <v>107</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -4647,7 +4682,7 @@
       <c r="A54" s="22">
         <v>39</v>
       </c>
-      <c r="B54" s="24"/>
+      <c r="B54" s="29"/>
       <c r="C54" s="4" t="s">
         <v>71</v>
       </c>
@@ -4676,7 +4711,7 @@
       <c r="A55" s="22">
         <v>40</v>
       </c>
-      <c r="B55" s="24"/>
+      <c r="B55" s="29"/>
       <c r="C55" s="4" t="s">
         <v>74</v>
       </c>
@@ -4705,7 +4740,7 @@
       <c r="A56" s="22">
         <v>41</v>
       </c>
-      <c r="B56" s="24"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="4" t="s">
         <v>74</v>
       </c>
@@ -4734,7 +4769,7 @@
       <c r="A57" s="22">
         <v>42</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="30"/>
       <c r="C57" s="4" t="s">
         <v>74</v>
       </c>
@@ -4763,14 +4798,14 @@
       <c r="A58" s="22">
         <v>43</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="41" t="s">
         <v>19</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>122</v>
@@ -4792,8 +4827,8 @@
       <c r="A59" s="22">
         <v>44</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="31"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="41"/>
       <c r="D59" s="5" t="s">
         <v>123</v>
       </c>
@@ -4817,8 +4852,8 @@
       <c r="A60" s="22">
         <v>45</v>
       </c>
-      <c r="B60" s="30"/>
-      <c r="C60" s="31"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="41"/>
       <c r="D60" s="5" t="s">
         <v>125</v>
       </c>
@@ -4842,13 +4877,13 @@
       <c r="A61" s="22">
         <v>46</v>
       </c>
-      <c r="B61" s="30"/>
-      <c r="C61" s="31"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="41"/>
       <c r="D61" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="11" t="s">
@@ -4867,13 +4902,13 @@
       <c r="A62" s="22">
         <v>47</v>
       </c>
-      <c r="B62" s="30"/>
-      <c r="C62" s="31"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="41"/>
       <c r="D62" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>598</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>599</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="11" t="s">
@@ -4892,10 +4927,10 @@
       <c r="A63" s="22">
         <v>48</v>
       </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="31"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="41"/>
       <c r="D63" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>127</v>
@@ -4917,17 +4952,17 @@
       <c r="A64" s="22">
         <v>49</v>
       </c>
-      <c r="B64" s="23" t="s">
+      <c r="B64" s="28" t="s">
+        <v>599</v>
+      </c>
+      <c r="C64" s="21" t="s">
         <v>600</v>
       </c>
-      <c r="C64" s="21" t="s">
-        <v>601</v>
-      </c>
       <c r="D64" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>603</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>604</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="11" t="s">
@@ -4946,9 +4981,9 @@
       <c r="A65" s="22">
         <v>50</v>
       </c>
-      <c r="B65" s="24"/>
+      <c r="B65" s="29"/>
       <c r="C65" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>139</v>
@@ -4973,15 +5008,15 @@
       <c r="A66" s="22">
         <v>51</v>
       </c>
-      <c r="B66" s="24"/>
+      <c r="B66" s="29"/>
       <c r="C66" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>596</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>597</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="22" t="s">
@@ -5000,15 +5035,15 @@
       <c r="A67" s="22">
         <v>52</v>
       </c>
-      <c r="B67" s="25"/>
-      <c r="C67" s="45" t="s">
+      <c r="B67" s="30"/>
+      <c r="C67" s="24" t="s">
         <v>228</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>250</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="11" t="s">
@@ -5027,10 +5062,10 @@
       <c r="A68" s="22">
         <v>53</v>
       </c>
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="31" t="s">
         <v>129</v>
       </c>
       <c r="D68" s="5" t="s">
@@ -5056,7 +5091,7 @@
       <c r="A69" s="22">
         <v>54</v>
       </c>
-      <c r="B69" s="24"/>
+      <c r="B69" s="29"/>
       <c r="C69" s="32"/>
       <c r="D69" s="5" t="s">
         <v>133</v>
@@ -5083,8 +5118,8 @@
       <c r="A70" s="22">
         <v>55</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="27"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="33"/>
       <c r="D70" s="5" t="s">
         <v>136</v>
       </c>
@@ -5110,7 +5145,7 @@
       <c r="A71" s="22">
         <v>56</v>
       </c>
-      <c r="B71" s="24"/>
+      <c r="B71" s="29"/>
       <c r="C71" s="4" t="s">
         <v>138</v>
       </c>
@@ -5137,8 +5172,8 @@
       <c r="A72" s="22">
         <v>57</v>
       </c>
-      <c r="B72" s="24"/>
-      <c r="C72" s="31" t="s">
+      <c r="B72" s="29"/>
+      <c r="C72" s="41" t="s">
         <v>141</v>
       </c>
       <c r="D72" s="5" t="s">
@@ -5164,8 +5199,8 @@
       <c r="A73" s="22">
         <v>58</v>
       </c>
-      <c r="B73" s="24"/>
-      <c r="C73" s="31"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="41"/>
       <c r="D73" s="5" t="s">
         <v>144</v>
       </c>
@@ -5189,8 +5224,8 @@
       <c r="A74" s="22">
         <v>59</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="31"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="41"/>
       <c r="D74" s="5" t="s">
         <v>146</v>
       </c>
@@ -5214,7 +5249,7 @@
       <c r="A75" s="22">
         <v>60</v>
       </c>
-      <c r="B75" s="24"/>
+      <c r="B75" s="29"/>
       <c r="C75" s="22" t="s">
         <v>228</v>
       </c>
@@ -5222,7 +5257,7 @@
         <v>250</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="11" t="s">
@@ -5241,7 +5276,7 @@
       <c r="A76" s="22">
         <v>61</v>
       </c>
-      <c r="B76" s="25"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="4"/>
       <c r="D76" s="5" t="s">
         <v>148</v>
@@ -5266,10 +5301,10 @@
       <c r="A77" s="22">
         <v>62</v>
       </c>
-      <c r="B77" s="23" t="s">
+      <c r="B77" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="C77" s="31" t="s">
+      <c r="C77" s="41" t="s">
         <v>151</v>
       </c>
       <c r="D77" s="5" t="s">
@@ -5297,8 +5332,8 @@
       <c r="A78" s="22">
         <v>63</v>
       </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="31"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="41"/>
       <c r="D78" s="5" t="s">
         <v>155</v>
       </c>
@@ -5322,8 +5357,8 @@
       <c r="A79" s="22">
         <v>64</v>
       </c>
-      <c r="B79" s="24"/>
-      <c r="C79" s="31" t="s">
+      <c r="B79" s="29"/>
+      <c r="C79" s="41" t="s">
         <v>157</v>
       </c>
       <c r="D79" s="5" t="s">
@@ -5349,8 +5384,8 @@
       <c r="A80" s="22">
         <v>65</v>
       </c>
-      <c r="B80" s="24"/>
-      <c r="C80" s="31"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="41"/>
       <c r="D80" s="5" t="s">
         <v>160</v>
       </c>
@@ -5374,8 +5409,8 @@
       <c r="A81" s="22">
         <v>66</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="31"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="41"/>
       <c r="D81" s="5" t="s">
         <v>162</v>
       </c>
@@ -5399,8 +5434,8 @@
       <c r="A82" s="22">
         <v>67</v>
       </c>
-      <c r="B82" s="24"/>
-      <c r="C82" s="31"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="41"/>
       <c r="D82" s="5" t="s">
         <v>164</v>
       </c>
@@ -5424,15 +5459,15 @@
       <c r="A83" s="22">
         <v>68</v>
       </c>
-      <c r="B83" s="24"/>
+      <c r="B83" s="29"/>
       <c r="C83" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>596</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>597</v>
       </c>
       <c r="F83" s="5"/>
       <c r="G83" s="22" t="s">
@@ -5451,7 +5486,7 @@
       <c r="A84" s="22">
         <v>69</v>
       </c>
-      <c r="B84" s="24"/>
+      <c r="B84" s="29"/>
       <c r="C84" s="4" t="s">
         <v>138</v>
       </c>
@@ -5478,7 +5513,7 @@
       <c r="A85" s="22">
         <v>70</v>
       </c>
-      <c r="B85" s="24"/>
+      <c r="B85" s="29"/>
       <c r="C85" s="22" t="s">
         <v>228</v>
       </c>
@@ -5486,7 +5521,7 @@
         <v>250</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F85" s="5"/>
       <c r="G85" s="11" t="s">
@@ -5505,7 +5540,7 @@
       <c r="A86" s="22">
         <v>71</v>
       </c>
-      <c r="B86" s="25"/>
+      <c r="B86" s="30"/>
       <c r="C86" s="4"/>
       <c r="D86" s="5" t="s">
         <v>148</v>
@@ -5530,10 +5565,10 @@
       <c r="A87" s="22">
         <v>72</v>
       </c>
-      <c r="B87" s="30" t="s">
+      <c r="B87" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="C87" s="31" t="s">
+      <c r="C87" s="41" t="s">
         <v>151</v>
       </c>
       <c r="D87" s="5" t="s">
@@ -5559,8 +5594,8 @@
       <c r="A88" s="22">
         <v>73</v>
       </c>
-      <c r="B88" s="30"/>
-      <c r="C88" s="31"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="41"/>
       <c r="D88" s="5" t="s">
         <v>155</v>
       </c>
@@ -5584,8 +5619,8 @@
       <c r="A89" s="22">
         <v>74</v>
       </c>
-      <c r="B89" s="30"/>
-      <c r="C89" s="31" t="s">
+      <c r="B89" s="40"/>
+      <c r="C89" s="41" t="s">
         <v>157</v>
       </c>
       <c r="D89" s="5" t="s">
@@ -5611,8 +5646,8 @@
       <c r="A90" s="22">
         <v>75</v>
       </c>
-      <c r="B90" s="30"/>
-      <c r="C90" s="31"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="41"/>
       <c r="D90" s="5" t="s">
         <v>160</v>
       </c>
@@ -5636,8 +5671,8 @@
       <c r="A91" s="22">
         <v>76</v>
       </c>
-      <c r="B91" s="30"/>
-      <c r="C91" s="31"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="41"/>
       <c r="D91" s="5" t="s">
         <v>162</v>
       </c>
@@ -5661,8 +5696,8 @@
       <c r="A92" s="22">
         <v>77</v>
       </c>
-      <c r="B92" s="30"/>
-      <c r="C92" s="31"/>
+      <c r="B92" s="40"/>
+      <c r="C92" s="41"/>
       <c r="D92" s="5" t="s">
         <v>164</v>
       </c>
@@ -5686,15 +5721,15 @@
       <c r="A93" s="22">
         <v>78</v>
       </c>
-      <c r="B93" s="30"/>
+      <c r="B93" s="40"/>
       <c r="C93" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="E93" s="5" t="s">
         <v>596</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>597</v>
       </c>
       <c r="F93" s="5"/>
       <c r="G93" s="22" t="s">
@@ -5713,7 +5748,7 @@
       <c r="A94" s="22">
         <v>79</v>
       </c>
-      <c r="B94" s="30"/>
+      <c r="B94" s="40"/>
       <c r="C94" s="4" t="s">
         <v>138</v>
       </c>
@@ -5740,7 +5775,7 @@
       <c r="A95" s="22">
         <v>80</v>
       </c>
-      <c r="B95" s="30"/>
+      <c r="B95" s="40"/>
       <c r="C95" s="22" t="s">
         <v>228</v>
       </c>
@@ -5748,7 +5783,7 @@
         <v>250</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F95" s="5"/>
       <c r="G95" s="11" t="s">
@@ -5767,7 +5802,7 @@
       <c r="A96" s="22">
         <v>81</v>
       </c>
-      <c r="B96" s="30"/>
+      <c r="B96" s="40"/>
       <c r="C96" s="4"/>
       <c r="D96" s="5" t="s">
         <v>148</v>
@@ -5792,7 +5827,7 @@
       <c r="A97" s="22">
         <v>82</v>
       </c>
-      <c r="B97" s="30" t="s">
+      <c r="B97" s="40" t="s">
         <v>168</v>
       </c>
       <c r="C97" s="4" t="s">
@@ -5821,7 +5856,7 @@
       <c r="A98" s="22">
         <v>83</v>
       </c>
-      <c r="B98" s="30"/>
+      <c r="B98" s="40"/>
       <c r="C98" s="22" t="s">
         <v>228</v>
       </c>
@@ -5829,7 +5864,7 @@
         <v>250</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F98" s="5"/>
       <c r="G98" s="22" t="s">
@@ -5848,7 +5883,7 @@
       <c r="A99" s="22">
         <v>84</v>
       </c>
-      <c r="B99" s="30"/>
+      <c r="B99" s="40"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5" t="s">
         <v>148</v>
@@ -5873,7 +5908,7 @@
       <c r="A100" s="22">
         <v>85</v>
       </c>
-      <c r="B100" s="30" t="s">
+      <c r="B100" s="40" t="s">
         <v>172</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -5902,7 +5937,7 @@
       <c r="A101" s="22">
         <v>86</v>
       </c>
-      <c r="B101" s="30"/>
+      <c r="B101" s="40"/>
       <c r="C101" s="4" t="s">
         <v>173</v>
       </c>
@@ -5929,15 +5964,15 @@
       <c r="A102" s="22">
         <v>87</v>
       </c>
-      <c r="B102" s="30"/>
-      <c r="C102" s="31" t="s">
+      <c r="B102" s="40"/>
+      <c r="C102" s="41" t="s">
         <v>176</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F102" s="5"/>
       <c r="G102" s="4" t="s">
@@ -5950,7 +5985,7 @@
         <v>22</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K102" s="7"/>
     </row>
@@ -5958,13 +5993,13 @@
       <c r="A103" s="22">
         <v>88</v>
       </c>
-      <c r="B103" s="30"/>
-      <c r="C103" s="31"/>
+      <c r="B103" s="40"/>
+      <c r="C103" s="41"/>
       <c r="D103" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F103" s="5"/>
       <c r="G103" s="4" t="s">
@@ -5977,7 +6012,7 @@
         <v>22</v>
       </c>
       <c r="J103" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K103" s="7"/>
     </row>
@@ -5985,13 +6020,13 @@
       <c r="A104" s="22">
         <v>89</v>
       </c>
-      <c r="B104" s="30"/>
-      <c r="C104" s="31"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="41"/>
       <c r="D104" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F104" s="5"/>
       <c r="G104" s="4" t="s">
@@ -6004,7 +6039,7 @@
         <v>22</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K104" s="7"/>
     </row>
@@ -6012,13 +6047,13 @@
       <c r="A105" s="22">
         <v>90</v>
       </c>
-      <c r="B105" s="30"/>
-      <c r="C105" s="31"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="41"/>
       <c r="D105" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="4" t="s">
@@ -6031,7 +6066,7 @@
         <v>22</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K105" s="7"/>
     </row>
@@ -6039,7 +6074,7 @@
       <c r="A106" s="22">
         <v>91</v>
       </c>
-      <c r="B106" s="30"/>
+      <c r="B106" s="40"/>
       <c r="C106" s="4" t="s">
         <v>228</v>
       </c>
@@ -6047,7 +6082,7 @@
         <v>250</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="22" t="s">
@@ -6066,7 +6101,7 @@
       <c r="A107" s="22">
         <v>92</v>
       </c>
-      <c r="B107" s="30"/>
+      <c r="B107" s="40"/>
       <c r="C107" s="4"/>
       <c r="D107" s="5" t="s">
         <v>148</v>
@@ -6091,10 +6126,10 @@
       <c r="A108" s="22">
         <v>93</v>
       </c>
-      <c r="B108" s="30" t="s">
+      <c r="B108" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="C108" s="26" t="s">
+      <c r="C108" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D108" s="5" t="s">
@@ -6120,7 +6155,7 @@
       <c r="A109" s="22">
         <v>94</v>
       </c>
-      <c r="B109" s="30"/>
+      <c r="B109" s="40"/>
       <c r="C109" s="32"/>
       <c r="D109" s="5" t="s">
         <v>181</v>
@@ -6145,10 +6180,10 @@
       <c r="A110" s="22">
         <v>95</v>
       </c>
-      <c r="B110" s="30"/>
+      <c r="B110" s="40"/>
       <c r="C110" s="32"/>
       <c r="D110" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>183</v>
@@ -6170,10 +6205,10 @@
       <c r="A111" s="22">
         <v>96</v>
       </c>
-      <c r="B111" s="30"/>
-      <c r="C111" s="27"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="33"/>
       <c r="D111" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>184</v>
@@ -6195,7 +6230,7 @@
       <c r="A112" s="22">
         <v>97</v>
       </c>
-      <c r="B112" s="30" t="s">
+      <c r="B112" s="40" t="s">
         <v>185</v>
       </c>
       <c r="C112" s="4" t="s">
@@ -6224,8 +6259,8 @@
       <c r="A113" s="22">
         <v>98</v>
       </c>
-      <c r="B113" s="30"/>
-      <c r="C113" s="31" t="s">
+      <c r="B113" s="40"/>
+      <c r="C113" s="41" t="s">
         <v>189</v>
       </c>
       <c r="D113" s="5" t="s">
@@ -6251,8 +6286,8 @@
       <c r="A114" s="22">
         <v>99</v>
       </c>
-      <c r="B114" s="30"/>
-      <c r="C114" s="31"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="41"/>
       <c r="D114" s="5" t="s">
         <v>192</v>
       </c>
@@ -6276,8 +6311,8 @@
       <c r="A115" s="22">
         <v>100</v>
       </c>
-      <c r="B115" s="30"/>
-      <c r="C115" s="31"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="41"/>
       <c r="D115" s="5" t="s">
         <v>194</v>
       </c>
@@ -6301,8 +6336,8 @@
       <c r="A116" s="22">
         <v>101</v>
       </c>
-      <c r="B116" s="30"/>
-      <c r="C116" s="31"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="41"/>
       <c r="D116" s="5" t="s">
         <v>196</v>
       </c>
@@ -6326,8 +6361,8 @@
       <c r="A117" s="22">
         <v>102</v>
       </c>
-      <c r="B117" s="30"/>
-      <c r="C117" s="31" t="s">
+      <c r="B117" s="40"/>
+      <c r="C117" s="41" t="s">
         <v>197</v>
       </c>
       <c r="D117" s="5" t="s">
@@ -6353,8 +6388,8 @@
       <c r="A118" s="22">
         <v>103</v>
       </c>
-      <c r="B118" s="30"/>
-      <c r="C118" s="31"/>
+      <c r="B118" s="40"/>
+      <c r="C118" s="41"/>
       <c r="D118" s="5" t="s">
         <v>200</v>
       </c>
@@ -6378,8 +6413,8 @@
       <c r="A119" s="22">
         <v>104</v>
       </c>
-      <c r="B119" s="30"/>
-      <c r="C119" s="31"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="41"/>
       <c r="D119" s="5" t="s">
         <v>202</v>
       </c>
@@ -6403,8 +6438,8 @@
       <c r="A120" s="22">
         <v>105</v>
       </c>
-      <c r="B120" s="30"/>
-      <c r="C120" s="31"/>
+      <c r="B120" s="40"/>
+      <c r="C120" s="41"/>
       <c r="D120" s="5" t="s">
         <v>203</v>
       </c>
@@ -6428,8 +6463,8 @@
       <c r="A121" s="22">
         <v>106</v>
       </c>
-      <c r="B121" s="30"/>
-      <c r="C121" s="31" t="s">
+      <c r="B121" s="40"/>
+      <c r="C121" s="41" t="s">
         <v>204</v>
       </c>
       <c r="D121" s="5" t="s">
@@ -6455,8 +6490,8 @@
       <c r="A122" s="22">
         <v>107</v>
       </c>
-      <c r="B122" s="30"/>
-      <c r="C122" s="31"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="41"/>
       <c r="D122" s="5" t="s">
         <v>207</v>
       </c>
@@ -6480,8 +6515,8 @@
       <c r="A123" s="22">
         <v>108</v>
       </c>
-      <c r="B123" s="30"/>
-      <c r="C123" s="31"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="41"/>
       <c r="D123" s="5" t="s">
         <v>208</v>
       </c>
@@ -6505,8 +6540,8 @@
       <c r="A124" s="22">
         <v>109</v>
       </c>
-      <c r="B124" s="30"/>
-      <c r="C124" s="31" t="s">
+      <c r="B124" s="40"/>
+      <c r="C124" s="41" t="s">
         <v>210</v>
       </c>
       <c r="D124" s="5" t="s">
@@ -6532,8 +6567,8 @@
       <c r="A125" s="22">
         <v>110</v>
       </c>
-      <c r="B125" s="30"/>
-      <c r="C125" s="31"/>
+      <c r="B125" s="40"/>
+      <c r="C125" s="41"/>
       <c r="D125" s="5" t="s">
         <v>213</v>
       </c>
@@ -6557,8 +6592,8 @@
       <c r="A126" s="22">
         <v>111</v>
       </c>
-      <c r="B126" s="30"/>
-      <c r="C126" s="31" t="s">
+      <c r="B126" s="40"/>
+      <c r="C126" s="41" t="s">
         <v>215</v>
       </c>
       <c r="D126" s="5" t="s">
@@ -6584,8 +6619,8 @@
       <c r="A127" s="22">
         <v>112</v>
       </c>
-      <c r="B127" s="30"/>
-      <c r="C127" s="31"/>
+      <c r="B127" s="40"/>
+      <c r="C127" s="41"/>
       <c r="D127" s="5" t="s">
         <v>218</v>
       </c>
@@ -6609,8 +6644,8 @@
       <c r="A128" s="22">
         <v>113</v>
       </c>
-      <c r="B128" s="30"/>
-      <c r="C128" s="31"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="41"/>
       <c r="D128" s="5" t="s">
         <v>220</v>
       </c>
@@ -6634,7 +6669,7 @@
       <c r="A129" s="22">
         <v>114</v>
       </c>
-      <c r="B129" s="30"/>
+      <c r="B129" s="40"/>
       <c r="C129" s="4"/>
       <c r="D129" s="8" t="s">
         <v>148</v>
@@ -6659,10 +6694,10 @@
       <c r="A130" s="22">
         <v>115</v>
       </c>
-      <c r="B130" s="30" t="s">
+      <c r="B130" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="C130" s="31" t="s">
+      <c r="C130" s="41" t="s">
         <v>224</v>
       </c>
       <c r="D130" s="5" t="s">
@@ -6688,8 +6723,8 @@
       <c r="A131" s="22">
         <v>116</v>
       </c>
-      <c r="B131" s="30"/>
-      <c r="C131" s="31"/>
+      <c r="B131" s="40"/>
+      <c r="C131" s="41"/>
       <c r="D131" s="5" t="s">
         <v>231</v>
       </c>
@@ -6713,8 +6748,8 @@
       <c r="A132" s="22">
         <v>117</v>
       </c>
-      <c r="B132" s="30"/>
-      <c r="C132" s="31"/>
+      <c r="B132" s="40"/>
+      <c r="C132" s="41"/>
       <c r="D132" s="5" t="s">
         <v>232</v>
       </c>
@@ -6738,8 +6773,8 @@
       <c r="A133" s="22">
         <v>118</v>
       </c>
-      <c r="B133" s="30"/>
-      <c r="C133" s="26" t="s">
+      <c r="B133" s="40"/>
+      <c r="C133" s="31" t="s">
         <v>225</v>
       </c>
       <c r="D133" s="5" t="s">
@@ -6765,8 +6800,8 @@
       <c r="A134" s="22">
         <v>119</v>
       </c>
-      <c r="B134" s="30"/>
-      <c r="C134" s="27"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="33"/>
       <c r="D134" s="5" t="s">
         <v>230</v>
       </c>
@@ -6790,8 +6825,8 @@
       <c r="A135" s="22">
         <v>120</v>
       </c>
-      <c r="B135" s="30"/>
-      <c r="C135" s="26" t="s">
+      <c r="B135" s="40"/>
+      <c r="C135" s="31" t="s">
         <v>226</v>
       </c>
       <c r="D135" s="5" t="s">
@@ -6817,7 +6852,7 @@
       <c r="A136" s="22">
         <v>121</v>
       </c>
-      <c r="B136" s="30"/>
+      <c r="B136" s="40"/>
       <c r="C136" s="32"/>
       <c r="D136" s="5" t="s">
         <v>238</v>
@@ -6842,8 +6877,8 @@
       <c r="A137" s="22">
         <v>122</v>
       </c>
-      <c r="B137" s="30"/>
-      <c r="C137" s="27"/>
+      <c r="B137" s="40"/>
+      <c r="C137" s="33"/>
       <c r="D137" s="5" t="s">
         <v>240</v>
       </c>
@@ -6867,8 +6902,8 @@
       <c r="A138" s="22">
         <v>123</v>
       </c>
-      <c r="B138" s="30"/>
-      <c r="C138" s="26" t="s">
+      <c r="B138" s="40"/>
+      <c r="C138" s="31" t="s">
         <v>227</v>
       </c>
       <c r="D138" s="5" t="s">
@@ -6894,7 +6929,7 @@
       <c r="A139" s="22">
         <v>124</v>
       </c>
-      <c r="B139" s="30"/>
+      <c r="B139" s="40"/>
       <c r="C139" s="32"/>
       <c r="D139" s="5" t="s">
         <v>244</v>
@@ -6919,7 +6954,7 @@
       <c r="A140" s="22">
         <v>125</v>
       </c>
-      <c r="B140" s="30"/>
+      <c r="B140" s="40"/>
       <c r="C140" s="32"/>
       <c r="D140" s="5" t="s">
         <v>246</v>
@@ -6944,7 +6979,7 @@
       <c r="A141" s="22">
         <v>126</v>
       </c>
-      <c r="B141" s="30"/>
+      <c r="B141" s="40"/>
       <c r="C141" s="32"/>
       <c r="D141" s="5" t="s">
         <v>245</v>
@@ -6969,7 +7004,7 @@
       <c r="A142" s="22">
         <v>127</v>
       </c>
-      <c r="B142" s="30"/>
+      <c r="B142" s="40"/>
       <c r="C142" s="32"/>
       <c r="D142" s="5" t="s">
         <v>247</v>
@@ -6994,8 +7029,8 @@
       <c r="A143" s="22">
         <v>128</v>
       </c>
-      <c r="B143" s="30"/>
-      <c r="C143" s="27"/>
+      <c r="B143" s="40"/>
+      <c r="C143" s="33"/>
       <c r="D143" s="5" t="s">
         <v>249</v>
       </c>
@@ -7019,7 +7054,7 @@
       <c r="A144" s="22">
         <v>129</v>
       </c>
-      <c r="B144" s="30"/>
+      <c r="B144" s="40"/>
       <c r="C144" s="7" t="s">
         <v>228</v>
       </c>
@@ -7046,7 +7081,7 @@
       <c r="A145" s="22">
         <v>130</v>
       </c>
-      <c r="B145" s="30"/>
+      <c r="B145" s="40"/>
       <c r="C145" s="7"/>
       <c r="D145" s="5" t="s">
         <v>148</v>
@@ -7071,10 +7106,10 @@
       <c r="A146" s="22">
         <v>131</v>
       </c>
-      <c r="B146" s="30" t="s">
+      <c r="B146" s="40" t="s">
         <v>251</v>
       </c>
-      <c r="C146" s="31" t="s">
+      <c r="C146" s="41" t="s">
         <v>252</v>
       </c>
       <c r="D146" s="5" t="s">
@@ -7100,8 +7135,8 @@
       <c r="A147" s="22">
         <v>132</v>
       </c>
-      <c r="B147" s="30"/>
-      <c r="C147" s="31"/>
+      <c r="B147" s="40"/>
+      <c r="C147" s="41"/>
       <c r="D147" s="5" t="s">
         <v>255</v>
       </c>
@@ -7125,7 +7160,7 @@
       <c r="A148" s="22">
         <v>133</v>
       </c>
-      <c r="B148" s="30"/>
+      <c r="B148" s="40"/>
       <c r="C148" s="4"/>
       <c r="D148" s="5" t="s">
         <v>148</v>
@@ -7150,10 +7185,10 @@
       <c r="A149" s="22">
         <v>134</v>
       </c>
-      <c r="B149" s="23" t="s">
+      <c r="B149" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="C149" s="26" t="s">
+      <c r="C149" s="31" t="s">
         <v>258</v>
       </c>
       <c r="D149" s="5" t="s">
@@ -7179,7 +7214,7 @@
       <c r="A150" s="22">
         <v>135</v>
       </c>
-      <c r="B150" s="24"/>
+      <c r="B150" s="29"/>
       <c r="C150" s="32"/>
       <c r="D150" s="5" t="s">
         <v>261</v>
@@ -7204,7 +7239,7 @@
       <c r="A151" s="22">
         <v>136</v>
       </c>
-      <c r="B151" s="24"/>
+      <c r="B151" s="29"/>
       <c r="C151" s="32"/>
       <c r="D151" s="5" t="s">
         <v>263</v>
@@ -7229,8 +7264,8 @@
       <c r="A152" s="22">
         <v>137</v>
       </c>
-      <c r="B152" s="24"/>
-      <c r="C152" s="27"/>
+      <c r="B152" s="29"/>
+      <c r="C152" s="33"/>
       <c r="D152" s="5" t="s">
         <v>265</v>
       </c>
@@ -7254,8 +7289,8 @@
       <c r="A153" s="22">
         <v>138</v>
       </c>
-      <c r="B153" s="24"/>
-      <c r="C153" s="26" t="s">
+      <c r="B153" s="29"/>
+      <c r="C153" s="31" t="s">
         <v>252</v>
       </c>
       <c r="D153" s="5" t="s">
@@ -7281,8 +7316,8 @@
       <c r="A154" s="22">
         <v>139</v>
       </c>
-      <c r="B154" s="24"/>
-      <c r="C154" s="27"/>
+      <c r="B154" s="29"/>
+      <c r="C154" s="33"/>
       <c r="D154" s="5" t="s">
         <v>269</v>
       </c>
@@ -7306,7 +7341,7 @@
       <c r="A155" s="22">
         <v>140</v>
       </c>
-      <c r="B155" s="25"/>
+      <c r="B155" s="30"/>
       <c r="C155" s="4"/>
       <c r="D155" s="5" t="s">
         <v>148</v>
@@ -7331,7 +7366,7 @@
       <c r="A156" s="22">
         <v>141</v>
       </c>
-      <c r="B156" s="23" t="s">
+      <c r="B156" s="28" t="s">
         <v>271</v>
       </c>
       <c r="C156" s="4" t="s">
@@ -7360,7 +7395,7 @@
       <c r="A157" s="22">
         <v>142</v>
       </c>
-      <c r="B157" s="24"/>
+      <c r="B157" s="29"/>
       <c r="C157" s="4" t="s">
         <v>275</v>
       </c>
@@ -7387,7 +7422,7 @@
       <c r="A158" s="22">
         <v>143</v>
       </c>
-      <c r="B158" s="24"/>
+      <c r="B158" s="29"/>
       <c r="C158" s="4" t="s">
         <v>278</v>
       </c>
@@ -7414,7 +7449,7 @@
       <c r="A159" s="22">
         <v>144</v>
       </c>
-      <c r="B159" s="25"/>
+      <c r="B159" s="30"/>
       <c r="C159" s="4"/>
       <c r="D159" s="5" t="s">
         <v>148</v>
@@ -7439,7 +7474,7 @@
       <c r="A160" s="22">
         <v>145</v>
       </c>
-      <c r="B160" s="23" t="s">
+      <c r="B160" s="28" t="s">
         <v>281</v>
       </c>
       <c r="C160" s="4" t="s">
@@ -7468,8 +7503,8 @@
       <c r="A161" s="22">
         <v>146</v>
       </c>
-      <c r="B161" s="24"/>
-      <c r="C161" s="26" t="s">
+      <c r="B161" s="29"/>
+      <c r="C161" s="31" t="s">
         <v>284</v>
       </c>
       <c r="D161" s="5" t="s">
@@ -7495,8 +7530,8 @@
       <c r="A162" s="22">
         <v>147</v>
       </c>
-      <c r="B162" s="24"/>
-      <c r="C162" s="27"/>
+      <c r="B162" s="29"/>
+      <c r="C162" s="33"/>
       <c r="D162" s="5" t="s">
         <v>287</v>
       </c>
@@ -7520,8 +7555,8 @@
       <c r="A163" s="22">
         <v>148</v>
       </c>
-      <c r="B163" s="24"/>
-      <c r="C163" s="26" t="s">
+      <c r="B163" s="29"/>
+      <c r="C163" s="31" t="s">
         <v>289</v>
       </c>
       <c r="D163" s="5" t="s">
@@ -7547,8 +7582,8 @@
       <c r="A164" s="22">
         <v>149</v>
       </c>
-      <c r="B164" s="24"/>
-      <c r="C164" s="27"/>
+      <c r="B164" s="29"/>
+      <c r="C164" s="33"/>
       <c r="D164" s="5" t="s">
         <v>290</v>
       </c>
@@ -7572,7 +7607,7 @@
       <c r="A165" s="22">
         <v>150</v>
       </c>
-      <c r="B165" s="24"/>
+      <c r="B165" s="29"/>
       <c r="C165" s="4" t="s">
         <v>293</v>
       </c>
@@ -7599,8 +7634,8 @@
       <c r="A166" s="22">
         <v>151</v>
       </c>
-      <c r="B166" s="24"/>
-      <c r="C166" s="26" t="s">
+      <c r="B166" s="29"/>
+      <c r="C166" s="31" t="s">
         <v>296</v>
       </c>
       <c r="D166" s="5" t="s">
@@ -7626,8 +7661,8 @@
       <c r="A167" s="22">
         <v>152</v>
       </c>
-      <c r="B167" s="24"/>
-      <c r="C167" s="27"/>
+      <c r="B167" s="29"/>
+      <c r="C167" s="33"/>
       <c r="D167" s="5" t="s">
         <v>299</v>
       </c>
@@ -7651,8 +7686,8 @@
       <c r="A168" s="22">
         <v>153</v>
       </c>
-      <c r="B168" s="24"/>
-      <c r="C168" s="26" t="s">
+      <c r="B168" s="29"/>
+      <c r="C168" s="31" t="s">
         <v>301</v>
       </c>
       <c r="D168" s="5" t="s">
@@ -7678,8 +7713,8 @@
       <c r="A169" s="22">
         <v>154</v>
       </c>
-      <c r="B169" s="24"/>
-      <c r="C169" s="27"/>
+      <c r="B169" s="29"/>
+      <c r="C169" s="33"/>
       <c r="D169" s="5" t="s">
         <v>304</v>
       </c>
@@ -7703,8 +7738,8 @@
       <c r="A170" s="22">
         <v>155</v>
       </c>
-      <c r="B170" s="24"/>
-      <c r="C170" s="26" t="s">
+      <c r="B170" s="29"/>
+      <c r="C170" s="31" t="s">
         <v>306</v>
       </c>
       <c r="D170" s="5" t="s">
@@ -7730,7 +7765,7 @@
       <c r="A171" s="22">
         <v>156</v>
       </c>
-      <c r="B171" s="24"/>
+      <c r="B171" s="29"/>
       <c r="C171" s="32"/>
       <c r="D171" s="5" t="s">
         <v>309</v>
@@ -7755,8 +7790,8 @@
       <c r="A172" s="22">
         <v>157</v>
       </c>
-      <c r="B172" s="24"/>
-      <c r="C172" s="27"/>
+      <c r="B172" s="29"/>
+      <c r="C172" s="33"/>
       <c r="D172" s="5" t="s">
         <v>311</v>
       </c>
@@ -7780,8 +7815,8 @@
       <c r="A173" s="22">
         <v>158</v>
       </c>
-      <c r="B173" s="24"/>
-      <c r="C173" s="26" t="s">
+      <c r="B173" s="29"/>
+      <c r="C173" s="31" t="s">
         <v>313</v>
       </c>
       <c r="D173" s="5" t="s">
@@ -7807,8 +7842,8 @@
       <c r="A174" s="22">
         <v>159</v>
       </c>
-      <c r="B174" s="24"/>
-      <c r="C174" s="27"/>
+      <c r="B174" s="29"/>
+      <c r="C174" s="33"/>
       <c r="D174" s="5" t="s">
         <v>314</v>
       </c>
@@ -7832,7 +7867,7 @@
       <c r="A175" s="22">
         <v>160</v>
       </c>
-      <c r="B175" s="24" t="s">
+      <c r="B175" s="29" t="s">
         <v>317</v>
       </c>
       <c r="C175" s="4" t="s">
@@ -7861,7 +7896,7 @@
       <c r="A176" s="22">
         <v>161</v>
       </c>
-      <c r="B176" s="24"/>
+      <c r="B176" s="29"/>
       <c r="C176" s="4" t="s">
         <v>319</v>
       </c>
@@ -7888,8 +7923,8 @@
       <c r="A177" s="22">
         <v>162</v>
       </c>
-      <c r="B177" s="24"/>
-      <c r="C177" s="26" t="s">
+      <c r="B177" s="29"/>
+      <c r="C177" s="31" t="s">
         <v>322</v>
       </c>
       <c r="D177" s="5" t="s">
@@ -7915,8 +7950,8 @@
       <c r="A178" s="22">
         <v>163</v>
       </c>
-      <c r="B178" s="25"/>
-      <c r="C178" s="27"/>
+      <c r="B178" s="30"/>
+      <c r="C178" s="33"/>
       <c r="D178" s="5" t="s">
         <v>323</v>
       </c>
@@ -7940,10 +7975,10 @@
       <c r="A179" s="22">
         <v>164</v>
       </c>
-      <c r="B179" s="30" t="s">
+      <c r="B179" s="40" t="s">
         <v>326</v>
       </c>
-      <c r="C179" s="26" t="s">
+      <c r="C179" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D179" s="5" t="s">
@@ -7954,13 +7989,13 @@
       </c>
       <c r="F179" s="6"/>
       <c r="G179" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H179" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I179" s="4" t="s">
-        <v>177</v>
+        <v>22</v>
+      </c>
+      <c r="H179" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I179" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="J179" s="6"/>
       <c r="K179" s="7"/>
@@ -7969,7 +8004,7 @@
       <c r="A180" s="22">
         <v>165</v>
       </c>
-      <c r="B180" s="30"/>
+      <c r="B180" s="40"/>
       <c r="C180" s="32"/>
       <c r="D180" s="5" t="s">
         <v>329</v>
@@ -7978,14 +8013,14 @@
         <v>330</v>
       </c>
       <c r="F180" s="6"/>
-      <c r="G180" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H180" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I180" s="4" t="s">
-        <v>177</v>
+      <c r="G180" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H180" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I180" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="J180" s="6"/>
       <c r="K180" s="7"/>
@@ -7994,7 +8029,7 @@
       <c r="A181" s="22">
         <v>166</v>
       </c>
-      <c r="B181" s="30"/>
+      <c r="B181" s="40"/>
       <c r="C181" s="32"/>
       <c r="D181" s="5" t="s">
         <v>331</v>
@@ -8003,14 +8038,14 @@
         <v>332</v>
       </c>
       <c r="F181" s="6"/>
-      <c r="G181" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H181" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I181" s="4" t="s">
-        <v>177</v>
+      <c r="G181" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H181" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I181" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="J181" s="6"/>
       <c r="K181" s="7"/>
@@ -8019,8 +8054,8 @@
       <c r="A182" s="22">
         <v>167</v>
       </c>
-      <c r="B182" s="30"/>
-      <c r="C182" s="27"/>
+      <c r="B182" s="40"/>
+      <c r="C182" s="33"/>
       <c r="D182" s="5" t="s">
         <v>333</v>
       </c>
@@ -8028,14 +8063,14 @@
         <v>334</v>
       </c>
       <c r="F182" s="6"/>
-      <c r="G182" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H182" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I182" s="4" t="s">
-        <v>177</v>
+      <c r="G182" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H182" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I182" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="J182" s="6"/>
       <c r="K182" s="7"/>
@@ -8044,7 +8079,7 @@
       <c r="A183" s="22">
         <v>168</v>
       </c>
-      <c r="B183" s="23" t="s">
+      <c r="B183" s="28" t="s">
         <v>335</v>
       </c>
       <c r="C183" s="4" t="s">
@@ -8073,7 +8108,7 @@
       <c r="A184" s="22">
         <v>169</v>
       </c>
-      <c r="B184" s="24"/>
+      <c r="B184" s="29"/>
       <c r="C184" s="4" t="s">
         <v>339</v>
       </c>
@@ -8100,7 +8135,7 @@
       <c r="A185" s="22">
         <v>170</v>
       </c>
-      <c r="B185" s="25"/>
+      <c r="B185" s="30"/>
       <c r="C185" s="4" t="s">
         <v>342</v>
       </c>
@@ -8127,7 +8162,7 @@
       <c r="A186" s="22">
         <v>171</v>
       </c>
-      <c r="B186" s="30" t="s">
+      <c r="B186" s="40" t="s">
         <v>345</v>
       </c>
       <c r="C186" s="4" t="s">
@@ -8156,7 +8191,7 @@
       <c r="A187" s="22">
         <v>172</v>
       </c>
-      <c r="B187" s="30"/>
+      <c r="B187" s="40"/>
       <c r="C187" s="4" t="s">
         <v>349</v>
       </c>
@@ -8183,7 +8218,7 @@
       <c r="A188" s="22">
         <v>173</v>
       </c>
-      <c r="B188" s="30"/>
+      <c r="B188" s="40"/>
       <c r="C188" s="4" t="s">
         <v>352</v>
       </c>
@@ -8210,7 +8245,7 @@
       <c r="A189" s="22">
         <v>174</v>
       </c>
-      <c r="B189" s="30"/>
+      <c r="B189" s="40"/>
       <c r="C189" s="4" t="s">
         <v>355</v>
       </c>
@@ -8237,7 +8272,7 @@
       <c r="A190" s="22">
         <v>175</v>
       </c>
-      <c r="B190" s="30"/>
+      <c r="B190" s="40"/>
       <c r="C190" s="4" t="s">
         <v>357</v>
       </c>
@@ -8264,7 +8299,7 @@
       <c r="A191" s="22">
         <v>176</v>
       </c>
-      <c r="B191" s="30" t="s">
+      <c r="B191" s="40" t="s">
         <v>359</v>
       </c>
       <c r="C191" s="4" t="s">
@@ -8293,7 +8328,7 @@
       <c r="A192" s="22">
         <v>177</v>
       </c>
-      <c r="B192" s="30"/>
+      <c r="B192" s="40"/>
       <c r="C192" s="4"/>
       <c r="D192" s="5" t="s">
         <v>363</v>
@@ -8318,7 +8353,7 @@
       <c r="A193" s="22">
         <v>178</v>
       </c>
-      <c r="B193" s="30"/>
+      <c r="B193" s="40"/>
       <c r="C193" s="4"/>
       <c r="D193" s="5" t="s">
         <v>365</v>
@@ -8343,7 +8378,7 @@
       <c r="A194" s="22">
         <v>179</v>
       </c>
-      <c r="B194" s="30"/>
+      <c r="B194" s="40"/>
       <c r="C194" s="4"/>
       <c r="D194" s="5" t="s">
         <v>367</v>
@@ -8368,7 +8403,7 @@
       <c r="A195" s="22">
         <v>180</v>
       </c>
-      <c r="B195" s="30"/>
+      <c r="B195" s="40"/>
       <c r="C195" s="4" t="s">
         <v>369</v>
       </c>
@@ -8395,7 +8430,7 @@
       <c r="A196" s="22">
         <v>181</v>
       </c>
-      <c r="B196" s="30"/>
+      <c r="B196" s="40"/>
       <c r="C196" s="4" t="s">
         <v>372</v>
       </c>
@@ -8422,7 +8457,7 @@
       <c r="A197" s="22">
         <v>182</v>
       </c>
-      <c r="B197" s="30"/>
+      <c r="B197" s="40"/>
       <c r="C197" s="4"/>
       <c r="D197" s="5" t="s">
         <v>375</v>
@@ -8447,7 +8482,7 @@
       <c r="A198" s="22">
         <v>183</v>
       </c>
-      <c r="B198" s="30"/>
+      <c r="B198" s="40"/>
       <c r="C198" s="4"/>
       <c r="D198" s="5" t="s">
         <v>377</v>
@@ -8472,7 +8507,7 @@
       <c r="A199" s="22">
         <v>184</v>
       </c>
-      <c r="B199" s="30"/>
+      <c r="B199" s="40"/>
       <c r="C199" s="4" t="s">
         <v>379</v>
       </c>
@@ -8499,7 +8534,7 @@
       <c r="A200" s="22">
         <v>185</v>
       </c>
-      <c r="B200" s="30"/>
+      <c r="B200" s="40"/>
       <c r="C200" s="4" t="s">
         <v>357</v>
       </c>
@@ -8526,7 +8561,7 @@
       <c r="A201" s="22">
         <v>186</v>
       </c>
-      <c r="B201" s="30"/>
+      <c r="B201" s="40"/>
       <c r="C201" s="4" t="s">
         <v>382</v>
       </c>
@@ -8553,7 +8588,7 @@
       <c r="A202" s="22">
         <v>187</v>
       </c>
-      <c r="B202" s="30" t="s">
+      <c r="B202" s="40" t="s">
         <v>384</v>
       </c>
       <c r="C202" s="4" t="s">
@@ -8582,7 +8617,7 @@
       <c r="A203" s="22">
         <v>188</v>
       </c>
-      <c r="B203" s="30"/>
+      <c r="B203" s="40"/>
       <c r="C203" s="4"/>
       <c r="D203" s="5" t="s">
         <v>353</v>
@@ -8607,7 +8642,7 @@
       <c r="A204" s="22">
         <v>189</v>
       </c>
-      <c r="B204" s="30"/>
+      <c r="B204" s="40"/>
       <c r="C204" s="4" t="s">
         <v>382</v>
       </c>
@@ -8634,7 +8669,7 @@
       <c r="A205" s="22">
         <v>190</v>
       </c>
-      <c r="B205" s="30"/>
+      <c r="B205" s="40"/>
       <c r="C205" s="4" t="s">
         <v>388</v>
       </c>
@@ -8661,7 +8696,7 @@
       <c r="A206" s="22">
         <v>191</v>
       </c>
-      <c r="B206" s="30"/>
+      <c r="B206" s="40"/>
       <c r="C206" s="16" t="s">
         <v>391</v>
       </c>
@@ -8688,7 +8723,7 @@
       <c r="A207" s="22">
         <v>192</v>
       </c>
-      <c r="B207" s="23" t="s">
+      <c r="B207" s="28" t="s">
         <v>394</v>
       </c>
       <c r="C207" s="4" t="s">
@@ -8717,8 +8752,8 @@
       <c r="A208" s="22">
         <v>193</v>
       </c>
-      <c r="B208" s="24"/>
-      <c r="C208" s="26" t="s">
+      <c r="B208" s="29"/>
+      <c r="C208" s="31" t="s">
         <v>397</v>
       </c>
       <c r="D208" s="5" t="s">
@@ -8744,7 +8779,7 @@
       <c r="A209" s="22">
         <v>194</v>
       </c>
-      <c r="B209" s="24"/>
+      <c r="B209" s="29"/>
       <c r="C209" s="32"/>
       <c r="D209" s="5" t="s">
         <v>400</v>
@@ -8769,8 +8804,8 @@
       <c r="A210" s="22">
         <v>195</v>
       </c>
-      <c r="B210" s="24"/>
-      <c r="C210" s="27"/>
+      <c r="B210" s="29"/>
+      <c r="C210" s="33"/>
       <c r="D210" s="5" t="s">
         <v>402</v>
       </c>
@@ -8794,7 +8829,7 @@
       <c r="A211" s="22">
         <v>196</v>
       </c>
-      <c r="B211" s="24"/>
+      <c r="B211" s="29"/>
       <c r="C211" s="4" t="s">
         <v>404</v>
       </c>
@@ -8821,7 +8856,7 @@
       <c r="A212" s="22">
         <v>197</v>
       </c>
-      <c r="B212" s="24"/>
+      <c r="B212" s="29"/>
       <c r="C212" s="4" t="s">
         <v>407</v>
       </c>
@@ -8848,8 +8883,8 @@
       <c r="A213" s="22">
         <v>198</v>
       </c>
-      <c r="B213" s="24"/>
-      <c r="C213" s="26" t="s">
+      <c r="B213" s="29"/>
+      <c r="C213" s="31" t="s">
         <v>410</v>
       </c>
       <c r="D213" s="5" t="s">
@@ -8875,7 +8910,7 @@
       <c r="A214" s="22">
         <v>199</v>
       </c>
-      <c r="B214" s="24"/>
+      <c r="B214" s="29"/>
       <c r="C214" s="32"/>
       <c r="D214" s="5" t="s">
         <v>411</v>
@@ -8900,8 +8935,8 @@
       <c r="A215" s="22">
         <v>200</v>
       </c>
-      <c r="B215" s="24"/>
-      <c r="C215" s="27"/>
+      <c r="B215" s="29"/>
+      <c r="C215" s="33"/>
       <c r="D215" s="5" t="s">
         <v>411</v>
       </c>
@@ -8925,7 +8960,7 @@
       <c r="A216" s="22">
         <v>201</v>
       </c>
-      <c r="B216" s="24"/>
+      <c r="B216" s="29"/>
       <c r="C216" s="4" t="s">
         <v>357</v>
       </c>
@@ -8952,7 +8987,7 @@
       <c r="A217" s="22">
         <v>202</v>
       </c>
-      <c r="B217" s="24"/>
+      <c r="B217" s="29"/>
       <c r="C217" s="4" t="s">
         <v>382</v>
       </c>
@@ -8979,7 +9014,7 @@
       <c r="A218" s="22">
         <v>203</v>
       </c>
-      <c r="B218" s="25"/>
+      <c r="B218" s="30"/>
       <c r="C218" s="4" t="s">
         <v>418</v>
       </c>
@@ -9006,7 +9041,7 @@
       <c r="A219" s="22">
         <v>204</v>
       </c>
-      <c r="B219" s="36" t="s">
+      <c r="B219" s="37" t="s">
         <v>421</v>
       </c>
       <c r="C219" s="4" t="s">
@@ -9035,8 +9070,8 @@
       <c r="A220" s="22">
         <v>205</v>
       </c>
-      <c r="B220" s="37"/>
-      <c r="C220" s="26" t="s">
+      <c r="B220" s="38"/>
+      <c r="C220" s="31" t="s">
         <v>397</v>
       </c>
       <c r="D220" s="5" t="s">
@@ -9062,7 +9097,7 @@
       <c r="A221" s="22">
         <v>206</v>
       </c>
-      <c r="B221" s="37"/>
+      <c r="B221" s="38"/>
       <c r="C221" s="32"/>
       <c r="D221" s="5" t="s">
         <v>424</v>
@@ -9087,8 +9122,8 @@
       <c r="A222" s="22">
         <v>207</v>
       </c>
-      <c r="B222" s="37"/>
-      <c r="C222" s="27"/>
+      <c r="B222" s="38"/>
+      <c r="C222" s="33"/>
       <c r="D222" s="5" t="s">
         <v>424</v>
       </c>
@@ -9112,7 +9147,7 @@
       <c r="A223" s="22">
         <v>208</v>
       </c>
-      <c r="B223" s="37"/>
+      <c r="B223" s="38"/>
       <c r="C223" s="4" t="s">
         <v>407</v>
       </c>
@@ -9139,8 +9174,8 @@
       <c r="A224" s="22">
         <v>209</v>
       </c>
-      <c r="B224" s="37"/>
-      <c r="C224" s="26" t="s">
+      <c r="B224" s="38"/>
+      <c r="C224" s="31" t="s">
         <v>410</v>
       </c>
       <c r="D224" s="5" t="s">
@@ -9166,7 +9201,7 @@
       <c r="A225" s="22">
         <v>210</v>
       </c>
-      <c r="B225" s="37"/>
+      <c r="B225" s="38"/>
       <c r="C225" s="32"/>
       <c r="D225" s="5" t="s">
         <v>426</v>
@@ -9191,8 +9226,8 @@
       <c r="A226" s="22">
         <v>211</v>
       </c>
-      <c r="B226" s="37"/>
-      <c r="C226" s="27"/>
+      <c r="B226" s="38"/>
+      <c r="C226" s="33"/>
       <c r="D226" s="5" t="s">
         <v>426</v>
       </c>
@@ -9216,7 +9251,7 @@
       <c r="A227" s="22">
         <v>212</v>
       </c>
-      <c r="B227" s="37"/>
+      <c r="B227" s="38"/>
       <c r="C227" s="4" t="s">
         <v>357</v>
       </c>
@@ -9243,7 +9278,7 @@
       <c r="A228" s="22">
         <v>213</v>
       </c>
-      <c r="B228" s="38"/>
+      <c r="B228" s="39"/>
       <c r="C228" s="4" t="s">
         <v>382</v>
       </c>
@@ -9270,7 +9305,7 @@
       <c r="A229" s="22">
         <v>214</v>
       </c>
-      <c r="B229" s="39" t="s">
+      <c r="B229" s="25" t="s">
         <v>429</v>
       </c>
       <c r="C229" s="4" t="s">
@@ -9299,8 +9334,8 @@
       <c r="A230" s="22">
         <v>215</v>
       </c>
-      <c r="B230" s="40"/>
-      <c r="C230" s="26" t="s">
+      <c r="B230" s="26"/>
+      <c r="C230" s="31" t="s">
         <v>397</v>
       </c>
       <c r="D230" s="5" t="s">
@@ -9326,7 +9361,7 @@
       <c r="A231" s="22">
         <v>216</v>
       </c>
-      <c r="B231" s="40"/>
+      <c r="B231" s="26"/>
       <c r="C231" s="32"/>
       <c r="D231" s="5" t="s">
         <v>433</v>
@@ -9351,8 +9386,8 @@
       <c r="A232" s="22">
         <v>217</v>
       </c>
-      <c r="B232" s="40"/>
-      <c r="C232" s="27"/>
+      <c r="B232" s="26"/>
+      <c r="C232" s="33"/>
       <c r="D232" s="5" t="s">
         <v>433</v>
       </c>
@@ -9376,7 +9411,7 @@
       <c r="A233" s="22">
         <v>218</v>
       </c>
-      <c r="B233" s="40"/>
+      <c r="B233" s="26"/>
       <c r="C233" s="4" t="s">
         <v>407</v>
       </c>
@@ -9403,8 +9438,8 @@
       <c r="A234" s="22">
         <v>219</v>
       </c>
-      <c r="B234" s="40"/>
-      <c r="C234" s="26" t="s">
+      <c r="B234" s="26"/>
+      <c r="C234" s="31" t="s">
         <v>410</v>
       </c>
       <c r="D234" s="5" t="s">
@@ -9430,7 +9465,7 @@
       <c r="A235" s="22">
         <v>220</v>
       </c>
-      <c r="B235" s="40"/>
+      <c r="B235" s="26"/>
       <c r="C235" s="32"/>
       <c r="D235" s="5" t="s">
         <v>435</v>
@@ -9455,8 +9490,8 @@
       <c r="A236" s="22">
         <v>221</v>
       </c>
-      <c r="B236" s="40"/>
-      <c r="C236" s="27"/>
+      <c r="B236" s="26"/>
+      <c r="C236" s="33"/>
       <c r="D236" s="5" t="s">
         <v>435</v>
       </c>
@@ -9480,7 +9515,7 @@
       <c r="A237" s="22">
         <v>222</v>
       </c>
-      <c r="B237" s="40"/>
+      <c r="B237" s="26"/>
       <c r="C237" s="4" t="s">
         <v>357</v>
       </c>
@@ -9507,7 +9542,7 @@
       <c r="A238" s="22">
         <v>223</v>
       </c>
-      <c r="B238" s="40"/>
+      <c r="B238" s="26"/>
       <c r="C238" s="4" t="s">
         <v>382</v>
       </c>
@@ -9534,7 +9569,7 @@
       <c r="A239" s="22">
         <v>224</v>
       </c>
-      <c r="B239" s="41"/>
+      <c r="B239" s="27"/>
       <c r="C239" s="4" t="s">
         <v>404</v>
       </c>
@@ -9561,7 +9596,7 @@
       <c r="A240" s="22">
         <v>225</v>
       </c>
-      <c r="B240" s="39" t="s">
+      <c r="B240" s="25" t="s">
         <v>439</v>
       </c>
       <c r="C240" s="4" t="s">
@@ -9590,7 +9625,7 @@
       <c r="A241" s="22">
         <v>226</v>
       </c>
-      <c r="B241" s="40"/>
+      <c r="B241" s="26"/>
       <c r="C241" s="4" t="s">
         <v>442</v>
       </c>
@@ -9617,7 +9652,7 @@
       <c r="A242" s="22">
         <v>227</v>
       </c>
-      <c r="B242" s="40"/>
+      <c r="B242" s="26"/>
       <c r="C242" s="4" t="s">
         <v>445</v>
       </c>
@@ -9644,7 +9679,7 @@
       <c r="A243" s="22">
         <v>228</v>
       </c>
-      <c r="B243" s="40"/>
+      <c r="B243" s="26"/>
       <c r="C243" s="4"/>
       <c r="D243" s="5" t="s">
         <v>448</v>
@@ -9669,7 +9704,7 @@
       <c r="A244" s="22">
         <v>229</v>
       </c>
-      <c r="B244" s="41"/>
+      <c r="B244" s="27"/>
       <c r="C244" s="4"/>
       <c r="D244" s="5" t="s">
         <v>450</v>
@@ -9694,7 +9729,7 @@
       <c r="A245" s="22">
         <v>230</v>
       </c>
-      <c r="B245" s="39" t="s">
+      <c r="B245" s="25" t="s">
         <v>452</v>
       </c>
       <c r="C245" s="4" t="s">
@@ -9723,8 +9758,8 @@
       <c r="A246" s="22">
         <v>231</v>
       </c>
-      <c r="B246" s="40"/>
-      <c r="C246" s="26" t="s">
+      <c r="B246" s="26"/>
+      <c r="C246" s="31" t="s">
         <v>455</v>
       </c>
       <c r="D246" s="5" t="s">
@@ -9750,7 +9785,7 @@
       <c r="A247" s="22">
         <v>232</v>
       </c>
-      <c r="B247" s="40"/>
+      <c r="B247" s="26"/>
       <c r="C247" s="32"/>
       <c r="D247" s="5" t="s">
         <v>458</v>
@@ -9775,7 +9810,7 @@
       <c r="A248" s="22">
         <v>233</v>
       </c>
-      <c r="B248" s="40"/>
+      <c r="B248" s="26"/>
       <c r="C248" s="32"/>
       <c r="D248" s="5" t="s">
         <v>460</v>
@@ -9800,8 +9835,8 @@
       <c r="A249" s="22">
         <v>234</v>
       </c>
-      <c r="B249" s="40"/>
-      <c r="C249" s="27"/>
+      <c r="B249" s="26"/>
+      <c r="C249" s="33"/>
       <c r="D249" s="5" t="s">
         <v>462</v>
       </c>
@@ -9825,7 +9860,7 @@
       <c r="A250" s="22">
         <v>235</v>
       </c>
-      <c r="B250" s="40"/>
+      <c r="B250" s="26"/>
       <c r="C250" s="4" t="s">
         <v>464</v>
       </c>
@@ -9852,7 +9887,7 @@
       <c r="A251" s="22">
         <v>236</v>
       </c>
-      <c r="B251" s="40"/>
+      <c r="B251" s="26"/>
       <c r="C251" s="4" t="s">
         <v>467</v>
       </c>
@@ -9879,7 +9914,7 @@
       <c r="A252" s="22">
         <v>237</v>
       </c>
-      <c r="B252" s="40"/>
+      <c r="B252" s="26"/>
       <c r="C252" s="4" t="s">
         <v>470</v>
       </c>
@@ -9906,7 +9941,7 @@
       <c r="A253" s="22">
         <v>238</v>
       </c>
-      <c r="B253" s="40"/>
+      <c r="B253" s="26"/>
       <c r="C253" s="4" t="s">
         <v>473</v>
       </c>
@@ -9933,7 +9968,7 @@
       <c r="A254" s="22">
         <v>239</v>
       </c>
-      <c r="B254" s="41"/>
+      <c r="B254" s="27"/>
       <c r="C254" s="4" t="s">
         <v>476</v>
       </c>
@@ -9960,7 +9995,7 @@
       <c r="A255" s="22">
         <v>240</v>
       </c>
-      <c r="B255" s="39" t="s">
+      <c r="B255" s="25" t="s">
         <v>479</v>
       </c>
       <c r="C255" s="4" t="s">
@@ -9989,7 +10024,7 @@
       <c r="A256" s="22">
         <v>241</v>
       </c>
-      <c r="B256" s="40"/>
+      <c r="B256" s="26"/>
       <c r="C256" s="4" t="s">
         <v>482</v>
       </c>
@@ -10016,7 +10051,7 @@
       <c r="A257" s="22">
         <v>242</v>
       </c>
-      <c r="B257" s="40"/>
+      <c r="B257" s="26"/>
       <c r="C257" s="4" t="s">
         <v>151</v>
       </c>
@@ -10043,8 +10078,8 @@
       <c r="A258" s="22">
         <v>243</v>
       </c>
-      <c r="B258" s="40"/>
-      <c r="C258" s="26" t="s">
+      <c r="B258" s="26"/>
+      <c r="C258" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D258" s="5" t="s">
@@ -10070,7 +10105,7 @@
       <c r="A259" s="22">
         <v>244</v>
       </c>
-      <c r="B259" s="40"/>
+      <c r="B259" s="26"/>
       <c r="C259" s="32"/>
       <c r="D259" s="5" t="s">
         <v>490</v>
@@ -10095,8 +10130,8 @@
       <c r="A260" s="22">
         <v>245</v>
       </c>
-      <c r="B260" s="40"/>
-      <c r="C260" s="27"/>
+      <c r="B260" s="26"/>
+      <c r="C260" s="33"/>
       <c r="D260" s="5" t="s">
         <v>492</v>
       </c>
@@ -10120,7 +10155,7 @@
       <c r="A261" s="22">
         <v>246</v>
       </c>
-      <c r="B261" s="40"/>
+      <c r="B261" s="26"/>
       <c r="C261" s="17" t="s">
         <v>494</v>
       </c>
@@ -10147,7 +10182,7 @@
       <c r="A262" s="22">
         <v>247</v>
       </c>
-      <c r="B262" s="40"/>
+      <c r="B262" s="26"/>
       <c r="C262" s="4" t="s">
         <v>497</v>
       </c>
@@ -10174,7 +10209,7 @@
       <c r="A263" s="22">
         <v>248</v>
       </c>
-      <c r="B263" s="40"/>
+      <c r="B263" s="26"/>
       <c r="C263" s="4" t="s">
         <v>500</v>
       </c>
@@ -10201,7 +10236,7 @@
       <c r="A264" s="22">
         <v>249</v>
       </c>
-      <c r="B264" s="41"/>
+      <c r="B264" s="27"/>
       <c r="C264" s="4" t="s">
         <v>503</v>
       </c>
@@ -10228,7 +10263,7 @@
       <c r="A265" s="22">
         <v>250</v>
       </c>
-      <c r="B265" s="39" t="s">
+      <c r="B265" s="25" t="s">
         <v>506</v>
       </c>
       <c r="C265" s="4" t="s">
@@ -10257,7 +10292,7 @@
       <c r="A266" s="22">
         <v>251</v>
       </c>
-      <c r="B266" s="40"/>
+      <c r="B266" s="26"/>
       <c r="C266" s="4" t="s">
         <v>509</v>
       </c>
@@ -10284,7 +10319,7 @@
       <c r="A267" s="22">
         <v>252</v>
       </c>
-      <c r="B267" s="40"/>
+      <c r="B267" s="26"/>
       <c r="C267" s="4" t="s">
         <v>512</v>
       </c>
@@ -10311,7 +10346,7 @@
       <c r="A268" s="22">
         <v>253</v>
       </c>
-      <c r="B268" s="40"/>
+      <c r="B268" s="26"/>
       <c r="C268" s="4" t="s">
         <v>515</v>
       </c>
@@ -10338,7 +10373,7 @@
       <c r="A269" s="22">
         <v>254</v>
       </c>
-      <c r="B269" s="40"/>
+      <c r="B269" s="26"/>
       <c r="C269" s="4" t="s">
         <v>500</v>
       </c>
@@ -10365,7 +10400,7 @@
       <c r="A270" s="22">
         <v>255</v>
       </c>
-      <c r="B270" s="41"/>
+      <c r="B270" s="27"/>
       <c r="C270" s="4" t="s">
         <v>497</v>
       </c>
@@ -10392,7 +10427,7 @@
       <c r="A271" s="22">
         <v>256</v>
       </c>
-      <c r="B271" s="39" t="s">
+      <c r="B271" s="25" t="s">
         <v>520</v>
       </c>
       <c r="C271" s="4" t="s">
@@ -10421,7 +10456,7 @@
       <c r="A272" s="22">
         <v>257</v>
       </c>
-      <c r="B272" s="40"/>
+      <c r="B272" s="26"/>
       <c r="C272" s="4" t="s">
         <v>482</v>
       </c>
@@ -10448,7 +10483,7 @@
       <c r="A273" s="22">
         <v>258</v>
       </c>
-      <c r="B273" s="40"/>
+      <c r="B273" s="26"/>
       <c r="C273" s="4" t="s">
         <v>151</v>
       </c>
@@ -10475,8 +10510,8 @@
       <c r="A274" s="22">
         <v>259</v>
       </c>
-      <c r="B274" s="40"/>
-      <c r="C274" s="26" t="s">
+      <c r="B274" s="26"/>
+      <c r="C274" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D274" s="5" t="s">
@@ -10502,7 +10537,7 @@
       <c r="A275" s="22">
         <v>260</v>
       </c>
-      <c r="B275" s="40"/>
+      <c r="B275" s="26"/>
       <c r="C275" s="32"/>
       <c r="D275" s="5" t="s">
         <v>490</v>
@@ -10527,8 +10562,8 @@
       <c r="A276" s="22">
         <v>261</v>
       </c>
-      <c r="B276" s="40"/>
-      <c r="C276" s="27"/>
+      <c r="B276" s="26"/>
+      <c r="C276" s="33"/>
       <c r="D276" s="5" t="s">
         <v>492</v>
       </c>
@@ -10552,7 +10587,7 @@
       <c r="A277" s="22">
         <v>262</v>
       </c>
-      <c r="B277" s="40"/>
+      <c r="B277" s="26"/>
       <c r="C277" s="17" t="s">
         <v>494</v>
       </c>
@@ -10579,7 +10614,7 @@
       <c r="A278" s="22">
         <v>263</v>
       </c>
-      <c r="B278" s="40"/>
+      <c r="B278" s="26"/>
       <c r="C278" s="4" t="s">
         <v>497</v>
       </c>
@@ -10606,7 +10641,7 @@
       <c r="A279" s="22">
         <v>264</v>
       </c>
-      <c r="B279" s="41"/>
+      <c r="B279" s="27"/>
       <c r="C279" s="4" t="s">
         <v>500</v>
       </c>
@@ -10633,7 +10668,7 @@
       <c r="A280" s="22">
         <v>265</v>
       </c>
-      <c r="B280" s="39" t="s">
+      <c r="B280" s="25" t="s">
         <v>530</v>
       </c>
       <c r="C280" s="4" t="s">
@@ -10662,7 +10697,7 @@
       <c r="A281" s="22">
         <v>266</v>
       </c>
-      <c r="B281" s="40"/>
+      <c r="B281" s="26"/>
       <c r="C281" s="4" t="s">
         <v>482</v>
       </c>
@@ -10689,7 +10724,7 @@
       <c r="A282" s="22">
         <v>267</v>
       </c>
-      <c r="B282" s="40"/>
+      <c r="B282" s="26"/>
       <c r="C282" s="4" t="s">
         <v>151</v>
       </c>
@@ -10716,7 +10751,7 @@
       <c r="A283" s="22">
         <v>268</v>
       </c>
-      <c r="B283" s="40"/>
+      <c r="B283" s="26"/>
       <c r="C283" s="4" t="s">
         <v>500</v>
       </c>
@@ -10743,7 +10778,7 @@
       <c r="A284" s="22">
         <v>269</v>
       </c>
-      <c r="B284" s="40"/>
+      <c r="B284" s="26"/>
       <c r="C284" s="4" t="s">
         <v>497</v>
       </c>
@@ -10770,8 +10805,8 @@
       <c r="A285" s="22">
         <v>270</v>
       </c>
-      <c r="B285" s="40"/>
-      <c r="C285" s="26" t="s">
+      <c r="B285" s="26"/>
+      <c r="C285" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D285" s="5" t="s">
@@ -10797,7 +10832,7 @@
       <c r="A286" s="22">
         <v>271</v>
       </c>
-      <c r="B286" s="40"/>
+      <c r="B286" s="26"/>
       <c r="C286" s="32"/>
       <c r="D286" s="5" t="s">
         <v>490</v>
@@ -10822,7 +10857,7 @@
       <c r="A287" s="22">
         <v>272</v>
       </c>
-      <c r="B287" s="40"/>
+      <c r="B287" s="26"/>
       <c r="C287" s="32"/>
       <c r="D287" s="5" t="s">
         <v>492</v>
@@ -10847,7 +10882,7 @@
       <c r="A288" s="22">
         <v>273</v>
       </c>
-      <c r="B288" s="40"/>
+      <c r="B288" s="26"/>
       <c r="C288" s="32"/>
       <c r="D288" s="5" t="s">
         <v>539</v>
@@ -10872,7 +10907,7 @@
       <c r="A289" s="22">
         <v>274</v>
       </c>
-      <c r="B289" s="40"/>
+      <c r="B289" s="26"/>
       <c r="C289" s="32"/>
       <c r="D289" s="5" t="s">
         <v>541</v>
@@ -10897,8 +10932,8 @@
       <c r="A290" s="22">
         <v>275</v>
       </c>
-      <c r="B290" s="41"/>
-      <c r="C290" s="27"/>
+      <c r="B290" s="27"/>
+      <c r="C290" s="33"/>
       <c r="D290" s="5" t="s">
         <v>541</v>
       </c>
@@ -10922,7 +10957,7 @@
       <c r="A291" s="22">
         <v>276</v>
       </c>
-      <c r="B291" s="39" t="s">
+      <c r="B291" s="25" t="s">
         <v>544</v>
       </c>
       <c r="C291" s="4" t="s">
@@ -10951,7 +10986,7 @@
       <c r="A292" s="22">
         <v>277</v>
       </c>
-      <c r="B292" s="40"/>
+      <c r="B292" s="26"/>
       <c r="C292" s="4" t="s">
         <v>482</v>
       </c>
@@ -10978,7 +11013,7 @@
       <c r="A293" s="22">
         <v>278</v>
       </c>
-      <c r="B293" s="40"/>
+      <c r="B293" s="26"/>
       <c r="C293" s="4" t="s">
         <v>151</v>
       </c>
@@ -11005,7 +11040,7 @@
       <c r="A294" s="22">
         <v>279</v>
       </c>
-      <c r="B294" s="40"/>
+      <c r="B294" s="26"/>
       <c r="C294" s="4" t="s">
         <v>497</v>
       </c>
@@ -11032,8 +11067,8 @@
       <c r="A295" s="22">
         <v>280</v>
       </c>
-      <c r="B295" s="40"/>
-      <c r="C295" s="26" t="s">
+      <c r="B295" s="26"/>
+      <c r="C295" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D295" s="5" t="s">
@@ -11059,7 +11094,7 @@
       <c r="A296" s="22">
         <v>281</v>
       </c>
-      <c r="B296" s="40"/>
+      <c r="B296" s="26"/>
       <c r="C296" s="32"/>
       <c r="D296" s="5" t="s">
         <v>490</v>
@@ -11084,7 +11119,7 @@
       <c r="A297" s="22">
         <v>282</v>
       </c>
-      <c r="B297" s="40"/>
+      <c r="B297" s="26"/>
       <c r="C297" s="32"/>
       <c r="D297" s="5" t="s">
         <v>492</v>
@@ -11109,8 +11144,8 @@
       <c r="A298" s="22">
         <v>283</v>
       </c>
-      <c r="B298" s="40"/>
-      <c r="C298" s="27"/>
+      <c r="B298" s="26"/>
+      <c r="C298" s="33"/>
       <c r="D298" s="5" t="s">
         <v>550</v>
       </c>
@@ -11134,7 +11169,7 @@
       <c r="A299" s="22">
         <v>284</v>
       </c>
-      <c r="B299" s="40"/>
+      <c r="B299" s="26"/>
       <c r="C299" s="4" t="s">
         <v>552</v>
       </c>
@@ -11161,7 +11196,7 @@
       <c r="A300" s="22">
         <v>285</v>
       </c>
-      <c r="B300" s="41"/>
+      <c r="B300" s="27"/>
       <c r="C300" s="4" t="s">
         <v>500</v>
       </c>
@@ -11188,7 +11223,7 @@
       <c r="A301" s="22">
         <v>286</v>
       </c>
-      <c r="B301" s="42" t="s">
+      <c r="B301" s="34" t="s">
         <v>556</v>
       </c>
       <c r="C301" s="4" t="s">
@@ -11217,7 +11252,7 @@
       <c r="A302" s="22">
         <v>287</v>
       </c>
-      <c r="B302" s="43"/>
+      <c r="B302" s="35"/>
       <c r="C302" s="4" t="s">
         <v>552</v>
       </c>
@@ -11244,7 +11279,7 @@
       <c r="A303" s="22">
         <v>288</v>
       </c>
-      <c r="B303" s="43"/>
+      <c r="B303" s="35"/>
       <c r="C303" s="4" t="s">
         <v>500</v>
       </c>
@@ -11271,7 +11306,7 @@
       <c r="A304" s="22">
         <v>289</v>
       </c>
-      <c r="B304" s="43"/>
+      <c r="B304" s="35"/>
       <c r="C304" s="4" t="s">
         <v>497</v>
       </c>
@@ -11298,7 +11333,7 @@
       <c r="A305" s="22">
         <v>290</v>
       </c>
-      <c r="B305" s="44"/>
+      <c r="B305" s="36"/>
       <c r="C305" s="4" t="s">
         <v>561</v>
       </c>
@@ -11325,7 +11360,7 @@
       <c r="A306" s="22">
         <v>291</v>
       </c>
-      <c r="B306" s="39" t="s">
+      <c r="B306" s="25" t="s">
         <v>564</v>
       </c>
       <c r="C306" s="4" t="s">
@@ -11354,7 +11389,7 @@
       <c r="A307" s="22">
         <v>292</v>
       </c>
-      <c r="B307" s="40"/>
+      <c r="B307" s="26"/>
       <c r="C307" s="4" t="s">
         <v>500</v>
       </c>
@@ -11381,7 +11416,7 @@
       <c r="A308" s="22">
         <v>293</v>
       </c>
-      <c r="B308" s="40"/>
+      <c r="B308" s="26"/>
       <c r="C308" s="4" t="s">
         <v>497</v>
       </c>
@@ -11408,8 +11443,8 @@
       <c r="A309" s="22">
         <v>294</v>
       </c>
-      <c r="B309" s="40"/>
-      <c r="C309" s="26" t="s">
+      <c r="B309" s="26"/>
+      <c r="C309" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D309" s="5" t="s">
@@ -11435,7 +11470,7 @@
       <c r="A310" s="22">
         <v>295</v>
       </c>
-      <c r="B310" s="40"/>
+      <c r="B310" s="26"/>
       <c r="C310" s="32"/>
       <c r="D310" s="5" t="s">
         <v>490</v>
@@ -11460,8 +11495,8 @@
       <c r="A311" s="22">
         <v>296</v>
       </c>
-      <c r="B311" s="40"/>
-      <c r="C311" s="27"/>
+      <c r="B311" s="26"/>
+      <c r="C311" s="33"/>
       <c r="D311" s="5" t="s">
         <v>492</v>
       </c>
@@ -11485,8 +11520,8 @@
       <c r="A312" s="22">
         <v>297</v>
       </c>
-      <c r="B312" s="40"/>
-      <c r="C312" s="26" t="s">
+      <c r="B312" s="26"/>
+      <c r="C312" s="31" t="s">
         <v>569</v>
       </c>
       <c r="D312" s="5" t="s">
@@ -11512,7 +11547,7 @@
       <c r="A313" s="22">
         <v>298</v>
       </c>
-      <c r="B313" s="40"/>
+      <c r="B313" s="26"/>
       <c r="C313" s="32"/>
       <c r="D313" s="5" t="s">
         <v>572</v>
@@ -11537,8 +11572,8 @@
       <c r="A314" s="22">
         <v>299</v>
       </c>
-      <c r="B314" s="40"/>
-      <c r="C314" s="27"/>
+      <c r="B314" s="26"/>
+      <c r="C314" s="33"/>
       <c r="D314" s="5" t="s">
         <v>574</v>
       </c>
@@ -11562,8 +11597,8 @@
       <c r="A315" s="22">
         <v>300</v>
       </c>
-      <c r="B315" s="40"/>
-      <c r="C315" s="26" t="s">
+      <c r="B315" s="26"/>
+      <c r="C315" s="31" t="s">
         <v>576</v>
       </c>
       <c r="D315" s="5" t="s">
@@ -11589,8 +11624,8 @@
       <c r="A316" s="22">
         <v>301</v>
       </c>
-      <c r="B316" s="40"/>
-      <c r="C316" s="27"/>
+      <c r="B316" s="26"/>
+      <c r="C316" s="33"/>
       <c r="D316" s="5" t="s">
         <v>579</v>
       </c>
@@ -11614,7 +11649,7 @@
       <c r="A317" s="22">
         <v>302</v>
       </c>
-      <c r="B317" s="41"/>
+      <c r="B317" s="27"/>
       <c r="C317" s="4" t="s">
         <v>581</v>
       </c>
@@ -11641,7 +11676,7 @@
       <c r="A318" s="22">
         <v>303</v>
       </c>
-      <c r="B318" s="39" t="s">
+      <c r="B318" s="25" t="s">
         <v>584</v>
       </c>
       <c r="C318" s="4" t="s">
@@ -11670,7 +11705,7 @@
       <c r="A319" s="22">
         <v>304</v>
       </c>
-      <c r="B319" s="40"/>
+      <c r="B319" s="26"/>
       <c r="C319" s="4" t="s">
         <v>494</v>
       </c>
@@ -11697,7 +11732,7 @@
       <c r="A320" s="22">
         <v>305</v>
       </c>
-      <c r="B320" s="40"/>
+      <c r="B320" s="26"/>
       <c r="C320" s="4" t="s">
         <v>500</v>
       </c>
@@ -11724,7 +11759,7 @@
       <c r="A321" s="22">
         <v>306</v>
       </c>
-      <c r="B321" s="41"/>
+      <c r="B321" s="27"/>
       <c r="C321" s="4" t="s">
         <v>497</v>
       </c>
@@ -11749,6 +11784,76 @@
     </row>
   </sheetData>
   <mergeCells count="86">
+    <mergeCell ref="B22:B36"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="C58:C63"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="B112:B129"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="B100:B107"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="C117:C120"/>
+    <mergeCell ref="C121:C123"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C126:C128"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="B87:B96"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C92"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B68:B76"/>
+    <mergeCell ref="B77:B86"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="C138:C143"/>
+    <mergeCell ref="B146:B148"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="B130:B145"/>
+    <mergeCell ref="C130:C132"/>
+    <mergeCell ref="B149:B155"/>
+    <mergeCell ref="C149:C152"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B156:B159"/>
+    <mergeCell ref="B160:B174"/>
+    <mergeCell ref="C161:C162"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="C166:C167"/>
+    <mergeCell ref="C168:C169"/>
+    <mergeCell ref="C170:C172"/>
+    <mergeCell ref="B219:B228"/>
+    <mergeCell ref="C220:C222"/>
+    <mergeCell ref="C224:C226"/>
+    <mergeCell ref="C173:C174"/>
+    <mergeCell ref="B175:B178"/>
+    <mergeCell ref="C177:C178"/>
+    <mergeCell ref="B179:B182"/>
+    <mergeCell ref="B186:B190"/>
+    <mergeCell ref="B191:B201"/>
+    <mergeCell ref="B202:B206"/>
+    <mergeCell ref="B207:B218"/>
+    <mergeCell ref="C208:C210"/>
+    <mergeCell ref="C213:C215"/>
+    <mergeCell ref="C179:C182"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="B255:B264"/>
+    <mergeCell ref="C258:C260"/>
+    <mergeCell ref="B265:B270"/>
+    <mergeCell ref="B271:B279"/>
+    <mergeCell ref="C274:C276"/>
     <mergeCell ref="B318:B321"/>
     <mergeCell ref="B183:B185"/>
     <mergeCell ref="B291:B300"/>
@@ -11765,82 +11870,12 @@
     <mergeCell ref="C234:C236"/>
     <mergeCell ref="B240:B244"/>
     <mergeCell ref="B245:B254"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="B255:B264"/>
-    <mergeCell ref="C258:C260"/>
-    <mergeCell ref="B265:B270"/>
-    <mergeCell ref="B271:B279"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="B219:B228"/>
-    <mergeCell ref="C220:C222"/>
-    <mergeCell ref="C224:C226"/>
-    <mergeCell ref="C173:C174"/>
-    <mergeCell ref="B175:B178"/>
-    <mergeCell ref="C177:C178"/>
-    <mergeCell ref="B179:B182"/>
-    <mergeCell ref="B186:B190"/>
-    <mergeCell ref="B191:B201"/>
-    <mergeCell ref="B202:B206"/>
-    <mergeCell ref="B207:B218"/>
-    <mergeCell ref="C208:C210"/>
-    <mergeCell ref="C213:C215"/>
-    <mergeCell ref="C179:C182"/>
-    <mergeCell ref="B149:B155"/>
-    <mergeCell ref="C149:C152"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="B156:B159"/>
-    <mergeCell ref="B160:B174"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="C166:C167"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="C170:C172"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="C135:C137"/>
-    <mergeCell ref="C138:C143"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="B130:B145"/>
-    <mergeCell ref="C130:C132"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="B87:B96"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C92"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B68:B76"/>
-    <mergeCell ref="B77:B86"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="C58:C63"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="B112:B129"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="B100:B107"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="C121:C123"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="C126:C128"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="B22:B36"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 K54:K57 K59:K211" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 K54:K57 K59:K211">
       <formula1>$C$2:$C$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G16:I321" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G16:I321">
       <formula1>$B$1:$B$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
upate 1 so testcase
</commit_message>
<xml_diff>
--- a/TestCase-Reup.xlsx
+++ b/TestCase-Reup.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ChuyenDe12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PTDiDong12\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96B278C-B65A-426D-86FA-A4E41A65C26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2566,7 +2567,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2730,7 +2731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2810,13 +2811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2831,10 +2826,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2846,139 +2880,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -3422,11 +3328,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G280" sqref="G280:I290"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J156" sqref="J156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3616,11 +3522,11 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
       <c r="J13" s="2"/>
       <c r="K13" s="9"/>
     </row>
@@ -3641,11 +3547,11 @@
       <c r="F14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="2"/>
       <c r="K14" s="9"/>
     </row>
@@ -3688,7 +3594,7 @@
       <c r="A16" s="4">
         <v>1</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -3717,7 +3623,7 @@
       <c r="A17" s="4">
         <v>2</v>
       </c>
-      <c r="B17" s="31"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="4" t="s">
         <v>23</v>
       </c>
@@ -3746,7 +3652,7 @@
       <c r="A18" s="22">
         <v>3</v>
       </c>
-      <c r="B18" s="31"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
@@ -3775,7 +3681,7 @@
       <c r="A19" s="22">
         <v>4</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
@@ -3804,7 +3710,7 @@
       <c r="A20" s="22">
         <v>5</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3833,7 +3739,7 @@
       <c r="A21" s="22">
         <v>6</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
@@ -3860,10 +3766,10 @@
       <c r="A22" s="22">
         <v>7</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -3889,8 +3795,8 @@
       <c r="A23" s="22">
         <v>8</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="35"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="5" t="s">
         <v>42</v>
       </c>
@@ -3914,8 +3820,8 @@
       <c r="A24" s="22">
         <v>9</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="33" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="31" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -3941,8 +3847,8 @@
       <c r="A25" s="22">
         <v>10</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="5" t="s">
         <v>42</v>
       </c>
@@ -3966,7 +3872,7 @@
       <c r="A26" s="22">
         <v>11</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="4" t="s">
         <v>46</v>
       </c>
@@ -3993,7 +3899,7 @@
       <c r="A27" s="22">
         <v>12</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="4" t="s">
         <v>49</v>
       </c>
@@ -4020,7 +3926,7 @@
       <c r="A28" s="22">
         <v>13</v>
       </c>
-      <c r="B28" s="31"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
@@ -4047,7 +3953,7 @@
       <c r="A29" s="22">
         <v>14</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="4" t="s">
         <v>54</v>
       </c>
@@ -4074,7 +3980,7 @@
       <c r="A30" s="22">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="4" t="s">
         <v>55</v>
       </c>
@@ -4103,7 +4009,7 @@
       <c r="A31" s="22">
         <v>16</v>
       </c>
-      <c r="B31" s="31"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="4" t="s">
         <v>58</v>
       </c>
@@ -4132,7 +4038,7 @@
       <c r="A32" s="22">
         <v>17</v>
       </c>
-      <c r="B32" s="31"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="4" t="s">
         <v>58</v>
       </c>
@@ -4161,7 +4067,7 @@
       <c r="A33" s="22">
         <v>18</v>
       </c>
-      <c r="B33" s="31"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="4" t="s">
         <v>61</v>
       </c>
@@ -4192,7 +4098,7 @@
       <c r="A34" s="22">
         <v>19</v>
       </c>
-      <c r="B34" s="31"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="4" t="s">
         <v>64</v>
       </c>
@@ -4219,7 +4125,7 @@
       <c r="A35" s="22">
         <v>20</v>
       </c>
-      <c r="B35" s="31"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="4" t="s">
         <v>65</v>
       </c>
@@ -4246,7 +4152,7 @@
       <c r="A36" s="22">
         <v>21</v>
       </c>
-      <c r="B36" s="32"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="4" t="s">
         <v>65</v>
       </c>
@@ -4273,7 +4179,7 @@
       <c r="A37" s="22">
         <v>22</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -4302,7 +4208,7 @@
       <c r="A38" s="22">
         <v>23</v>
       </c>
-      <c r="B38" s="31"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="4" t="s">
         <v>71</v>
       </c>
@@ -4331,7 +4237,7 @@
       <c r="A39" s="22">
         <v>24</v>
       </c>
-      <c r="B39" s="31"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="4" t="s">
         <v>74</v>
       </c>
@@ -4360,7 +4266,7 @@
       <c r="A40" s="22">
         <v>25</v>
       </c>
-      <c r="B40" s="31"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="4" t="s">
         <v>76</v>
       </c>
@@ -4389,7 +4295,7 @@
       <c r="A41" s="22">
         <v>26</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="4" t="s">
         <v>79</v>
       </c>
@@ -4418,7 +4324,7 @@
       <c r="A42" s="22">
         <v>27</v>
       </c>
-      <c r="B42" s="31"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="4" t="s">
         <v>81</v>
       </c>
@@ -4445,7 +4351,7 @@
       <c r="A43" s="22">
         <v>28</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="4" t="s">
         <v>84</v>
       </c>
@@ -4472,7 +4378,7 @@
       <c r="A44" s="22">
         <v>29</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -4501,7 +4407,7 @@
       <c r="A45" s="22">
         <v>30</v>
       </c>
-      <c r="B45" s="31"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="4" t="s">
         <v>89</v>
       </c>
@@ -4528,7 +4434,7 @@
       <c r="A46" s="22">
         <v>31</v>
       </c>
-      <c r="B46" s="31"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="4" t="s">
         <v>71</v>
       </c>
@@ -4557,7 +4463,7 @@
       <c r="A47" s="22">
         <v>32</v>
       </c>
-      <c r="B47" s="31"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="4" t="s">
         <v>74</v>
       </c>
@@ -4586,7 +4492,7 @@
       <c r="A48" s="22">
         <v>33</v>
       </c>
-      <c r="B48" s="31"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="4" t="s">
         <v>92</v>
       </c>
@@ -4615,7 +4521,7 @@
       <c r="A49" s="22">
         <v>34</v>
       </c>
-      <c r="B49" s="32"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="4" t="s">
         <v>96</v>
       </c>
@@ -4644,7 +4550,7 @@
       <c r="A50" s="22">
         <v>35</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="38" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -4673,7 +4579,7 @@
       <c r="A51" s="22">
         <v>36</v>
       </c>
-      <c r="B51" s="45"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="4" t="s">
         <v>71</v>
       </c>
@@ -4702,7 +4608,7 @@
       <c r="A52" s="22">
         <v>37</v>
       </c>
-      <c r="B52" s="46"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="4" t="s">
         <v>74</v>
       </c>
@@ -4729,7 +4635,7 @@
       <c r="A53" s="22">
         <v>38</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="28" t="s">
         <v>107</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -4758,7 +4664,7 @@
       <c r="A54" s="22">
         <v>39</v>
       </c>
-      <c r="B54" s="31"/>
+      <c r="B54" s="29"/>
       <c r="C54" s="4" t="s">
         <v>71</v>
       </c>
@@ -4787,7 +4693,7 @@
       <c r="A55" s="22">
         <v>40</v>
       </c>
-      <c r="B55" s="31"/>
+      <c r="B55" s="29"/>
       <c r="C55" s="4" t="s">
         <v>74</v>
       </c>
@@ -4816,7 +4722,7 @@
       <c r="A56" s="22">
         <v>41</v>
       </c>
-      <c r="B56" s="31"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="4" t="s">
         <v>74</v>
       </c>
@@ -4845,7 +4751,7 @@
       <c r="A57" s="22">
         <v>42</v>
       </c>
-      <c r="B57" s="32"/>
+      <c r="B57" s="30"/>
       <c r="C57" s="4" t="s">
         <v>74</v>
       </c>
@@ -4874,10 +4780,10 @@
       <c r="A58" s="22">
         <v>43</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="43" t="s">
+      <c r="C58" s="36" t="s">
         <v>19</v>
       </c>
       <c r="D58" s="5" t="s">
@@ -4903,8 +4809,8 @@
       <c r="A59" s="22">
         <v>44</v>
       </c>
-      <c r="B59" s="42"/>
-      <c r="C59" s="43"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="5" t="s">
         <v>123</v>
       </c>
@@ -4928,8 +4834,8 @@
       <c r="A60" s="22">
         <v>45</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="43"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="5" t="s">
         <v>125</v>
       </c>
@@ -4953,8 +4859,8 @@
       <c r="A61" s="22">
         <v>46</v>
       </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="43"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="36"/>
       <c r="D61" s="5" t="s">
         <v>593</v>
       </c>
@@ -4978,8 +4884,8 @@
       <c r="A62" s="22">
         <v>47</v>
       </c>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="36"/>
       <c r="D62" s="5" t="s">
         <v>597</v>
       </c>
@@ -5003,8 +4909,8 @@
       <c r="A63" s="22">
         <v>48</v>
       </c>
-      <c r="B63" s="42"/>
-      <c r="C63" s="43"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="5" t="s">
         <v>592</v>
       </c>
@@ -5028,7 +4934,7 @@
       <c r="A64" s="22">
         <v>49</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="28" t="s">
         <v>599</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -5057,7 +4963,7 @@
       <c r="A65" s="22">
         <v>50</v>
       </c>
-      <c r="B65" s="31"/>
+      <c r="B65" s="29"/>
       <c r="C65" s="21" t="s">
         <v>601</v>
       </c>
@@ -5084,7 +4990,7 @@
       <c r="A66" s="22">
         <v>51</v>
       </c>
-      <c r="B66" s="31"/>
+      <c r="B66" s="29"/>
       <c r="C66" s="22" t="s">
         <v>594</v>
       </c>
@@ -5111,7 +5017,7 @@
       <c r="A67" s="22">
         <v>52</v>
       </c>
-      <c r="B67" s="32"/>
+      <c r="B67" s="30"/>
       <c r="C67" s="24" t="s">
         <v>228</v>
       </c>
@@ -5138,10 +5044,10 @@
       <c r="A68" s="22">
         <v>53</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="C68" s="33" t="s">
+      <c r="C68" s="31" t="s">
         <v>129</v>
       </c>
       <c r="D68" s="5" t="s">
@@ -5167,8 +5073,8 @@
       <c r="A69" s="22">
         <v>54</v>
       </c>
-      <c r="B69" s="31"/>
-      <c r="C69" s="34"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="37"/>
       <c r="D69" s="5" t="s">
         <v>133</v>
       </c>
@@ -5194,8 +5100,8 @@
       <c r="A70" s="22">
         <v>55</v>
       </c>
-      <c r="B70" s="31"/>
-      <c r="C70" s="35"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="32"/>
       <c r="D70" s="5" t="s">
         <v>136</v>
       </c>
@@ -5221,7 +5127,7 @@
       <c r="A71" s="22">
         <v>56</v>
       </c>
-      <c r="B71" s="31"/>
+      <c r="B71" s="29"/>
       <c r="C71" s="4" t="s">
         <v>138</v>
       </c>
@@ -5248,8 +5154,8 @@
       <c r="A72" s="22">
         <v>57</v>
       </c>
-      <c r="B72" s="31"/>
-      <c r="C72" s="43" t="s">
+      <c r="B72" s="29"/>
+      <c r="C72" s="36" t="s">
         <v>141</v>
       </c>
       <c r="D72" s="5" t="s">
@@ -5275,8 +5181,8 @@
       <c r="A73" s="22">
         <v>58</v>
       </c>
-      <c r="B73" s="31"/>
-      <c r="C73" s="43"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="36"/>
       <c r="D73" s="5" t="s">
         <v>144</v>
       </c>
@@ -5300,8 +5206,8 @@
       <c r="A74" s="22">
         <v>59</v>
       </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="43"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="36"/>
       <c r="D74" s="5" t="s">
         <v>146</v>
       </c>
@@ -5325,7 +5231,7 @@
       <c r="A75" s="22">
         <v>60</v>
       </c>
-      <c r="B75" s="31"/>
+      <c r="B75" s="29"/>
       <c r="C75" s="22" t="s">
         <v>228</v>
       </c>
@@ -5352,7 +5258,7 @@
       <c r="A76" s="22">
         <v>61</v>
       </c>
-      <c r="B76" s="32"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="4"/>
       <c r="D76" s="5" t="s">
         <v>148</v>
@@ -5377,10 +5283,10 @@
       <c r="A77" s="22">
         <v>62</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="C77" s="43" t="s">
+      <c r="C77" s="36" t="s">
         <v>151</v>
       </c>
       <c r="D77" s="5" t="s">
@@ -5408,8 +5314,8 @@
       <c r="A78" s="22">
         <v>63</v>
       </c>
-      <c r="B78" s="31"/>
-      <c r="C78" s="43"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="36"/>
       <c r="D78" s="5" t="s">
         <v>155</v>
       </c>
@@ -5433,8 +5339,8 @@
       <c r="A79" s="22">
         <v>64</v>
       </c>
-      <c r="B79" s="31"/>
-      <c r="C79" s="43" t="s">
+      <c r="B79" s="29"/>
+      <c r="C79" s="36" t="s">
         <v>157</v>
       </c>
       <c r="D79" s="5" t="s">
@@ -5460,8 +5366,8 @@
       <c r="A80" s="22">
         <v>65</v>
       </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="43"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="36"/>
       <c r="D80" s="5" t="s">
         <v>160</v>
       </c>
@@ -5485,8 +5391,8 @@
       <c r="A81" s="22">
         <v>66</v>
       </c>
-      <c r="B81" s="31"/>
-      <c r="C81" s="43"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="36"/>
       <c r="D81" s="5" t="s">
         <v>162</v>
       </c>
@@ -5510,8 +5416,8 @@
       <c r="A82" s="22">
         <v>67</v>
       </c>
-      <c r="B82" s="31"/>
-      <c r="C82" s="43"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="36"/>
       <c r="D82" s="5" t="s">
         <v>164</v>
       </c>
@@ -5535,7 +5441,7 @@
       <c r="A83" s="22">
         <v>68</v>
       </c>
-      <c r="B83" s="31"/>
+      <c r="B83" s="29"/>
       <c r="C83" s="22" t="s">
         <v>594</v>
       </c>
@@ -5562,7 +5468,7 @@
       <c r="A84" s="22">
         <v>69</v>
       </c>
-      <c r="B84" s="31"/>
+      <c r="B84" s="29"/>
       <c r="C84" s="4" t="s">
         <v>138</v>
       </c>
@@ -5589,7 +5495,7 @@
       <c r="A85" s="22">
         <v>70</v>
       </c>
-      <c r="B85" s="31"/>
+      <c r="B85" s="29"/>
       <c r="C85" s="22" t="s">
         <v>228</v>
       </c>
@@ -5616,7 +5522,7 @@
       <c r="A86" s="22">
         <v>71</v>
       </c>
-      <c r="B86" s="32"/>
+      <c r="B86" s="30"/>
       <c r="C86" s="4"/>
       <c r="D86" s="5" t="s">
         <v>148</v>
@@ -5641,10 +5547,10 @@
       <c r="A87" s="22">
         <v>72</v>
       </c>
-      <c r="B87" s="42" t="s">
+      <c r="B87" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="C87" s="43" t="s">
+      <c r="C87" s="36" t="s">
         <v>151</v>
       </c>
       <c r="D87" s="5" t="s">
@@ -5670,8 +5576,8 @@
       <c r="A88" s="22">
         <v>73</v>
       </c>
-      <c r="B88" s="42"/>
-      <c r="C88" s="43"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="36"/>
       <c r="D88" s="5" t="s">
         <v>155</v>
       </c>
@@ -5695,8 +5601,8 @@
       <c r="A89" s="22">
         <v>74</v>
       </c>
-      <c r="B89" s="42"/>
-      <c r="C89" s="43" t="s">
+      <c r="B89" s="35"/>
+      <c r="C89" s="36" t="s">
         <v>157</v>
       </c>
       <c r="D89" s="5" t="s">
@@ -5722,8 +5628,8 @@
       <c r="A90" s="22">
         <v>75</v>
       </c>
-      <c r="B90" s="42"/>
-      <c r="C90" s="43"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="36"/>
       <c r="D90" s="5" t="s">
         <v>160</v>
       </c>
@@ -5747,8 +5653,8 @@
       <c r="A91" s="22">
         <v>76</v>
       </c>
-      <c r="B91" s="42"/>
-      <c r="C91" s="43"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="36"/>
       <c r="D91" s="5" t="s">
         <v>162</v>
       </c>
@@ -5772,8 +5678,8 @@
       <c r="A92" s="22">
         <v>77</v>
       </c>
-      <c r="B92" s="42"/>
-      <c r="C92" s="43"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="36"/>
       <c r="D92" s="5" t="s">
         <v>164</v>
       </c>
@@ -5797,7 +5703,7 @@
       <c r="A93" s="22">
         <v>78</v>
       </c>
-      <c r="B93" s="42"/>
+      <c r="B93" s="35"/>
       <c r="C93" s="22" t="s">
         <v>594</v>
       </c>
@@ -5824,7 +5730,7 @@
       <c r="A94" s="22">
         <v>79</v>
       </c>
-      <c r="B94" s="42"/>
+      <c r="B94" s="35"/>
       <c r="C94" s="4" t="s">
         <v>138</v>
       </c>
@@ -5851,7 +5757,7 @@
       <c r="A95" s="22">
         <v>80</v>
       </c>
-      <c r="B95" s="42"/>
+      <c r="B95" s="35"/>
       <c r="C95" s="22" t="s">
         <v>228</v>
       </c>
@@ -5878,7 +5784,7 @@
       <c r="A96" s="22">
         <v>81</v>
       </c>
-      <c r="B96" s="42"/>
+      <c r="B96" s="35"/>
       <c r="C96" s="4"/>
       <c r="D96" s="5" t="s">
         <v>148</v>
@@ -5903,7 +5809,7 @@
       <c r="A97" s="22">
         <v>82</v>
       </c>
-      <c r="B97" s="42" t="s">
+      <c r="B97" s="35" t="s">
         <v>168</v>
       </c>
       <c r="C97" s="4" t="s">
@@ -5932,7 +5838,7 @@
       <c r="A98" s="22">
         <v>83</v>
       </c>
-      <c r="B98" s="42"/>
+      <c r="B98" s="35"/>
       <c r="C98" s="22" t="s">
         <v>228</v>
       </c>
@@ -5959,7 +5865,7 @@
       <c r="A99" s="22">
         <v>84</v>
       </c>
-      <c r="B99" s="42"/>
+      <c r="B99" s="35"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5" t="s">
         <v>148</v>
@@ -5984,7 +5890,7 @@
       <c r="A100" s="22">
         <v>85</v>
       </c>
-      <c r="B100" s="42" t="s">
+      <c r="B100" s="35" t="s">
         <v>172</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -6013,7 +5919,7 @@
       <c r="A101" s="22">
         <v>86</v>
       </c>
-      <c r="B101" s="42"/>
+      <c r="B101" s="35"/>
       <c r="C101" s="4" t="s">
         <v>173</v>
       </c>
@@ -6040,8 +5946,8 @@
       <c r="A102" s="22">
         <v>87</v>
       </c>
-      <c r="B102" s="42"/>
-      <c r="C102" s="43" t="s">
+      <c r="B102" s="35"/>
+      <c r="C102" s="36" t="s">
         <v>176</v>
       </c>
       <c r="D102" s="5" t="s">
@@ -6069,8 +5975,8 @@
       <c r="A103" s="22">
         <v>88</v>
       </c>
-      <c r="B103" s="42"/>
-      <c r="C103" s="43"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="36"/>
       <c r="D103" s="5" t="s">
         <v>608</v>
       </c>
@@ -6096,8 +6002,8 @@
       <c r="A104" s="22">
         <v>89</v>
       </c>
-      <c r="B104" s="42"/>
-      <c r="C104" s="43"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="36"/>
       <c r="D104" s="5" t="s">
         <v>609</v>
       </c>
@@ -6123,8 +6029,8 @@
       <c r="A105" s="22">
         <v>90</v>
       </c>
-      <c r="B105" s="42"/>
-      <c r="C105" s="43"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="36"/>
       <c r="D105" s="5" t="s">
         <v>610</v>
       </c>
@@ -6150,7 +6056,7 @@
       <c r="A106" s="22">
         <v>91</v>
       </c>
-      <c r="B106" s="42"/>
+      <c r="B106" s="35"/>
       <c r="C106" s="4" t="s">
         <v>228</v>
       </c>
@@ -6177,7 +6083,7 @@
       <c r="A107" s="22">
         <v>92</v>
       </c>
-      <c r="B107" s="42"/>
+      <c r="B107" s="35"/>
       <c r="C107" s="4"/>
       <c r="D107" s="5" t="s">
         <v>148</v>
@@ -6202,10 +6108,10 @@
       <c r="A108" s="22">
         <v>93</v>
       </c>
-      <c r="B108" s="42" t="s">
+      <c r="B108" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="C108" s="33" t="s">
+      <c r="C108" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D108" s="5" t="s">
@@ -6231,8 +6137,8 @@
       <c r="A109" s="22">
         <v>94</v>
       </c>
-      <c r="B109" s="42"/>
-      <c r="C109" s="34"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="37"/>
       <c r="D109" s="5" t="s">
         <v>181</v>
       </c>
@@ -6256,8 +6162,8 @@
       <c r="A110" s="22">
         <v>95</v>
       </c>
-      <c r="B110" s="42"/>
-      <c r="C110" s="34"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="37"/>
       <c r="D110" s="5" t="s">
         <v>606</v>
       </c>
@@ -6281,8 +6187,8 @@
       <c r="A111" s="22">
         <v>96</v>
       </c>
-      <c r="B111" s="42"/>
-      <c r="C111" s="35"/>
+      <c r="B111" s="35"/>
+      <c r="C111" s="32"/>
       <c r="D111" s="5" t="s">
         <v>605</v>
       </c>
@@ -6306,7 +6212,7 @@
       <c r="A112" s="22">
         <v>97</v>
       </c>
-      <c r="B112" s="42" t="s">
+      <c r="B112" s="35" t="s">
         <v>185</v>
       </c>
       <c r="C112" s="4" t="s">
@@ -6335,8 +6241,8 @@
       <c r="A113" s="22">
         <v>98</v>
       </c>
-      <c r="B113" s="42"/>
-      <c r="C113" s="43" t="s">
+      <c r="B113" s="35"/>
+      <c r="C113" s="36" t="s">
         <v>189</v>
       </c>
       <c r="D113" s="5" t="s">
@@ -6362,8 +6268,8 @@
       <c r="A114" s="22">
         <v>99</v>
       </c>
-      <c r="B114" s="42"/>
-      <c r="C114" s="43"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="36"/>
       <c r="D114" s="5" t="s">
         <v>192</v>
       </c>
@@ -6387,8 +6293,8 @@
       <c r="A115" s="22">
         <v>100</v>
       </c>
-      <c r="B115" s="42"/>
-      <c r="C115" s="43"/>
+      <c r="B115" s="35"/>
+      <c r="C115" s="36"/>
       <c r="D115" s="5" t="s">
         <v>194</v>
       </c>
@@ -6412,8 +6318,8 @@
       <c r="A116" s="22">
         <v>101</v>
       </c>
-      <c r="B116" s="42"/>
-      <c r="C116" s="43"/>
+      <c r="B116" s="35"/>
+      <c r="C116" s="36"/>
       <c r="D116" s="5" t="s">
         <v>196</v>
       </c>
@@ -6437,8 +6343,8 @@
       <c r="A117" s="22">
         <v>102</v>
       </c>
-      <c r="B117" s="42"/>
-      <c r="C117" s="43" t="s">
+      <c r="B117" s="35"/>
+      <c r="C117" s="36" t="s">
         <v>197</v>
       </c>
       <c r="D117" s="5" t="s">
@@ -6464,8 +6370,8 @@
       <c r="A118" s="22">
         <v>103</v>
       </c>
-      <c r="B118" s="42"/>
-      <c r="C118" s="43"/>
+      <c r="B118" s="35"/>
+      <c r="C118" s="36"/>
       <c r="D118" s="5" t="s">
         <v>200</v>
       </c>
@@ -6489,8 +6395,8 @@
       <c r="A119" s="22">
         <v>104</v>
       </c>
-      <c r="B119" s="42"/>
-      <c r="C119" s="43"/>
+      <c r="B119" s="35"/>
+      <c r="C119" s="36"/>
       <c r="D119" s="5" t="s">
         <v>202</v>
       </c>
@@ -6514,8 +6420,8 @@
       <c r="A120" s="22">
         <v>105</v>
       </c>
-      <c r="B120" s="42"/>
-      <c r="C120" s="43"/>
+      <c r="B120" s="35"/>
+      <c r="C120" s="36"/>
       <c r="D120" s="5" t="s">
         <v>203</v>
       </c>
@@ -6539,8 +6445,8 @@
       <c r="A121" s="22">
         <v>106</v>
       </c>
-      <c r="B121" s="42"/>
-      <c r="C121" s="43" t="s">
+      <c r="B121" s="35"/>
+      <c r="C121" s="36" t="s">
         <v>204</v>
       </c>
       <c r="D121" s="5" t="s">
@@ -6566,8 +6472,8 @@
       <c r="A122" s="22">
         <v>107</v>
       </c>
-      <c r="B122" s="42"/>
-      <c r="C122" s="43"/>
+      <c r="B122" s="35"/>
+      <c r="C122" s="36"/>
       <c r="D122" s="5" t="s">
         <v>207</v>
       </c>
@@ -6591,8 +6497,8 @@
       <c r="A123" s="22">
         <v>108</v>
       </c>
-      <c r="B123" s="42"/>
-      <c r="C123" s="43"/>
+      <c r="B123" s="35"/>
+      <c r="C123" s="36"/>
       <c r="D123" s="5" t="s">
         <v>208</v>
       </c>
@@ -6616,8 +6522,8 @@
       <c r="A124" s="22">
         <v>109</v>
       </c>
-      <c r="B124" s="42"/>
-      <c r="C124" s="43" t="s">
+      <c r="B124" s="35"/>
+      <c r="C124" s="36" t="s">
         <v>210</v>
       </c>
       <c r="D124" s="5" t="s">
@@ -6643,8 +6549,8 @@
       <c r="A125" s="22">
         <v>110</v>
       </c>
-      <c r="B125" s="42"/>
-      <c r="C125" s="43"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="36"/>
       <c r="D125" s="5" t="s">
         <v>213</v>
       </c>
@@ -6668,8 +6574,8 @@
       <c r="A126" s="22">
         <v>111</v>
       </c>
-      <c r="B126" s="42"/>
-      <c r="C126" s="43" t="s">
+      <c r="B126" s="35"/>
+      <c r="C126" s="36" t="s">
         <v>215</v>
       </c>
       <c r="D126" s="5" t="s">
@@ -6695,8 +6601,8 @@
       <c r="A127" s="22">
         <v>112</v>
       </c>
-      <c r="B127" s="42"/>
-      <c r="C127" s="43"/>
+      <c r="B127" s="35"/>
+      <c r="C127" s="36"/>
       <c r="D127" s="5" t="s">
         <v>218</v>
       </c>
@@ -6720,8 +6626,8 @@
       <c r="A128" s="22">
         <v>113</v>
       </c>
-      <c r="B128" s="42"/>
-      <c r="C128" s="43"/>
+      <c r="B128" s="35"/>
+      <c r="C128" s="36"/>
       <c r="D128" s="5" t="s">
         <v>220</v>
       </c>
@@ -6745,7 +6651,7 @@
       <c r="A129" s="22">
         <v>114</v>
       </c>
-      <c r="B129" s="42"/>
+      <c r="B129" s="35"/>
       <c r="C129" s="4"/>
       <c r="D129" s="8" t="s">
         <v>148</v>
@@ -6770,10 +6676,10 @@
       <c r="A130" s="22">
         <v>115</v>
       </c>
-      <c r="B130" s="42" t="s">
+      <c r="B130" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="C130" s="43" t="s">
+      <c r="C130" s="36" t="s">
         <v>224</v>
       </c>
       <c r="D130" s="5" t="s">
@@ -6799,8 +6705,8 @@
       <c r="A131" s="22">
         <v>116</v>
       </c>
-      <c r="B131" s="42"/>
-      <c r="C131" s="43"/>
+      <c r="B131" s="35"/>
+      <c r="C131" s="36"/>
       <c r="D131" s="5" t="s">
         <v>231</v>
       </c>
@@ -6824,8 +6730,8 @@
       <c r="A132" s="22">
         <v>117</v>
       </c>
-      <c r="B132" s="42"/>
-      <c r="C132" s="43"/>
+      <c r="B132" s="35"/>
+      <c r="C132" s="36"/>
       <c r="D132" s="5" t="s">
         <v>232</v>
       </c>
@@ -6849,8 +6755,8 @@
       <c r="A133" s="22">
         <v>118</v>
       </c>
-      <c r="B133" s="42"/>
-      <c r="C133" s="33" t="s">
+      <c r="B133" s="35"/>
+      <c r="C133" s="31" t="s">
         <v>225</v>
       </c>
       <c r="D133" s="5" t="s">
@@ -6876,8 +6782,8 @@
       <c r="A134" s="22">
         <v>119</v>
       </c>
-      <c r="B134" s="42"/>
-      <c r="C134" s="35"/>
+      <c r="B134" s="35"/>
+      <c r="C134" s="32"/>
       <c r="D134" s="5" t="s">
         <v>230</v>
       </c>
@@ -6901,8 +6807,8 @@
       <c r="A135" s="22">
         <v>120</v>
       </c>
-      <c r="B135" s="42"/>
-      <c r="C135" s="33" t="s">
+      <c r="B135" s="35"/>
+      <c r="C135" s="31" t="s">
         <v>226</v>
       </c>
       <c r="D135" s="5" t="s">
@@ -6928,8 +6834,8 @@
       <c r="A136" s="22">
         <v>121</v>
       </c>
-      <c r="B136" s="42"/>
-      <c r="C136" s="34"/>
+      <c r="B136" s="35"/>
+      <c r="C136" s="37"/>
       <c r="D136" s="5" t="s">
         <v>238</v>
       </c>
@@ -6953,8 +6859,8 @@
       <c r="A137" s="22">
         <v>122</v>
       </c>
-      <c r="B137" s="42"/>
-      <c r="C137" s="35"/>
+      <c r="B137" s="35"/>
+      <c r="C137" s="32"/>
       <c r="D137" s="5" t="s">
         <v>240</v>
       </c>
@@ -6978,8 +6884,8 @@
       <c r="A138" s="22">
         <v>123</v>
       </c>
-      <c r="B138" s="42"/>
-      <c r="C138" s="33" t="s">
+      <c r="B138" s="35"/>
+      <c r="C138" s="31" t="s">
         <v>227</v>
       </c>
       <c r="D138" s="5" t="s">
@@ -7005,8 +6911,8 @@
       <c r="A139" s="22">
         <v>124</v>
       </c>
-      <c r="B139" s="42"/>
-      <c r="C139" s="34"/>
+      <c r="B139" s="35"/>
+      <c r="C139" s="37"/>
       <c r="D139" s="5" t="s">
         <v>244</v>
       </c>
@@ -7030,8 +6936,8 @@
       <c r="A140" s="22">
         <v>125</v>
       </c>
-      <c r="B140" s="42"/>
-      <c r="C140" s="34"/>
+      <c r="B140" s="35"/>
+      <c r="C140" s="37"/>
       <c r="D140" s="5" t="s">
         <v>246</v>
       </c>
@@ -7055,8 +6961,8 @@
       <c r="A141" s="22">
         <v>126</v>
       </c>
-      <c r="B141" s="42"/>
-      <c r="C141" s="34"/>
+      <c r="B141" s="35"/>
+      <c r="C141" s="37"/>
       <c r="D141" s="5" t="s">
         <v>245</v>
       </c>
@@ -7080,8 +6986,8 @@
       <c r="A142" s="22">
         <v>127</v>
       </c>
-      <c r="B142" s="42"/>
-      <c r="C142" s="34"/>
+      <c r="B142" s="35"/>
+      <c r="C142" s="37"/>
       <c r="D142" s="5" t="s">
         <v>247</v>
       </c>
@@ -7105,8 +7011,8 @@
       <c r="A143" s="22">
         <v>128</v>
       </c>
-      <c r="B143" s="42"/>
-      <c r="C143" s="35"/>
+      <c r="B143" s="35"/>
+      <c r="C143" s="32"/>
       <c r="D143" s="5" t="s">
         <v>249</v>
       </c>
@@ -7130,7 +7036,7 @@
       <c r="A144" s="22">
         <v>129</v>
       </c>
-      <c r="B144" s="42"/>
+      <c r="B144" s="35"/>
       <c r="C144" s="7" t="s">
         <v>228</v>
       </c>
@@ -7157,7 +7063,7 @@
       <c r="A145" s="22">
         <v>130</v>
       </c>
-      <c r="B145" s="42"/>
+      <c r="B145" s="35"/>
       <c r="C145" s="7"/>
       <c r="D145" s="5" t="s">
         <v>148</v>
@@ -7182,10 +7088,10 @@
       <c r="A146" s="22">
         <v>131</v>
       </c>
-      <c r="B146" s="42" t="s">
+      <c r="B146" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="C146" s="43" t="s">
+      <c r="C146" s="36" t="s">
         <v>252</v>
       </c>
       <c r="D146" s="5" t="s">
@@ -7211,8 +7117,8 @@
       <c r="A147" s="22">
         <v>132</v>
       </c>
-      <c r="B147" s="42"/>
-      <c r="C147" s="43"/>
+      <c r="B147" s="35"/>
+      <c r="C147" s="36"/>
       <c r="D147" s="5" t="s">
         <v>255</v>
       </c>
@@ -7236,7 +7142,7 @@
       <c r="A148" s="22">
         <v>133</v>
       </c>
-      <c r="B148" s="42"/>
+      <c r="B148" s="35"/>
       <c r="C148" s="4"/>
       <c r="D148" s="5" t="s">
         <v>148</v>
@@ -7261,10 +7167,10 @@
       <c r="A149" s="22">
         <v>134</v>
       </c>
-      <c r="B149" s="30" t="s">
+      <c r="B149" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="C149" s="33" t="s">
+      <c r="C149" s="31" t="s">
         <v>258</v>
       </c>
       <c r="D149" s="5" t="s">
@@ -7290,8 +7196,8 @@
       <c r="A150" s="22">
         <v>135</v>
       </c>
-      <c r="B150" s="31"/>
-      <c r="C150" s="34"/>
+      <c r="B150" s="29"/>
+      <c r="C150" s="37"/>
       <c r="D150" s="5" t="s">
         <v>261</v>
       </c>
@@ -7315,8 +7221,8 @@
       <c r="A151" s="22">
         <v>136</v>
       </c>
-      <c r="B151" s="31"/>
-      <c r="C151" s="34"/>
+      <c r="B151" s="29"/>
+      <c r="C151" s="37"/>
       <c r="D151" s="5" t="s">
         <v>263</v>
       </c>
@@ -7340,8 +7246,8 @@
       <c r="A152" s="22">
         <v>137</v>
       </c>
-      <c r="B152" s="31"/>
-      <c r="C152" s="35"/>
+      <c r="B152" s="29"/>
+      <c r="C152" s="32"/>
       <c r="D152" s="5" t="s">
         <v>265</v>
       </c>
@@ -7365,8 +7271,8 @@
       <c r="A153" s="22">
         <v>138</v>
       </c>
-      <c r="B153" s="31"/>
-      <c r="C153" s="33" t="s">
+      <c r="B153" s="29"/>
+      <c r="C153" s="31" t="s">
         <v>252</v>
       </c>
       <c r="D153" s="5" t="s">
@@ -7392,8 +7298,8 @@
       <c r="A154" s="22">
         <v>139</v>
       </c>
-      <c r="B154" s="31"/>
-      <c r="C154" s="35"/>
+      <c r="B154" s="29"/>
+      <c r="C154" s="32"/>
       <c r="D154" s="5" t="s">
         <v>269</v>
       </c>
@@ -7417,7 +7323,7 @@
       <c r="A155" s="22">
         <v>140</v>
       </c>
-      <c r="B155" s="32"/>
+      <c r="B155" s="30"/>
       <c r="C155" s="4"/>
       <c r="D155" s="5" t="s">
         <v>148</v>
@@ -7442,7 +7348,7 @@
       <c r="A156" s="22">
         <v>141</v>
       </c>
-      <c r="B156" s="30" t="s">
+      <c r="B156" s="28" t="s">
         <v>271</v>
       </c>
       <c r="C156" s="4" t="s">
@@ -7455,14 +7361,14 @@
         <v>274</v>
       </c>
       <c r="F156" s="5"/>
-      <c r="G156" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H156" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I156" s="4" t="s">
-        <v>177</v>
+      <c r="G156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I156" s="27" t="s">
+        <v>22</v>
       </c>
       <c r="J156" s="6"/>
       <c r="K156" s="7"/>
@@ -7471,7 +7377,7 @@
       <c r="A157" s="22">
         <v>142</v>
       </c>
-      <c r="B157" s="31"/>
+      <c r="B157" s="29"/>
       <c r="C157" s="4" t="s">
         <v>275</v>
       </c>
@@ -7498,7 +7404,7 @@
       <c r="A158" s="22">
         <v>143</v>
       </c>
-      <c r="B158" s="31"/>
+      <c r="B158" s="29"/>
       <c r="C158" s="4" t="s">
         <v>278</v>
       </c>
@@ -7525,7 +7431,7 @@
       <c r="A159" s="22">
         <v>144</v>
       </c>
-      <c r="B159" s="32"/>
+      <c r="B159" s="30"/>
       <c r="C159" s="4"/>
       <c r="D159" s="5" t="s">
         <v>148</v>
@@ -7550,7 +7456,7 @@
       <c r="A160" s="22">
         <v>145</v>
       </c>
-      <c r="B160" s="30" t="s">
+      <c r="B160" s="28" t="s">
         <v>281</v>
       </c>
       <c r="C160" s="4" t="s">
@@ -7579,8 +7485,8 @@
       <c r="A161" s="22">
         <v>146</v>
       </c>
-      <c r="B161" s="31"/>
-      <c r="C161" s="33" t="s">
+      <c r="B161" s="29"/>
+      <c r="C161" s="31" t="s">
         <v>284</v>
       </c>
       <c r="D161" s="5" t="s">
@@ -7606,8 +7512,8 @@
       <c r="A162" s="22">
         <v>147</v>
       </c>
-      <c r="B162" s="31"/>
-      <c r="C162" s="35"/>
+      <c r="B162" s="29"/>
+      <c r="C162" s="32"/>
       <c r="D162" s="5" t="s">
         <v>287</v>
       </c>
@@ -7631,8 +7537,8 @@
       <c r="A163" s="22">
         <v>148</v>
       </c>
-      <c r="B163" s="31"/>
-      <c r="C163" s="33" t="s">
+      <c r="B163" s="29"/>
+      <c r="C163" s="31" t="s">
         <v>289</v>
       </c>
       <c r="D163" s="5" t="s">
@@ -7658,8 +7564,8 @@
       <c r="A164" s="22">
         <v>149</v>
       </c>
-      <c r="B164" s="31"/>
-      <c r="C164" s="35"/>
+      <c r="B164" s="29"/>
+      <c r="C164" s="32"/>
       <c r="D164" s="5" t="s">
         <v>290</v>
       </c>
@@ -7683,7 +7589,7 @@
       <c r="A165" s="22">
         <v>150</v>
       </c>
-      <c r="B165" s="31"/>
+      <c r="B165" s="29"/>
       <c r="C165" s="4" t="s">
         <v>293</v>
       </c>
@@ -7710,8 +7616,8 @@
       <c r="A166" s="22">
         <v>151</v>
       </c>
-      <c r="B166" s="31"/>
-      <c r="C166" s="33" t="s">
+      <c r="B166" s="29"/>
+      <c r="C166" s="31" t="s">
         <v>296</v>
       </c>
       <c r="D166" s="5" t="s">
@@ -7737,8 +7643,8 @@
       <c r="A167" s="22">
         <v>152</v>
       </c>
-      <c r="B167" s="31"/>
-      <c r="C167" s="35"/>
+      <c r="B167" s="29"/>
+      <c r="C167" s="32"/>
       <c r="D167" s="5" t="s">
         <v>299</v>
       </c>
@@ -7762,8 +7668,8 @@
       <c r="A168" s="22">
         <v>153</v>
       </c>
-      <c r="B168" s="31"/>
-      <c r="C168" s="33" t="s">
+      <c r="B168" s="29"/>
+      <c r="C168" s="31" t="s">
         <v>301</v>
       </c>
       <c r="D168" s="5" t="s">
@@ -7789,8 +7695,8 @@
       <c r="A169" s="22">
         <v>154</v>
       </c>
-      <c r="B169" s="31"/>
-      <c r="C169" s="35"/>
+      <c r="B169" s="29"/>
+      <c r="C169" s="32"/>
       <c r="D169" s="5" t="s">
         <v>304</v>
       </c>
@@ -7814,8 +7720,8 @@
       <c r="A170" s="22">
         <v>155</v>
       </c>
-      <c r="B170" s="31"/>
-      <c r="C170" s="33" t="s">
+      <c r="B170" s="29"/>
+      <c r="C170" s="31" t="s">
         <v>306</v>
       </c>
       <c r="D170" s="5" t="s">
@@ -7841,8 +7747,8 @@
       <c r="A171" s="22">
         <v>156</v>
       </c>
-      <c r="B171" s="31"/>
-      <c r="C171" s="34"/>
+      <c r="B171" s="29"/>
+      <c r="C171" s="37"/>
       <c r="D171" s="5" t="s">
         <v>309</v>
       </c>
@@ -7866,8 +7772,8 @@
       <c r="A172" s="22">
         <v>157</v>
       </c>
-      <c r="B172" s="31"/>
-      <c r="C172" s="35"/>
+      <c r="B172" s="29"/>
+      <c r="C172" s="32"/>
       <c r="D172" s="5" t="s">
         <v>311</v>
       </c>
@@ -7891,8 +7797,8 @@
       <c r="A173" s="22">
         <v>158</v>
       </c>
-      <c r="B173" s="31"/>
-      <c r="C173" s="33" t="s">
+      <c r="B173" s="29"/>
+      <c r="C173" s="31" t="s">
         <v>313</v>
       </c>
       <c r="D173" s="5" t="s">
@@ -7918,8 +7824,8 @@
       <c r="A174" s="22">
         <v>159</v>
       </c>
-      <c r="B174" s="31"/>
-      <c r="C174" s="35"/>
+      <c r="B174" s="29"/>
+      <c r="C174" s="32"/>
       <c r="D174" s="5" t="s">
         <v>314</v>
       </c>
@@ -7943,7 +7849,7 @@
       <c r="A175" s="22">
         <v>160</v>
       </c>
-      <c r="B175" s="31" t="s">
+      <c r="B175" s="29" t="s">
         <v>317</v>
       </c>
       <c r="C175" s="4" t="s">
@@ -7972,7 +7878,7 @@
       <c r="A176" s="22">
         <v>161</v>
       </c>
-      <c r="B176" s="31"/>
+      <c r="B176" s="29"/>
       <c r="C176" s="4" t="s">
         <v>319</v>
       </c>
@@ -7999,8 +7905,8 @@
       <c r="A177" s="22">
         <v>162</v>
       </c>
-      <c r="B177" s="31"/>
-      <c r="C177" s="33" t="s">
+      <c r="B177" s="29"/>
+      <c r="C177" s="31" t="s">
         <v>322</v>
       </c>
       <c r="D177" s="5" t="s">
@@ -8026,8 +7932,8 @@
       <c r="A178" s="22">
         <v>163</v>
       </c>
-      <c r="B178" s="32"/>
-      <c r="C178" s="35"/>
+      <c r="B178" s="30"/>
+      <c r="C178" s="32"/>
       <c r="D178" s="5" t="s">
         <v>323</v>
       </c>
@@ -8051,10 +7957,10 @@
       <c r="A179" s="22">
         <v>164</v>
       </c>
-      <c r="B179" s="42" t="s">
+      <c r="B179" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="C179" s="33" t="s">
+      <c r="C179" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D179" s="5" t="s">
@@ -8080,8 +7986,8 @@
       <c r="A180" s="22">
         <v>165</v>
       </c>
-      <c r="B180" s="42"/>
-      <c r="C180" s="34"/>
+      <c r="B180" s="35"/>
+      <c r="C180" s="37"/>
       <c r="D180" s="5" t="s">
         <v>329</v>
       </c>
@@ -8105,8 +8011,8 @@
       <c r="A181" s="22">
         <v>166</v>
       </c>
-      <c r="B181" s="42"/>
-      <c r="C181" s="34"/>
+      <c r="B181" s="35"/>
+      <c r="C181" s="37"/>
       <c r="D181" s="5" t="s">
         <v>331</v>
       </c>
@@ -8130,8 +8036,8 @@
       <c r="A182" s="22">
         <v>167</v>
       </c>
-      <c r="B182" s="42"/>
-      <c r="C182" s="35"/>
+      <c r="B182" s="35"/>
+      <c r="C182" s="32"/>
       <c r="D182" s="5" t="s">
         <v>333</v>
       </c>
@@ -8155,7 +8061,7 @@
       <c r="A183" s="22">
         <v>168</v>
       </c>
-      <c r="B183" s="30" t="s">
+      <c r="B183" s="28" t="s">
         <v>335</v>
       </c>
       <c r="C183" s="4" t="s">
@@ -8184,7 +8090,7 @@
       <c r="A184" s="22">
         <v>169</v>
       </c>
-      <c r="B184" s="31"/>
+      <c r="B184" s="29"/>
       <c r="C184" s="4" t="s">
         <v>339</v>
       </c>
@@ -8211,7 +8117,7 @@
       <c r="A185" s="22">
         <v>170</v>
       </c>
-      <c r="B185" s="32"/>
+      <c r="B185" s="30"/>
       <c r="C185" s="4" t="s">
         <v>342</v>
       </c>
@@ -8238,7 +8144,7 @@
       <c r="A186" s="22">
         <v>171</v>
       </c>
-      <c r="B186" s="42" t="s">
+      <c r="B186" s="35" t="s">
         <v>345</v>
       </c>
       <c r="C186" s="4" t="s">
@@ -8267,7 +8173,7 @@
       <c r="A187" s="22">
         <v>172</v>
       </c>
-      <c r="B187" s="42"/>
+      <c r="B187" s="35"/>
       <c r="C187" s="4" t="s">
         <v>349</v>
       </c>
@@ -8294,7 +8200,7 @@
       <c r="A188" s="22">
         <v>173</v>
       </c>
-      <c r="B188" s="42"/>
+      <c r="B188" s="35"/>
       <c r="C188" s="4" t="s">
         <v>352</v>
       </c>
@@ -8321,7 +8227,7 @@
       <c r="A189" s="22">
         <v>174</v>
       </c>
-      <c r="B189" s="42"/>
+      <c r="B189" s="35"/>
       <c r="C189" s="4" t="s">
         <v>355</v>
       </c>
@@ -8348,7 +8254,7 @@
       <c r="A190" s="22">
         <v>175</v>
       </c>
-      <c r="B190" s="42"/>
+      <c r="B190" s="35"/>
       <c r="C190" s="4" t="s">
         <v>357</v>
       </c>
@@ -8375,7 +8281,7 @@
       <c r="A191" s="22">
         <v>176</v>
       </c>
-      <c r="B191" s="42" t="s">
+      <c r="B191" s="35" t="s">
         <v>359</v>
       </c>
       <c r="C191" s="4" t="s">
@@ -8404,7 +8310,7 @@
       <c r="A192" s="22">
         <v>177</v>
       </c>
-      <c r="B192" s="42"/>
+      <c r="B192" s="35"/>
       <c r="C192" s="4"/>
       <c r="D192" s="5" t="s">
         <v>363</v>
@@ -8429,7 +8335,7 @@
       <c r="A193" s="22">
         <v>178</v>
       </c>
-      <c r="B193" s="42"/>
+      <c r="B193" s="35"/>
       <c r="C193" s="4"/>
       <c r="D193" s="5" t="s">
         <v>365</v>
@@ -8454,7 +8360,7 @@
       <c r="A194" s="22">
         <v>179</v>
       </c>
-      <c r="B194" s="42"/>
+      <c r="B194" s="35"/>
       <c r="C194" s="4"/>
       <c r="D194" s="5" t="s">
         <v>367</v>
@@ -8479,7 +8385,7 @@
       <c r="A195" s="22">
         <v>180</v>
       </c>
-      <c r="B195" s="42"/>
+      <c r="B195" s="35"/>
       <c r="C195" s="4" t="s">
         <v>369</v>
       </c>
@@ -8506,7 +8412,7 @@
       <c r="A196" s="22">
         <v>181</v>
       </c>
-      <c r="B196" s="42"/>
+      <c r="B196" s="35"/>
       <c r="C196" s="4" t="s">
         <v>372</v>
       </c>
@@ -8533,7 +8439,7 @@
       <c r="A197" s="22">
         <v>182</v>
       </c>
-      <c r="B197" s="42"/>
+      <c r="B197" s="35"/>
       <c r="C197" s="4"/>
       <c r="D197" s="5" t="s">
         <v>375</v>
@@ -8558,7 +8464,7 @@
       <c r="A198" s="22">
         <v>183</v>
       </c>
-      <c r="B198" s="42"/>
+      <c r="B198" s="35"/>
       <c r="C198" s="4"/>
       <c r="D198" s="5" t="s">
         <v>377</v>
@@ -8583,7 +8489,7 @@
       <c r="A199" s="22">
         <v>184</v>
       </c>
-      <c r="B199" s="42"/>
+      <c r="B199" s="35"/>
       <c r="C199" s="4" t="s">
         <v>379</v>
       </c>
@@ -8610,7 +8516,7 @@
       <c r="A200" s="22">
         <v>185</v>
       </c>
-      <c r="B200" s="42"/>
+      <c r="B200" s="35"/>
       <c r="C200" s="4" t="s">
         <v>357</v>
       </c>
@@ -8637,7 +8543,7 @@
       <c r="A201" s="22">
         <v>186</v>
       </c>
-      <c r="B201" s="42"/>
+      <c r="B201" s="35"/>
       <c r="C201" s="4" t="s">
         <v>382</v>
       </c>
@@ -8664,7 +8570,7 @@
       <c r="A202" s="22">
         <v>187</v>
       </c>
-      <c r="B202" s="42" t="s">
+      <c r="B202" s="35" t="s">
         <v>384</v>
       </c>
       <c r="C202" s="4" t="s">
@@ -8693,7 +8599,7 @@
       <c r="A203" s="22">
         <v>188</v>
       </c>
-      <c r="B203" s="42"/>
+      <c r="B203" s="35"/>
       <c r="C203" s="4"/>
       <c r="D203" s="5" t="s">
         <v>353</v>
@@ -8718,7 +8624,7 @@
       <c r="A204" s="22">
         <v>189</v>
       </c>
-      <c r="B204" s="42"/>
+      <c r="B204" s="35"/>
       <c r="C204" s="4" t="s">
         <v>382</v>
       </c>
@@ -8745,7 +8651,7 @@
       <c r="A205" s="22">
         <v>190</v>
       </c>
-      <c r="B205" s="42"/>
+      <c r="B205" s="35"/>
       <c r="C205" s="4" t="s">
         <v>388</v>
       </c>
@@ -8772,7 +8678,7 @@
       <c r="A206" s="22">
         <v>191</v>
       </c>
-      <c r="B206" s="42"/>
+      <c r="B206" s="35"/>
       <c r="C206" s="16" t="s">
         <v>391</v>
       </c>
@@ -8799,7 +8705,7 @@
       <c r="A207" s="22">
         <v>192</v>
       </c>
-      <c r="B207" s="30" t="s">
+      <c r="B207" s="28" t="s">
         <v>394</v>
       </c>
       <c r="C207" s="4" t="s">
@@ -8828,8 +8734,8 @@
       <c r="A208" s="22">
         <v>193</v>
       </c>
-      <c r="B208" s="31"/>
-      <c r="C208" s="33" t="s">
+      <c r="B208" s="29"/>
+      <c r="C208" s="31" t="s">
         <v>397</v>
       </c>
       <c r="D208" s="5" t="s">
@@ -8855,8 +8761,8 @@
       <c r="A209" s="22">
         <v>194</v>
       </c>
-      <c r="B209" s="31"/>
-      <c r="C209" s="34"/>
+      <c r="B209" s="29"/>
+      <c r="C209" s="37"/>
       <c r="D209" s="5" t="s">
         <v>400</v>
       </c>
@@ -8880,8 +8786,8 @@
       <c r="A210" s="22">
         <v>195</v>
       </c>
-      <c r="B210" s="31"/>
-      <c r="C210" s="35"/>
+      <c r="B210" s="29"/>
+      <c r="C210" s="32"/>
       <c r="D210" s="5" t="s">
         <v>402</v>
       </c>
@@ -8905,7 +8811,7 @@
       <c r="A211" s="22">
         <v>196</v>
       </c>
-      <c r="B211" s="31"/>
+      <c r="B211" s="29"/>
       <c r="C211" s="4" t="s">
         <v>404</v>
       </c>
@@ -8932,7 +8838,7 @@
       <c r="A212" s="22">
         <v>197</v>
       </c>
-      <c r="B212" s="31"/>
+      <c r="B212" s="29"/>
       <c r="C212" s="4" t="s">
         <v>407</v>
       </c>
@@ -8959,8 +8865,8 @@
       <c r="A213" s="22">
         <v>198</v>
       </c>
-      <c r="B213" s="31"/>
-      <c r="C213" s="33" t="s">
+      <c r="B213" s="29"/>
+      <c r="C213" s="31" t="s">
         <v>410</v>
       </c>
       <c r="D213" s="5" t="s">
@@ -8986,8 +8892,8 @@
       <c r="A214" s="22">
         <v>199</v>
       </c>
-      <c r="B214" s="31"/>
-      <c r="C214" s="34"/>
+      <c r="B214" s="29"/>
+      <c r="C214" s="37"/>
       <c r="D214" s="5" t="s">
         <v>411</v>
       </c>
@@ -9011,8 +8917,8 @@
       <c r="A215" s="22">
         <v>200</v>
       </c>
-      <c r="B215" s="31"/>
-      <c r="C215" s="35"/>
+      <c r="B215" s="29"/>
+      <c r="C215" s="32"/>
       <c r="D215" s="5" t="s">
         <v>411</v>
       </c>
@@ -9036,7 +8942,7 @@
       <c r="A216" s="22">
         <v>201</v>
       </c>
-      <c r="B216" s="31"/>
+      <c r="B216" s="29"/>
       <c r="C216" s="4" t="s">
         <v>357</v>
       </c>
@@ -9063,7 +8969,7 @@
       <c r="A217" s="22">
         <v>202</v>
       </c>
-      <c r="B217" s="31"/>
+      <c r="B217" s="29"/>
       <c r="C217" s="4" t="s">
         <v>382</v>
       </c>
@@ -9090,7 +8996,7 @@
       <c r="A218" s="22">
         <v>203</v>
       </c>
-      <c r="B218" s="32"/>
+      <c r="B218" s="30"/>
       <c r="C218" s="4" t="s">
         <v>418</v>
       </c>
@@ -9117,7 +9023,7 @@
       <c r="A219" s="22">
         <v>204</v>
       </c>
-      <c r="B219" s="39" t="s">
+      <c r="B219" s="41" t="s">
         <v>421</v>
       </c>
       <c r="C219" s="4" t="s">
@@ -9146,8 +9052,8 @@
       <c r="A220" s="22">
         <v>205</v>
       </c>
-      <c r="B220" s="40"/>
-      <c r="C220" s="33" t="s">
+      <c r="B220" s="42"/>
+      <c r="C220" s="31" t="s">
         <v>397</v>
       </c>
       <c r="D220" s="5" t="s">
@@ -9173,8 +9079,8 @@
       <c r="A221" s="22">
         <v>206</v>
       </c>
-      <c r="B221" s="40"/>
-      <c r="C221" s="34"/>
+      <c r="B221" s="42"/>
+      <c r="C221" s="37"/>
       <c r="D221" s="5" t="s">
         <v>424</v>
       </c>
@@ -9198,8 +9104,8 @@
       <c r="A222" s="22">
         <v>207</v>
       </c>
-      <c r="B222" s="40"/>
-      <c r="C222" s="35"/>
+      <c r="B222" s="42"/>
+      <c r="C222" s="32"/>
       <c r="D222" s="5" t="s">
         <v>424</v>
       </c>
@@ -9223,7 +9129,7 @@
       <c r="A223" s="22">
         <v>208</v>
       </c>
-      <c r="B223" s="40"/>
+      <c r="B223" s="42"/>
       <c r="C223" s="4" t="s">
         <v>407</v>
       </c>
@@ -9250,8 +9156,8 @@
       <c r="A224" s="22">
         <v>209</v>
       </c>
-      <c r="B224" s="40"/>
-      <c r="C224" s="33" t="s">
+      <c r="B224" s="42"/>
+      <c r="C224" s="31" t="s">
         <v>410</v>
       </c>
       <c r="D224" s="5" t="s">
@@ -9277,8 +9183,8 @@
       <c r="A225" s="22">
         <v>210</v>
       </c>
-      <c r="B225" s="40"/>
-      <c r="C225" s="34"/>
+      <c r="B225" s="42"/>
+      <c r="C225" s="37"/>
       <c r="D225" s="5" t="s">
         <v>426</v>
       </c>
@@ -9302,8 +9208,8 @@
       <c r="A226" s="22">
         <v>211</v>
       </c>
-      <c r="B226" s="40"/>
-      <c r="C226" s="35"/>
+      <c r="B226" s="42"/>
+      <c r="C226" s="32"/>
       <c r="D226" s="5" t="s">
         <v>426</v>
       </c>
@@ -9327,7 +9233,7 @@
       <c r="A227" s="22">
         <v>212</v>
       </c>
-      <c r="B227" s="40"/>
+      <c r="B227" s="42"/>
       <c r="C227" s="4" t="s">
         <v>357</v>
       </c>
@@ -9354,7 +9260,7 @@
       <c r="A228" s="22">
         <v>213</v>
       </c>
-      <c r="B228" s="41"/>
+      <c r="B228" s="43"/>
       <c r="C228" s="4" t="s">
         <v>382</v>
       </c>
@@ -9381,7 +9287,7 @@
       <c r="A229" s="22">
         <v>214</v>
       </c>
-      <c r="B229" s="27" t="s">
+      <c r="B229" s="44" t="s">
         <v>429</v>
       </c>
       <c r="C229" s="4" t="s">
@@ -9410,8 +9316,8 @@
       <c r="A230" s="22">
         <v>215</v>
       </c>
-      <c r="B230" s="28"/>
-      <c r="C230" s="33" t="s">
+      <c r="B230" s="45"/>
+      <c r="C230" s="31" t="s">
         <v>397</v>
       </c>
       <c r="D230" s="5" t="s">
@@ -9437,8 +9343,8 @@
       <c r="A231" s="22">
         <v>216</v>
       </c>
-      <c r="B231" s="28"/>
-      <c r="C231" s="34"/>
+      <c r="B231" s="45"/>
+      <c r="C231" s="37"/>
       <c r="D231" s="5" t="s">
         <v>433</v>
       </c>
@@ -9462,8 +9368,8 @@
       <c r="A232" s="22">
         <v>217</v>
       </c>
-      <c r="B232" s="28"/>
-      <c r="C232" s="35"/>
+      <c r="B232" s="45"/>
+      <c r="C232" s="32"/>
       <c r="D232" s="5" t="s">
         <v>433</v>
       </c>
@@ -9487,7 +9393,7 @@
       <c r="A233" s="22">
         <v>218</v>
       </c>
-      <c r="B233" s="28"/>
+      <c r="B233" s="45"/>
       <c r="C233" s="4" t="s">
         <v>407</v>
       </c>
@@ -9514,8 +9420,8 @@
       <c r="A234" s="22">
         <v>219</v>
       </c>
-      <c r="B234" s="28"/>
-      <c r="C234" s="33" t="s">
+      <c r="B234" s="45"/>
+      <c r="C234" s="31" t="s">
         <v>410</v>
       </c>
       <c r="D234" s="5" t="s">
@@ -9541,8 +9447,8 @@
       <c r="A235" s="22">
         <v>220</v>
       </c>
-      <c r="B235" s="28"/>
-      <c r="C235" s="34"/>
+      <c r="B235" s="45"/>
+      <c r="C235" s="37"/>
       <c r="D235" s="5" t="s">
         <v>435</v>
       </c>
@@ -9566,8 +9472,8 @@
       <c r="A236" s="22">
         <v>221</v>
       </c>
-      <c r="B236" s="28"/>
-      <c r="C236" s="35"/>
+      <c r="B236" s="45"/>
+      <c r="C236" s="32"/>
       <c r="D236" s="5" t="s">
         <v>435</v>
       </c>
@@ -9591,7 +9497,7 @@
       <c r="A237" s="22">
         <v>222</v>
       </c>
-      <c r="B237" s="28"/>
+      <c r="B237" s="45"/>
       <c r="C237" s="4" t="s">
         <v>357</v>
       </c>
@@ -9618,7 +9524,7 @@
       <c r="A238" s="22">
         <v>223</v>
       </c>
-      <c r="B238" s="28"/>
+      <c r="B238" s="45"/>
       <c r="C238" s="4" t="s">
         <v>382</v>
       </c>
@@ -9645,7 +9551,7 @@
       <c r="A239" s="22">
         <v>224</v>
       </c>
-      <c r="B239" s="29"/>
+      <c r="B239" s="46"/>
       <c r="C239" s="4" t="s">
         <v>404</v>
       </c>
@@ -9672,7 +9578,7 @@
       <c r="A240" s="22">
         <v>225</v>
       </c>
-      <c r="B240" s="27" t="s">
+      <c r="B240" s="44" t="s">
         <v>439</v>
       </c>
       <c r="C240" s="4" t="s">
@@ -9701,7 +9607,7 @@
       <c r="A241" s="22">
         <v>226</v>
       </c>
-      <c r="B241" s="28"/>
+      <c r="B241" s="45"/>
       <c r="C241" s="4" t="s">
         <v>442</v>
       </c>
@@ -9728,7 +9634,7 @@
       <c r="A242" s="22">
         <v>227</v>
       </c>
-      <c r="B242" s="28"/>
+      <c r="B242" s="45"/>
       <c r="C242" s="4" t="s">
         <v>445</v>
       </c>
@@ -9755,7 +9661,7 @@
       <c r="A243" s="22">
         <v>228</v>
       </c>
-      <c r="B243" s="28"/>
+      <c r="B243" s="45"/>
       <c r="C243" s="4"/>
       <c r="D243" s="5" t="s">
         <v>448</v>
@@ -9780,7 +9686,7 @@
       <c r="A244" s="22">
         <v>229</v>
       </c>
-      <c r="B244" s="29"/>
+      <c r="B244" s="46"/>
       <c r="C244" s="4"/>
       <c r="D244" s="5" t="s">
         <v>450</v>
@@ -9805,7 +9711,7 @@
       <c r="A245" s="22">
         <v>230</v>
       </c>
-      <c r="B245" s="27" t="s">
+      <c r="B245" s="44" t="s">
         <v>452</v>
       </c>
       <c r="C245" s="4" t="s">
@@ -9834,8 +9740,8 @@
       <c r="A246" s="22">
         <v>231</v>
       </c>
-      <c r="B246" s="28"/>
-      <c r="C246" s="33" t="s">
+      <c r="B246" s="45"/>
+      <c r="C246" s="31" t="s">
         <v>455</v>
       </c>
       <c r="D246" s="5" t="s">
@@ -9861,8 +9767,8 @@
       <c r="A247" s="22">
         <v>232</v>
       </c>
-      <c r="B247" s="28"/>
-      <c r="C247" s="34"/>
+      <c r="B247" s="45"/>
+      <c r="C247" s="37"/>
       <c r="D247" s="5" t="s">
         <v>458</v>
       </c>
@@ -9886,8 +9792,8 @@
       <c r="A248" s="22">
         <v>233</v>
       </c>
-      <c r="B248" s="28"/>
-      <c r="C248" s="34"/>
+      <c r="B248" s="45"/>
+      <c r="C248" s="37"/>
       <c r="D248" s="5" t="s">
         <v>460</v>
       </c>
@@ -9911,8 +9817,8 @@
       <c r="A249" s="22">
         <v>234</v>
       </c>
-      <c r="B249" s="28"/>
-      <c r="C249" s="35"/>
+      <c r="B249" s="45"/>
+      <c r="C249" s="32"/>
       <c r="D249" s="5" t="s">
         <v>462</v>
       </c>
@@ -9936,7 +9842,7 @@
       <c r="A250" s="22">
         <v>235</v>
       </c>
-      <c r="B250" s="28"/>
+      <c r="B250" s="45"/>
       <c r="C250" s="4" t="s">
         <v>464</v>
       </c>
@@ -9963,7 +9869,7 @@
       <c r="A251" s="22">
         <v>236</v>
       </c>
-      <c r="B251" s="28"/>
+      <c r="B251" s="45"/>
       <c r="C251" s="4" t="s">
         <v>467</v>
       </c>
@@ -9990,7 +9896,7 @@
       <c r="A252" s="22">
         <v>237</v>
       </c>
-      <c r="B252" s="28"/>
+      <c r="B252" s="45"/>
       <c r="C252" s="4" t="s">
         <v>470</v>
       </c>
@@ -10017,7 +9923,7 @@
       <c r="A253" s="22">
         <v>238</v>
       </c>
-      <c r="B253" s="28"/>
+      <c r="B253" s="45"/>
       <c r="C253" s="4" t="s">
         <v>473</v>
       </c>
@@ -10044,7 +9950,7 @@
       <c r="A254" s="22">
         <v>239</v>
       </c>
-      <c r="B254" s="29"/>
+      <c r="B254" s="46"/>
       <c r="C254" s="4" t="s">
         <v>476</v>
       </c>
@@ -10071,7 +9977,7 @@
       <c r="A255" s="22">
         <v>240</v>
       </c>
-      <c r="B255" s="27" t="s">
+      <c r="B255" s="44" t="s">
         <v>479</v>
       </c>
       <c r="C255" s="4" t="s">
@@ -10100,7 +10006,7 @@
       <c r="A256" s="22">
         <v>241</v>
       </c>
-      <c r="B256" s="28"/>
+      <c r="B256" s="45"/>
       <c r="C256" s="4" t="s">
         <v>482</v>
       </c>
@@ -10127,7 +10033,7 @@
       <c r="A257" s="22">
         <v>242</v>
       </c>
-      <c r="B257" s="28"/>
+      <c r="B257" s="45"/>
       <c r="C257" s="4" t="s">
         <v>151</v>
       </c>
@@ -10154,8 +10060,8 @@
       <c r="A258" s="22">
         <v>243</v>
       </c>
-      <c r="B258" s="28"/>
-      <c r="C258" s="33" t="s">
+      <c r="B258" s="45"/>
+      <c r="C258" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D258" s="5" t="s">
@@ -10181,8 +10087,8 @@
       <c r="A259" s="22">
         <v>244</v>
       </c>
-      <c r="B259" s="28"/>
-      <c r="C259" s="34"/>
+      <c r="B259" s="45"/>
+      <c r="C259" s="37"/>
       <c r="D259" s="5" t="s">
         <v>490</v>
       </c>
@@ -10206,8 +10112,8 @@
       <c r="A260" s="22">
         <v>245</v>
       </c>
-      <c r="B260" s="28"/>
-      <c r="C260" s="35"/>
+      <c r="B260" s="45"/>
+      <c r="C260" s="32"/>
       <c r="D260" s="5" t="s">
         <v>492</v>
       </c>
@@ -10231,7 +10137,7 @@
       <c r="A261" s="22">
         <v>246</v>
       </c>
-      <c r="B261" s="28"/>
+      <c r="B261" s="45"/>
       <c r="C261" s="17" t="s">
         <v>494</v>
       </c>
@@ -10258,7 +10164,7 @@
       <c r="A262" s="22">
         <v>247</v>
       </c>
-      <c r="B262" s="28"/>
+      <c r="B262" s="45"/>
       <c r="C262" s="4" t="s">
         <v>497</v>
       </c>
@@ -10285,7 +10191,7 @@
       <c r="A263" s="22">
         <v>248</v>
       </c>
-      <c r="B263" s="28"/>
+      <c r="B263" s="45"/>
       <c r="C263" s="4" t="s">
         <v>500</v>
       </c>
@@ -10312,7 +10218,7 @@
       <c r="A264" s="22">
         <v>249</v>
       </c>
-      <c r="B264" s="29"/>
+      <c r="B264" s="46"/>
       <c r="C264" s="4" t="s">
         <v>503</v>
       </c>
@@ -10339,7 +10245,7 @@
       <c r="A265" s="22">
         <v>250</v>
       </c>
-      <c r="B265" s="27" t="s">
+      <c r="B265" s="44" t="s">
         <v>506</v>
       </c>
       <c r="C265" s="4" t="s">
@@ -10368,7 +10274,7 @@
       <c r="A266" s="22">
         <v>251</v>
       </c>
-      <c r="B266" s="28"/>
+      <c r="B266" s="45"/>
       <c r="C266" s="4" t="s">
         <v>509</v>
       </c>
@@ -10395,7 +10301,7 @@
       <c r="A267" s="22">
         <v>252</v>
       </c>
-      <c r="B267" s="28"/>
+      <c r="B267" s="45"/>
       <c r="C267" s="4" t="s">
         <v>512</v>
       </c>
@@ -10422,7 +10328,7 @@
       <c r="A268" s="22">
         <v>253</v>
       </c>
-      <c r="B268" s="28"/>
+      <c r="B268" s="45"/>
       <c r="C268" s="4" t="s">
         <v>515</v>
       </c>
@@ -10449,7 +10355,7 @@
       <c r="A269" s="22">
         <v>254</v>
       </c>
-      <c r="B269" s="28"/>
+      <c r="B269" s="45"/>
       <c r="C269" s="4" t="s">
         <v>500</v>
       </c>
@@ -10476,7 +10382,7 @@
       <c r="A270" s="22">
         <v>255</v>
       </c>
-      <c r="B270" s="29"/>
+      <c r="B270" s="46"/>
       <c r="C270" s="4" t="s">
         <v>497</v>
       </c>
@@ -10503,7 +10409,7 @@
       <c r="A271" s="22">
         <v>256</v>
       </c>
-      <c r="B271" s="27" t="s">
+      <c r="B271" s="44" t="s">
         <v>520</v>
       </c>
       <c r="C271" s="4" t="s">
@@ -10532,7 +10438,7 @@
       <c r="A272" s="22">
         <v>257</v>
       </c>
-      <c r="B272" s="28"/>
+      <c r="B272" s="45"/>
       <c r="C272" s="4" t="s">
         <v>482</v>
       </c>
@@ -10559,7 +10465,7 @@
       <c r="A273" s="22">
         <v>258</v>
       </c>
-      <c r="B273" s="28"/>
+      <c r="B273" s="45"/>
       <c r="C273" s="4" t="s">
         <v>151</v>
       </c>
@@ -10586,8 +10492,8 @@
       <c r="A274" s="22">
         <v>259</v>
       </c>
-      <c r="B274" s="28"/>
-      <c r="C274" s="33" t="s">
+      <c r="B274" s="45"/>
+      <c r="C274" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D274" s="5" t="s">
@@ -10613,8 +10519,8 @@
       <c r="A275" s="22">
         <v>260</v>
       </c>
-      <c r="B275" s="28"/>
-      <c r="C275" s="34"/>
+      <c r="B275" s="45"/>
+      <c r="C275" s="37"/>
       <c r="D275" s="5" t="s">
         <v>490</v>
       </c>
@@ -10638,8 +10544,8 @@
       <c r="A276" s="22">
         <v>261</v>
       </c>
-      <c r="B276" s="28"/>
-      <c r="C276" s="35"/>
+      <c r="B276" s="45"/>
+      <c r="C276" s="32"/>
       <c r="D276" s="5" t="s">
         <v>492</v>
       </c>
@@ -10663,7 +10569,7 @@
       <c r="A277" s="22">
         <v>262</v>
       </c>
-      <c r="B277" s="28"/>
+      <c r="B277" s="45"/>
       <c r="C277" s="17" t="s">
         <v>494</v>
       </c>
@@ -10690,7 +10596,7 @@
       <c r="A278" s="22">
         <v>263</v>
       </c>
-      <c r="B278" s="28"/>
+      <c r="B278" s="45"/>
       <c r="C278" s="4" t="s">
         <v>497</v>
       </c>
@@ -10717,7 +10623,7 @@
       <c r="A279" s="22">
         <v>264</v>
       </c>
-      <c r="B279" s="29"/>
+      <c r="B279" s="46"/>
       <c r="C279" s="4" t="s">
         <v>500</v>
       </c>
@@ -10744,7 +10650,7 @@
       <c r="A280" s="22">
         <v>265</v>
       </c>
-      <c r="B280" s="27" t="s">
+      <c r="B280" s="44" t="s">
         <v>530</v>
       </c>
       <c r="C280" s="4" t="s">
@@ -10773,7 +10679,7 @@
       <c r="A281" s="22">
         <v>266</v>
       </c>
-      <c r="B281" s="28"/>
+      <c r="B281" s="45"/>
       <c r="C281" s="4" t="s">
         <v>482</v>
       </c>
@@ -10800,7 +10706,7 @@
       <c r="A282" s="22">
         <v>267</v>
       </c>
-      <c r="B282" s="28"/>
+      <c r="B282" s="45"/>
       <c r="C282" s="4" t="s">
         <v>151</v>
       </c>
@@ -10827,7 +10733,7 @@
       <c r="A283" s="22">
         <v>268</v>
       </c>
-      <c r="B283" s="28"/>
+      <c r="B283" s="45"/>
       <c r="C283" s="4" t="s">
         <v>500</v>
       </c>
@@ -10854,7 +10760,7 @@
       <c r="A284" s="22">
         <v>269</v>
       </c>
-      <c r="B284" s="28"/>
+      <c r="B284" s="45"/>
       <c r="C284" s="4" t="s">
         <v>497</v>
       </c>
@@ -10881,8 +10787,8 @@
       <c r="A285" s="22">
         <v>270</v>
       </c>
-      <c r="B285" s="28"/>
-      <c r="C285" s="33" t="s">
+      <c r="B285" s="45"/>
+      <c r="C285" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D285" s="5" t="s">
@@ -10908,8 +10814,8 @@
       <c r="A286" s="22">
         <v>271</v>
       </c>
-      <c r="B286" s="28"/>
-      <c r="C286" s="34"/>
+      <c r="B286" s="45"/>
+      <c r="C286" s="37"/>
       <c r="D286" s="5" t="s">
         <v>490</v>
       </c>
@@ -10933,8 +10839,8 @@
       <c r="A287" s="22">
         <v>272</v>
       </c>
-      <c r="B287" s="28"/>
-      <c r="C287" s="34"/>
+      <c r="B287" s="45"/>
+      <c r="C287" s="37"/>
       <c r="D287" s="5" t="s">
         <v>492</v>
       </c>
@@ -10958,8 +10864,8 @@
       <c r="A288" s="22">
         <v>273</v>
       </c>
-      <c r="B288" s="28"/>
-      <c r="C288" s="34"/>
+      <c r="B288" s="45"/>
+      <c r="C288" s="37"/>
       <c r="D288" s="5" t="s">
         <v>539</v>
       </c>
@@ -10983,8 +10889,8 @@
       <c r="A289" s="22">
         <v>274</v>
       </c>
-      <c r="B289" s="28"/>
-      <c r="C289" s="34"/>
+      <c r="B289" s="45"/>
+      <c r="C289" s="37"/>
       <c r="D289" s="5" t="s">
         <v>541</v>
       </c>
@@ -11008,8 +10914,8 @@
       <c r="A290" s="22">
         <v>275</v>
       </c>
-      <c r="B290" s="29"/>
-      <c r="C290" s="35"/>
+      <c r="B290" s="46"/>
+      <c r="C290" s="32"/>
       <c r="D290" s="5" t="s">
         <v>541</v>
       </c>
@@ -11033,7 +10939,7 @@
       <c r="A291" s="22">
         <v>276</v>
       </c>
-      <c r="B291" s="27" t="s">
+      <c r="B291" s="44" t="s">
         <v>544</v>
       </c>
       <c r="C291" s="4" t="s">
@@ -11062,7 +10968,7 @@
       <c r="A292" s="22">
         <v>277</v>
       </c>
-      <c r="B292" s="28"/>
+      <c r="B292" s="45"/>
       <c r="C292" s="4" t="s">
         <v>482</v>
       </c>
@@ -11089,7 +10995,7 @@
       <c r="A293" s="22">
         <v>278</v>
       </c>
-      <c r="B293" s="28"/>
+      <c r="B293" s="45"/>
       <c r="C293" s="4" t="s">
         <v>151</v>
       </c>
@@ -11116,7 +11022,7 @@
       <c r="A294" s="22">
         <v>279</v>
       </c>
-      <c r="B294" s="28"/>
+      <c r="B294" s="45"/>
       <c r="C294" s="4" t="s">
         <v>497</v>
       </c>
@@ -11143,8 +11049,8 @@
       <c r="A295" s="22">
         <v>280</v>
       </c>
-      <c r="B295" s="28"/>
-      <c r="C295" s="33" t="s">
+      <c r="B295" s="45"/>
+      <c r="C295" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D295" s="5" t="s">
@@ -11170,8 +11076,8 @@
       <c r="A296" s="22">
         <v>281</v>
       </c>
-      <c r="B296" s="28"/>
-      <c r="C296" s="34"/>
+      <c r="B296" s="45"/>
+      <c r="C296" s="37"/>
       <c r="D296" s="5" t="s">
         <v>490</v>
       </c>
@@ -11195,8 +11101,8 @@
       <c r="A297" s="22">
         <v>282</v>
       </c>
-      <c r="B297" s="28"/>
-      <c r="C297" s="34"/>
+      <c r="B297" s="45"/>
+      <c r="C297" s="37"/>
       <c r="D297" s="5" t="s">
         <v>492</v>
       </c>
@@ -11220,8 +11126,8 @@
       <c r="A298" s="22">
         <v>283</v>
       </c>
-      <c r="B298" s="28"/>
-      <c r="C298" s="35"/>
+      <c r="B298" s="45"/>
+      <c r="C298" s="32"/>
       <c r="D298" s="5" t="s">
         <v>550</v>
       </c>
@@ -11245,7 +11151,7 @@
       <c r="A299" s="22">
         <v>284</v>
       </c>
-      <c r="B299" s="28"/>
+      <c r="B299" s="45"/>
       <c r="C299" s="4" t="s">
         <v>552</v>
       </c>
@@ -11272,7 +11178,7 @@
       <c r="A300" s="22">
         <v>285</v>
       </c>
-      <c r="B300" s="29"/>
+      <c r="B300" s="46"/>
       <c r="C300" s="4" t="s">
         <v>500</v>
       </c>
@@ -11299,7 +11205,7 @@
       <c r="A301" s="22">
         <v>286</v>
       </c>
-      <c r="B301" s="36" t="s">
+      <c r="B301" s="47" t="s">
         <v>556</v>
       </c>
       <c r="C301" s="4" t="s">
@@ -11328,7 +11234,7 @@
       <c r="A302" s="22">
         <v>287</v>
       </c>
-      <c r="B302" s="37"/>
+      <c r="B302" s="48"/>
       <c r="C302" s="4" t="s">
         <v>552</v>
       </c>
@@ -11355,7 +11261,7 @@
       <c r="A303" s="22">
         <v>288</v>
       </c>
-      <c r="B303" s="37"/>
+      <c r="B303" s="48"/>
       <c r="C303" s="4" t="s">
         <v>500</v>
       </c>
@@ -11382,7 +11288,7 @@
       <c r="A304" s="22">
         <v>289</v>
       </c>
-      <c r="B304" s="37"/>
+      <c r="B304" s="48"/>
       <c r="C304" s="4" t="s">
         <v>497</v>
       </c>
@@ -11409,7 +11315,7 @@
       <c r="A305" s="22">
         <v>290</v>
       </c>
-      <c r="B305" s="38"/>
+      <c r="B305" s="49"/>
       <c r="C305" s="4" t="s">
         <v>561</v>
       </c>
@@ -11436,7 +11342,7 @@
       <c r="A306" s="22">
         <v>291</v>
       </c>
-      <c r="B306" s="27" t="s">
+      <c r="B306" s="44" t="s">
         <v>564</v>
       </c>
       <c r="C306" s="4" t="s">
@@ -11465,7 +11371,7 @@
       <c r="A307" s="22">
         <v>292</v>
       </c>
-      <c r="B307" s="28"/>
+      <c r="B307" s="45"/>
       <c r="C307" s="4" t="s">
         <v>500</v>
       </c>
@@ -11492,7 +11398,7 @@
       <c r="A308" s="22">
         <v>293</v>
       </c>
-      <c r="B308" s="28"/>
+      <c r="B308" s="45"/>
       <c r="C308" s="4" t="s">
         <v>497</v>
       </c>
@@ -11519,8 +11425,8 @@
       <c r="A309" s="22">
         <v>294</v>
       </c>
-      <c r="B309" s="28"/>
-      <c r="C309" s="33" t="s">
+      <c r="B309" s="45"/>
+      <c r="C309" s="31" t="s">
         <v>487</v>
       </c>
       <c r="D309" s="5" t="s">
@@ -11546,8 +11452,8 @@
       <c r="A310" s="22">
         <v>295</v>
       </c>
-      <c r="B310" s="28"/>
-      <c r="C310" s="34"/>
+      <c r="B310" s="45"/>
+      <c r="C310" s="37"/>
       <c r="D310" s="5" t="s">
         <v>490</v>
       </c>
@@ -11571,8 +11477,8 @@
       <c r="A311" s="22">
         <v>296</v>
       </c>
-      <c r="B311" s="28"/>
-      <c r="C311" s="35"/>
+      <c r="B311" s="45"/>
+      <c r="C311" s="32"/>
       <c r="D311" s="5" t="s">
         <v>492</v>
       </c>
@@ -11596,8 +11502,8 @@
       <c r="A312" s="22">
         <v>297</v>
       </c>
-      <c r="B312" s="28"/>
-      <c r="C312" s="33" t="s">
+      <c r="B312" s="45"/>
+      <c r="C312" s="31" t="s">
         <v>569</v>
       </c>
       <c r="D312" s="5" t="s">
@@ -11623,8 +11529,8 @@
       <c r="A313" s="22">
         <v>298</v>
       </c>
-      <c r="B313" s="28"/>
-      <c r="C313" s="34"/>
+      <c r="B313" s="45"/>
+      <c r="C313" s="37"/>
       <c r="D313" s="5" t="s">
         <v>572</v>
       </c>
@@ -11648,8 +11554,8 @@
       <c r="A314" s="22">
         <v>299</v>
       </c>
-      <c r="B314" s="28"/>
-      <c r="C314" s="35"/>
+      <c r="B314" s="45"/>
+      <c r="C314" s="32"/>
       <c r="D314" s="5" t="s">
         <v>574</v>
       </c>
@@ -11673,8 +11579,8 @@
       <c r="A315" s="22">
         <v>300</v>
       </c>
-      <c r="B315" s="28"/>
-      <c r="C315" s="33" t="s">
+      <c r="B315" s="45"/>
+      <c r="C315" s="31" t="s">
         <v>576</v>
       </c>
       <c r="D315" s="5" t="s">
@@ -11700,8 +11606,8 @@
       <c r="A316" s="22">
         <v>301</v>
       </c>
-      <c r="B316" s="28"/>
-      <c r="C316" s="35"/>
+      <c r="B316" s="45"/>
+      <c r="C316" s="32"/>
       <c r="D316" s="5" t="s">
         <v>579</v>
       </c>
@@ -11725,7 +11631,7 @@
       <c r="A317" s="22">
         <v>302</v>
       </c>
-      <c r="B317" s="29"/>
+      <c r="B317" s="46"/>
       <c r="C317" s="4" t="s">
         <v>581</v>
       </c>
@@ -11752,7 +11658,7 @@
       <c r="A318" s="22">
         <v>303</v>
       </c>
-      <c r="B318" s="27" t="s">
+      <c r="B318" s="44" t="s">
         <v>584</v>
       </c>
       <c r="C318" s="4" t="s">
@@ -11781,7 +11687,7 @@
       <c r="A319" s="22">
         <v>304</v>
       </c>
-      <c r="B319" s="28"/>
+      <c r="B319" s="45"/>
       <c r="C319" s="4" t="s">
         <v>494</v>
       </c>
@@ -11808,7 +11714,7 @@
       <c r="A320" s="22">
         <v>305</v>
       </c>
-      <c r="B320" s="28"/>
+      <c r="B320" s="45"/>
       <c r="C320" s="4" t="s">
         <v>500</v>
       </c>
@@ -11835,7 +11741,7 @@
       <c r="A321" s="22">
         <v>306</v>
       </c>
-      <c r="B321" s="29"/>
+      <c r="B321" s="46"/>
       <c r="C321" s="4" t="s">
         <v>497</v>
       </c>
@@ -11860,76 +11766,6 @@
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="B22:B36"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="B112:B129"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="B100:B107"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="C121:C123"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="C126:C128"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="B87:B96"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="C58:C63"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C92"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B68:B76"/>
-    <mergeCell ref="B77:B86"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="C135:C137"/>
-    <mergeCell ref="C138:C143"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="B130:B145"/>
-    <mergeCell ref="C130:C132"/>
-    <mergeCell ref="B149:B155"/>
-    <mergeCell ref="C149:C152"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="B156:B159"/>
-    <mergeCell ref="B160:B174"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="C166:C167"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="C170:C172"/>
-    <mergeCell ref="B219:B228"/>
-    <mergeCell ref="C220:C222"/>
-    <mergeCell ref="C224:C226"/>
-    <mergeCell ref="C173:C174"/>
-    <mergeCell ref="B175:B178"/>
-    <mergeCell ref="C177:C178"/>
-    <mergeCell ref="B179:B182"/>
-    <mergeCell ref="B186:B190"/>
-    <mergeCell ref="B191:B201"/>
-    <mergeCell ref="B202:B206"/>
-    <mergeCell ref="B207:B218"/>
-    <mergeCell ref="C208:C210"/>
-    <mergeCell ref="C213:C215"/>
-    <mergeCell ref="C179:C182"/>
-    <mergeCell ref="C246:C249"/>
-    <mergeCell ref="B255:B264"/>
-    <mergeCell ref="C258:C260"/>
-    <mergeCell ref="B265:B270"/>
-    <mergeCell ref="B271:B279"/>
-    <mergeCell ref="C274:C276"/>
     <mergeCell ref="B318:B321"/>
     <mergeCell ref="B183:B185"/>
     <mergeCell ref="B291:B300"/>
@@ -11946,12 +11782,82 @@
     <mergeCell ref="C234:C236"/>
     <mergeCell ref="B240:B244"/>
     <mergeCell ref="B245:B254"/>
+    <mergeCell ref="C246:C249"/>
+    <mergeCell ref="B255:B264"/>
+    <mergeCell ref="C258:C260"/>
+    <mergeCell ref="B265:B270"/>
+    <mergeCell ref="B271:B279"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="B219:B228"/>
+    <mergeCell ref="C220:C222"/>
+    <mergeCell ref="C224:C226"/>
+    <mergeCell ref="C173:C174"/>
+    <mergeCell ref="B175:B178"/>
+    <mergeCell ref="C177:C178"/>
+    <mergeCell ref="B179:B182"/>
+    <mergeCell ref="B186:B190"/>
+    <mergeCell ref="B191:B201"/>
+    <mergeCell ref="B202:B206"/>
+    <mergeCell ref="B207:B218"/>
+    <mergeCell ref="C208:C210"/>
+    <mergeCell ref="C213:C215"/>
+    <mergeCell ref="C179:C182"/>
+    <mergeCell ref="B149:B155"/>
+    <mergeCell ref="C149:C152"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B156:B159"/>
+    <mergeCell ref="B160:B174"/>
+    <mergeCell ref="C161:C162"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="C166:C167"/>
+    <mergeCell ref="C168:C169"/>
+    <mergeCell ref="C170:C172"/>
+    <mergeCell ref="B77:B86"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="C138:C143"/>
+    <mergeCell ref="B146:B148"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="B130:B145"/>
+    <mergeCell ref="C130:C132"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="C58:C63"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B68:B76"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="B112:B129"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="B100:B107"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="C117:C120"/>
+    <mergeCell ref="C121:C123"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C126:C128"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="B87:B96"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C92"/>
+    <mergeCell ref="B22:B36"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 K54:K57 K59:K211">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3 K54:K57 K59:K211" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$C$2:$C$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G16:I321">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 G16:I321" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$B$1:$B$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>